<commit_message>
will test lp time
</commit_message>
<xml_diff>
--- a/stats/stats_compilation.xlsx
+++ b/stats/stats_compilation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="984" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="weights" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="30">
   <si>
     <t xml:space="preserve">stats</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t xml:space="preserve">without_lp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lp_time</t>
   </si>
   <si>
     <t xml:space="preserve">batch_size(J)</t>
@@ -114,8 +117,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="0.000000"/>
+    <numFmt numFmtId="166" formatCode="0.0000"/>
   </numFmts>
   <fonts count="4">
     <font>
@@ -182,8 +187,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -206,21 +219,20 @@
   </sheetPr>
   <dimension ref="A1:H31"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.4438775510204"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="4.86224489795918"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.1734693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="4.72448979591837"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.04591836734694"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -642,20 +654,22 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G51"/>
+  <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B18" activeCellId="0" sqref="B18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G40" activeCellId="0" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="14.9030612244898"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="13.2397959183673"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.93877551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="14.9030612244898"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="0" width="13.2397959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="8" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.8010204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.8163265306122"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.9132653061224"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.0204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.8010204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.9132653061224"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="9.54591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -697,13 +711,13 @@
       <c r="B5" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="1" t="n">
         <v>0.000165</v>
       </c>
       <c r="E5" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F5" s="0" t="n">
+      <c r="F5" s="1" t="n">
         <f aca="false">AVERAGE(C5,C10,C15,C20,C25)</f>
         <v>0.0001382</v>
       </c>
@@ -715,13 +729,13 @@
       <c r="B6" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
         <v>0.000167</v>
       </c>
       <c r="E6" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="F6" s="0" t="n">
+      <c r="F6" s="1" t="n">
         <f aca="false">AVERAGE(C6,C11,C16,C21,C26)</f>
         <v>0.000157</v>
       </c>
@@ -733,13 +747,13 @@
       <c r="B7" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7" s="1" t="n">
         <v>0.000192</v>
       </c>
       <c r="E7" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="F7" s="0" t="n">
+      <c r="F7" s="1" t="n">
         <f aca="false">AVERAGE(C7,C12,C17,C22,C27)</f>
         <v>0.0001812</v>
       </c>
@@ -751,13 +765,13 @@
       <c r="B8" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8" s="1" t="n">
         <v>0.000193</v>
       </c>
       <c r="E8" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="F8" s="0" t="n">
+      <c r="F8" s="1" t="n">
         <f aca="false">AVERAGE(C8,C13,C18,C23,C28)</f>
         <v>0.0001964</v>
       </c>
@@ -769,13 +783,13 @@
       <c r="B9" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9" s="1" t="n">
         <v>0.000388</v>
       </c>
       <c r="E9" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="F9" s="0" t="n">
+      <c r="F9" s="1" t="n">
         <f aca="false">AVERAGE(C9,C14,C19,C24,C29)</f>
         <v>0.0003564</v>
       </c>
@@ -787,7 +801,7 @@
       <c r="B10" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10" s="1" t="n">
         <v>0.000128</v>
       </c>
     </row>
@@ -798,7 +812,7 @@
       <c r="B11" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11" s="1" t="n">
         <v>0.000153</v>
       </c>
       <c r="E11" s="0" t="s">
@@ -815,13 +829,13 @@
       <c r="B12" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12" s="1" t="n">
         <v>0.00017</v>
       </c>
       <c r="E12" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="F12" s="0" t="n">
+      <c r="F12" s="1" t="n">
         <f aca="false">AVERAGE(C4:C9)</f>
         <v>0.000221</v>
       </c>
@@ -833,13 +847,13 @@
       <c r="B13" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="C13" s="1" t="n">
         <v>0.000195</v>
       </c>
       <c r="E13" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="F13" s="0" t="n">
+      <c r="F13" s="1" t="n">
         <f aca="false">AVERAGE(C10:C14)</f>
         <v>0.0002022</v>
       </c>
@@ -851,13 +865,13 @@
       <c r="B14" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="C14" s="1" t="n">
         <v>0.000365</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="F14" s="0" t="n">
+      <c r="F14" s="1" t="n">
         <f aca="false">AVERAGE(C15:C19)</f>
         <v>0.000198</v>
       </c>
@@ -869,13 +883,13 @@
       <c r="B15" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C15" s="0" t="n">
+      <c r="C15" s="1" t="n">
         <v>0.000123</v>
       </c>
       <c r="E15" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="F15" s="0" t="n">
+      <c r="F15" s="1" t="n">
         <f aca="false">AVERAGE(C20:C24)</f>
         <v>0.0002184</v>
       </c>
@@ -887,13 +901,13 @@
       <c r="B16" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C16" s="0" t="n">
+      <c r="C16" s="1" t="n">
         <v>0.000156</v>
       </c>
       <c r="E16" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="F16" s="0" t="n">
+      <c r="F16" s="1" t="n">
         <f aca="false">AVERAGE(C25:C29)</f>
         <v>0.0001896</v>
       </c>
@@ -905,7 +919,7 @@
       <c r="B17" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C17" s="0" t="n">
+      <c r="C17" s="1" t="n">
         <v>0.000181</v>
       </c>
     </row>
@@ -916,7 +930,7 @@
       <c r="B18" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C18" s="0" t="n">
+      <c r="C18" s="1" t="n">
         <v>0.000187</v>
       </c>
     </row>
@@ -927,7 +941,7 @@
       <c r="B19" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C19" s="0" t="n">
+      <c r="C19" s="1" t="n">
         <v>0.000343</v>
       </c>
     </row>
@@ -938,7 +952,7 @@
       <c r="B20" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C20" s="0" t="n">
+      <c r="C20" s="1" t="n">
         <v>0.000144</v>
       </c>
     </row>
@@ -949,7 +963,7 @@
       <c r="B21" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C21" s="0" t="n">
+      <c r="C21" s="1" t="n">
         <v>0.000153</v>
       </c>
     </row>
@@ -960,7 +974,7 @@
       <c r="B22" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C22" s="0" t="n">
+      <c r="C22" s="1" t="n">
         <v>0.000202</v>
       </c>
     </row>
@@ -971,7 +985,7 @@
       <c r="B23" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C23" s="0" t="n">
+      <c r="C23" s="1" t="n">
         <v>0.000228</v>
       </c>
     </row>
@@ -982,7 +996,7 @@
       <c r="B24" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C24" s="0" t="n">
+      <c r="C24" s="1" t="n">
         <v>0.000365</v>
       </c>
     </row>
@@ -993,7 +1007,7 @@
       <c r="B25" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="C25" s="0" t="n">
+      <c r="C25" s="1" t="n">
         <v>0.000131</v>
       </c>
     </row>
@@ -1004,7 +1018,7 @@
       <c r="B26" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="C26" s="0" t="n">
+      <c r="C26" s="1" t="n">
         <v>0.000156</v>
       </c>
     </row>
@@ -1015,7 +1029,7 @@
       <c r="B27" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="C27" s="0" t="n">
+      <c r="C27" s="1" t="n">
         <v>0.000161</v>
       </c>
     </row>
@@ -1026,7 +1040,7 @@
       <c r="B28" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="C28" s="0" t="n">
+      <c r="C28" s="1" t="n">
         <v>0.000179</v>
       </c>
     </row>
@@ -1037,12 +1051,12 @@
       <c r="B29" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="C29" s="0" t="n">
+      <c r="C29" s="1" t="n">
         <v>0.000321</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C30" s="0" t="n">
+      <c r="C30" s="1" t="n">
         <f aca="false">AVERAGE(C5:C29)</f>
         <v>0.00020584</v>
       </c>
@@ -1054,10 +1068,13 @@
       <c r="E32" s="0" t="s">
         <v>26</v>
       </c>
+      <c r="G32" s="0" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>3</v>
@@ -1072,6 +1089,12 @@
         <v>14</v>
       </c>
       <c r="F33" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="G33" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="H33" s="0" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1082,6 +1105,26 @@
       <c r="B34" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="C34" s="2" t="n">
+        <v>16.7756</v>
+      </c>
+      <c r="D34" s="2" t="n">
+        <v>7.8467</v>
+      </c>
+      <c r="E34" s="2" t="n">
+        <v>5.8991</v>
+      </c>
+      <c r="F34" s="2" t="n">
+        <v>1.1224</v>
+      </c>
+      <c r="G34" s="2" t="n">
+        <f aca="false">C34-E34</f>
+        <v>10.8765</v>
+      </c>
+      <c r="H34" s="2" t="n">
+        <f aca="false">D34-F34</f>
+        <v>6.7243</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
@@ -1090,6 +1133,26 @@
       <c r="B35" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="C35" s="2" t="n">
+        <v>18.2741</v>
+      </c>
+      <c r="D35" s="2" t="n">
+        <v>7.9524</v>
+      </c>
+      <c r="E35" s="2" t="n">
+        <v>5.7696</v>
+      </c>
+      <c r="F35" s="2" t="n">
+        <v>1.1043</v>
+      </c>
+      <c r="G35" s="2" t="n">
+        <f aca="false">C35-E35</f>
+        <v>12.5045</v>
+      </c>
+      <c r="H35" s="2" t="n">
+        <f aca="false">D35-F35</f>
+        <v>6.8481</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
@@ -1098,6 +1161,26 @@
       <c r="B36" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="C36" s="2" t="n">
+        <v>17.095</v>
+      </c>
+      <c r="D36" s="2" t="n">
+        <v>7.7072</v>
+      </c>
+      <c r="E36" s="2" t="n">
+        <v>6.3547</v>
+      </c>
+      <c r="F36" s="2" t="n">
+        <v>1.1154</v>
+      </c>
+      <c r="G36" s="2" t="n">
+        <f aca="false">C36-E36</f>
+        <v>10.7403</v>
+      </c>
+      <c r="H36" s="2" t="n">
+        <f aca="false">D36-F36</f>
+        <v>6.5918</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
@@ -1106,6 +1189,26 @@
       <c r="B37" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="C37" s="2" t="n">
+        <v>133.9213</v>
+      </c>
+      <c r="D37" s="2" t="n">
+        <v>47.453</v>
+      </c>
+      <c r="E37" s="2" t="n">
+        <v>9.9895</v>
+      </c>
+      <c r="F37" s="2" t="n">
+        <v>1.446</v>
+      </c>
+      <c r="G37" s="2" t="n">
+        <f aca="false">C37-E37</f>
+        <v>123.9318</v>
+      </c>
+      <c r="H37" s="2" t="n">
+        <f aca="false">D37-F37</f>
+        <v>46.007</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="n">
@@ -1114,6 +1217,26 @@
       <c r="B38" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="C38" s="2" t="n">
+        <v>135.2881</v>
+      </c>
+      <c r="D38" s="2" t="n">
+        <v>47.817</v>
+      </c>
+      <c r="E38" s="2" t="n">
+        <v>10.0232</v>
+      </c>
+      <c r="F38" s="2" t="n">
+        <v>1.4357</v>
+      </c>
+      <c r="G38" s="2" t="n">
+        <f aca="false">C38-E38</f>
+        <v>125.2649</v>
+      </c>
+      <c r="H38" s="2" t="n">
+        <f aca="false">D38-F38</f>
+        <v>46.3813</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="n">
@@ -1122,6 +1245,26 @@
       <c r="B39" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="C39" s="2" t="n">
+        <v>129.2066</v>
+      </c>
+      <c r="D39" s="2" t="n">
+        <v>47.4152</v>
+      </c>
+      <c r="E39" s="2" t="n">
+        <v>9.296</v>
+      </c>
+      <c r="F39" s="2" t="n">
+        <v>1.4497</v>
+      </c>
+      <c r="G39" s="2" t="n">
+        <f aca="false">C39-E39</f>
+        <v>119.9106</v>
+      </c>
+      <c r="H39" s="2" t="n">
+        <f aca="false">D39-F39</f>
+        <v>45.9655</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="n">
@@ -1130,6 +1273,26 @@
       <c r="B40" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="C40" s="2" t="n">
+        <v>274.0645</v>
+      </c>
+      <c r="D40" s="2" t="n">
+        <v>157.9343</v>
+      </c>
+      <c r="E40" s="2" t="n">
+        <v>14.5792</v>
+      </c>
+      <c r="F40" s="2" t="n">
+        <v>1.9266</v>
+      </c>
+      <c r="G40" s="2" t="n">
+        <f aca="false">C40-E40</f>
+        <v>259.4853</v>
+      </c>
+      <c r="H40" s="2" t="n">
+        <f aca="false">D40-F40</f>
+        <v>156.0077</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
@@ -1138,6 +1301,26 @@
       <c r="B41" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="C41" s="2" t="n">
+        <v>273.8888</v>
+      </c>
+      <c r="D41" s="2" t="n">
+        <v>155.35</v>
+      </c>
+      <c r="E41" s="2" t="n">
+        <v>17.5104</v>
+      </c>
+      <c r="F41" s="2" t="n">
+        <v>1.9399</v>
+      </c>
+      <c r="G41" s="2" t="n">
+        <f aca="false">C41-E41</f>
+        <v>256.3784</v>
+      </c>
+      <c r="H41" s="2" t="n">
+        <f aca="false">D41-F41</f>
+        <v>153.4101</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="n">
@@ -1146,6 +1329,26 @@
       <c r="B42" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="C42" s="2" t="n">
+        <v>274.3244</v>
+      </c>
+      <c r="D42" s="2" t="n">
+        <v>157.0729</v>
+      </c>
+      <c r="E42" s="2" t="n">
+        <v>16.8252</v>
+      </c>
+      <c r="F42" s="2" t="n">
+        <v>1.9495</v>
+      </c>
+      <c r="G42" s="2" t="n">
+        <f aca="false">C42-E42</f>
+        <v>257.4992</v>
+      </c>
+      <c r="H42" s="2" t="n">
+        <f aca="false">D42-F42</f>
+        <v>155.1234</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
@@ -1154,7 +1357,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B45" s="0" t="s">
         <v>14</v>
@@ -1179,87 +1382,87 @@
       <c r="A46" s="0" t="n">
         <v>11</v>
       </c>
-      <c r="B46" s="0" t="e">
+      <c r="B46" s="2" t="n">
         <f aca="false">AVERAGE(C34:C36)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C46" s="0" t="e">
+        <v>17.3815666666667</v>
+      </c>
+      <c r="C46" s="2" t="n">
         <f aca="false">AVERAGE(D34:D36)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D46" s="0" t="e">
+        <v>7.83543333333333</v>
+      </c>
+      <c r="D46" s="2" t="n">
         <f aca="false">B46/C46</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E46" s="0" t="e">
+        <v>2.21832870336888</v>
+      </c>
+      <c r="E46" s="2" t="n">
         <f aca="false">AVERAGE(E34:E36)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F46" s="0" t="e">
+        <v>6.0078</v>
+      </c>
+      <c r="F46" s="2" t="n">
         <f aca="false">AVERAGE(F34:F36)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G46" s="0" t="e">
+        <v>1.11403333333333</v>
+      </c>
+      <c r="G46" s="2" t="n">
         <f aca="false">E46/F46</f>
-        <v>#DIV/0!</v>
+        <v>5.39283683911313</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="n">
         <v>55</v>
       </c>
-      <c r="B47" s="0" t="e">
+      <c r="B47" s="2" t="n">
         <f aca="false">AVERAGE(C37:C39)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C47" s="0" t="e">
+        <v>132.805333333333</v>
+      </c>
+      <c r="C47" s="2" t="n">
         <f aca="false">AVERAGE(D37:D39)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D47" s="0" t="e">
+        <v>47.5617333333333</v>
+      </c>
+      <c r="D47" s="2" t="n">
         <f aca="false">B47/C47</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E47" s="0" t="e">
+        <v>2.79227277951743</v>
+      </c>
+      <c r="E47" s="2" t="n">
         <f aca="false">AVERAGE(E37:E39)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F47" s="0" t="e">
+        <v>9.76956666666667</v>
+      </c>
+      <c r="F47" s="2" t="n">
         <f aca="false">AVERAGE(F37:F39)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G47" s="0" t="e">
+        <v>1.4438</v>
+      </c>
+      <c r="G47" s="2" t="n">
         <f aca="false">E47/F47</f>
-        <v>#DIV/0!</v>
+        <v>6.76656508288313</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="n">
         <v>116</v>
       </c>
-      <c r="B48" s="0" t="e">
+      <c r="B48" s="2" t="n">
         <f aca="false">AVERAGE(C40:C42)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C48" s="0" t="e">
+        <v>274.092566666667</v>
+      </c>
+      <c r="C48" s="2" t="n">
         <f aca="false">AVERAGE(D40:D42)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="D48" s="0" t="e">
+        <v>156.785733333333</v>
+      </c>
+      <c r="D48" s="2" t="n">
         <f aca="false">B48/C48</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E48" s="0" t="e">
+        <v>1.74819839049982</v>
+      </c>
+      <c r="E48" s="2" t="n">
         <f aca="false">AVERAGE(E40:E42)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="F48" s="0" t="e">
+        <v>16.3049333333333</v>
+      </c>
+      <c r="F48" s="2" t="n">
         <f aca="false">AVERAGE(F40:F42)</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G48" s="0" t="e">
+        <v>1.93866666666667</v>
+      </c>
+      <c r="G48" s="2" t="n">
         <f aca="false">E48/F48</f>
-        <v>#DIV/0!</v>
+        <v>8.41038514442916</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1272,13 +1475,13 @@
       <c r="C50" s="0" t="s">
         <v>20</v>
       </c>
+      <c r="D50" s="0" t="s">
+        <v>18</v>
+      </c>
       <c r="E50" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="G50" s="0" t="s">
         <v>20</v>
       </c>
     </row>
@@ -1286,24 +1489,24 @@
       <c r="A51" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="B51" s="0" t="e">
+      <c r="B51" s="2" t="n">
         <f aca="false">B48/B46</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="C51" s="0" t="e">
+        <v>15.7691519943542</v>
+      </c>
+      <c r="C51" s="2" t="n">
         <f aca="false">C48/C46</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="E51" s="0" t="n">
+        <v>20.0098356610781</v>
+      </c>
+      <c r="D51" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="F51" s="0" t="e">
+      <c r="E51" s="2" t="n">
+        <f aca="false">E48/E46</f>
+        <v>2.71396073992698</v>
+      </c>
+      <c r="F51" s="2" t="n">
         <f aca="false">F48/F46</f>
-        <v>#DIV/0!</v>
-      </c>
-      <c r="G51" s="0" t="e">
-        <f aca="false">G48/G46</f>
-        <v>#DIV/0!</v>
+        <v>1.74022321294994</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
minor changes in appendix, writing experiment spec section
</commit_message>
<xml_diff>
--- a/stats/stats_compilation.xlsx
+++ b/stats/stats_compilation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="weights" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,12 +21,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="31">
   <si>
     <t xml:space="preserve">stats</t>
   </si>
   <si>
     <t xml:space="preserve">find_weights</t>
+  </si>
+  <si>
+    <t xml:space="preserve">hiddenlayer</t>
   </si>
   <si>
     <t xml:space="preserve">ORIG</t>
@@ -217,22 +220,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H31"/>
+  <dimension ref="A1:Q31"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.1734693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.5561224489796"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="4.72448979591837"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.6173469387755"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1020408163265"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.9132653061224"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.75510204081633"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="5.18367346938776"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.36224489795918"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.64795918367347"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.4285714285714"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.6377551020408"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.0102040816327"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.4183673469388"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.75510204081633"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="5.18367346938776"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="8.36224489795918"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="9.64795918367347"/>
+    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -244,36 +257,66 @@
       <c r="A2" s="0" t="s">
         <v>1</v>
       </c>
+      <c r="J2" s="0" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="0" t="s">
+        <v>9</v>
+      </c>
+      <c r="G4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="J4" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="K4" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="L4" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="M4" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="0" t="s">
+      <c r="N4" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="0" t="s">
+      <c r="O4" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="H4" s="0" t="s">
+      <c r="P4" s="0" t="s">
         <v>10</v>
+      </c>
+      <c r="Q4" s="0" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -296,12 +339,37 @@
         <v>0.01</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H5" s="0" t="n">
         <f aca="false">C5+D5</f>
         <v>0.1261</v>
       </c>
+      <c r="J5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>1808.7846</v>
+      </c>
+      <c r="L5" s="0" t="n">
+        <v>0.1625</v>
+      </c>
+      <c r="M5" s="0" t="n">
+        <v>0.3124</v>
+      </c>
+      <c r="N5" s="0" t="n">
+        <v>10000</v>
+      </c>
+      <c r="O5" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="P5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q5" s="0" t="n">
+        <f aca="false">L5+M5</f>
+        <v>0.4749</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -323,12 +391,37 @@
         <v>0.01</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H6" s="0" t="n">
         <f aca="false">C6+D6</f>
         <v>0.1472</v>
       </c>
+      <c r="J6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>1806.9126</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>0.1642</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <v>0.5044</v>
+      </c>
+      <c r="N6" s="0" t="n">
+        <v>10000</v>
+      </c>
+      <c r="O6" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="P6" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q6" s="0" t="n">
+        <f aca="false">L6+M6</f>
+        <v>0.6686</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -350,12 +443,37 @@
         <v>0.01</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H7" s="0" t="n">
         <f aca="false">C7+D7</f>
         <v>0.1774</v>
       </c>
+      <c r="J7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>1803.7836</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>0.1817</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <v>0.6462</v>
+      </c>
+      <c r="N7" s="0" t="n">
+        <v>10000</v>
+      </c>
+      <c r="O7" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="P7" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q7" s="0" t="n">
+        <f aca="false">L7+M7</f>
+        <v>0.8279</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -377,12 +495,37 @@
         <v>0.01</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H8" s="0" t="n">
         <f aca="false">C8+D8</f>
         <v>0.3008</v>
       </c>
+      <c r="J8" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>1798.6844</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <v>0.0839</v>
+      </c>
+      <c r="M8" s="0" t="n">
+        <v>0.5398</v>
+      </c>
+      <c r="N8" s="0" t="n">
+        <v>10000</v>
+      </c>
+      <c r="O8" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="P8" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q8" s="0" t="n">
+        <f aca="false">L8+M8</f>
+        <v>0.6237</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
@@ -404,11 +547,36 @@
         <v>0.01</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H9" s="0" t="n">
         <f aca="false">C9+D9</f>
         <v>0.162</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>1805.5194</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>0.1366</v>
+      </c>
+      <c r="M9" s="0" t="n">
+        <v>0.4672</v>
+      </c>
+      <c r="N9" s="0" t="n">
+        <v>10000</v>
+      </c>
+      <c r="O9" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="P9" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q9" s="0" t="n">
+        <f aca="false">L9+M9</f>
+        <v>0.6038</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -428,24 +596,36 @@
         <f aca="false">AVERAGE(H5:H9)</f>
         <v>0.1827</v>
       </c>
+      <c r="L10" s="0" t="n">
+        <f aca="false">AVERAGE(L5:L9)</f>
+        <v>0.14578</v>
+      </c>
+      <c r="M10" s="0" t="n">
+        <f aca="false">AVERAGE(M5:M9)</f>
+        <v>0.494</v>
+      </c>
+      <c r="Q10" s="0" t="n">
+        <f aca="false">AVERAGE(Q5:Q9)</f>
+        <v>0.63978</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -497,6 +677,12 @@
       <c r="B17" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="C17" s="0" t="n">
+        <v>544.7114</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>61.2416</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
@@ -505,6 +691,12 @@
       <c r="B18" s="0" t="n">
         <v>2</v>
       </c>
+      <c r="C18" s="0" t="n">
+        <v>538.4962</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>60.9564</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="n">
@@ -513,6 +705,12 @@
       <c r="B19" s="0" t="n">
         <v>3</v>
       </c>
+      <c r="C19" s="0" t="n">
+        <v>537.11</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>60.8781</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
@@ -558,21 +756,21 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -596,6 +794,18 @@
       <c r="A27" s="0" t="n">
         <v>85</v>
       </c>
+      <c r="B27" s="0" t="n">
+        <f aca="false">AVERAGE(C17:C19)</f>
+        <v>540.105866666667</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <f aca="false">AVERAGE(D17:D19)</f>
+        <v>61.0253666666667</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <f aca="false">B27/C27</f>
+        <v>8.8505140758406</v>
+      </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="n">
@@ -616,13 +826,13 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -656,20 +866,19 @@
   </sheetPr>
   <dimension ref="A1:H51"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G40" activeCellId="0" sqref="G40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.8010204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.8163265306122"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="13.9132653061224"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.0204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.8010204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.9132653061224"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="9.54591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -679,29 +888,29 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" s="0" t="s">
         <v>23</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>22</v>
-      </c>
       <c r="F4" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -816,10 +1025,10 @@
         <v>0.000153</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1063,39 +1272,39 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D33" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="E33" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="E33" s="0" t="s">
-        <v>14</v>
-      </c>
       <c r="F33" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="G33" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="G33" s="0" t="s">
-        <v>14</v>
-      </c>
       <c r="H33" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1352,30 +1561,30 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C45" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="E45" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="D45" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="E45" s="0" t="s">
-        <v>14</v>
-      </c>
       <c r="F45" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1467,22 +1676,22 @@
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B50" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C50" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D50" s="0" t="s">
         <v>19</v>
       </c>
-      <c r="C50" s="0" t="s">
+      <c r="E50" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="D50" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E50" s="0" t="s">
-        <v>19</v>
-      </c>
       <c r="F50" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
writing results section, plotting result and speedup values in the report
</commit_message>
<xml_diff>
--- a/stats/stats_compilation.xlsx
+++ b/stats/stats_compilation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="weights" sheetId="1" state="visible" r:id="rId2"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="32">
   <si>
     <t xml:space="preserve">stats</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t xml:space="preserve">sum_loss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">diff_loss</t>
   </si>
   <si>
     <t xml:space="preserve">gpu</t>
@@ -220,32 +223,32 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Q31"/>
+  <dimension ref="A1:T31"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.6173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="16.1020408163265"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.9132653061224"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.75510204081633"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="5.18367346938776"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.36224489795918"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.64795918367347"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="11.4285714285714"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="10.6377551020408"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="14.0102040816327"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.4183673469388"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="7.75510204081633"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="5.18367346938776"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="8.36224489795918"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="9.64795918367347"/>
-    <col collapsed="false" hidden="false" max="1025" min="18" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.9285714285714"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.7142857142857"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="4.99489795918367"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="10" min="9" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="0" width="4.99489795918367"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="0" width="9.58673469387755"/>
+    <col collapsed="false" hidden="false" max="1025" min="19" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -257,7 +260,7 @@
       <c r="A2" s="0" t="s">
         <v>1</v>
       </c>
-      <c r="J2" s="0" t="s">
+      <c r="K2" s="0" t="s">
         <v>2</v>
       </c>
     </row>
@@ -265,7 +268,7 @@
       <c r="A3" s="0" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="0" t="s">
+      <c r="K3" s="0" t="s">
         <v>3</v>
       </c>
     </row>
@@ -294,29 +297,35 @@
       <c r="H4" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="0" t="s">
+      <c r="I4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" s="0" t="s">
         <v>4</v>
       </c>
-      <c r="K4" s="0" t="s">
+      <c r="L4" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="L4" s="0" t="s">
+      <c r="M4" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="M4" s="0" t="s">
+      <c r="N4" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="N4" s="0" t="s">
+      <c r="O4" s="0" t="s">
         <v>8</v>
       </c>
-      <c r="O4" s="0" t="s">
+      <c r="P4" s="0" t="s">
         <v>9</v>
       </c>
-      <c r="P4" s="0" t="s">
+      <c r="Q4" s="0" t="s">
         <v>10</v>
       </c>
-      <c r="Q4" s="0" t="s">
+      <c r="R4" s="0" t="s">
         <v>11</v>
+      </c>
+      <c r="S4" s="0" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -339,36 +348,52 @@
         <v>0.01</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H5" s="0" t="n">
         <f aca="false">C5+D5</f>
         <v>0.1261</v>
       </c>
+      <c r="I5" s="0" t="n">
+        <f aca="false">D5-C5</f>
+        <v>0.0579</v>
+      </c>
       <c r="J5" s="0" t="n">
-        <v>1</v>
+        <f aca="false">ABS($I$10-I5)</f>
+        <v>0.04872</v>
       </c>
       <c r="K5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="L5" s="0" t="n">
         <v>1808.7846</v>
       </c>
-      <c r="L5" s="0" t="n">
+      <c r="M5" s="0" t="n">
         <v>0.1625</v>
       </c>
-      <c r="M5" s="0" t="n">
+      <c r="N5" s="0" t="n">
         <v>0.3124</v>
       </c>
-      <c r="N5" s="0" t="n">
+      <c r="O5" s="0" t="n">
         <v>10000</v>
       </c>
-      <c r="O5" s="0" t="n">
+      <c r="P5" s="0" t="n">
         <v>0.01</v>
       </c>
-      <c r="P5" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q5" s="0" t="n">
-        <f aca="false">L5+M5</f>
+      <c r="Q5" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="R5" s="0" t="n">
+        <f aca="false">M5+N5</f>
         <v>0.4749</v>
+      </c>
+      <c r="S5" s="0" t="n">
+        <f aca="false">N5-M5</f>
+        <v>0.1499</v>
+      </c>
+      <c r="T5" s="0" t="n">
+        <f aca="false">ABS($S$10-S5)</f>
+        <v>0.19832</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -391,36 +416,52 @@
         <v>0.01</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H6" s="0" t="n">
         <f aca="false">C6+D6</f>
         <v>0.1472</v>
       </c>
+      <c r="I6" s="0" t="n">
+        <f aca="false">D6-C6</f>
+        <v>0.0826</v>
+      </c>
       <c r="J6" s="0" t="n">
-        <v>2</v>
+        <f aca="false">ABS($I$10-I6)</f>
+        <v>0.02402</v>
       </c>
       <c r="K6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="L6" s="0" t="n">
         <v>1806.9126</v>
       </c>
-      <c r="L6" s="0" t="n">
+      <c r="M6" s="0" t="n">
         <v>0.1642</v>
       </c>
-      <c r="M6" s="0" t="n">
+      <c r="N6" s="0" t="n">
         <v>0.5044</v>
       </c>
-      <c r="N6" s="0" t="n">
+      <c r="O6" s="0" t="n">
         <v>10000</v>
       </c>
-      <c r="O6" s="0" t="n">
+      <c r="P6" s="0" t="n">
         <v>0.01</v>
       </c>
-      <c r="P6" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q6" s="0" t="n">
-        <f aca="false">L6+M6</f>
+      <c r="Q6" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="R6" s="0" t="n">
+        <f aca="false">M6+N6</f>
         <v>0.6686</v>
+      </c>
+      <c r="S6" s="0" t="n">
+        <f aca="false">N6-M6</f>
+        <v>0.3402</v>
+      </c>
+      <c r="T6" s="0" t="n">
+        <f aca="false">ABS($S$10-S6)</f>
+        <v>0.00801999999999997</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -443,36 +484,52 @@
         <v>0.01</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H7" s="0" t="n">
         <f aca="false">C7+D7</f>
         <v>0.1774</v>
       </c>
+      <c r="I7" s="0" t="n">
+        <f aca="false">D7-C7</f>
+        <v>0.0496</v>
+      </c>
       <c r="J7" s="0" t="n">
-        <v>3</v>
+        <f aca="false">ABS($I$10-I7)</f>
+        <v>0.05702</v>
       </c>
       <c r="K7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="L7" s="0" t="n">
         <v>1803.7836</v>
       </c>
-      <c r="L7" s="0" t="n">
+      <c r="M7" s="0" t="n">
         <v>0.1817</v>
       </c>
-      <c r="M7" s="0" t="n">
+      <c r="N7" s="0" t="n">
         <v>0.6462</v>
       </c>
-      <c r="N7" s="0" t="n">
+      <c r="O7" s="0" t="n">
         <v>10000</v>
       </c>
-      <c r="O7" s="0" t="n">
+      <c r="P7" s="0" t="n">
         <v>0.01</v>
       </c>
-      <c r="P7" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q7" s="0" t="n">
-        <f aca="false">L7+M7</f>
+      <c r="Q7" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="R7" s="0" t="n">
+        <f aca="false">M7+N7</f>
         <v>0.8279</v>
+      </c>
+      <c r="S7" s="0" t="n">
+        <f aca="false">N7-M7</f>
+        <v>0.4645</v>
+      </c>
+      <c r="T7" s="0" t="n">
+        <f aca="false">ABS($S$10-S7)</f>
+        <v>0.11628</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -495,36 +552,52 @@
         <v>0.01</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H8" s="0" t="n">
         <f aca="false">C8+D8</f>
         <v>0.3008</v>
       </c>
+      <c r="I8" s="0" t="n">
+        <f aca="false">D8-C8</f>
+        <v>0.2452</v>
+      </c>
       <c r="J8" s="0" t="n">
+        <f aca="false">ABS($I$10-I8)</f>
+        <v>0.13858</v>
+      </c>
+      <c r="K8" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="K8" s="0" t="n">
+      <c r="L8" s="0" t="n">
         <v>1798.6844</v>
       </c>
-      <c r="L8" s="0" t="n">
+      <c r="M8" s="0" t="n">
         <v>0.0839</v>
       </c>
-      <c r="M8" s="0" t="n">
+      <c r="N8" s="0" t="n">
         <v>0.5398</v>
       </c>
-      <c r="N8" s="0" t="n">
+      <c r="O8" s="0" t="n">
         <v>10000</v>
       </c>
-      <c r="O8" s="0" t="n">
+      <c r="P8" s="0" t="n">
         <v>0.01</v>
       </c>
-      <c r="P8" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q8" s="0" t="n">
-        <f aca="false">L8+M8</f>
+      <c r="Q8" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="R8" s="0" t="n">
+        <f aca="false">M8+N8</f>
         <v>0.6237</v>
+      </c>
+      <c r="S8" s="0" t="n">
+        <f aca="false">N8-M8</f>
+        <v>0.4559</v>
+      </c>
+      <c r="T8" s="0" t="n">
+        <f aca="false">ABS($S$10-S8)</f>
+        <v>0.10768</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -547,36 +620,52 @@
         <v>0.01</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H9" s="0" t="n">
         <f aca="false">C9+D9</f>
         <v>0.162</v>
       </c>
+      <c r="I9" s="0" t="n">
+        <f aca="false">D9-C9</f>
+        <v>0.0978</v>
+      </c>
       <c r="J9" s="0" t="n">
+        <f aca="false">ABS($I$10-I9)</f>
+        <v>0.00882</v>
+      </c>
+      <c r="K9" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="K9" s="0" t="n">
+      <c r="L9" s="0" t="n">
         <v>1805.5194</v>
       </c>
-      <c r="L9" s="0" t="n">
+      <c r="M9" s="0" t="n">
         <v>0.1366</v>
       </c>
-      <c r="M9" s="0" t="n">
+      <c r="N9" s="0" t="n">
         <v>0.4672</v>
       </c>
-      <c r="N9" s="0" t="n">
+      <c r="O9" s="0" t="n">
         <v>10000</v>
       </c>
-      <c r="O9" s="0" t="n">
+      <c r="P9" s="0" t="n">
         <v>0.01</v>
       </c>
-      <c r="P9" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="Q9" s="0" t="n">
-        <f aca="false">L9+M9</f>
+      <c r="Q9" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="R9" s="0" t="n">
+        <f aca="false">M9+N9</f>
         <v>0.6038</v>
+      </c>
+      <c r="S9" s="0" t="n">
+        <f aca="false">N9-M9</f>
+        <v>0.3306</v>
+      </c>
+      <c r="T9" s="0" t="n">
+        <f aca="false">ABS($S$10-S9)</f>
+        <v>0.01762</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -596,36 +685,52 @@
         <f aca="false">AVERAGE(H5:H9)</f>
         <v>0.1827</v>
       </c>
-      <c r="L10" s="0" t="n">
-        <f aca="false">AVERAGE(L5:L9)</f>
-        <v>0.14578</v>
+      <c r="I10" s="0" t="n">
+        <f aca="false">AVERAGE(I5:I9)</f>
+        <v>0.10662</v>
+      </c>
+      <c r="J10" s="0" t="n">
+        <f aca="false">AVERAGE(J5:J9)</f>
+        <v>0.055432</v>
       </c>
       <c r="M10" s="0" t="n">
         <f aca="false">AVERAGE(M5:M9)</f>
+        <v>0.14578</v>
+      </c>
+      <c r="N10" s="0" t="n">
+        <f aca="false">AVERAGE(N5:N9)</f>
         <v>0.494</v>
       </c>
-      <c r="Q10" s="0" t="n">
-        <f aca="false">AVERAGE(Q5:Q9)</f>
+      <c r="R10" s="0" t="n">
+        <f aca="false">AVERAGE(R5:R9)</f>
         <v>0.63978</v>
+      </c>
+      <c r="S10" s="0" t="n">
+        <f aca="false">AVERAGE(S5:S9)</f>
+        <v>0.34822</v>
+      </c>
+      <c r="T10" s="0" t="n">
+        <f aca="false">AVERAGE(T5:T9)</f>
+        <v>0.089584</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>4</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -756,21 +861,21 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -826,13 +931,13 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -840,12 +945,16 @@
         <v>10</v>
       </c>
       <c r="B31" s="0" t="n">
-        <f aca="false">B28/B26</f>
-        <v>5.19246639823407</v>
+        <f aca="false">(B28-B26)/(A28-A26)</f>
+        <v>4.6645829059829</v>
       </c>
       <c r="C31" s="0" t="n">
-        <f aca="false">C28/C26</f>
-        <v>12.6696352458605</v>
+        <f aca="false">(C28-C26)/(A28-A26)</f>
+        <v>0.745891666666667</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <f aca="false">B31/C31</f>
+        <v>6.25370025492921</v>
       </c>
     </row>
   </sheetData>
@@ -864,21 +973,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G40" activeCellId="0" sqref="G40"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J51" activeCellId="0" sqref="J51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="6" min="5" style="0" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="10" min="8" style="0" width="9.31632653061224"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -888,7 +996,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -898,19 +1006,19 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B4" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="F4" s="0" t="s">
-        <v>26</v>
+      <c r="G4" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -923,13 +1031,14 @@
       <c r="C5" s="1" t="n">
         <v>0.000165</v>
       </c>
-      <c r="E5" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F5" s="1" t="n">
+      <c r="F5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G5" s="1" t="n">
         <f aca="false">AVERAGE(C5,C10,C15,C20,C25)</f>
         <v>0.0001382</v>
       </c>
+      <c r="H5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -941,13 +1050,14 @@
       <c r="C6" s="1" t="n">
         <v>0.000167</v>
       </c>
-      <c r="E6" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="F6" s="1" t="n">
+      <c r="F6" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G6" s="1" t="n">
         <f aca="false">AVERAGE(C6,C11,C16,C21,C26)</f>
         <v>0.000157</v>
       </c>
+      <c r="H6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -959,13 +1069,14 @@
       <c r="C7" s="1" t="n">
         <v>0.000192</v>
       </c>
-      <c r="E7" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="F7" s="1" t="n">
+      <c r="F7" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G7" s="1" t="n">
         <f aca="false">AVERAGE(C7,C12,C17,C22,C27)</f>
         <v>0.0001812</v>
       </c>
+      <c r="H7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -977,13 +1088,14 @@
       <c r="C8" s="1" t="n">
         <v>0.000193</v>
       </c>
-      <c r="E8" s="0" t="n">
+      <c r="F8" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="F8" s="1" t="n">
+      <c r="G8" s="1" t="n">
         <f aca="false">AVERAGE(C8,C13,C18,C23,C28)</f>
         <v>0.0001964</v>
       </c>
+      <c r="H8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
@@ -995,13 +1107,14 @@
       <c r="C9" s="1" t="n">
         <v>0.000388</v>
       </c>
-      <c r="E9" s="0" t="n">
+      <c r="F9" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="F9" s="1" t="n">
+      <c r="G9" s="1" t="n">
         <f aca="false">AVERAGE(C9,C14,C19,C24,C29)</f>
         <v>0.0003564</v>
       </c>
+      <c r="H9" s="1"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
@@ -1024,11 +1137,11 @@
       <c r="C11" s="1" t="n">
         <v>0.000153</v>
       </c>
-      <c r="E11" s="0" t="s">
-        <v>24</v>
-      </c>
       <c r="F11" s="0" t="s">
-        <v>26</v>
+        <v>25</v>
+      </c>
+      <c r="G11" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1041,13 +1154,14 @@
       <c r="C12" s="1" t="n">
         <v>0.00017</v>
       </c>
-      <c r="E12" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F12" s="1" t="n">
+      <c r="F12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G12" s="1" t="n">
         <f aca="false">AVERAGE(C4:C9)</f>
         <v>0.000221</v>
       </c>
+      <c r="H12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
@@ -1059,13 +1173,14 @@
       <c r="C13" s="1" t="n">
         <v>0.000195</v>
       </c>
-      <c r="E13" s="0" t="n">
-        <v>2</v>
-      </c>
-      <c r="F13" s="1" t="n">
+      <c r="F13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="G13" s="1" t="n">
         <f aca="false">AVERAGE(C10:C14)</f>
         <v>0.0002022</v>
       </c>
+      <c r="H13" s="1"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
@@ -1077,13 +1192,14 @@
       <c r="C14" s="1" t="n">
         <v>0.000365</v>
       </c>
-      <c r="E14" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="F14" s="1" t="n">
+      <c r="F14" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G14" s="1" t="n">
         <f aca="false">AVERAGE(C15:C19)</f>
         <v>0.000198</v>
       </c>
+      <c r="H14" s="1"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
@@ -1095,13 +1211,14 @@
       <c r="C15" s="1" t="n">
         <v>0.000123</v>
       </c>
-      <c r="E15" s="0" t="n">
+      <c r="F15" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="F15" s="1" t="n">
+      <c r="G15" s="1" t="n">
         <f aca="false">AVERAGE(C20:C24)</f>
         <v>0.0002184</v>
       </c>
+      <c r="H15" s="1"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
@@ -1113,13 +1230,14 @@
       <c r="C16" s="1" t="n">
         <v>0.000156</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="F16" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="F16" s="1" t="n">
+      <c r="G16" s="1" t="n">
         <f aca="false">AVERAGE(C25:C29)</f>
         <v>0.0001896</v>
       </c>
+      <c r="H16" s="1"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
@@ -1272,39 +1390,39 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E32" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="G32" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F32" s="0" t="s">
         <v>28</v>
+      </c>
+      <c r="I32" s="0" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>4</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="E33" s="0" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F33" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H33" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="I33" s="0" t="s">
         <v>16</v>
+      </c>
+      <c r="J33" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1320,18 +1438,20 @@
       <c r="D34" s="2" t="n">
         <v>7.8467</v>
       </c>
-      <c r="E34" s="2" t="n">
+      <c r="E34" s="2"/>
+      <c r="F34" s="2" t="n">
         <v>5.8991</v>
       </c>
-      <c r="F34" s="2" t="n">
+      <c r="G34" s="2" t="n">
         <v>1.1224</v>
       </c>
-      <c r="G34" s="2" t="n">
-        <f aca="false">C34-E34</f>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2" t="n">
+        <f aca="false">C34-F34</f>
         <v>10.8765</v>
       </c>
-      <c r="H34" s="2" t="n">
-        <f aca="false">D34-F34</f>
+      <c r="J34" s="2" t="n">
+        <f aca="false">D34-G34</f>
         <v>6.7243</v>
       </c>
     </row>
@@ -1348,18 +1468,20 @@
       <c r="D35" s="2" t="n">
         <v>7.9524</v>
       </c>
-      <c r="E35" s="2" t="n">
+      <c r="E35" s="2"/>
+      <c r="F35" s="2" t="n">
         <v>5.7696</v>
       </c>
-      <c r="F35" s="2" t="n">
+      <c r="G35" s="2" t="n">
         <v>1.1043</v>
       </c>
-      <c r="G35" s="2" t="n">
-        <f aca="false">C35-E35</f>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2" t="n">
+        <f aca="false">C35-F35</f>
         <v>12.5045</v>
       </c>
-      <c r="H35" s="2" t="n">
-        <f aca="false">D35-F35</f>
+      <c r="J35" s="2" t="n">
+        <f aca="false">D35-G35</f>
         <v>6.8481</v>
       </c>
     </row>
@@ -1376,18 +1498,20 @@
       <c r="D36" s="2" t="n">
         <v>7.7072</v>
       </c>
-      <c r="E36" s="2" t="n">
+      <c r="E36" s="2"/>
+      <c r="F36" s="2" t="n">
         <v>6.3547</v>
       </c>
-      <c r="F36" s="2" t="n">
+      <c r="G36" s="2" t="n">
         <v>1.1154</v>
       </c>
-      <c r="G36" s="2" t="n">
-        <f aca="false">C36-E36</f>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2" t="n">
+        <f aca="false">C36-F36</f>
         <v>10.7403</v>
       </c>
-      <c r="H36" s="2" t="n">
-        <f aca="false">D36-F36</f>
+      <c r="J36" s="2" t="n">
+        <f aca="false">D36-G36</f>
         <v>6.5918</v>
       </c>
     </row>
@@ -1404,18 +1528,20 @@
       <c r="D37" s="2" t="n">
         <v>47.453</v>
       </c>
-      <c r="E37" s="2" t="n">
+      <c r="E37" s="2"/>
+      <c r="F37" s="2" t="n">
         <v>9.9895</v>
       </c>
-      <c r="F37" s="2" t="n">
+      <c r="G37" s="2" t="n">
         <v>1.446</v>
       </c>
-      <c r="G37" s="2" t="n">
-        <f aca="false">C37-E37</f>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2" t="n">
+        <f aca="false">C37-F37</f>
         <v>123.9318</v>
       </c>
-      <c r="H37" s="2" t="n">
-        <f aca="false">D37-F37</f>
+      <c r="J37" s="2" t="n">
+        <f aca="false">D37-G37</f>
         <v>46.007</v>
       </c>
     </row>
@@ -1432,18 +1558,20 @@
       <c r="D38" s="2" t="n">
         <v>47.817</v>
       </c>
-      <c r="E38" s="2" t="n">
+      <c r="E38" s="2"/>
+      <c r="F38" s="2" t="n">
         <v>10.0232</v>
       </c>
-      <c r="F38" s="2" t="n">
+      <c r="G38" s="2" t="n">
         <v>1.4357</v>
       </c>
-      <c r="G38" s="2" t="n">
-        <f aca="false">C38-E38</f>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2" t="n">
+        <f aca="false">C38-F38</f>
         <v>125.2649</v>
       </c>
-      <c r="H38" s="2" t="n">
-        <f aca="false">D38-F38</f>
+      <c r="J38" s="2" t="n">
+        <f aca="false">D38-G38</f>
         <v>46.3813</v>
       </c>
     </row>
@@ -1460,18 +1588,20 @@
       <c r="D39" s="2" t="n">
         <v>47.4152</v>
       </c>
-      <c r="E39" s="2" t="n">
+      <c r="E39" s="2"/>
+      <c r="F39" s="2" t="n">
         <v>9.296</v>
       </c>
-      <c r="F39" s="2" t="n">
+      <c r="G39" s="2" t="n">
         <v>1.4497</v>
       </c>
-      <c r="G39" s="2" t="n">
-        <f aca="false">C39-E39</f>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2" t="n">
+        <f aca="false">C39-F39</f>
         <v>119.9106</v>
       </c>
-      <c r="H39" s="2" t="n">
-        <f aca="false">D39-F39</f>
+      <c r="J39" s="2" t="n">
+        <f aca="false">D39-G39</f>
         <v>45.9655</v>
       </c>
     </row>
@@ -1488,18 +1618,20 @@
       <c r="D40" s="2" t="n">
         <v>157.9343</v>
       </c>
-      <c r="E40" s="2" t="n">
+      <c r="E40" s="2"/>
+      <c r="F40" s="2" t="n">
         <v>14.5792</v>
       </c>
-      <c r="F40" s="2" t="n">
+      <c r="G40" s="2" t="n">
         <v>1.9266</v>
       </c>
-      <c r="G40" s="2" t="n">
-        <f aca="false">C40-E40</f>
+      <c r="H40" s="2"/>
+      <c r="I40" s="2" t="n">
+        <f aca="false">C40-F40</f>
         <v>259.4853</v>
       </c>
-      <c r="H40" s="2" t="n">
-        <f aca="false">D40-F40</f>
+      <c r="J40" s="2" t="n">
+        <f aca="false">D40-G40</f>
         <v>156.0077</v>
       </c>
     </row>
@@ -1516,18 +1648,20 @@
       <c r="D41" s="2" t="n">
         <v>155.35</v>
       </c>
-      <c r="E41" s="2" t="n">
+      <c r="E41" s="2"/>
+      <c r="F41" s="2" t="n">
         <v>17.5104</v>
       </c>
-      <c r="F41" s="2" t="n">
+      <c r="G41" s="2" t="n">
         <v>1.9399</v>
       </c>
-      <c r="G41" s="2" t="n">
-        <f aca="false">C41-E41</f>
+      <c r="H41" s="2"/>
+      <c r="I41" s="2" t="n">
+        <f aca="false">C41-F41</f>
         <v>256.3784</v>
       </c>
-      <c r="H41" s="2" t="n">
-        <f aca="false">D41-F41</f>
+      <c r="J41" s="2" t="n">
+        <f aca="false">D41-G41</f>
         <v>153.4101</v>
       </c>
     </row>
@@ -1544,47 +1678,52 @@
       <c r="D42" s="2" t="n">
         <v>157.0729</v>
       </c>
-      <c r="E42" s="2" t="n">
+      <c r="E42" s="2"/>
+      <c r="F42" s="2" t="n">
         <v>16.8252</v>
       </c>
-      <c r="F42" s="2" t="n">
+      <c r="G42" s="2" t="n">
         <v>1.9495</v>
       </c>
-      <c r="G42" s="2" t="n">
-        <f aca="false">C42-E42</f>
+      <c r="H42" s="2"/>
+      <c r="I42" s="2" t="n">
+        <f aca="false">C42-F42</f>
         <v>257.4992</v>
       </c>
-      <c r="H42" s="2" t="n">
-        <f aca="false">D42-F42</f>
+      <c r="J42" s="2" t="n">
+        <f aca="false">D42-G42</f>
         <v>155.1234</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B45" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C45" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D45" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="E45" s="0" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="F45" s="0" t="s">
         <v>16</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>18</v>
+        <v>17</v>
+      </c>
+      <c r="I45" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="J45" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1603,17 +1742,23 @@
         <f aca="false">B46/C46</f>
         <v>2.21832870336888</v>
       </c>
-      <c r="E46" s="2" t="n">
-        <f aca="false">AVERAGE(E34:E36)</f>
-        <v>6.0078</v>
-      </c>
+      <c r="E46" s="2"/>
       <c r="F46" s="2" t="n">
         <f aca="false">AVERAGE(F34:F36)</f>
+        <v>6.0078</v>
+      </c>
+      <c r="G46" s="2" t="n">
+        <f aca="false">AVERAGE(G34:G36)</f>
         <v>1.11403333333333</v>
       </c>
-      <c r="G46" s="2" t="n">
-        <f aca="false">E46/F46</f>
-        <v>5.39283683911313</v>
+      <c r="H46" s="2"/>
+      <c r="I46" s="2" t="n">
+        <f aca="false">AVERAGE(I34:I36)</f>
+        <v>11.3737666666667</v>
+      </c>
+      <c r="J46" s="2" t="n">
+        <f aca="false">AVERAGE(J34:J36)</f>
+        <v>6.7214</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1632,17 +1777,23 @@
         <f aca="false">B47/C47</f>
         <v>2.79227277951743</v>
       </c>
-      <c r="E47" s="2" t="n">
-        <f aca="false">AVERAGE(E37:E39)</f>
-        <v>9.76956666666667</v>
-      </c>
+      <c r="E47" s="2"/>
       <c r="F47" s="2" t="n">
         <f aca="false">AVERAGE(F37:F39)</f>
+        <v>9.76956666666667</v>
+      </c>
+      <c r="G47" s="2" t="n">
+        <f aca="false">AVERAGE(G37:G39)</f>
         <v>1.4438</v>
       </c>
-      <c r="G47" s="2" t="n">
-        <f aca="false">E47/F47</f>
-        <v>6.76656508288313</v>
+      <c r="H47" s="2"/>
+      <c r="I47" s="2" t="n">
+        <f aca="false">AVERAGE(I37:I39)</f>
+        <v>123.035766666667</v>
+      </c>
+      <c r="J47" s="2" t="n">
+        <f aca="false">AVERAGE(J37:J39)</f>
+        <v>46.1179333333333</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1661,37 +1812,49 @@
         <f aca="false">B48/C48</f>
         <v>1.74819839049982</v>
       </c>
-      <c r="E48" s="2" t="n">
-        <f aca="false">AVERAGE(E40:E42)</f>
-        <v>16.3049333333333</v>
-      </c>
+      <c r="E48" s="2"/>
       <c r="F48" s="2" t="n">
         <f aca="false">AVERAGE(F40:F42)</f>
+        <v>16.3049333333333</v>
+      </c>
+      <c r="G48" s="2" t="n">
+        <f aca="false">AVERAGE(G40:G42)</f>
         <v>1.93866666666667</v>
       </c>
-      <c r="G48" s="2" t="n">
-        <f aca="false">E48/F48</f>
-        <v>8.41038514442916</v>
+      <c r="H48" s="2"/>
+      <c r="I48" s="2" t="n">
+        <f aca="false">AVERAGE(I40:I42)</f>
+        <v>257.787633333333</v>
+      </c>
+      <c r="J48" s="2" t="n">
+        <f aca="false">AVERAGE(J40:J42)</f>
+        <v>154.847066666667</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="E50" s="0" t="s">
         <v>20</v>
       </c>
       <c r="F50" s="0" t="s">
         <v>21</v>
+      </c>
+      <c r="G50" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="I50" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="J50" s="0" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1699,23 +1862,46 @@
         <v>10</v>
       </c>
       <c r="B51" s="2" t="n">
-        <f aca="false">B48/B46</f>
-        <v>15.7691519943542</v>
+        <f aca="false">(B48-B46)/($A$48-$A$46)</f>
+        <v>2.44486666666667</v>
       </c>
       <c r="C51" s="2" t="n">
-        <f aca="false">C48/C46</f>
-        <v>20.0098356610781</v>
+        <f aca="false">(C48-C46)/($A$48-$A$46)</f>
+        <v>1.41857428571428</v>
       </c>
       <c r="D51" s="0" t="n">
         <v>10</v>
       </c>
-      <c r="E51" s="2" t="n">
-        <f aca="false">E48/E46</f>
-        <v>2.71396073992698</v>
-      </c>
       <c r="F51" s="2" t="n">
-        <f aca="false">F48/F46</f>
-        <v>1.74022321294994</v>
+        <f aca="false">(F48-F46)/($A$48-$A$46)</f>
+        <v>0.0980679365079362</v>
+      </c>
+      <c r="G51" s="2" t="n">
+        <f aca="false">(G48-G46)/($A$48-$A$46)</f>
+        <v>0.00785365079365086</v>
+      </c>
+      <c r="H51" s="2"/>
+      <c r="I51" s="2" t="n">
+        <f aca="false">(I48-I46)/($A$48-$A$46)</f>
+        <v>2.34679873015873</v>
+      </c>
+      <c r="J51" s="2" t="n">
+        <f aca="false">(J48-J46)/($A$48-$A$46)</f>
+        <v>1.41072063492064</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D52" s="0" t="n">
+        <f aca="false">B51/C51</f>
+        <v>1.72346749217693</v>
+      </c>
+      <c r="G52" s="0" t="n">
+        <f aca="false">F51/G51</f>
+        <v>12.486923481143</v>
+      </c>
+      <c r="J52" s="0" t="n">
+        <f aca="false">I51/J51</f>
+        <v>1.66354604311204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
baseline rewards testing, pricing problem results in the report
</commit_message>
<xml_diff>
--- a/stats/stats_compilation.xlsx
+++ b/stats/stats_compilation.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="38">
   <si>
     <t xml:space="preserve">stats</t>
   </si>
@@ -95,6 +95,12 @@
     <t xml:space="preserve">find_rewards</t>
   </si>
   <si>
+    <t xml:space="preserve">BASELINES</t>
+  </si>
+  <si>
+    <t xml:space="preserve">weights_seed</t>
+  </si>
+  <si>
     <t xml:space="preserve">weight_file_seed</t>
   </si>
   <si>
@@ -105,6 +111,18 @@
   </si>
   <si>
     <t xml:space="preserve">average_loss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">proport</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rand1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rand2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rand3</t>
   </si>
   <si>
     <t xml:space="preserve">without_lp</t>
@@ -973,10 +991,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J52"/>
+  <dimension ref="A1:L52"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J51" activeCellId="0" sqref="J51"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E17" activeCellId="0" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1003,22 +1021,41 @@
       <c r="A3" s="0" t="s">
         <v>3</v>
       </c>
+      <c r="I3" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C4" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="0" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="0" t="s">
-        <v>24</v>
-      </c>
       <c r="G4" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="I4" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K4" s="0" t="n">
+        <v>0.00139</v>
+      </c>
+      <c r="L4" s="0" t="n">
+        <f aca="false">AVERAGE(K4:K8)</f>
+        <v>0.00161</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1039,6 +1076,12 @@
         <v>0.0001382</v>
       </c>
       <c r="H5" s="1"/>
+      <c r="J5" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="K5" s="0" t="n">
+        <v>0.00167</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="n">
@@ -1058,6 +1101,12 @@
         <v>0.000157</v>
       </c>
       <c r="H6" s="1"/>
+      <c r="J6" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>0.00155</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="n">
@@ -1077,6 +1126,12 @@
         <v>0.0001812</v>
       </c>
       <c r="H7" s="1"/>
+      <c r="J7" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>0.00195</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="n">
@@ -1096,6 +1151,12 @@
         <v>0.0001964</v>
       </c>
       <c r="H8" s="1"/>
+      <c r="J8" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>0.00149</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
@@ -1115,6 +1176,19 @@
         <v>0.0003564</v>
       </c>
       <c r="H9" s="1"/>
+      <c r="I9" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="J9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>0.0013</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <f aca="false">AVERAGE(K9:K23)</f>
+        <v>0.001602</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
@@ -1126,6 +1200,12 @@
       <c r="C10" s="1" t="n">
         <v>0.000128</v>
       </c>
+      <c r="J10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="K10" s="0" t="n">
+        <v>0.00149</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
@@ -1138,10 +1218,16 @@
         <v>0.000153</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
+      </c>
+      <c r="J11" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="K11" s="0" t="n">
+        <v>0.00177</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1162,6 +1248,12 @@
         <v>0.000221</v>
       </c>
       <c r="H12" s="1"/>
+      <c r="J12" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="K12" s="0" t="n">
+        <v>0.00219</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
@@ -1181,6 +1273,12 @@
         <v>0.0002022</v>
       </c>
       <c r="H13" s="1"/>
+      <c r="J13" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="K13" s="0" t="n">
+        <v>0.00145</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
@@ -1200,6 +1298,15 @@
         <v>0.000198</v>
       </c>
       <c r="H14" s="1"/>
+      <c r="I14" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="J14" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K14" s="0" t="n">
+        <v>0.00132</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
@@ -1219,6 +1326,12 @@
         <v>0.0002184</v>
       </c>
       <c r="H15" s="1"/>
+      <c r="J15" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="K15" s="0" t="n">
+        <v>0.0015</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
@@ -1238,6 +1351,12 @@
         <v>0.0001896</v>
       </c>
       <c r="H16" s="1"/>
+      <c r="J16" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="K16" s="0" t="n">
+        <v>0.00166</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="n">
@@ -1249,6 +1368,12 @@
       <c r="C17" s="1" t="n">
         <v>0.000181</v>
       </c>
+      <c r="J17" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="K17" s="0" t="n">
+        <v>0.00219</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="n">
@@ -1259,6 +1384,12 @@
       </c>
       <c r="C18" s="1" t="n">
         <v>0.000187</v>
+      </c>
+      <c r="J18" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="K18" s="0" t="n">
+        <v>0.00145</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1271,6 +1402,15 @@
       <c r="C19" s="1" t="n">
         <v>0.000343</v>
       </c>
+      <c r="I19" s="0" t="s">
+        <v>33</v>
+      </c>
+      <c r="J19" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="K19" s="0" t="n">
+        <v>0.0013</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="n">
@@ -1282,6 +1422,12 @@
       <c r="C20" s="1" t="n">
         <v>0.000144</v>
       </c>
+      <c r="J20" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="K20" s="0" t="n">
+        <v>0.00144</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
@@ -1293,6 +1439,12 @@
       <c r="C21" s="1" t="n">
         <v>0.000153</v>
       </c>
+      <c r="J21" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="K21" s="0" t="n">
+        <v>0.00167</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
@@ -1304,6 +1456,12 @@
       <c r="C22" s="1" t="n">
         <v>0.000202</v>
       </c>
+      <c r="J22" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="K22" s="0" t="n">
+        <v>0.00196</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
@@ -1314,6 +1472,12 @@
       </c>
       <c r="C23" s="1" t="n">
         <v>0.000228</v>
+      </c>
+      <c r="J23" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="K23" s="0" t="n">
+        <v>0.00134</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1393,15 +1557,15 @@
         <v>14</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="B33" s="0" t="s">
         <v>4</v>
@@ -1702,7 +1866,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
       <c r="B45" s="0" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
updated stats records with orig and rand reward results, modified bash script for testing
</commit_message>
<xml_diff>
--- a/stats/stats_compilation.xlsx
+++ b/stats/stats_compilation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="weights" sheetId="1" state="visible" r:id="rId2"/>
@@ -33,6 +33,7 @@
             <sz val="10"/>
             <rFont val="Arial"/>
             <family val="2"/>
+            <charset val="1"/>
           </rPr>
           <t xml:space="preserve">plotting the best test losses, on average results are diff</t>
         </r>
@@ -56,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="38">
   <si>
     <t xml:space="preserve">stats</t>
   </si>
@@ -119,6 +120,9 @@
   </si>
   <si>
     <t xml:space="preserve">find_rewards</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lr=0.001</t>
   </si>
   <si>
     <t xml:space="preserve">BASELINES</t>
@@ -179,7 +183,7 @@
     <numFmt numFmtId="166" formatCode="0.00000"/>
     <numFmt numFmtId="167" formatCode="0.000000"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -207,11 +211,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -307,7 +306,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -390,49 +389,85 @@
   </sheetPr>
   <dimension ref="A1:N53"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K23" activeCellId="0" sqref="K23"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.6173469387755"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.8163265306122"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.9132653061224"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.6377551020408"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.0102040816327"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.4183673469388"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="8.36224489795918"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="7.36224489795918"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.4285714285714"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.6377551020408"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="14.0102040816327"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="13.4183673469388"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="8.36224489795918"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="7.36224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="1" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="7.29081632653061"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="1" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="0"/>
+      <c r="C1" s="0"/>
+      <c r="D1" s="0"/>
+      <c r="E1" s="0"/>
+      <c r="F1" s="0"/>
+      <c r="G1" s="0"/>
+      <c r="H1" s="0"/>
+      <c r="I1" s="0"/>
+      <c r="J1" s="0"/>
+      <c r="K1" s="0"/>
+      <c r="L1" s="0"/>
+      <c r="M1" s="0"/>
+      <c r="N1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="B2" s="0"/>
+      <c r="C2" s="0"/>
+      <c r="D2" s="0"/>
+      <c r="E2" s="0"/>
+      <c r="F2" s="0"/>
+      <c r="G2" s="0"/>
+      <c r="H2" s="0"/>
       <c r="I2" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="J2" s="0"/>
+      <c r="K2" s="0"/>
+      <c r="L2" s="0"/>
+      <c r="M2" s="0"/>
+      <c r="N2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B3" s="0"/>
+      <c r="C3" s="0"/>
+      <c r="D3" s="0"/>
+      <c r="E3" s="0"/>
+      <c r="F3" s="0"/>
+      <c r="G3" s="0"/>
+      <c r="H3" s="0"/>
       <c r="I3" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="J3" s="0"/>
+      <c r="K3" s="0"/>
+      <c r="L3" s="0"/>
+      <c r="M3" s="0"/>
+      <c r="N3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -701,6 +736,9 @@
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0"/>
+      <c r="B10" s="0"/>
+      <c r="C10" s="0"/>
       <c r="D10" s="1" t="n">
         <f aca="false">AVERAGE(D5:D9)</f>
         <v>1300.55738</v>
@@ -742,6 +780,21 @@
         <v>0.089584</v>
       </c>
     </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0"/>
+      <c r="B11" s="0"/>
+      <c r="C11" s="0"/>
+      <c r="D11" s="0"/>
+      <c r="E11" s="0"/>
+      <c r="F11" s="0"/>
+      <c r="G11" s="0"/>
+      <c r="H11" s="0"/>
+      <c r="J11" s="0"/>
+      <c r="K11" s="0"/>
+      <c r="L11" s="0"/>
+      <c r="M11" s="0"/>
+      <c r="N11" s="0"/>
+    </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
         <v>1</v>
@@ -968,6 +1021,9 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0"/>
+      <c r="B17" s="0"/>
+      <c r="C17" s="0"/>
       <c r="D17" s="1" t="n">
         <f aca="false">AVERAGE(D12:D16)</f>
         <v>1224.29658</v>
@@ -1009,6 +1065,21 @@
         <v>0.04732</v>
       </c>
     </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0"/>
+      <c r="B18" s="0"/>
+      <c r="C18" s="0"/>
+      <c r="D18" s="0"/>
+      <c r="E18" s="0"/>
+      <c r="F18" s="0"/>
+      <c r="G18" s="0"/>
+      <c r="H18" s="0"/>
+      <c r="J18" s="0"/>
+      <c r="K18" s="0"/>
+      <c r="L18" s="0"/>
+      <c r="M18" s="0"/>
+      <c r="N18" s="0"/>
+    </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
         <v>1</v>
@@ -1235,6 +1306,9 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0"/>
+      <c r="B24" s="0"/>
+      <c r="C24" s="0"/>
       <c r="D24" s="1" t="n">
         <f aca="false">AVERAGE(D19:D23)</f>
         <v>1175.0596</v>
@@ -1276,6 +1350,21 @@
         <v>0.071664</v>
       </c>
     </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0"/>
+      <c r="B25" s="0"/>
+      <c r="C25" s="0"/>
+      <c r="D25" s="0"/>
+      <c r="E25" s="0"/>
+      <c r="F25" s="0"/>
+      <c r="G25" s="0"/>
+      <c r="H25" s="0"/>
+      <c r="J25" s="0"/>
+      <c r="K25" s="0"/>
+      <c r="L25" s="0"/>
+      <c r="M25" s="0"/>
+      <c r="N25" s="0"/>
+    </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
         <v>1</v>
@@ -1502,6 +1591,9 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0"/>
+      <c r="B31" s="0"/>
+      <c r="C31" s="0"/>
       <c r="D31" s="1" t="n">
         <f aca="false">AVERAGE(D26:D30)</f>
         <v>1230.32994</v>
@@ -1543,6 +1635,12 @@
         <v>0.068896</v>
       </c>
     </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0"/>
+      <c r="B32" s="0"/>
+      <c r="C32" s="0"/>
+      <c r="D32" s="0"/>
+    </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
         <v>12</v>
@@ -1691,15 +1789,25 @@
         <v>126.5676</v>
       </c>
     </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0"/>
+      <c r="B44" s="0"/>
+      <c r="C44" s="0"/>
+      <c r="D44" s="0"/>
+    </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="B45" s="0"/>
+      <c r="C45" s="0"/>
+      <c r="D45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="B46" s="0"/>
       <c r="C46" s="1" t="s">
         <v>14</v>
       </c>
@@ -1711,6 +1819,7 @@
       <c r="A47" s="1" t="n">
         <v>17</v>
       </c>
+      <c r="B47" s="0"/>
       <c r="C47" s="1" t="n">
         <f aca="false">AVERAGE(C35:C37)</f>
         <v>173.567266666667</v>
@@ -1724,6 +1833,7 @@
       <c r="A48" s="1" t="n">
         <v>85</v>
       </c>
+      <c r="B48" s="0"/>
       <c r="C48" s="1" t="n">
         <f aca="false">AVERAGE(C38:C40)</f>
         <v>540.105866666667</v>
@@ -1737,6 +1847,7 @@
       <c r="A49" s="1" t="n">
         <v>173</v>
       </c>
+      <c r="B49" s="0"/>
       <c r="C49" s="1" t="n">
         <f aca="false">AVERAGE(C41:C43)</f>
         <v>901.2422</v>
@@ -1746,7 +1857,15 @@
         <v>126.3302</v>
       </c>
     </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0"/>
+      <c r="B50" s="0"/>
+      <c r="C50" s="0"/>
+      <c r="D50" s="0"/>
+    </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0"/>
+      <c r="B51" s="0"/>
       <c r="C51" s="1" t="s">
         <v>17</v>
       </c>
@@ -1758,6 +1877,7 @@
       <c r="A52" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="B52" s="0"/>
       <c r="C52" s="1" t="n">
         <f aca="false">SLOPE(C47:C49,$A$47:$A$49)</f>
         <v>4.63769375908166</v>
@@ -1795,61 +1915,88 @@
   </sheetPr>
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H51" activeCellId="0" sqref="H51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.8010204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="13.8163265306122"/>
-    <col collapsed="false" hidden="false" max="4" min="3" style="1" width="13.9132653061224"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.8010204081633"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="1" width="13.9132653061224"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.45918367346939"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.54591836734694"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="1" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="1" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.6581632653061"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="1" width="13.6326530612245"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="1" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="0"/>
+      <c r="C1" s="0"/>
+      <c r="D1" s="0"/>
+      <c r="E1" s="0"/>
+      <c r="F1" s="0"/>
+      <c r="G1" s="0"/>
+      <c r="H1" s="0"/>
+      <c r="I1" s="0"/>
+      <c r="J1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="B2" s="0"/>
+      <c r="C2" s="0"/>
+      <c r="D2" s="0"/>
+      <c r="E2" s="0"/>
+      <c r="F2" s="0"/>
+      <c r="G2" s="0"/>
+      <c r="H2" s="0"/>
+      <c r="I2" s="0"/>
+      <c r="J2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="B3" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="C3" s="0"/>
+      <c r="D3" s="0"/>
+      <c r="E3" s="0"/>
+      <c r="F3" s="0"/>
       <c r="G3" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>22</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="I3" s="0"/>
+      <c r="J3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D4" s="0"/>
+      <c r="E4" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>23</v>
-      </c>
       <c r="F4" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="H4" s="1" t="n">
         <v>1</v>
@@ -1870,15 +2017,17 @@
         <v>1</v>
       </c>
       <c r="C5" s="7" t="n">
-        <v>0.000165</v>
-      </c>
+        <v>0.000152</v>
+      </c>
+      <c r="D5" s="0"/>
       <c r="E5" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F5" s="7" t="n">
         <f aca="false">AVERAGE(C5,C10,C15,C20,C25)</f>
-        <v>0.0001382</v>
-      </c>
+        <v>0.0001518</v>
+      </c>
+      <c r="G5" s="0"/>
       <c r="H5" s="1" t="n">
         <v>2</v>
       </c>
@@ -1895,15 +2044,17 @@
         <v>1</v>
       </c>
       <c r="C6" s="7" t="n">
-        <v>0.000167</v>
-      </c>
+        <v>7.4E-005</v>
+      </c>
+      <c r="D6" s="0"/>
       <c r="E6" s="1" t="n">
         <v>2</v>
       </c>
       <c r="F6" s="7" t="n">
         <f aca="false">AVERAGE(C6,C11,C16,C21,C26)</f>
-        <v>0.000157</v>
-      </c>
+        <v>7.88E-005</v>
+      </c>
+      <c r="G6" s="0"/>
       <c r="H6" s="1" t="n">
         <v>3</v>
       </c>
@@ -1920,15 +2071,17 @@
         <v>1</v>
       </c>
       <c r="C7" s="7" t="n">
-        <v>0.000192</v>
-      </c>
+        <v>0.000137</v>
+      </c>
+      <c r="D7" s="0"/>
       <c r="E7" s="1" t="n">
         <v>3</v>
       </c>
       <c r="F7" s="7" t="n">
         <f aca="false">AVERAGE(C7,C12,C17,C22,C27)</f>
-        <v>0.0001812</v>
-      </c>
+        <v>0.0001386</v>
+      </c>
+      <c r="G7" s="0"/>
       <c r="H7" s="1" t="n">
         <v>4</v>
       </c>
@@ -1945,15 +2098,17 @@
         <v>1</v>
       </c>
       <c r="C8" s="7" t="n">
-        <v>0.000193</v>
-      </c>
+        <v>0.000133</v>
+      </c>
+      <c r="D8" s="0"/>
       <c r="E8" s="1" t="n">
         <v>4</v>
       </c>
       <c r="F8" s="7" t="n">
         <f aca="false">AVERAGE(C8,C13,C18,C23,C28)</f>
-        <v>0.0001964</v>
-      </c>
+        <v>0.0001294</v>
+      </c>
+      <c r="G8" s="0"/>
       <c r="H8" s="1" t="n">
         <v>5</v>
       </c>
@@ -1970,17 +2125,18 @@
         <v>1</v>
       </c>
       <c r="C9" s="7" t="n">
-        <v>0.000388</v>
-      </c>
+        <v>0.000156</v>
+      </c>
+      <c r="D9" s="0"/>
       <c r="E9" s="1" t="n">
         <v>5</v>
       </c>
       <c r="F9" s="7" t="n">
         <f aca="false">AVERAGE(C9,C14,C19,C24,C29)</f>
-        <v>0.0003564</v>
+        <v>0.000155</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H9" s="1" t="n">
         <v>1</v>
@@ -2001,8 +2157,12 @@
         <v>2</v>
       </c>
       <c r="C10" s="7" t="n">
-        <v>0.000128</v>
-      </c>
+        <v>0.000151</v>
+      </c>
+      <c r="D10" s="0"/>
+      <c r="E10" s="0"/>
+      <c r="F10" s="0"/>
+      <c r="G10" s="0"/>
       <c r="H10" s="1" t="n">
         <v>2</v>
       </c>
@@ -2019,14 +2179,16 @@
         <v>2</v>
       </c>
       <c r="C11" s="7" t="n">
-        <v>0.000153</v>
-      </c>
+        <v>9E-005</v>
+      </c>
+      <c r="D11" s="0"/>
       <c r="E11" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>26</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="G11" s="0"/>
       <c r="H11" s="1" t="n">
         <v>3</v>
       </c>
@@ -2043,15 +2205,17 @@
         <v>2</v>
       </c>
       <c r="C12" s="7" t="n">
-        <v>0.00017</v>
-      </c>
+        <v>0.000141</v>
+      </c>
+      <c r="D12" s="0"/>
       <c r="E12" s="1" t="n">
         <v>1</v>
       </c>
       <c r="F12" s="7" t="n">
         <f aca="false">AVERAGE(C4:C9)</f>
-        <v>0.000221</v>
-      </c>
+        <v>0.0001304</v>
+      </c>
+      <c r="G12" s="0"/>
       <c r="H12" s="1" t="n">
         <v>4</v>
       </c>
@@ -2068,15 +2232,17 @@
         <v>2</v>
       </c>
       <c r="C13" s="7" t="n">
-        <v>0.000195</v>
-      </c>
+        <v>0.000131</v>
+      </c>
+      <c r="D13" s="0"/>
       <c r="E13" s="1" t="n">
         <v>2</v>
       </c>
       <c r="F13" s="7" t="n">
         <f aca="false">AVERAGE(C10:C14)</f>
-        <v>0.0002022</v>
-      </c>
+        <v>0.000134</v>
+      </c>
+      <c r="G13" s="0"/>
       <c r="H13" s="1" t="n">
         <v>5</v>
       </c>
@@ -2093,17 +2259,18 @@
         <v>2</v>
       </c>
       <c r="C14" s="7" t="n">
-        <v>0.000365</v>
-      </c>
+        <v>0.000157</v>
+      </c>
+      <c r="D14" s="0"/>
       <c r="E14" s="1" t="n">
         <v>3</v>
       </c>
       <c r="F14" s="7" t="n">
         <f aca="false">AVERAGE(C15:C19)</f>
-        <v>0.000198</v>
+        <v>0.0001284</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H14" s="1" t="n">
         <v>1</v>
@@ -2121,15 +2288,17 @@
         <v>3</v>
       </c>
       <c r="C15" s="7" t="n">
-        <v>0.000123</v>
-      </c>
+        <v>0.000151</v>
+      </c>
+      <c r="D15" s="0"/>
       <c r="E15" s="1" t="n">
         <v>4</v>
       </c>
       <c r="F15" s="7" t="n">
         <f aca="false">AVERAGE(C20:C24)</f>
-        <v>0.0002184</v>
-      </c>
+        <v>0.0001292</v>
+      </c>
+      <c r="G15" s="0"/>
       <c r="H15" s="1" t="n">
         <v>2</v>
       </c>
@@ -2146,15 +2315,17 @@
         <v>3</v>
       </c>
       <c r="C16" s="7" t="n">
-        <v>0.000156</v>
-      </c>
+        <v>7.9E-005</v>
+      </c>
+      <c r="D16" s="0"/>
       <c r="E16" s="1" t="n">
         <v>5</v>
       </c>
       <c r="F16" s="7" t="n">
         <f aca="false">AVERAGE(C25:C29)</f>
-        <v>0.0001896</v>
-      </c>
+        <v>0.0001316</v>
+      </c>
+      <c r="G16" s="0"/>
       <c r="H16" s="1" t="n">
         <v>3</v>
       </c>
@@ -2171,8 +2342,12 @@
         <v>3</v>
       </c>
       <c r="C17" s="7" t="n">
-        <v>0.000181</v>
-      </c>
+        <v>0.000133</v>
+      </c>
+      <c r="D17" s="0"/>
+      <c r="E17" s="0"/>
+      <c r="F17" s="0"/>
+      <c r="G17" s="0"/>
       <c r="H17" s="1" t="n">
         <v>4</v>
       </c>
@@ -2189,8 +2364,12 @@
         <v>3</v>
       </c>
       <c r="C18" s="7" t="n">
-        <v>0.000187</v>
-      </c>
+        <v>0.000128</v>
+      </c>
+      <c r="D18" s="0"/>
+      <c r="E18" s="0"/>
+      <c r="F18" s="0"/>
+      <c r="G18" s="0"/>
       <c r="H18" s="1" t="n">
         <v>5</v>
       </c>
@@ -2207,10 +2386,13 @@
         <v>3</v>
       </c>
       <c r="C19" s="7" t="n">
-        <v>0.000343</v>
-      </c>
+        <v>0.000151</v>
+      </c>
+      <c r="D19" s="0"/>
+      <c r="E19" s="0"/>
+      <c r="F19" s="0"/>
       <c r="G19" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H19" s="1" t="n">
         <v>1</v>
@@ -2228,8 +2410,12 @@
         <v>4</v>
       </c>
       <c r="C20" s="7" t="n">
-        <v>0.000144</v>
-      </c>
+        <v>0.000151</v>
+      </c>
+      <c r="D20" s="0"/>
+      <c r="E20" s="0"/>
+      <c r="F20" s="0"/>
+      <c r="G20" s="0"/>
       <c r="H20" s="1" t="n">
         <v>2</v>
       </c>
@@ -2246,8 +2432,12 @@
         <v>4</v>
       </c>
       <c r="C21" s="7" t="n">
-        <v>0.000153</v>
-      </c>
+        <v>7.1E-005</v>
+      </c>
+      <c r="D21" s="0"/>
+      <c r="E21" s="0"/>
+      <c r="F21" s="0"/>
+      <c r="G21" s="0"/>
       <c r="H21" s="1" t="n">
         <v>3</v>
       </c>
@@ -2264,8 +2454,12 @@
         <v>4</v>
       </c>
       <c r="C22" s="7" t="n">
-        <v>0.000202</v>
-      </c>
+        <v>0.000139</v>
+      </c>
+      <c r="D22" s="0"/>
+      <c r="E22" s="0"/>
+      <c r="F22" s="0"/>
+      <c r="G22" s="0"/>
       <c r="H22" s="1" t="n">
         <v>4</v>
       </c>
@@ -2282,8 +2476,12 @@
         <v>4</v>
       </c>
       <c r="C23" s="7" t="n">
-        <v>0.000228</v>
-      </c>
+        <v>0.000129</v>
+      </c>
+      <c r="D23" s="0"/>
+      <c r="E23" s="0"/>
+      <c r="F23" s="0"/>
+      <c r="G23" s="0"/>
       <c r="H23" s="1" t="n">
         <v>5</v>
       </c>
@@ -2300,8 +2498,13 @@
         <v>4</v>
       </c>
       <c r="C24" s="7" t="n">
-        <v>0.000365</v>
-      </c>
+        <v>0.000156</v>
+      </c>
+      <c r="D24" s="0"/>
+      <c r="E24" s="0"/>
+      <c r="F24" s="0"/>
+      <c r="G24" s="0"/>
+      <c r="H24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
@@ -2311,8 +2514,13 @@
         <v>5</v>
       </c>
       <c r="C25" s="7" t="n">
-        <v>0.000131</v>
-      </c>
+        <v>0.000154</v>
+      </c>
+      <c r="D25" s="0"/>
+      <c r="E25" s="0"/>
+      <c r="F25" s="0"/>
+      <c r="G25" s="0"/>
+      <c r="H25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
@@ -2322,8 +2530,13 @@
         <v>5</v>
       </c>
       <c r="C26" s="7" t="n">
-        <v>0.000156</v>
-      </c>
+        <v>8E-005</v>
+      </c>
+      <c r="D26" s="0"/>
+      <c r="E26" s="0"/>
+      <c r="F26" s="0"/>
+      <c r="G26" s="0"/>
+      <c r="H26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
@@ -2333,8 +2546,13 @@
         <v>5</v>
       </c>
       <c r="C27" s="7" t="n">
-        <v>0.000161</v>
-      </c>
+        <v>0.000143</v>
+      </c>
+      <c r="D27" s="0"/>
+      <c r="E27" s="0"/>
+      <c r="F27" s="0"/>
+      <c r="G27" s="0"/>
+      <c r="H27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
@@ -2344,8 +2562,13 @@
         <v>5</v>
       </c>
       <c r="C28" s="7" t="n">
-        <v>0.000179</v>
-      </c>
+        <v>0.000126</v>
+      </c>
+      <c r="D28" s="0"/>
+      <c r="E28" s="0"/>
+      <c r="F28" s="0"/>
+      <c r="G28" s="0"/>
+      <c r="H28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
@@ -2355,14 +2578,36 @@
         <v>5</v>
       </c>
       <c r="C29" s="7" t="n">
-        <v>0.000321</v>
-      </c>
+        <v>0.000155</v>
+      </c>
+      <c r="D29" s="0"/>
+      <c r="E29" s="0"/>
+      <c r="F29" s="0"/>
+      <c r="G29" s="0"/>
+      <c r="H29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0"/>
+      <c r="B30" s="0"/>
       <c r="C30" s="7" t="n">
         <f aca="false">MIN(C5:C29)</f>
-        <v>0.000123</v>
-      </c>
+        <v>7.1E-005</v>
+      </c>
+      <c r="D30" s="0"/>
+      <c r="E30" s="0"/>
+      <c r="F30" s="0"/>
+      <c r="G30" s="0"/>
+      <c r="H30" s="0"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0"/>
+      <c r="B31" s="0"/>
+      <c r="C31" s="0"/>
+      <c r="D31" s="0"/>
+      <c r="E31" s="0"/>
+      <c r="F31" s="0"/>
+      <c r="G31" s="0"/>
+      <c r="H31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
@@ -2370,21 +2615,21 @@
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="8" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D32" s="8"/>
       <c r="E32" s="8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F32" s="8"/>
       <c r="G32" s="8" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H32" s="8"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>4</v>
@@ -2416,24 +2661,24 @@
         <v>1</v>
       </c>
       <c r="C34" s="1" t="n">
-        <v>13.8086</v>
+        <v>13.9195</v>
       </c>
       <c r="D34" s="1" t="n">
-        <v>8.0567</v>
+        <v>8.151</v>
       </c>
       <c r="E34" s="1" t="n">
-        <v>12.5993</v>
+        <v>12.7189</v>
       </c>
       <c r="F34" s="1" t="n">
-        <v>6.6326</v>
+        <v>6.7243</v>
       </c>
       <c r="G34" s="1" t="n">
         <f aca="false">C34-E34</f>
-        <v>1.2093</v>
+        <v>1.2006</v>
       </c>
       <c r="H34" s="1" t="n">
         <f aca="false">D34-F34</f>
-        <v>1.4241</v>
+        <v>1.4267</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2444,24 +2689,24 @@
         <v>2</v>
       </c>
       <c r="C35" s="1" t="n">
-        <v>13.238</v>
+        <v>14.2646</v>
       </c>
       <c r="D35" s="1" t="n">
-        <v>8.0258</v>
+        <v>8.1344</v>
       </c>
       <c r="E35" s="1" t="n">
-        <v>12.0873</v>
+        <v>13.0006</v>
       </c>
       <c r="F35" s="1" t="n">
-        <v>6.5976</v>
+        <v>6.6935</v>
       </c>
       <c r="G35" s="1" t="n">
         <f aca="false">C35-E35</f>
-        <v>1.1507</v>
+        <v>1.264</v>
       </c>
       <c r="H35" s="1" t="n">
         <f aca="false">D35-F35</f>
-        <v>1.4282</v>
+        <v>1.4409</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2472,24 +2717,24 @@
         <v>3</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>14.0211</v>
+        <v>14.4436</v>
       </c>
       <c r="D36" s="1" t="n">
-        <v>8.0105</v>
+        <v>8.1168</v>
       </c>
       <c r="E36" s="1" t="n">
-        <v>12.7343</v>
+        <v>13.1529</v>
       </c>
       <c r="F36" s="1" t="n">
-        <v>6.5839</v>
+        <v>6.6934</v>
       </c>
       <c r="G36" s="1" t="n">
         <f aca="false">C36-E36</f>
-        <v>1.2868</v>
+        <v>1.2907</v>
       </c>
       <c r="H36" s="1" t="n">
         <f aca="false">D36-F36</f>
-        <v>1.4266</v>
+        <v>1.4234</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2500,24 +2745,24 @@
         <v>1</v>
       </c>
       <c r="C37" s="1" t="n">
-        <v>77.8923</v>
+        <v>80.3965</v>
       </c>
       <c r="D37" s="1" t="n">
-        <v>48.2504</v>
+        <v>48.0494</v>
       </c>
       <c r="E37" s="1" t="n">
-        <v>75.3074</v>
+        <v>77.837</v>
       </c>
       <c r="F37" s="1" t="n">
-        <v>46.1819</v>
+        <v>45.9833</v>
       </c>
       <c r="G37" s="1" t="n">
         <f aca="false">C37-E37</f>
-        <v>2.5849</v>
+        <v>2.5595</v>
       </c>
       <c r="H37" s="1" t="n">
         <f aca="false">D37-F37</f>
-        <v>2.0685</v>
+        <v>2.0661</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2528,24 +2773,24 @@
         <v>2</v>
       </c>
       <c r="C38" s="1" t="n">
-        <v>75.1551</v>
+        <v>82.2621</v>
       </c>
       <c r="D38" s="1" t="n">
-        <v>48.6702</v>
+        <v>47.99</v>
       </c>
       <c r="E38" s="1" t="n">
-        <v>72.67</v>
+        <v>79.559</v>
       </c>
       <c r="F38" s="1" t="n">
-        <v>46.6197</v>
+        <v>45.9413</v>
       </c>
       <c r="G38" s="1" t="n">
         <f aca="false">C38-E38</f>
-        <v>2.4851</v>
+        <v>2.70310000000001</v>
       </c>
       <c r="H38" s="1" t="n">
         <f aca="false">D38-F38</f>
-        <v>2.0505</v>
+        <v>2.0487</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2556,24 +2801,24 @@
         <v>3</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>83.7482</v>
+        <v>77.5451</v>
       </c>
       <c r="D39" s="1" t="n">
-        <v>50.2861</v>
+        <v>49.4514</v>
       </c>
       <c r="E39" s="1" t="n">
-        <v>80.9484</v>
+        <v>75.0593</v>
       </c>
       <c r="F39" s="1" t="n">
-        <v>48.2188</v>
+        <v>47.4115</v>
       </c>
       <c r="G39" s="1" t="n">
         <f aca="false">C39-E39</f>
-        <v>2.79979999999999</v>
+        <v>2.48580000000001</v>
       </c>
       <c r="H39" s="1" t="n">
         <f aca="false">D39-F39</f>
-        <v>2.0673</v>
+        <v>2.0399</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2584,24 +2829,24 @@
         <v>1</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>294.9207</v>
+        <v>299.8727</v>
       </c>
       <c r="D40" s="1" t="n">
-        <v>160.6785</v>
+        <v>163.6952</v>
       </c>
       <c r="E40" s="1" t="n">
-        <v>285.7749</v>
+        <v>290.2085</v>
       </c>
       <c r="F40" s="1" t="n">
-        <v>157.7023</v>
+        <v>160.7069</v>
       </c>
       <c r="G40" s="1" t="n">
         <f aca="false">C40-E40</f>
-        <v>9.14580000000001</v>
+        <v>9.66419999999999</v>
       </c>
       <c r="H40" s="1" t="n">
         <f aca="false">D40-F40</f>
-        <v>2.97620000000001</v>
+        <v>2.98830000000001</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2612,24 +2857,24 @@
         <v>2</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>282.7204</v>
+        <v>314.5035</v>
       </c>
       <c r="D41" s="1" t="n">
-        <v>153.5427</v>
+        <v>158.9194</v>
       </c>
       <c r="E41" s="1" t="n">
-        <v>273.5776</v>
+        <v>304.5913</v>
       </c>
       <c r="F41" s="1" t="n">
-        <v>150.5596</v>
+        <v>155.9664</v>
       </c>
       <c r="G41" s="1" t="n">
         <f aca="false">C41-E41</f>
-        <v>9.14279999999997</v>
+        <v>9.91219999999998</v>
       </c>
       <c r="H41" s="1" t="n">
         <f aca="false">D41-F41</f>
-        <v>2.98310000000001</v>
+        <v>2.953</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2640,35 +2885,53 @@
         <v>3</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>292.2481</v>
+        <v>317.9456</v>
       </c>
       <c r="D42" s="1" t="n">
-        <v>159.8252</v>
+        <v>166.705</v>
       </c>
       <c r="E42" s="1" t="n">
-        <v>282.5553</v>
+        <v>307.8481</v>
       </c>
       <c r="F42" s="1" t="n">
-        <v>156.8683</v>
+        <v>163.6936</v>
       </c>
       <c r="G42" s="1" t="n">
         <f aca="false">C42-E42</f>
-        <v>9.69280000000003</v>
+        <v>10.0975</v>
       </c>
       <c r="H42" s="1" t="n">
         <f aca="false">D42-F42</f>
-        <v>2.95689999999999</v>
-      </c>
+        <v>3.01140000000001</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0"/>
+      <c r="B43" s="0"/>
+      <c r="C43" s="0"/>
+      <c r="D43" s="0"/>
+      <c r="E43" s="0"/>
+      <c r="F43" s="0"/>
+      <c r="G43" s="0"/>
+      <c r="H43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="B44" s="0"/>
+      <c r="C44" s="0"/>
+      <c r="D44" s="0"/>
+      <c r="E44" s="0"/>
+      <c r="F44" s="0"/>
+      <c r="G44" s="0"/>
+      <c r="H44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>35</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B45" s="0"/>
       <c r="C45" s="1" t="s">
         <v>14</v>
       </c>
@@ -2692,90 +2955,105 @@
       <c r="A46" s="1" t="n">
         <v>11</v>
       </c>
+      <c r="B46" s="0"/>
       <c r="C46" s="1" t="n">
         <f aca="false">AVERAGE(C34:C36)</f>
-        <v>13.6892333333333</v>
+        <v>14.2092333333333</v>
       </c>
       <c r="D46" s="1" t="n">
         <f aca="false">AVERAGE(D34:D36)</f>
-        <v>8.031</v>
+        <v>8.13406666666667</v>
       </c>
       <c r="E46" s="1" t="n">
         <f aca="false">AVERAGE(E34:E36)</f>
-        <v>12.4736333333333</v>
+        <v>12.9574666666667</v>
       </c>
       <c r="F46" s="1" t="n">
         <f aca="false">AVERAGE(F34:F36)</f>
-        <v>6.6047</v>
+        <v>6.70373333333333</v>
       </c>
       <c r="G46" s="1" t="n">
         <f aca="false">AVERAGE(G34:G36)</f>
-        <v>1.2156</v>
+        <v>1.25176666666667</v>
       </c>
       <c r="H46" s="1" t="n">
         <f aca="false">AVERAGE(H34:H36)</f>
-        <v>1.4263</v>
+        <v>1.43033333333333</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="n">
         <v>55</v>
       </c>
+      <c r="B47" s="0"/>
       <c r="C47" s="1" t="n">
         <f aca="false">AVERAGE(C37:C39)</f>
-        <v>78.9318666666667</v>
+        <v>80.0679</v>
       </c>
       <c r="D47" s="1" t="n">
         <f aca="false">AVERAGE(D37:D39)</f>
-        <v>49.0689</v>
+        <v>48.4969333333333</v>
       </c>
       <c r="E47" s="1" t="n">
         <f aca="false">AVERAGE(E37:E39)</f>
-        <v>76.3086</v>
+        <v>77.4851</v>
       </c>
       <c r="F47" s="1" t="n">
         <f aca="false">AVERAGE(F37:F39)</f>
-        <v>47.0068</v>
+        <v>46.4453666666667</v>
       </c>
       <c r="G47" s="1" t="n">
         <f aca="false">AVERAGE(G37:G39)</f>
-        <v>2.62326666666667</v>
+        <v>2.58280000000001</v>
       </c>
       <c r="H47" s="1" t="n">
         <f aca="false">AVERAGE(H37:H39)</f>
-        <v>2.0621</v>
+        <v>2.05156666666667</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="n">
         <v>116</v>
       </c>
+      <c r="B48" s="0"/>
       <c r="C48" s="1" t="n">
         <f aca="false">AVERAGE(C40:C42)</f>
-        <v>289.963066666667</v>
+        <v>310.773933333333</v>
       </c>
       <c r="D48" s="1" t="n">
         <f aca="false">AVERAGE(D40:D42)</f>
-        <v>158.015466666667</v>
+        <v>163.106533333333</v>
       </c>
       <c r="E48" s="1" t="n">
         <f aca="false">AVERAGE(E40:E42)</f>
-        <v>280.635933333333</v>
+        <v>300.882633333333</v>
       </c>
       <c r="F48" s="1" t="n">
         <f aca="false">AVERAGE(F40:F42)</f>
-        <v>155.0434</v>
+        <v>160.1223</v>
       </c>
       <c r="G48" s="1" t="n">
         <f aca="false">AVERAGE(G40:G42)</f>
-        <v>9.32713333333334</v>
+        <v>9.8913</v>
       </c>
       <c r="H48" s="1" t="n">
         <f aca="false">AVERAGE(H40:H42)</f>
-        <v>2.97206666666667</v>
-      </c>
+        <v>2.98423333333334</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0"/>
+      <c r="B49" s="0"/>
+      <c r="C49" s="0"/>
+      <c r="D49" s="0"/>
+      <c r="E49" s="0"/>
+      <c r="F49" s="0"/>
+      <c r="G49" s="0"/>
+      <c r="H49" s="0"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0"/>
+      <c r="B50" s="0"/>
       <c r="C50" s="1" t="s">
         <v>17</v>
       </c>
@@ -2799,50 +3077,51 @@
       <c r="A51" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="B51" s="0"/>
       <c r="C51" s="1" t="n">
         <f aca="false">SLOPE(C46:C48,$A$46:$A$48)</f>
-        <v>2.68267183591096</v>
+        <v>2.88395533309355</v>
       </c>
       <c r="D51" s="1" t="n">
         <f aca="false">SLOPE(D46:D48,$A$46:$A$48)</f>
-        <v>1.45065203013228</v>
+        <v>1.50097474723255</v>
       </c>
       <c r="E51" s="1" t="n">
         <f aca="false">SLOPE(E46:E48,$A$46:$A$48)</f>
-        <v>2.60338972345442</v>
+        <v>2.79934108020621</v>
       </c>
       <c r="F51" s="1" t="n">
         <f aca="false">SLOPE(F46:F48,$A$46:$A$48)</f>
-        <v>1.43591826519602</v>
+        <v>1.48614520441194</v>
       </c>
       <c r="G51" s="1" t="n">
         <f aca="false">SLOPE(G46:G48,$A$46:$A$48)</f>
-        <v>0.07928211245654</v>
+        <v>0.0846142528873437</v>
       </c>
       <c r="H51" s="1" t="n">
         <f aca="false">SLOPE(H46:H48,$A$46:$A$48)</f>
-        <v>0.0147337649362587</v>
+        <v>0.0148295428206051</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="5" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B52" s="5"/>
       <c r="C52" s="5"/>
       <c r="D52" s="5" t="n">
         <f aca="false">C51/D51</f>
-        <v>1.84928692766269</v>
+        <v>1.92138831010376</v>
       </c>
       <c r="E52" s="5"/>
       <c r="F52" s="5" t="n">
         <f aca="false">E51/F51</f>
-        <v>1.81304868567782</v>
+        <v>1.8836255514574</v>
       </c>
       <c r="G52" s="5"/>
       <c r="H52" s="5" t="n">
         <f aca="false">G51/H51</f>
-        <v>5.38098122235091</v>
+        <v>5.70578971387946</v>
       </c>
     </row>
   </sheetData>
@@ -2851,6 +3130,30 @@
     <mergeCell ref="E32:F32"/>
     <mergeCell ref="G32:H32"/>
   </mergeCells>
+  <conditionalFormatting sqref="C5:C29">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF00CC00"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5:F9">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max" val="0"/>
+        <color rgb="FF00CC00"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FFFF0000"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
more stats, revising results section
</commit_message>
<xml_diff>
--- a/stats/stats_compilation.xlsx
+++ b/stats/stats_compilation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="weights" sheetId="1" state="visible" r:id="rId2"/>
@@ -39,7 +39,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="I12" authorId="0">
+    <comment ref="J12" authorId="0">
       <text>
         <r>
           <rPr>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="39">
   <si>
     <t xml:space="preserve">stats</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t xml:space="preserve">end_test_loss</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+-testloss</t>
   </si>
   <si>
     <t xml:space="preserve">diff_loss</t>
@@ -273,7 +276,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -286,11 +289,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -387,28 +398,30 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N53"/>
+  <dimension ref="A1:P53"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D27" activeCellId="0" sqref="D27"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E7" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M28" activeCellId="0" sqref="M28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.3928571428571"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="7.29081632653061"/>
-    <col collapsed="false" hidden="false" max="1025" min="15" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.5"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="9.4234693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="10.2602040816327"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="13.5"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="9.4234693877551"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="7.1530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="1" width="11.0714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -428,6 +441,8 @@
       <c r="L1" s="0"/>
       <c r="M1" s="0"/>
       <c r="N1" s="0"/>
+      <c r="O1" s="0"/>
+      <c r="P1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -440,14 +455,16 @@
       <c r="F2" s="0"/>
       <c r="G2" s="0"/>
       <c r="H2" s="0"/>
-      <c r="I2" s="1" t="s">
+      <c r="I2" s="0"/>
+      <c r="J2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="0"/>
       <c r="K2" s="0"/>
       <c r="L2" s="0"/>
       <c r="M2" s="0"/>
       <c r="N2" s="0"/>
+      <c r="O2" s="0"/>
+      <c r="P2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
@@ -460,14 +477,16 @@
       <c r="F3" s="0"/>
       <c r="G3" s="0"/>
       <c r="H3" s="0"/>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="0"/>
+      <c r="J3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="J3" s="0"/>
       <c r="K3" s="0"/>
       <c r="L3" s="0"/>
       <c r="M3" s="0"/>
       <c r="N3" s="0"/>
+      <c r="O3" s="0"/>
+      <c r="P3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -494,20 +513,26 @@
       <c r="H4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="I4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="K4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L4" s="1" t="s">
+      <c r="M4" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N4" s="1" t="s">
+      <c r="O4" s="1" t="s">
         <v>11</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -530,28 +555,36 @@
         <v>0.092</v>
       </c>
       <c r="G5" s="2" t="n">
+        <f aca="false">ABS($F$10-F5)</f>
+        <v>0.0765</v>
+      </c>
+      <c r="H5" s="2" t="n">
         <f aca="false">F5-E5</f>
         <v>0.0579</v>
       </c>
-      <c r="H5" s="2" t="n">
-        <f aca="false">ABS($G$10-G5)</f>
+      <c r="I5" s="2" t="n">
+        <f aca="false">ABS($H$10-H5)</f>
         <v>0.07256</v>
       </c>
-      <c r="J5" s="1" t="n">
+      <c r="K5" s="1" t="n">
         <v>1653.3931</v>
       </c>
-      <c r="K5" s="1" t="n">
+      <c r="L5" s="1" t="n">
         <v>0.1625</v>
       </c>
-      <c r="L5" s="1" t="n">
+      <c r="M5" s="1" t="n">
         <v>0.3124</v>
       </c>
-      <c r="M5" s="1" t="n">
-        <f aca="false">L5-K5</f>
+      <c r="N5" s="2" t="n">
+        <f aca="false">ABS($M$10-M5)</f>
+        <v>0.1816</v>
+      </c>
+      <c r="O5" s="1" t="n">
+        <f aca="false">M5-L5</f>
         <v>0.1499</v>
       </c>
-      <c r="N5" s="1" t="n">
-        <f aca="false">ABS($M$10-M5)</f>
+      <c r="P5" s="1" t="n">
+        <f aca="false">ABS($O$10-O5)</f>
         <v>0.19832</v>
       </c>
     </row>
@@ -574,29 +607,37 @@
       <c r="F6" s="1" t="n">
         <v>0.1149</v>
       </c>
-      <c r="G6" s="1" t="n">
+      <c r="G6" s="3" t="n">
+        <f aca="false">ABS($F$10-F6)</f>
+        <v>0.0536</v>
+      </c>
+      <c r="H6" s="1" t="n">
         <f aca="false">F6-E6</f>
         <v>0.0826</v>
       </c>
-      <c r="H6" s="1" t="n">
-        <f aca="false">ABS($G$10-G6)</f>
+      <c r="I6" s="1" t="n">
+        <f aca="false">ABS($H$10-H6)</f>
         <v>0.04786</v>
       </c>
-      <c r="J6" s="1" t="n">
+      <c r="K6" s="1" t="n">
         <v>1766.2634</v>
       </c>
-      <c r="K6" s="1" t="n">
+      <c r="L6" s="1" t="n">
         <v>0.1642</v>
       </c>
-      <c r="L6" s="1" t="n">
+      <c r="M6" s="1" t="n">
         <v>0.5044</v>
       </c>
-      <c r="M6" s="1" t="n">
-        <f aca="false">L6-K6</f>
+      <c r="N6" s="3" t="n">
+        <f aca="false">ABS($M$10-M6)</f>
+        <v>0.0104000000000001</v>
+      </c>
+      <c r="O6" s="1" t="n">
+        <f aca="false">M6-L6</f>
         <v>0.3402</v>
       </c>
-      <c r="N6" s="1" t="n">
-        <f aca="false">ABS($M$10-M6)</f>
+      <c r="P6" s="1" t="n">
+        <f aca="false">ABS($O$10-O6)</f>
         <v>0.00801999999999997</v>
       </c>
     </row>
@@ -619,29 +660,37 @@
       <c r="F7" s="1" t="n">
         <v>0.2327</v>
       </c>
-      <c r="G7" s="1" t="n">
+      <c r="G7" s="3" t="n">
+        <f aca="false">ABS($F$10-F7)</f>
+        <v>0.0642</v>
+      </c>
+      <c r="H7" s="1" t="n">
         <f aca="false">F7-E7</f>
         <v>0.1688</v>
       </c>
-      <c r="H7" s="1" t="n">
-        <f aca="false">ABS($G$10-G7)</f>
+      <c r="I7" s="1" t="n">
+        <f aca="false">ABS($H$10-H7)</f>
         <v>0.03834</v>
       </c>
-      <c r="J7" s="1" t="n">
+      <c r="K7" s="1" t="n">
         <v>1638.3491</v>
       </c>
-      <c r="K7" s="1" t="n">
+      <c r="L7" s="1" t="n">
         <v>0.1817</v>
       </c>
-      <c r="L7" s="1" t="n">
+      <c r="M7" s="1" t="n">
         <v>0.6462</v>
       </c>
-      <c r="M7" s="1" t="n">
-        <f aca="false">L7-K7</f>
+      <c r="N7" s="3" t="n">
+        <f aca="false">ABS($M$10-M7)</f>
+        <v>0.1522</v>
+      </c>
+      <c r="O7" s="1" t="n">
+        <f aca="false">M7-L7</f>
         <v>0.4645</v>
       </c>
-      <c r="N7" s="1" t="n">
-        <f aca="false">ABS($M$10-M7)</f>
+      <c r="P7" s="1" t="n">
+        <f aca="false">ABS($O$10-O7)</f>
         <v>0.11628</v>
       </c>
     </row>
@@ -664,29 +713,37 @@
       <c r="F8" s="1" t="n">
         <v>0.273</v>
       </c>
-      <c r="G8" s="1" t="n">
+      <c r="G8" s="3" t="n">
+        <f aca="false">ABS($F$10-F8)</f>
+        <v>0.1045</v>
+      </c>
+      <c r="H8" s="1" t="n">
         <f aca="false">F8-E8</f>
         <v>0.2452</v>
       </c>
-      <c r="H8" s="1" t="n">
-        <f aca="false">ABS($G$10-G8)</f>
+      <c r="I8" s="1" t="n">
+        <f aca="false">ABS($H$10-H8)</f>
         <v>0.11474</v>
       </c>
-      <c r="J8" s="1" t="n">
+      <c r="K8" s="1" t="n">
         <v>1771.6125</v>
       </c>
-      <c r="K8" s="1" t="n">
+      <c r="L8" s="1" t="n">
         <v>0.0839</v>
       </c>
-      <c r="L8" s="1" t="n">
+      <c r="M8" s="1" t="n">
         <v>0.5398</v>
       </c>
-      <c r="M8" s="1" t="n">
-        <f aca="false">L8-K8</f>
+      <c r="N8" s="3" t="n">
+        <f aca="false">ABS($M$10-M8)</f>
+        <v>0.0458000000000001</v>
+      </c>
+      <c r="O8" s="1" t="n">
+        <f aca="false">M8-L8</f>
         <v>0.4559</v>
       </c>
-      <c r="N8" s="1" t="n">
-        <f aca="false">ABS($M$10-M8)</f>
+      <c r="P8" s="1" t="n">
+        <f aca="false">ABS($O$10-O8)</f>
         <v>0.10768</v>
       </c>
     </row>
@@ -709,29 +766,37 @@
       <c r="F9" s="1" t="n">
         <v>0.1299</v>
       </c>
-      <c r="G9" s="1" t="n">
+      <c r="G9" s="3" t="n">
+        <f aca="false">ABS($F$10-F9)</f>
+        <v>0.0386</v>
+      </c>
+      <c r="H9" s="1" t="n">
         <f aca="false">F9-E9</f>
         <v>0.0978</v>
       </c>
-      <c r="H9" s="1" t="n">
-        <f aca="false">ABS($G$10-G9)</f>
+      <c r="I9" s="1" t="n">
+        <f aca="false">ABS($H$10-H9)</f>
         <v>0.03266</v>
       </c>
-      <c r="J9" s="1" t="n">
+      <c r="K9" s="1" t="n">
         <v>1834.9186</v>
       </c>
-      <c r="K9" s="1" t="n">
+      <c r="L9" s="1" t="n">
         <v>0.1366</v>
       </c>
-      <c r="L9" s="1" t="n">
+      <c r="M9" s="1" t="n">
         <v>0.4672</v>
       </c>
-      <c r="M9" s="1" t="n">
-        <f aca="false">L9-K9</f>
+      <c r="N9" s="3" t="n">
+        <f aca="false">ABS($M$10-M9)</f>
+        <v>0.0268</v>
+      </c>
+      <c r="O9" s="1" t="n">
+        <f aca="false">M9-L9</f>
         <v>0.3306</v>
       </c>
-      <c r="N9" s="1" t="n">
-        <f aca="false">ABS($M$10-M9)</f>
+      <c r="P9" s="1" t="n">
+        <f aca="false">ABS($O$10-O9)</f>
         <v>0.01762</v>
       </c>
     </row>
@@ -753,30 +818,38 @@
       </c>
       <c r="G10" s="1" t="n">
         <f aca="false">AVERAGE(G5:G9)</f>
-        <v>0.13046</v>
+        <v>0.06748</v>
       </c>
       <c r="H10" s="1" t="n">
         <f aca="false">AVERAGE(H5:H9)</f>
+        <v>0.13046</v>
+      </c>
+      <c r="I10" s="1" t="n">
+        <f aca="false">AVERAGE(I5:I9)</f>
         <v>0.061232</v>
       </c>
-      <c r="J10" s="1" t="n">
-        <f aca="false">AVERAGE(J5:J9)</f>
+      <c r="K10" s="1" t="n">
+        <f aca="false">AVERAGE(K5:K9)</f>
         <v>1732.90734</v>
       </c>
-      <c r="K10" s="3" t="n">
-        <f aca="false">AVERAGE(K5:K9)</f>
+      <c r="L10" s="4" t="n">
+        <f aca="false">AVERAGE(L5:L9)</f>
         <v>0.14578</v>
       </c>
-      <c r="L10" s="3" t="n">
-        <f aca="false">AVERAGE(L5:L9)</f>
+      <c r="M10" s="4" t="n">
+        <f aca="false">AVERAGE(M5:M9)</f>
         <v>0.494</v>
       </c>
-      <c r="M10" s="3" t="n">
-        <f aca="false">AVERAGE(M5:M9)</f>
+      <c r="N10" s="1" t="n">
+        <f aca="false">AVERAGE(N5:N9)</f>
+        <v>0.08336</v>
+      </c>
+      <c r="O10" s="4" t="n">
+        <f aca="false">AVERAGE(O5:O9)</f>
         <v>0.34822</v>
       </c>
-      <c r="N10" s="3" t="n">
-        <f aca="false">AVERAGE(N5:N9)</f>
+      <c r="P10" s="4" t="n">
+        <f aca="false">AVERAGE(P5:P9)</f>
         <v>0.089584</v>
       </c>
     </row>
@@ -789,11 +862,13 @@
       <c r="F11" s="0"/>
       <c r="G11" s="0"/>
       <c r="H11" s="0"/>
-      <c r="J11" s="0"/>
+      <c r="I11" s="0"/>
       <c r="K11" s="0"/>
       <c r="L11" s="0"/>
       <c r="M11" s="0"/>
       <c r="N11" s="0"/>
+      <c r="O11" s="0"/>
+      <c r="P11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
@@ -815,28 +890,36 @@
         <v>0.0991</v>
       </c>
       <c r="G12" s="2" t="n">
+        <f aca="false">ABS($F$17-F12)</f>
+        <v>0.01976</v>
+      </c>
+      <c r="H12" s="2" t="n">
         <f aca="false">F12-E12</f>
         <v>0.0645</v>
       </c>
-      <c r="H12" s="2" t="n">
-        <f aca="false">ABS($G$17-G12)</f>
+      <c r="I12" s="2" t="n">
+        <f aca="false">ABS($H$17-H12)</f>
         <v>0.02312</v>
       </c>
-      <c r="J12" s="1" t="n">
+      <c r="K12" s="1" t="n">
         <v>1685.7548</v>
       </c>
-      <c r="K12" s="1" t="n">
+      <c r="L12" s="1" t="n">
         <v>0.0601</v>
       </c>
-      <c r="L12" s="1" t="n">
+      <c r="M12" s="1" t="n">
         <v>0.1579</v>
       </c>
-      <c r="M12" s="1" t="n">
-        <f aca="false">L12-K12</f>
+      <c r="N12" s="2" t="n">
+        <f aca="false">ABS($M$17-M12)</f>
+        <v>0.06992</v>
+      </c>
+      <c r="O12" s="1" t="n">
+        <f aca="false">M12-L12</f>
         <v>0.0978</v>
       </c>
-      <c r="N12" s="1" t="n">
-        <f aca="false">ABS($M$17-M12)</f>
+      <c r="P12" s="1" t="n">
+        <f aca="false">ABS($O$17-O12)</f>
         <v>0.0699</v>
       </c>
     </row>
@@ -859,29 +942,37 @@
       <c r="F13" s="1" t="n">
         <v>0.1155</v>
       </c>
-      <c r="G13" s="1" t="n">
+      <c r="G13" s="3" t="n">
+        <f aca="false">ABS($F$17-F13)</f>
+        <v>0.00336</v>
+      </c>
+      <c r="H13" s="1" t="n">
         <f aca="false">F13-E13</f>
         <v>0.0828</v>
       </c>
-      <c r="H13" s="1" t="n">
-        <f aca="false">ABS($G$17-G13)</f>
+      <c r="I13" s="1" t="n">
+        <f aca="false">ABS($H$17-H13)</f>
         <v>0.00481999999999999</v>
       </c>
-      <c r="J13" s="1" t="n">
+      <c r="K13" s="1" t="n">
         <v>1623.1623</v>
       </c>
-      <c r="K13" s="1" t="n">
+      <c r="L13" s="1" t="n">
         <v>0.0918</v>
       </c>
-      <c r="L13" s="1" t="n">
+      <c r="M13" s="1" t="n">
         <v>0.2523</v>
       </c>
-      <c r="M13" s="1" t="n">
-        <f aca="false">L13-K13</f>
+      <c r="N13" s="3" t="n">
+        <f aca="false">ABS($M$17-M13)</f>
+        <v>0.02448</v>
+      </c>
+      <c r="O13" s="1" t="n">
+        <f aca="false">M13-L13</f>
         <v>0.1605</v>
       </c>
-      <c r="N13" s="1" t="n">
-        <f aca="false">ABS($M$17-M13)</f>
+      <c r="P13" s="1" t="n">
+        <f aca="false">ABS($O$17-O13)</f>
         <v>0.00719999999999998</v>
       </c>
     </row>
@@ -904,29 +995,37 @@
       <c r="F14" s="1" t="n">
         <v>0.1557</v>
       </c>
-      <c r="G14" s="1" t="n">
+      <c r="G14" s="3" t="n">
+        <f aca="false">ABS($F$17-F14)</f>
+        <v>0.03684</v>
+      </c>
+      <c r="H14" s="1" t="n">
         <f aca="false">F14-E14</f>
         <v>0.126</v>
       </c>
-      <c r="H14" s="1" t="n">
-        <f aca="false">ABS($G$17-G14)</f>
+      <c r="I14" s="1" t="n">
+        <f aca="false">ABS($H$17-H14)</f>
         <v>0.03838</v>
       </c>
-      <c r="J14" s="1" t="n">
+      <c r="K14" s="1" t="n">
         <v>1615.3793</v>
       </c>
-      <c r="K14" s="1" t="n">
+      <c r="L14" s="1" t="n">
         <v>0.0572</v>
       </c>
-      <c r="L14" s="1" t="n">
+      <c r="M14" s="1" t="n">
         <v>0.2702</v>
       </c>
-      <c r="M14" s="1" t="n">
-        <f aca="false">L14-K14</f>
+      <c r="N14" s="3" t="n">
+        <f aca="false">ABS($M$17-M14)</f>
+        <v>0.04238</v>
+      </c>
+      <c r="O14" s="1" t="n">
+        <f aca="false">M14-L14</f>
         <v>0.213</v>
       </c>
-      <c r="N14" s="1" t="n">
-        <f aca="false">ABS($M$17-M14)</f>
+      <c r="P14" s="1" t="n">
+        <f aca="false">ABS($O$17-O14)</f>
         <v>0.0453</v>
       </c>
     </row>
@@ -949,29 +1048,37 @@
       <c r="F15" s="1" t="n">
         <v>0.1032</v>
       </c>
-      <c r="G15" s="1" t="n">
+      <c r="G15" s="3" t="n">
+        <f aca="false">ABS($F$17-F15)</f>
+        <v>0.01566</v>
+      </c>
+      <c r="H15" s="1" t="n">
         <f aca="false">F15-E15</f>
         <v>0.0758</v>
       </c>
-      <c r="H15" s="1" t="n">
-        <f aca="false">ABS($G$17-G15)</f>
+      <c r="I15" s="1" t="n">
+        <f aca="false">ABS($H$17-H15)</f>
         <v>0.01182</v>
       </c>
-      <c r="J15" s="1" t="n">
+      <c r="K15" s="1" t="n">
         <v>1618.4652</v>
       </c>
-      <c r="K15" s="1" t="n">
+      <c r="L15" s="1" t="n">
         <v>0.039</v>
       </c>
-      <c r="L15" s="1" t="n">
+      <c r="M15" s="1" t="n">
         <v>0.2797</v>
       </c>
-      <c r="M15" s="1" t="n">
-        <f aca="false">L15-K15</f>
+      <c r="N15" s="3" t="n">
+        <f aca="false">ABS($M$17-M15)</f>
+        <v>0.05188</v>
+      </c>
+      <c r="O15" s="1" t="n">
+        <f aca="false">M15-L15</f>
         <v>0.2407</v>
       </c>
-      <c r="N15" s="1" t="n">
-        <f aca="false">ABS($M$17-M15)</f>
+      <c r="P15" s="1" t="n">
+        <f aca="false">ABS($O$17-O15)</f>
         <v>0.073</v>
       </c>
     </row>
@@ -994,29 +1101,37 @@
       <c r="F16" s="1" t="n">
         <v>0.1208</v>
       </c>
-      <c r="G16" s="1" t="n">
+      <c r="G16" s="3" t="n">
+        <f aca="false">ABS($F$17-F16)</f>
+        <v>0.00194</v>
+      </c>
+      <c r="H16" s="1" t="n">
         <f aca="false">F16-E16</f>
         <v>0.089</v>
       </c>
-      <c r="H16" s="1" t="n">
-        <f aca="false">ABS($G$17-G16)</f>
+      <c r="I16" s="1" t="n">
+        <f aca="false">ABS($H$17-H16)</f>
         <v>0.00137999999999999</v>
       </c>
-      <c r="J16" s="1" t="n">
+      <c r="K16" s="1" t="n">
         <v>1653.7931</v>
       </c>
-      <c r="K16" s="1" t="n">
+      <c r="L16" s="1" t="n">
         <v>0.0525</v>
       </c>
-      <c r="L16" s="1" t="n">
+      <c r="M16" s="1" t="n">
         <v>0.179</v>
       </c>
-      <c r="M16" s="1" t="n">
-        <f aca="false">L16-K16</f>
+      <c r="N16" s="3" t="n">
+        <f aca="false">ABS($M$17-M16)</f>
+        <v>0.04882</v>
+      </c>
+      <c r="O16" s="1" t="n">
+        <f aca="false">M16-L16</f>
         <v>0.1265</v>
       </c>
-      <c r="N16" s="1" t="n">
-        <f aca="false">ABS($M$17-M16)</f>
+      <c r="P16" s="1" t="n">
+        <f aca="false">ABS($O$17-O16)</f>
         <v>0.0412</v>
       </c>
     </row>
@@ -1028,40 +1143,48 @@
         <f aca="false">AVERAGE(D12:D16)</f>
         <v>1224.29658</v>
       </c>
-      <c r="E17" s="4" t="n">
+      <c r="E17" s="5" t="n">
         <f aca="false">AVERAGE(E12:E16)</f>
         <v>0.03124</v>
       </c>
-      <c r="F17" s="4" t="n">
+      <c r="F17" s="5" t="n">
         <f aca="false">AVERAGE(F12:F16)</f>
         <v>0.11886</v>
       </c>
-      <c r="G17" s="4" t="n">
+      <c r="G17" s="1" t="n">
         <f aca="false">AVERAGE(G12:G16)</f>
+        <v>0.015512</v>
+      </c>
+      <c r="H17" s="5" t="n">
+        <f aca="false">AVERAGE(H12:H16)</f>
         <v>0.08762</v>
       </c>
-      <c r="H17" s="4" t="n">
-        <f aca="false">AVERAGE(H12:H16)</f>
+      <c r="I17" s="5" t="n">
+        <f aca="false">AVERAGE(I12:I16)</f>
         <v>0.015904</v>
       </c>
-      <c r="J17" s="1" t="n">
-        <f aca="false">AVERAGE(J12:J16)</f>
+      <c r="K17" s="1" t="n">
+        <f aca="false">AVERAGE(K12:K16)</f>
         <v>1639.31094</v>
       </c>
-      <c r="K17" s="4" t="n">
-        <f aca="false">AVERAGE(K12:K16)</f>
+      <c r="L17" s="5" t="n">
+        <f aca="false">AVERAGE(L12:L16)</f>
         <v>0.06012</v>
       </c>
-      <c r="L17" s="4" t="n">
-        <f aca="false">AVERAGE(L12:L16)</f>
+      <c r="M17" s="5" t="n">
+        <f aca="false">AVERAGE(M12:M16)</f>
         <v>0.22782</v>
       </c>
-      <c r="M17" s="4" t="n">
-        <f aca="false">AVERAGE(M12:M16)</f>
+      <c r="N17" s="1" t="n">
+        <f aca="false">AVERAGE(N12:N16)</f>
+        <v>0.047496</v>
+      </c>
+      <c r="O17" s="5" t="n">
+        <f aca="false">AVERAGE(O12:O16)</f>
         <v>0.1677</v>
       </c>
-      <c r="N17" s="4" t="n">
-        <f aca="false">AVERAGE(N12:N16)</f>
+      <c r="P17" s="5" t="n">
+        <f aca="false">AVERAGE(P12:P16)</f>
         <v>0.04732</v>
       </c>
     </row>
@@ -1074,11 +1197,13 @@
       <c r="F18" s="0"/>
       <c r="G18" s="0"/>
       <c r="H18" s="0"/>
-      <c r="J18" s="0"/>
+      <c r="I18" s="0"/>
       <c r="K18" s="0"/>
       <c r="L18" s="0"/>
       <c r="M18" s="0"/>
       <c r="N18" s="0"/>
+      <c r="O18" s="0"/>
+      <c r="P18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
@@ -1100,28 +1225,36 @@
         <v>0.1037</v>
       </c>
       <c r="G19" s="2" t="n">
+        <f aca="false">ABS($F$24-F19)</f>
+        <v>0.04722</v>
+      </c>
+      <c r="H19" s="2" t="n">
         <f aca="false">F19-E19</f>
         <v>0.0648</v>
       </c>
-      <c r="H19" s="2" t="n">
-        <f aca="false">ABS($G$24-G19)</f>
+      <c r="I19" s="2" t="n">
+        <f aca="false">ABS($H$24-H19)</f>
         <v>0.05188</v>
       </c>
-      <c r="J19" s="1" t="n">
+      <c r="K19" s="1" t="n">
         <v>1684.8748</v>
       </c>
-      <c r="K19" s="1" t="n">
+      <c r="L19" s="1" t="n">
         <v>0.0653</v>
       </c>
-      <c r="L19" s="1" t="n">
+      <c r="M19" s="1" t="n">
         <v>0.1948</v>
       </c>
-      <c r="M19" s="1" t="n">
-        <f aca="false">L19-K19</f>
+      <c r="N19" s="2" t="n">
+        <f aca="false">ABS($M$24-M19)</f>
+        <v>0.04212</v>
+      </c>
+      <c r="O19" s="1" t="n">
+        <f aca="false">M19-L19</f>
         <v>0.1295</v>
       </c>
-      <c r="N19" s="1" t="n">
-        <f aca="false">ABS($M$24-M19)</f>
+      <c r="P19" s="1" t="n">
+        <f aca="false">ABS($O$24-O19)</f>
         <v>0.03912</v>
       </c>
     </row>
@@ -1144,29 +1277,37 @@
       <c r="F20" s="1" t="n">
         <v>0.1205</v>
       </c>
-      <c r="G20" s="1" t="n">
+      <c r="G20" s="3" t="n">
+        <f aca="false">ABS($F$24-F20)</f>
+        <v>0.03042</v>
+      </c>
+      <c r="H20" s="1" t="n">
         <f aca="false">F20-E20</f>
         <v>0.0846</v>
       </c>
-      <c r="H20" s="1" t="n">
-        <f aca="false">ABS($G$24-G20)</f>
+      <c r="I20" s="1" t="n">
+        <f aca="false">ABS($H$24-H20)</f>
         <v>0.03208</v>
       </c>
-      <c r="J20" s="1" t="n">
+      <c r="K20" s="1" t="n">
         <v>1633.1539</v>
       </c>
-      <c r="K20" s="1" t="n">
+      <c r="L20" s="1" t="n">
         <v>0.0931</v>
       </c>
-      <c r="L20" s="1" t="n">
+      <c r="M20" s="1" t="n">
         <v>0.1447</v>
       </c>
-      <c r="M20" s="1" t="n">
-        <f aca="false">L20-K20</f>
+      <c r="N20" s="3" t="n">
+        <f aca="false">ABS($M$24-M20)</f>
+        <v>0.09222</v>
+      </c>
+      <c r="O20" s="1" t="n">
+        <f aca="false">M20-L20</f>
         <v>0.0516</v>
       </c>
-      <c r="N20" s="1" t="n">
-        <f aca="false">ABS($M$24-M20)</f>
+      <c r="P20" s="1" t="n">
+        <f aca="false">ABS($O$24-O20)</f>
         <v>0.11702</v>
       </c>
     </row>
@@ -1189,29 +1330,37 @@
       <c r="F21" s="1" t="n">
         <v>0.1552</v>
       </c>
-      <c r="G21" s="1" t="n">
+      <c r="G21" s="3" t="n">
+        <f aca="false">ABS($F$24-F21)</f>
+        <v>0.00428000000000001</v>
+      </c>
+      <c r="H21" s="1" t="n">
         <f aca="false">F21-E21</f>
         <v>0.1239</v>
       </c>
-      <c r="H21" s="1" t="n">
-        <f aca="false">ABS($G$24-G21)</f>
+      <c r="I21" s="1" t="n">
+        <f aca="false">ABS($H$24-H21)</f>
         <v>0.00722</v>
       </c>
-      <c r="J21" s="1" t="n">
+      <c r="K21" s="1" t="n">
         <v>1671.0286</v>
       </c>
-      <c r="K21" s="1" t="n">
+      <c r="L21" s="1" t="n">
         <v>0.0816</v>
       </c>
-      <c r="L21" s="1" t="n">
+      <c r="M21" s="1" t="n">
         <v>0.3436</v>
       </c>
-      <c r="M21" s="1" t="n">
-        <f aca="false">L21-K21</f>
+      <c r="N21" s="3" t="n">
+        <f aca="false">ABS($M$24-M21)</f>
+        <v>0.10668</v>
+      </c>
+      <c r="O21" s="1" t="n">
+        <f aca="false">M21-L21</f>
         <v>0.262</v>
       </c>
-      <c r="N21" s="1" t="n">
-        <f aca="false">ABS($M$24-M21)</f>
+      <c r="P21" s="1" t="n">
+        <f aca="false">ABS($O$24-O21)</f>
         <v>0.09338</v>
       </c>
     </row>
@@ -1234,29 +1383,37 @@
       <c r="F22" s="1" t="n">
         <v>0.2459</v>
       </c>
-      <c r="G22" s="1" t="n">
+      <c r="G22" s="3" t="n">
+        <f aca="false">ABS($F$24-F22)</f>
+        <v>0.09498</v>
+      </c>
+      <c r="H22" s="1" t="n">
         <f aca="false">F22-E22</f>
         <v>0.2161</v>
       </c>
-      <c r="H22" s="1" t="n">
-        <f aca="false">ABS($G$24-G22)</f>
+      <c r="I22" s="1" t="n">
+        <f aca="false">ABS($H$24-H22)</f>
         <v>0.09942</v>
       </c>
-      <c r="J22" s="1" t="n">
+      <c r="K22" s="1" t="n">
         <v>1620.4096</v>
       </c>
-      <c r="K22" s="1" t="n">
+      <c r="L22" s="1" t="n">
         <v>0.0428</v>
       </c>
-      <c r="L22" s="1" t="n">
+      <c r="M22" s="1" t="n">
         <v>0.2972</v>
       </c>
-      <c r="M22" s="1" t="n">
-        <f aca="false">L22-K22</f>
+      <c r="N22" s="3" t="n">
+        <f aca="false">ABS($M$24-M22)</f>
+        <v>0.06028</v>
+      </c>
+      <c r="O22" s="1" t="n">
+        <f aca="false">M22-L22</f>
         <v>0.2544</v>
       </c>
-      <c r="N22" s="1" t="n">
-        <f aca="false">ABS($M$24-M22)</f>
+      <c r="P22" s="1" t="n">
+        <f aca="false">ABS($O$24-O22)</f>
         <v>0.08578</v>
       </c>
     </row>
@@ -1279,29 +1436,37 @@
       <c r="F23" s="1" t="n">
         <v>0.1293</v>
       </c>
-      <c r="G23" s="1" t="n">
+      <c r="G23" s="3" t="n">
+        <f aca="false">ABS($F$24-F23)</f>
+        <v>0.02162</v>
+      </c>
+      <c r="H23" s="1" t="n">
         <f aca="false">F23-E23</f>
         <v>0.094</v>
       </c>
-      <c r="H23" s="1" t="n">
-        <f aca="false">ABS($G$24-G23)</f>
+      <c r="I23" s="1" t="n">
+        <f aca="false">ABS($H$24-H23)</f>
         <v>0.02268</v>
       </c>
-      <c r="J23" s="1" t="n">
+      <c r="K23" s="1" t="n">
         <v>1852.252</v>
       </c>
-      <c r="K23" s="1" t="n">
+      <c r="L23" s="1" t="n">
         <v>0.0587</v>
       </c>
-      <c r="L23" s="1" t="n">
+      <c r="M23" s="1" t="n">
         <v>0.2043</v>
       </c>
-      <c r="M23" s="1" t="n">
-        <f aca="false">L23-K23</f>
+      <c r="N23" s="3" t="n">
+        <f aca="false">ABS($M$24-M23)</f>
+        <v>0.03262</v>
+      </c>
+      <c r="O23" s="1" t="n">
+        <f aca="false">M23-L23</f>
         <v>0.1456</v>
       </c>
-      <c r="N23" s="1" t="n">
-        <f aca="false">ABS($M$24-M23)</f>
+      <c r="P23" s="1" t="n">
+        <f aca="false">ABS($O$24-O23)</f>
         <v>0.02302</v>
       </c>
     </row>
@@ -1323,30 +1488,38 @@
       </c>
       <c r="G24" s="1" t="n">
         <f aca="false">AVERAGE(G19:G23)</f>
-        <v>0.11668</v>
+        <v>0.039704</v>
       </c>
       <c r="H24" s="1" t="n">
         <f aca="false">AVERAGE(H19:H23)</f>
+        <v>0.11668</v>
+      </c>
+      <c r="I24" s="1" t="n">
+        <f aca="false">AVERAGE(I19:I23)</f>
         <v>0.042656</v>
-      </c>
-      <c r="J24" s="1" t="n">
-        <f aca="false">AVERAGE(J19:J23)</f>
-        <v>1692.34378</v>
       </c>
       <c r="K24" s="1" t="n">
         <f aca="false">AVERAGE(K19:K23)</f>
-        <v>0.0683</v>
+        <v>1692.34378</v>
       </c>
       <c r="L24" s="1" t="n">
         <f aca="false">AVERAGE(L19:L23)</f>
-        <v>0.23692</v>
+        <v>0.0683</v>
       </c>
       <c r="M24" s="1" t="n">
         <f aca="false">AVERAGE(M19:M23)</f>
-        <v>0.16862</v>
+        <v>0.23692</v>
       </c>
       <c r="N24" s="1" t="n">
         <f aca="false">AVERAGE(N19:N23)</f>
+        <v>0.066784</v>
+      </c>
+      <c r="O24" s="1" t="n">
+        <f aca="false">AVERAGE(O19:O23)</f>
+        <v>0.16862</v>
+      </c>
+      <c r="P24" s="1" t="n">
+        <f aca="false">AVERAGE(P19:P23)</f>
         <v>0.071664</v>
       </c>
     </row>
@@ -1359,11 +1532,13 @@
       <c r="F25" s="0"/>
       <c r="G25" s="0"/>
       <c r="H25" s="0"/>
-      <c r="J25" s="0"/>
+      <c r="I25" s="0"/>
       <c r="K25" s="0"/>
       <c r="L25" s="0"/>
       <c r="M25" s="0"/>
       <c r="N25" s="0"/>
+      <c r="O25" s="0"/>
+      <c r="P25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
@@ -1384,29 +1559,37 @@
       <c r="F26" s="1" t="n">
         <v>0.1782</v>
       </c>
-      <c r="G26" s="1" t="n">
+      <c r="G26" s="2" t="n">
+        <f aca="false">ABS($F$31-F26)</f>
+        <v>0.03774</v>
+      </c>
+      <c r="H26" s="1" t="n">
         <f aca="false">F26-E26</f>
         <v>0.1149</v>
       </c>
-      <c r="H26" s="1" t="n">
-        <f aca="false">ABS($G$31-G26)</f>
+      <c r="I26" s="1" t="n">
+        <f aca="false">ABS($H$31-H26)</f>
         <v>0.04052</v>
       </c>
-      <c r="J26" s="1" t="n">
+      <c r="K26" s="1" t="n">
         <v>1618.4821</v>
       </c>
-      <c r="K26" s="1" t="n">
+      <c r="L26" s="1" t="n">
         <v>0.0753</v>
       </c>
-      <c r="L26" s="1" t="n">
+      <c r="M26" s="1" t="n">
         <v>0.2087</v>
       </c>
-      <c r="M26" s="1" t="n">
-        <f aca="false">L26-K26</f>
+      <c r="N26" s="2" t="n">
+        <f aca="false">ABS($M$31-M26)</f>
+        <v>0.11134</v>
+      </c>
+      <c r="O26" s="1" t="n">
+        <f aca="false">M26-L26</f>
         <v>0.1334</v>
       </c>
-      <c r="N26" s="1" t="n">
-        <f aca="false">ABS($M$31-M26)</f>
+      <c r="P26" s="1" t="n">
+        <f aca="false">ABS($O$31-O26)</f>
         <v>0.09868</v>
       </c>
     </row>
@@ -1429,29 +1612,37 @@
       <c r="F27" s="1" t="n">
         <v>0.1918</v>
       </c>
-      <c r="G27" s="1" t="n">
+      <c r="G27" s="3" t="n">
+        <f aca="false">ABS($F$31-F27)</f>
+        <v>0.02414</v>
+      </c>
+      <c r="H27" s="1" t="n">
         <f aca="false">F27-E27</f>
         <v>0.1242</v>
       </c>
-      <c r="H27" s="1" t="n">
-        <f aca="false">ABS($G$31-G27)</f>
+      <c r="I27" s="1" t="n">
+        <f aca="false">ABS($H$31-H27)</f>
         <v>0.03122</v>
       </c>
-      <c r="J27" s="1" t="n">
+      <c r="K27" s="1" t="n">
         <v>1637.5779</v>
       </c>
-      <c r="K27" s="1" t="n">
+      <c r="L27" s="1" t="n">
         <v>0.1165</v>
       </c>
-      <c r="L27" s="1" t="n">
+      <c r="M27" s="1" t="n">
         <v>0.3287</v>
       </c>
-      <c r="M27" s="1" t="n">
-        <f aca="false">L27-K27</f>
+      <c r="N27" s="3" t="n">
+        <f aca="false">ABS($M$31-M27)</f>
+        <v>0.00865999999999995</v>
+      </c>
+      <c r="O27" s="1" t="n">
+        <f aca="false">M27-L27</f>
         <v>0.2122</v>
       </c>
-      <c r="N27" s="1" t="n">
-        <f aca="false">ABS($M$31-M27)</f>
+      <c r="P27" s="1" t="n">
+        <f aca="false">ABS($O$31-O27)</f>
         <v>0.01988</v>
       </c>
     </row>
@@ -1474,29 +1665,37 @@
       <c r="F28" s="1" t="n">
         <v>0.2368</v>
       </c>
-      <c r="G28" s="1" t="n">
+      <c r="G28" s="3" t="n">
+        <f aca="false">ABS($F$31-F28)</f>
+        <v>0.02086</v>
+      </c>
+      <c r="H28" s="1" t="n">
         <f aca="false">F28-E28</f>
         <v>0.1773</v>
       </c>
-      <c r="H28" s="1" t="n">
-        <f aca="false">ABS($G$31-G28)</f>
+      <c r="I28" s="1" t="n">
+        <f aca="false">ABS($H$31-H28)</f>
         <v>0.02188</v>
       </c>
-      <c r="J28" s="1" t="n">
+      <c r="K28" s="1" t="n">
         <v>1625.8821</v>
       </c>
-      <c r="K28" s="1" t="n">
+      <c r="L28" s="1" t="n">
         <v>0.1044</v>
       </c>
-      <c r="L28" s="1" t="n">
+      <c r="M28" s="1" t="n">
         <v>0.4185</v>
       </c>
-      <c r="M28" s="1" t="n">
-        <f aca="false">L28-K28</f>
+      <c r="N28" s="3" t="n">
+        <f aca="false">ABS($M$31-M28)</f>
+        <v>0.09846</v>
+      </c>
+      <c r="O28" s="1" t="n">
+        <f aca="false">M28-L28</f>
         <v>0.3141</v>
       </c>
-      <c r="N28" s="1" t="n">
-        <f aca="false">ABS($M$31-M28)</f>
+      <c r="P28" s="1" t="n">
+        <f aca="false">ABS($O$31-O28)</f>
         <v>0.08202</v>
       </c>
     </row>
@@ -1519,29 +1718,37 @@
       <c r="F29" s="1" t="n">
         <v>0.2949</v>
       </c>
-      <c r="G29" s="1" t="n">
+      <c r="G29" s="3" t="n">
+        <f aca="false">ABS($F$31-F29)</f>
+        <v>0.07896</v>
+      </c>
+      <c r="H29" s="1" t="n">
         <f aca="false">F29-E29</f>
         <v>0.2395</v>
       </c>
-      <c r="H29" s="1" t="n">
-        <f aca="false">ABS($G$31-G29)</f>
+      <c r="I29" s="1" t="n">
+        <f aca="false">ABS($H$31-H29)</f>
         <v>0.08408</v>
       </c>
-      <c r="J29" s="1" t="n">
+      <c r="K29" s="1" t="n">
         <v>1617.4055</v>
       </c>
-      <c r="K29" s="1" t="n">
+      <c r="L29" s="1" t="n">
         <v>0.0587</v>
       </c>
-      <c r="L29" s="1" t="n">
+      <c r="M29" s="1" t="n">
         <v>0.381</v>
       </c>
-      <c r="M29" s="1" t="n">
-        <f aca="false">L29-K29</f>
+      <c r="N29" s="3" t="n">
+        <f aca="false">ABS($M$31-M29)</f>
+        <v>0.06096</v>
+      </c>
+      <c r="O29" s="1" t="n">
+        <f aca="false">M29-L29</f>
         <v>0.3223</v>
       </c>
-      <c r="N29" s="1" t="n">
-        <f aca="false">ABS($M$31-M29)</f>
+      <c r="P29" s="1" t="n">
+        <f aca="false">ABS($O$31-O29)</f>
         <v>0.09022</v>
       </c>
     </row>
@@ -1564,29 +1771,37 @@
       <c r="F30" s="2" t="n">
         <v>0.178</v>
       </c>
-      <c r="G30" s="2" t="n">
+      <c r="G30" s="3" t="n">
+        <f aca="false">ABS($F$31-F30)</f>
+        <v>0.03794</v>
+      </c>
+      <c r="H30" s="2" t="n">
         <f aca="false">F30-E30</f>
         <v>0.1212</v>
       </c>
-      <c r="H30" s="2" t="n">
-        <f aca="false">ABS($G$31-G30)</f>
+      <c r="I30" s="2" t="n">
+        <f aca="false">ABS($H$31-H30)</f>
         <v>0.03422</v>
       </c>
-      <c r="J30" s="1" t="n">
+      <c r="K30" s="1" t="n">
         <v>1742.5917</v>
       </c>
-      <c r="K30" s="1" t="n">
+      <c r="L30" s="1" t="n">
         <v>0.0849</v>
       </c>
-      <c r="L30" s="1" t="n">
+      <c r="M30" s="1" t="n">
         <v>0.2633</v>
       </c>
-      <c r="M30" s="1" t="n">
-        <f aca="false">L30-K30</f>
+      <c r="N30" s="3" t="n">
+        <f aca="false">ABS($M$31-M30)</f>
+        <v>0.05674</v>
+      </c>
+      <c r="O30" s="1" t="n">
+        <f aca="false">M30-L30</f>
         <v>0.1784</v>
       </c>
-      <c r="N30" s="1" t="n">
-        <f aca="false">ABS($M$31-M30)</f>
+      <c r="P30" s="1" t="n">
+        <f aca="false">ABS($O$31-O30)</f>
         <v>0.05368</v>
       </c>
     </row>
@@ -1598,40 +1813,48 @@
         <f aca="false">AVERAGE(D26:D30)</f>
         <v>1230.32994</v>
       </c>
-      <c r="E31" s="3" t="n">
+      <c r="E31" s="4" t="n">
         <f aca="false">AVERAGE(E26:E30)</f>
         <v>0.06052</v>
       </c>
-      <c r="F31" s="3" t="n">
+      <c r="F31" s="4" t="n">
         <f aca="false">AVERAGE(F26:F30)</f>
         <v>0.21594</v>
       </c>
-      <c r="G31" s="3" t="n">
+      <c r="G31" s="1" t="n">
         <f aca="false">AVERAGE(G26:G30)</f>
+        <v>0.039928</v>
+      </c>
+      <c r="H31" s="4" t="n">
+        <f aca="false">AVERAGE(H26:H30)</f>
         <v>0.15542</v>
       </c>
-      <c r="H31" s="3" t="n">
-        <f aca="false">AVERAGE(H26:H30)</f>
+      <c r="I31" s="4" t="n">
+        <f aca="false">AVERAGE(I26:I30)</f>
         <v>0.042384</v>
-      </c>
-      <c r="J31" s="1" t="n">
-        <f aca="false">AVERAGE(J26:J30)</f>
-        <v>1648.38786</v>
       </c>
       <c r="K31" s="1" t="n">
         <f aca="false">AVERAGE(K26:K30)</f>
-        <v>0.08796</v>
+        <v>1648.38786</v>
       </c>
       <c r="L31" s="1" t="n">
         <f aca="false">AVERAGE(L26:L30)</f>
-        <v>0.32004</v>
+        <v>0.08796</v>
       </c>
       <c r="M31" s="1" t="n">
         <f aca="false">AVERAGE(M26:M30)</f>
-        <v>0.23208</v>
+        <v>0.32004</v>
       </c>
       <c r="N31" s="1" t="n">
         <f aca="false">AVERAGE(N26:N30)</f>
+        <v>0.067232</v>
+      </c>
+      <c r="O31" s="1" t="n">
+        <f aca="false">AVERAGE(O26:O30)</f>
+        <v>0.23208</v>
+      </c>
+      <c r="P31" s="1" t="n">
+        <f aca="false">AVERAGE(P26:P30)</f>
         <v>0.068896</v>
       </c>
     </row>
@@ -1639,11 +1862,14 @@
       <c r="A32" s="0"/>
       <c r="B32" s="0"/>
       <c r="C32" s="0"/>
-      <c r="D32" s="0"/>
+      <c r="D32" s="6" t="n">
+        <f aca="false">AVERAGE(D10,D17,D24,D31)</f>
+        <v>1232.560875</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -1651,16 +1877,16 @@
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1797,7 +2023,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B45" s="0"/>
       <c r="C45" s="0"/>
@@ -1805,14 +2031,14 @@
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B46" s="0"/>
       <c r="C46" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1867,15 +2093,15 @@
       <c r="A51" s="0"/>
       <c r="B51" s="0"/>
       <c r="C51" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B52" s="0"/>
       <c r="C52" s="1" t="n">
@@ -1888,10 +2114,10 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="5"/>
-      <c r="B53" s="5"/>
-      <c r="C53" s="5"/>
-      <c r="D53" s="5" t="n">
+      <c r="A53" s="7"/>
+      <c r="B53" s="7"/>
+      <c r="C53" s="7"/>
+      <c r="D53" s="7" t="n">
         <f aca="false">C52/D52</f>
         <v>6.21916638891868</v>
       </c>
@@ -1915,19 +2141,19 @@
   </sheetPr>
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H51" activeCellId="0" sqref="H51"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D37" activeCellId="0" sqref="D37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="1" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.6581632653061"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="1" width="13.6326530612245"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.44897959183673"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="1" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="1" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.5255102040816"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="1" width="13.3622448979592"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="1" width="11.0714285714286"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1946,7 +2172,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B2" s="0"/>
       <c r="C2" s="0"/>
@@ -1963,48 +2189,48 @@
         <v>3</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C3" s="0"/>
       <c r="D3" s="0"/>
       <c r="E3" s="0"/>
       <c r="F3" s="0"/>
       <c r="G3" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="I3" s="0"/>
       <c r="J3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D4" s="0"/>
       <c r="E4" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="H4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I4" s="6" t="n">
+      <c r="I4" s="8" t="n">
         <v>0.00139</v>
       </c>
-      <c r="J4" s="6" t="n">
+      <c r="J4" s="8" t="n">
         <f aca="false">AVERAGE(I4:I8)</f>
         <v>0.00161</v>
       </c>
@@ -2016,14 +2242,14 @@
       <c r="B5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C5" s="7" t="n">
+      <c r="C5" s="9" t="n">
         <v>0.000152</v>
       </c>
       <c r="D5" s="0"/>
       <c r="E5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F5" s="7" t="n">
+      <c r="F5" s="9" t="n">
         <f aca="false">AVERAGE(C5,C10,C15,C20,C25)</f>
         <v>0.0001518</v>
       </c>
@@ -2031,10 +2257,10 @@
       <c r="H5" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I5" s="6" t="n">
+      <c r="I5" s="8" t="n">
         <v>0.00167</v>
       </c>
-      <c r="J5" s="6"/>
+      <c r="J5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
@@ -2043,14 +2269,14 @@
       <c r="B6" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C6" s="7" t="n">
+      <c r="C6" s="9" t="n">
         <v>7.4E-005</v>
       </c>
       <c r="D6" s="0"/>
       <c r="E6" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F6" s="7" t="n">
+      <c r="F6" s="9" t="n">
         <f aca="false">AVERAGE(C6,C11,C16,C21,C26)</f>
         <v>7.88E-005</v>
       </c>
@@ -2058,10 +2284,10 @@
       <c r="H6" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="I6" s="6" t="n">
+      <c r="I6" s="8" t="n">
         <v>0.00155</v>
       </c>
-      <c r="J6" s="6"/>
+      <c r="J6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
@@ -2070,14 +2296,14 @@
       <c r="B7" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C7" s="7" t="n">
+      <c r="C7" s="9" t="n">
         <v>0.000137</v>
       </c>
       <c r="D7" s="0"/>
       <c r="E7" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F7" s="7" t="n">
+      <c r="F7" s="9" t="n">
         <f aca="false">AVERAGE(C7,C12,C17,C22,C27)</f>
         <v>0.0001386</v>
       </c>
@@ -2085,10 +2311,10 @@
       <c r="H7" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="I7" s="6" t="n">
+      <c r="I7" s="8" t="n">
         <v>0.00195</v>
       </c>
-      <c r="J7" s="6"/>
+      <c r="J7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
@@ -2097,14 +2323,14 @@
       <c r="B8" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C8" s="7" t="n">
+      <c r="C8" s="9" t="n">
         <v>0.000133</v>
       </c>
       <c r="D8" s="0"/>
       <c r="E8" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="F8" s="7" t="n">
+      <c r="F8" s="9" t="n">
         <f aca="false">AVERAGE(C8,C13,C18,C23,C28)</f>
         <v>0.0001294</v>
       </c>
@@ -2112,10 +2338,10 @@
       <c r="H8" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I8" s="6" t="n">
+      <c r="I8" s="8" t="n">
         <v>0.00149</v>
       </c>
-      <c r="J8" s="6"/>
+      <c r="J8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
@@ -2124,27 +2350,27 @@
       <c r="B9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C9" s="7" t="n">
+      <c r="C9" s="9" t="n">
         <v>0.000156</v>
       </c>
       <c r="D9" s="0"/>
       <c r="E9" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F9" s="7" t="n">
+      <c r="F9" s="9" t="n">
         <f aca="false">AVERAGE(C9,C14,C19,C24,C29)</f>
         <v>0.000155</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="H9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I9" s="6" t="n">
+      <c r="I9" s="8" t="n">
         <v>0.0013</v>
       </c>
-      <c r="J9" s="6" t="n">
+      <c r="J9" s="8" t="n">
         <f aca="false">AVERAGE(I9:I23)</f>
         <v>0.001602</v>
       </c>
@@ -2156,7 +2382,7 @@
       <c r="B10" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C10" s="7" t="n">
+      <c r="C10" s="9" t="n">
         <v>0.000151</v>
       </c>
       <c r="D10" s="0"/>
@@ -2166,10 +2392,10 @@
       <c r="H10" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I10" s="6" t="n">
+      <c r="I10" s="8" t="n">
         <v>0.00149</v>
       </c>
-      <c r="J10" s="6"/>
+      <c r="J10" s="8"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
@@ -2178,24 +2404,24 @@
       <c r="B11" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C11" s="7" t="n">
+      <c r="C11" s="9" t="n">
         <v>9E-005</v>
       </c>
       <c r="D11" s="0"/>
       <c r="E11" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="G11" s="0"/>
       <c r="H11" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="I11" s="6" t="n">
+      <c r="I11" s="8" t="n">
         <v>0.00177</v>
       </c>
-      <c r="J11" s="6"/>
+      <c r="J11" s="8"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
@@ -2204,14 +2430,14 @@
       <c r="B12" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C12" s="7" t="n">
+      <c r="C12" s="9" t="n">
         <v>0.000141</v>
       </c>
       <c r="D12" s="0"/>
       <c r="E12" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F12" s="7" t="n">
+      <c r="F12" s="9" t="n">
         <f aca="false">AVERAGE(C4:C9)</f>
         <v>0.0001304</v>
       </c>
@@ -2219,10 +2445,10 @@
       <c r="H12" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="I12" s="6" t="n">
+      <c r="I12" s="8" t="n">
         <v>0.00219</v>
       </c>
-      <c r="J12" s="6"/>
+      <c r="J12" s="8"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
@@ -2231,14 +2457,14 @@
       <c r="B13" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C13" s="7" t="n">
+      <c r="C13" s="9" t="n">
         <v>0.000131</v>
       </c>
       <c r="D13" s="0"/>
       <c r="E13" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F13" s="7" t="n">
+      <c r="F13" s="9" t="n">
         <f aca="false">AVERAGE(C10:C14)</f>
         <v>0.000134</v>
       </c>
@@ -2246,10 +2472,10 @@
       <c r="H13" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I13" s="6" t="n">
+      <c r="I13" s="8" t="n">
         <v>0.00145</v>
       </c>
-      <c r="J13" s="6"/>
+      <c r="J13" s="8"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
@@ -2258,27 +2484,27 @@
       <c r="B14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C14" s="7" t="n">
+      <c r="C14" s="9" t="n">
         <v>0.000157</v>
       </c>
       <c r="D14" s="0"/>
       <c r="E14" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F14" s="7" t="n">
+      <c r="F14" s="9" t="n">
         <f aca="false">AVERAGE(C15:C19)</f>
         <v>0.0001284</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H14" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I14" s="6" t="n">
+      <c r="I14" s="8" t="n">
         <v>0.00132</v>
       </c>
-      <c r="J14" s="6"/>
+      <c r="J14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
@@ -2287,14 +2513,14 @@
       <c r="B15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C15" s="7" t="n">
+      <c r="C15" s="9" t="n">
         <v>0.000151</v>
       </c>
       <c r="D15" s="0"/>
       <c r="E15" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="F15" s="7" t="n">
+      <c r="F15" s="9" t="n">
         <f aca="false">AVERAGE(C20:C24)</f>
         <v>0.0001292</v>
       </c>
@@ -2302,10 +2528,10 @@
       <c r="H15" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I15" s="6" t="n">
+      <c r="I15" s="8" t="n">
         <v>0.0015</v>
       </c>
-      <c r="J15" s="6"/>
+      <c r="J15" s="8"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
@@ -2314,14 +2540,14 @@
       <c r="B16" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C16" s="7" t="n">
+      <c r="C16" s="9" t="n">
         <v>7.9E-005</v>
       </c>
       <c r="D16" s="0"/>
       <c r="E16" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F16" s="7" t="n">
+      <c r="F16" s="9" t="n">
         <f aca="false">AVERAGE(C25:C29)</f>
         <v>0.0001316</v>
       </c>
@@ -2329,10 +2555,10 @@
       <c r="H16" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="I16" s="6" t="n">
+      <c r="I16" s="8" t="n">
         <v>0.00166</v>
       </c>
-      <c r="J16" s="6"/>
+      <c r="J16" s="8"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
@@ -2341,7 +2567,7 @@
       <c r="B17" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C17" s="7" t="n">
+      <c r="C17" s="9" t="n">
         <v>0.000133</v>
       </c>
       <c r="D17" s="0"/>
@@ -2351,10 +2577,10 @@
       <c r="H17" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="I17" s="6" t="n">
+      <c r="I17" s="8" t="n">
         <v>0.00219</v>
       </c>
-      <c r="J17" s="6"/>
+      <c r="J17" s="8"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
@@ -2363,7 +2589,7 @@
       <c r="B18" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C18" s="7" t="n">
+      <c r="C18" s="9" t="n">
         <v>0.000128</v>
       </c>
       <c r="D18" s="0"/>
@@ -2373,10 +2599,10 @@
       <c r="H18" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I18" s="6" t="n">
+      <c r="I18" s="8" t="n">
         <v>0.00145</v>
       </c>
-      <c r="J18" s="6"/>
+      <c r="J18" s="8"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
@@ -2385,22 +2611,22 @@
       <c r="B19" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C19" s="7" t="n">
+      <c r="C19" s="9" t="n">
         <v>0.000151</v>
       </c>
       <c r="D19" s="0"/>
       <c r="E19" s="0"/>
       <c r="F19" s="0"/>
       <c r="G19" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="H19" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I19" s="6" t="n">
+      <c r="I19" s="8" t="n">
         <v>0.0013</v>
       </c>
-      <c r="J19" s="6"/>
+      <c r="J19" s="8"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
@@ -2409,7 +2635,7 @@
       <c r="B20" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C20" s="7" t="n">
+      <c r="C20" s="9" t="n">
         <v>0.000151</v>
       </c>
       <c r="D20" s="0"/>
@@ -2419,10 +2645,10 @@
       <c r="H20" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I20" s="6" t="n">
+      <c r="I20" s="8" t="n">
         <v>0.00144</v>
       </c>
-      <c r="J20" s="6"/>
+      <c r="J20" s="8"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
@@ -2431,7 +2657,7 @@
       <c r="B21" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C21" s="7" t="n">
+      <c r="C21" s="9" t="n">
         <v>7.1E-005</v>
       </c>
       <c r="D21" s="0"/>
@@ -2441,10 +2667,10 @@
       <c r="H21" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="I21" s="6" t="n">
+      <c r="I21" s="8" t="n">
         <v>0.00167</v>
       </c>
-      <c r="J21" s="6"/>
+      <c r="J21" s="8"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
@@ -2453,7 +2679,7 @@
       <c r="B22" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C22" s="7" t="n">
+      <c r="C22" s="9" t="n">
         <v>0.000139</v>
       </c>
       <c r="D22" s="0"/>
@@ -2463,10 +2689,10 @@
       <c r="H22" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="I22" s="6" t="n">
+      <c r="I22" s="8" t="n">
         <v>0.00196</v>
       </c>
-      <c r="J22" s="6"/>
+      <c r="J22" s="8"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
@@ -2475,7 +2701,7 @@
       <c r="B23" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C23" s="7" t="n">
+      <c r="C23" s="9" t="n">
         <v>0.000129</v>
       </c>
       <c r="D23" s="0"/>
@@ -2485,10 +2711,10 @@
       <c r="H23" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I23" s="6" t="n">
+      <c r="I23" s="8" t="n">
         <v>0.00134</v>
       </c>
-      <c r="J23" s="6"/>
+      <c r="J23" s="8"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
@@ -2497,7 +2723,7 @@
       <c r="B24" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C24" s="7" t="n">
+      <c r="C24" s="9" t="n">
         <v>0.000156</v>
       </c>
       <c r="D24" s="0"/>
@@ -2513,7 +2739,7 @@
       <c r="B25" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C25" s="7" t="n">
+      <c r="C25" s="9" t="n">
         <v>0.000154</v>
       </c>
       <c r="D25" s="0"/>
@@ -2529,7 +2755,7 @@
       <c r="B26" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C26" s="7" t="n">
+      <c r="C26" s="9" t="n">
         <v>8E-005</v>
       </c>
       <c r="D26" s="0"/>
@@ -2545,7 +2771,7 @@
       <c r="B27" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C27" s="7" t="n">
+      <c r="C27" s="9" t="n">
         <v>0.000143</v>
       </c>
       <c r="D27" s="0"/>
@@ -2561,7 +2787,7 @@
       <c r="B28" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C28" s="7" t="n">
+      <c r="C28" s="9" t="n">
         <v>0.000126</v>
       </c>
       <c r="D28" s="0"/>
@@ -2577,7 +2803,7 @@
       <c r="B29" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C29" s="7" t="n">
+      <c r="C29" s="9" t="n">
         <v>0.000155</v>
       </c>
       <c r="D29" s="0"/>
@@ -2589,7 +2815,7 @@
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0"/>
       <c r="B30" s="0"/>
-      <c r="C30" s="7" t="n">
+      <c r="C30" s="9" t="n">
         <f aca="false">MIN(C5:C29)</f>
         <v>7.1E-005</v>
       </c>
@@ -2611,46 +2837,46 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B32" s="2"/>
-      <c r="C32" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8" t="s">
+      <c r="C32" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8" t="s">
+      <c r="D32" s="10"/>
+      <c r="E32" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="H32" s="8"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10" t="s">
+        <v>35</v>
+      </c>
+      <c r="H32" s="10"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D33" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E33" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="F33" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G33" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G33" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="H33" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2917,7 +3143,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B44" s="0"/>
       <c r="C44" s="0"/>
@@ -2929,26 +3155,26 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B45" s="0"/>
       <c r="C45" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="D45" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E45" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E45" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="F45" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G45" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G45" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="H45" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3055,27 +3281,27 @@
       <c r="A50" s="0"/>
       <c r="B50" s="0"/>
       <c r="C50" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D50" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E50" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="E50" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="F50" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="G50" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G50" s="1" t="s">
-        <v>17</v>
-      </c>
       <c r="H50" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B51" s="0"/>
       <c r="C51" s="1" t="n">
@@ -3104,22 +3330,22 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="5" t="s">
-        <v>37</v>
-      </c>
-      <c r="B52" s="5"/>
-      <c r="C52" s="5"/>
-      <c r="D52" s="5" t="n">
+      <c r="A52" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="B52" s="7"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="7" t="n">
         <f aca="false">C51/D51</f>
         <v>1.92138831010376</v>
       </c>
-      <c r="E52" s="5"/>
-      <c r="F52" s="5" t="n">
+      <c r="E52" s="7"/>
+      <c r="F52" s="7" t="n">
         <f aca="false">E51/F51</f>
         <v>1.8836255514574</v>
       </c>
-      <c r="G52" s="5"/>
-      <c r="H52" s="5" t="n">
+      <c r="G52" s="7"/>
+      <c r="H52" s="7" t="n">
         <f aca="false">G51/H51</f>
         <v>5.70578971387946</v>
       </c>

</xml_diff>

<commit_message>
completed iden prob result section but one graph
</commit_message>
<xml_diff>
--- a/stats/stats_compilation.xlsx
+++ b/stats/stats_compilation.xlsx
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="43">
   <si>
     <t xml:space="preserve">stats</t>
   </si>
@@ -110,7 +110,19 @@
     <t xml:space="preserve">gpu_time</t>
   </si>
   <si>
+    <t xml:space="preserve">+-cputime</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+-gputime</t>
+  </si>
+  <si>
     <t xml:space="preserve">averages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+-cpu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">+-gpu</t>
   </si>
   <si>
     <t xml:space="preserve">scaling on cpu</t>
@@ -400,8 +412,8 @@
   </sheetPr>
   <dimension ref="A1:P53"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="E7" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M28" activeCellId="0" sqref="M28"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G47" activeCellId="0" sqref="G47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1888,6 +1900,12 @@
       <c r="D34" s="1" t="s">
         <v>16</v>
       </c>
+      <c r="E34" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F34" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="n">
@@ -1902,6 +1920,14 @@
       <c r="D35" s="1" t="n">
         <v>9.945</v>
       </c>
+      <c r="E35" s="1" t="n">
+        <f aca="false">ABS(C$47-C35)</f>
+        <v>0.0036333333329992</v>
+      </c>
+      <c r="F35" s="1" t="n">
+        <f aca="false">ABS(D$47-D35)</f>
+        <v>0.0260999999999996</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="n">
@@ -1916,6 +1942,14 @@
       <c r="D36" s="1" t="n">
         <v>10.0032</v>
       </c>
+      <c r="E36" s="1" t="n">
+        <f aca="false">ABS(C$47-C36)</f>
+        <v>4.36783333333301</v>
+      </c>
+      <c r="F36" s="1" t="n">
+        <f aca="false">ABS(D$47-D36)</f>
+        <v>0.0320999999999998</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="n">
@@ -1930,6 +1964,14 @@
       <c r="D37" s="1" t="n">
         <v>9.9651</v>
       </c>
+      <c r="E37" s="1" t="n">
+        <f aca="false">ABS(C$47-C37)</f>
+        <v>4.371466666667</v>
+      </c>
+      <c r="F37" s="1" t="n">
+        <f aca="false">ABS(D$47-D37)</f>
+        <v>0.00600000000000023</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="n">
@@ -1944,6 +1986,14 @@
       <c r="D38" s="1" t="n">
         <v>61.2416</v>
       </c>
+      <c r="E38" s="1" t="n">
+        <f aca="false">ABS(C$48-C38)</f>
+        <v>4.60553333333303</v>
+      </c>
+      <c r="F38" s="1" t="n">
+        <f aca="false">ABS(D$48-D38)</f>
+        <v>0.2162333333333</v>
+      </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
@@ -1958,6 +2008,14 @@
       <c r="D39" s="1" t="n">
         <v>60.9564</v>
       </c>
+      <c r="E39" s="1" t="n">
+        <f aca="false">ABS(C$48-C39)</f>
+        <v>1.60966666666695</v>
+      </c>
+      <c r="F39" s="1" t="n">
+        <f aca="false">ABS(D$48-D39)</f>
+        <v>0.0689666666666966</v>
+      </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="n">
@@ -1972,6 +2030,14 @@
       <c r="D40" s="1" t="n">
         <v>60.8781</v>
       </c>
+      <c r="E40" s="1" t="n">
+        <f aca="false">ABS(C$48-C40)</f>
+        <v>2.99586666666698</v>
+      </c>
+      <c r="F40" s="1" t="n">
+        <f aca="false">ABS(D$48-D40)</f>
+        <v>0.147266666666695</v>
+      </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="n">
@@ -1986,6 +2052,14 @@
       <c r="D41" s="1" t="n">
         <v>126.035</v>
       </c>
+      <c r="E41" s="1" t="n">
+        <f aca="false">ABS(C$49-C41)</f>
+        <v>1.37840000000006</v>
+      </c>
+      <c r="F41" s="1" t="n">
+        <f aca="false">ABS(D$49-D41)</f>
+        <v>0.295200000000008</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
@@ -2000,6 +2074,14 @@
       <c r="D42" s="1" t="n">
         <v>126.388</v>
       </c>
+      <c r="E42" s="1" t="n">
+        <f aca="false">ABS(C$49-C42)</f>
+        <v>5.77999999999997</v>
+      </c>
+      <c r="F42" s="1" t="n">
+        <f aca="false">ABS(D$49-D42)</f>
+        <v>0.0578000000000003</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="n">
@@ -2013,6 +2095,14 @@
       </c>
       <c r="D43" s="1" t="n">
         <v>126.5676</v>
+      </c>
+      <c r="E43" s="1" t="n">
+        <f aca="false">ABS(C$49-C43)</f>
+        <v>4.40160000000003</v>
+      </c>
+      <c r="F43" s="1" t="n">
+        <f aca="false">ABS(D$49-D43)</f>
+        <v>0.237399999999994</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2023,7 +2113,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B45" s="0"/>
       <c r="C45" s="0"/>
@@ -2039,6 +2129,12 @@
       </c>
       <c r="D46" s="1" t="s">
         <v>16</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>21</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2054,6 +2150,14 @@
         <f aca="false">AVERAGE(D35:D37)</f>
         <v>9.9711</v>
       </c>
+      <c r="E47" s="1" t="n">
+        <f aca="false">AVERAGE(E35:E37)</f>
+        <v>2.914311111111</v>
+      </c>
+      <c r="F47" s="1" t="n">
+        <f aca="false">AVERAGE(F35:F37)</f>
+        <v>0.0213999999999999</v>
+      </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="n">
@@ -2068,6 +2172,14 @@
         <f aca="false">AVERAGE(D38:D40)</f>
         <v>61.0253666666667</v>
       </c>
+      <c r="E48" s="1" t="n">
+        <f aca="false">AVERAGE(E36:E38)</f>
+        <v>4.44827777777768</v>
+      </c>
+      <c r="F48" s="1" t="n">
+        <f aca="false">AVERAGE(F36:F38)</f>
+        <v>0.0847777777777665</v>
+      </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="n">
@@ -2081,6 +2193,14 @@
       <c r="D49" s="1" t="n">
         <f aca="false">AVERAGE(D41:D43)</f>
         <v>126.3302</v>
+      </c>
+      <c r="E49" s="1" t="n">
+        <f aca="false">AVERAGE(E37:E39)</f>
+        <v>3.52888888888899</v>
+      </c>
+      <c r="F49" s="1" t="n">
+        <f aca="false">AVERAGE(F37:F39)</f>
+        <v>0.0970666666666654</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2093,15 +2213,15 @@
       <c r="A51" s="0"/>
       <c r="B51" s="0"/>
       <c r="C51" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B52" s="0"/>
       <c r="C52" s="1" t="n">
@@ -2172,7 +2292,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B2" s="0"/>
       <c r="C2" s="0"/>
@@ -2189,40 +2309,40 @@
         <v>3</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C3" s="0"/>
       <c r="D3" s="0"/>
       <c r="E3" s="0"/>
       <c r="F3" s="0"/>
       <c r="G3" s="1" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="I3" s="0"/>
       <c r="J3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="D4" s="0"/>
       <c r="E4" s="1" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H4" s="1" t="n">
         <v>1</v>
@@ -2362,7 +2482,7 @@
         <v>0.000155</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="H9" s="1" t="n">
         <v>1</v>
@@ -2409,10 +2529,10 @@
       </c>
       <c r="D11" s="0"/>
       <c r="E11" s="1" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="G11" s="0"/>
       <c r="H11" s="1" t="n">
@@ -2496,7 +2616,7 @@
         <v>0.0001284</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="H14" s="1" t="n">
         <v>1</v>
@@ -2618,7 +2738,7 @@
       <c r="E19" s="0"/>
       <c r="F19" s="0"/>
       <c r="G19" s="1" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="H19" s="1" t="n">
         <v>1</v>
@@ -2841,21 +2961,21 @@
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="10" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="D32" s="10"/>
       <c r="E32" s="10" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="F32" s="10"/>
       <c r="G32" s="10" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="H32" s="10"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>4</v>
@@ -3143,7 +3263,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B44" s="0"/>
       <c r="C44" s="0"/>
@@ -3155,7 +3275,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="B45" s="0"/>
       <c r="C45" s="1" t="s">
@@ -3281,27 +3401,27 @@
       <c r="A50" s="0"/>
       <c r="B50" s="0"/>
       <c r="C50" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="H50" s="1" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>20</v>
+        <v>24</v>
       </c>
       <c r="B51" s="0"/>
       <c r="C51" s="1" t="n">
@@ -3331,7 +3451,7 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="7" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>

</xml_diff>

<commit_message>
writing optimizing reward section, stats, modified testing file
</commit_message>
<xml_diff>
--- a/stats/stats_compilation.xlsx
+++ b/stats/stats_compilation.xlsx
@@ -5,11 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="weights" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="rewards" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="best_rewards" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -57,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="43">
   <si>
     <t xml:space="preserve">stats</t>
   </si>
@@ -192,11 +193,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
     <numFmt numFmtId="166" formatCode="0.00000"/>
     <numFmt numFmtId="167" formatCode="0.000000"/>
+    <numFmt numFmtId="168" formatCode="0.000000000000000"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -228,7 +230,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -251,6 +253,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF99"/>
         <bgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -288,7 +296,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -331,6 +339,14 @@
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -412,8 +428,8 @@
   </sheetPr>
   <dimension ref="A1:P53"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G47" activeCellId="0" sqref="G47"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C40" activeCellId="0" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -801,7 +817,7 @@
       </c>
       <c r="N9" s="3" t="n">
         <f aca="false">ABS($M$10-M9)</f>
-        <v>0.0268</v>
+        <v>0.0267999999999999</v>
       </c>
       <c r="O9" s="1" t="n">
         <f aca="false">M9-L9</f>
@@ -1647,7 +1663,7 @@
       </c>
       <c r="N27" s="3" t="n">
         <f aca="false">ABS($M$31-M27)</f>
-        <v>0.00865999999999995</v>
+        <v>0.00866</v>
       </c>
       <c r="O27" s="1" t="n">
         <f aca="false">M27-L27</f>
@@ -1700,7 +1716,7 @@
       </c>
       <c r="N28" s="3" t="n">
         <f aca="false">ABS($M$31-M28)</f>
-        <v>0.09846</v>
+        <v>0.0984600000000001</v>
       </c>
       <c r="O28" s="1" t="n">
         <f aca="false">M28-L28</f>
@@ -1922,7 +1938,7 @@
       </c>
       <c r="E35" s="1" t="n">
         <f aca="false">ABS(C$47-C35)</f>
-        <v>0.0036333333329992</v>
+        <v>0.00363333333331184</v>
       </c>
       <c r="F35" s="1" t="n">
         <f aca="false">ABS(D$47-D35)</f>
@@ -1944,7 +1960,7 @@
       </c>
       <c r="E36" s="1" t="n">
         <f aca="false">ABS(C$47-C36)</f>
-        <v>4.36783333333301</v>
+        <v>4.36783333333332</v>
       </c>
       <c r="F36" s="1" t="n">
         <f aca="false">ABS(D$47-D36)</f>
@@ -1966,7 +1982,7 @@
       </c>
       <c r="E37" s="1" t="n">
         <f aca="false">ABS(C$47-C37)</f>
-        <v>4.371466666667</v>
+        <v>4.37146666666669</v>
       </c>
       <c r="F37" s="1" t="n">
         <f aca="false">ABS(D$47-D37)</f>
@@ -1988,11 +2004,11 @@
       </c>
       <c r="E38" s="1" t="n">
         <f aca="false">ABS(C$48-C38)</f>
-        <v>4.60553333333303</v>
+        <v>4.60553333333326</v>
       </c>
       <c r="F38" s="1" t="n">
         <f aca="false">ABS(D$48-D38)</f>
-        <v>0.2162333333333</v>
+        <v>0.216233333333335</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2010,11 +2026,11 @@
       </c>
       <c r="E39" s="1" t="n">
         <f aca="false">ABS(C$48-C39)</f>
-        <v>1.60966666666695</v>
+        <v>1.60966666666673</v>
       </c>
       <c r="F39" s="1" t="n">
         <f aca="false">ABS(D$48-D39)</f>
-        <v>0.0689666666666966</v>
+        <v>0.0689666666666611</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2032,11 +2048,11 @@
       </c>
       <c r="E40" s="1" t="n">
         <f aca="false">ABS(C$48-C40)</f>
-        <v>2.99586666666698</v>
+        <v>2.99586666666676</v>
       </c>
       <c r="F40" s="1" t="n">
         <f aca="false">ABS(D$48-D40)</f>
-        <v>0.147266666666695</v>
+        <v>0.14726666666666</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2058,7 +2074,7 @@
       </c>
       <c r="F41" s="1" t="n">
         <f aca="false">ABS(D$49-D41)</f>
-        <v>0.295200000000008</v>
+        <v>0.295199999999994</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2080,7 +2096,7 @@
       </c>
       <c r="F42" s="1" t="n">
         <f aca="false">ABS(D$49-D42)</f>
-        <v>0.0578000000000003</v>
+        <v>0.0578000000000145</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2102,7 +2118,7 @@
       </c>
       <c r="F43" s="1" t="n">
         <f aca="false">ABS(D$49-D43)</f>
-        <v>0.237399999999994</v>
+        <v>0.237400000000008</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2152,7 +2168,7 @@
       </c>
       <c r="E47" s="1" t="n">
         <f aca="false">AVERAGE(E35:E37)</f>
-        <v>2.914311111111</v>
+        <v>2.91431111111111</v>
       </c>
       <c r="F47" s="1" t="n">
         <f aca="false">AVERAGE(F35:F37)</f>
@@ -2174,11 +2190,11 @@
       </c>
       <c r="E48" s="1" t="n">
         <f aca="false">AVERAGE(E36:E38)</f>
-        <v>4.44827777777768</v>
+        <v>4.44827777777776</v>
       </c>
       <c r="F48" s="1" t="n">
         <f aca="false">AVERAGE(F36:F38)</f>
-        <v>0.0847777777777665</v>
+        <v>0.0847777777777784</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2196,7 +2212,7 @@
       </c>
       <c r="E49" s="1" t="n">
         <f aca="false">AVERAGE(E37:E39)</f>
-        <v>3.52888888888899</v>
+        <v>3.52888888888889</v>
       </c>
       <c r="F49" s="1" t="n">
         <f aca="false">AVERAGE(F37:F39)</f>
@@ -2259,10 +2275,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J52"/>
+  <dimension ref="1:52"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D37" activeCellId="0" sqref="D37"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2315,14 +2331,15 @@
       <c r="D3" s="0"/>
       <c r="E3" s="0"/>
       <c r="F3" s="0"/>
-      <c r="G3" s="1" t="s">
+      <c r="G3" s="0"/>
+      <c r="H3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="H3" s="1" t="s">
+      <c r="I3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="I3" s="0"/>
       <c r="J3" s="0"/>
+      <c r="K3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -2341,17 +2358,17 @@
       <c r="F4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G4" s="1" t="s">
+      <c r="H4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="H4" s="1" t="n">
+      <c r="I4" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I4" s="8" t="n">
+      <c r="J4" s="8" t="n">
         <v>0.00139</v>
       </c>
-      <c r="J4" s="8" t="n">
-        <f aca="false">AVERAGE(I4:I8)</f>
+      <c r="K4" s="8" t="n">
+        <f aca="false">AVERAGE(J4:J8)</f>
         <v>0.00161</v>
       </c>
     </row>
@@ -2365,7 +2382,10 @@
       <c r="C5" s="9" t="n">
         <v>0.000152</v>
       </c>
-      <c r="D5" s="0"/>
+      <c r="D5" s="0" t="n">
+        <f aca="false">ABS(F5-C5)</f>
+        <v>2.00000000000005E-007</v>
+      </c>
       <c r="E5" s="1" t="n">
         <v>1</v>
       </c>
@@ -2373,14 +2393,18 @@
         <f aca="false">AVERAGE(C5,C10,C15,C20,C25)</f>
         <v>0.0001518</v>
       </c>
-      <c r="G5" s="0"/>
-      <c r="H5" s="1" t="n">
+      <c r="G5" s="9" t="n">
+        <f aca="false">AVERAGE(D5,D10,D15,D20,D25)</f>
+        <v>9.60000000000002E-007</v>
+      </c>
+      <c r="H5" s="0"/>
+      <c r="I5" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I5" s="8" t="n">
+      <c r="J5" s="8" t="n">
         <v>0.00167</v>
       </c>
-      <c r="J5" s="8"/>
+      <c r="K5" s="8"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
@@ -2392,7 +2416,10 @@
       <c r="C6" s="9" t="n">
         <v>7.4E-005</v>
       </c>
-      <c r="D6" s="0"/>
+      <c r="D6" s="0" t="n">
+        <f aca="false">ABS(F6-C6)</f>
+        <v>4.79999999999999E-006</v>
+      </c>
       <c r="E6" s="1" t="n">
         <v>2</v>
       </c>
@@ -2400,14 +2427,18 @@
         <f aca="false">AVERAGE(C6,C11,C16,C21,C26)</f>
         <v>7.88E-005</v>
       </c>
-      <c r="G6" s="0"/>
-      <c r="H6" s="1" t="n">
+      <c r="G6" s="9" t="n">
+        <f aca="false">AVERAGE(D6,D11,D16,D21,D26)</f>
+        <v>5.04E-006</v>
+      </c>
+      <c r="H6" s="0"/>
+      <c r="I6" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="I6" s="8" t="n">
+      <c r="J6" s="8" t="n">
         <v>0.00155</v>
       </c>
-      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
@@ -2419,7 +2450,10 @@
       <c r="C7" s="9" t="n">
         <v>0.000137</v>
       </c>
-      <c r="D7" s="0"/>
+      <c r="D7" s="0" t="n">
+        <f aca="false">ABS(F7-C7)</f>
+        <v>1.59999999999998E-006</v>
+      </c>
       <c r="E7" s="1" t="n">
         <v>3</v>
       </c>
@@ -2427,14 +2461,18 @@
         <f aca="false">AVERAGE(C7,C12,C17,C22,C27)</f>
         <v>0.0001386</v>
       </c>
-      <c r="G7" s="0"/>
-      <c r="H7" s="1" t="n">
+      <c r="G7" s="9" t="n">
+        <f aca="false">AVERAGE(D7,D12,D17,D22,D27)</f>
+        <v>2.88E-006</v>
+      </c>
+      <c r="H7" s="0"/>
+      <c r="I7" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="I7" s="8" t="n">
+      <c r="J7" s="8" t="n">
         <v>0.00195</v>
       </c>
-      <c r="J7" s="8"/>
+      <c r="K7" s="8"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
@@ -2446,7 +2484,10 @@
       <c r="C8" s="9" t="n">
         <v>0.000133</v>
       </c>
-      <c r="D8" s="0"/>
+      <c r="D8" s="0" t="n">
+        <f aca="false">ABS(F8-C8)</f>
+        <v>3.60000000000001E-006</v>
+      </c>
       <c r="E8" s="1" t="n">
         <v>4</v>
       </c>
@@ -2454,14 +2495,18 @@
         <f aca="false">AVERAGE(C8,C13,C18,C23,C28)</f>
         <v>0.0001294</v>
       </c>
-      <c r="G8" s="0"/>
-      <c r="H8" s="1" t="n">
+      <c r="G8" s="9" t="n">
+        <f aca="false">AVERAGE(D8,D13,D18,D23,D28)</f>
+        <v>2.08E-006</v>
+      </c>
+      <c r="H8" s="0"/>
+      <c r="I8" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I8" s="8" t="n">
+      <c r="J8" s="8" t="n">
         <v>0.00149</v>
       </c>
-      <c r="J8" s="8"/>
+      <c r="K8" s="8"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
@@ -2473,7 +2518,10 @@
       <c r="C9" s="9" t="n">
         <v>0.000156</v>
       </c>
-      <c r="D9" s="0"/>
+      <c r="D9" s="0" t="n">
+        <f aca="false">ABS(F9-C9)</f>
+        <v>9.99999999999997E-007</v>
+      </c>
       <c r="E9" s="1" t="n">
         <v>5</v>
       </c>
@@ -2481,17 +2529,21 @@
         <f aca="false">AVERAGE(C9,C14,C19,C24,C29)</f>
         <v>0.000155</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="G9" s="9" t="n">
+        <f aca="false">AVERAGE(D9,D14,D19,D24,D29)</f>
+        <v>1.6E-006</v>
+      </c>
+      <c r="H9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H9" s="1" t="n">
+      <c r="I9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I9" s="8" t="n">
+      <c r="J9" s="8" t="n">
         <v>0.0013</v>
       </c>
-      <c r="J9" s="8" t="n">
-        <f aca="false">AVERAGE(I9:I23)</f>
+      <c r="K9" s="8" t="n">
+        <f aca="false">AVERAGE(J9:J23)</f>
         <v>0.001602</v>
       </c>
     </row>
@@ -2505,17 +2557,21 @@
       <c r="C10" s="9" t="n">
         <v>0.000151</v>
       </c>
-      <c r="D10" s="0"/>
+      <c r="D10" s="0" t="n">
+        <f aca="false">ABS(F5-C10)</f>
+        <v>7.99999999999992E-007</v>
+      </c>
       <c r="E10" s="0"/>
       <c r="F10" s="0"/>
       <c r="G10" s="0"/>
-      <c r="H10" s="1" t="n">
+      <c r="H10" s="0"/>
+      <c r="I10" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I10" s="8" t="n">
+      <c r="J10" s="8" t="n">
         <v>0.00149</v>
       </c>
-      <c r="J10" s="8"/>
+      <c r="K10" s="8"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
@@ -2527,21 +2583,24 @@
       <c r="C11" s="9" t="n">
         <v>9E-005</v>
       </c>
-      <c r="D11" s="0"/>
+      <c r="D11" s="0" t="n">
+        <f aca="false">ABS(F6-C11)</f>
+        <v>1.12E-005</v>
+      </c>
       <c r="E11" s="1" t="s">
         <v>30</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="G11" s="0"/>
-      <c r="H11" s="1" t="n">
+      <c r="H11" s="0"/>
+      <c r="I11" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="I11" s="8" t="n">
+      <c r="J11" s="8" t="n">
         <v>0.00177</v>
       </c>
-      <c r="J11" s="8"/>
+      <c r="K11" s="8"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
@@ -2553,7 +2612,10 @@
       <c r="C12" s="9" t="n">
         <v>0.000141</v>
       </c>
-      <c r="D12" s="0"/>
+      <c r="D12" s="0" t="n">
+        <f aca="false">ABS(F7-C12)</f>
+        <v>2.4E-006</v>
+      </c>
       <c r="E12" s="1" t="n">
         <v>1</v>
       </c>
@@ -2561,14 +2623,15 @@
         <f aca="false">AVERAGE(C4:C9)</f>
         <v>0.0001304</v>
       </c>
-      <c r="G12" s="0"/>
-      <c r="H12" s="1" t="n">
+      <c r="G12" s="9"/>
+      <c r="H12" s="0"/>
+      <c r="I12" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="I12" s="8" t="n">
+      <c r="J12" s="8" t="n">
         <v>0.00219</v>
       </c>
-      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
@@ -2580,7 +2643,10 @@
       <c r="C13" s="9" t="n">
         <v>0.000131</v>
       </c>
-      <c r="D13" s="0"/>
+      <c r="D13" s="0" t="n">
+        <f aca="false">ABS(F8-C13)</f>
+        <v>1.59999999999998E-006</v>
+      </c>
       <c r="E13" s="1" t="n">
         <v>2</v>
       </c>
@@ -2588,14 +2654,15 @@
         <f aca="false">AVERAGE(C10:C14)</f>
         <v>0.000134</v>
       </c>
-      <c r="G13" s="0"/>
-      <c r="H13" s="1" t="n">
+      <c r="G13" s="9"/>
+      <c r="H13" s="0"/>
+      <c r="I13" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I13" s="8" t="n">
+      <c r="J13" s="8" t="n">
         <v>0.00145</v>
       </c>
-      <c r="J13" s="8"/>
+      <c r="K13" s="8"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
@@ -2607,7 +2674,10 @@
       <c r="C14" s="9" t="n">
         <v>0.000157</v>
       </c>
-      <c r="D14" s="0"/>
+      <c r="D14" s="0" t="n">
+        <f aca="false">ABS(F9-C14)</f>
+        <v>2E-006</v>
+      </c>
       <c r="E14" s="1" t="n">
         <v>3</v>
       </c>
@@ -2615,16 +2685,17 @@
         <f aca="false">AVERAGE(C15:C19)</f>
         <v>0.0001284</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G14" s="9"/>
+      <c r="H14" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H14" s="1" t="n">
+      <c r="I14" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I14" s="8" t="n">
+      <c r="J14" s="8" t="n">
         <v>0.00132</v>
       </c>
-      <c r="J14" s="8"/>
+      <c r="K14" s="8"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
@@ -2636,7 +2707,10 @@
       <c r="C15" s="9" t="n">
         <v>0.000151</v>
       </c>
-      <c r="D15" s="0"/>
+      <c r="D15" s="0" t="n">
+        <f aca="false">ABS(F5-C15)</f>
+        <v>7.99999999999992E-007</v>
+      </c>
       <c r="E15" s="1" t="n">
         <v>4</v>
       </c>
@@ -2644,14 +2718,15 @@
         <f aca="false">AVERAGE(C20:C24)</f>
         <v>0.0001292</v>
       </c>
-      <c r="G15" s="0"/>
-      <c r="H15" s="1" t="n">
+      <c r="G15" s="9"/>
+      <c r="H15" s="0"/>
+      <c r="I15" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I15" s="8" t="n">
+      <c r="J15" s="8" t="n">
         <v>0.0015</v>
       </c>
-      <c r="J15" s="8"/>
+      <c r="K15" s="8"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
@@ -2663,7 +2738,10 @@
       <c r="C16" s="9" t="n">
         <v>7.9E-005</v>
       </c>
-      <c r="D16" s="0"/>
+      <c r="D16" s="0" t="n">
+        <f aca="false">ABS(F6-C16)</f>
+        <v>2.00000000000005E-007</v>
+      </c>
       <c r="E16" s="1" t="n">
         <v>5</v>
       </c>
@@ -2671,14 +2749,15 @@
         <f aca="false">AVERAGE(C25:C29)</f>
         <v>0.0001316</v>
       </c>
-      <c r="G16" s="0"/>
-      <c r="H16" s="1" t="n">
+      <c r="G16" s="9"/>
+      <c r="H16" s="0"/>
+      <c r="I16" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="I16" s="8" t="n">
+      <c r="J16" s="8" t="n">
         <v>0.00166</v>
       </c>
-      <c r="J16" s="8"/>
+      <c r="K16" s="8"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
@@ -2690,17 +2769,21 @@
       <c r="C17" s="9" t="n">
         <v>0.000133</v>
       </c>
-      <c r="D17" s="0"/>
+      <c r="D17" s="0" t="n">
+        <f aca="false">ABS(F7-C17)</f>
+        <v>5.59999999999997E-006</v>
+      </c>
       <c r="E17" s="0"/>
       <c r="F17" s="0"/>
       <c r="G17" s="0"/>
-      <c r="H17" s="1" t="n">
+      <c r="H17" s="0"/>
+      <c r="I17" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="I17" s="8" t="n">
+      <c r="J17" s="8" t="n">
         <v>0.00219</v>
       </c>
-      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
@@ -2712,17 +2795,21 @@
       <c r="C18" s="9" t="n">
         <v>0.000128</v>
       </c>
-      <c r="D18" s="0"/>
+      <c r="D18" s="0" t="n">
+        <f aca="false">ABS(F8-C18)</f>
+        <v>1.40000000000001E-006</v>
+      </c>
       <c r="E18" s="0"/>
       <c r="F18" s="0"/>
       <c r="G18" s="0"/>
-      <c r="H18" s="1" t="n">
+      <c r="H18" s="0"/>
+      <c r="I18" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I18" s="8" t="n">
+      <c r="J18" s="8" t="n">
         <v>0.00145</v>
       </c>
-      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
@@ -2734,19 +2821,23 @@
       <c r="C19" s="9" t="n">
         <v>0.000151</v>
       </c>
-      <c r="D19" s="0"/>
+      <c r="D19" s="0" t="n">
+        <f aca="false">ABS(F9-C19)</f>
+        <v>4.00000000000002E-006</v>
+      </c>
       <c r="E19" s="0"/>
       <c r="F19" s="0"/>
-      <c r="G19" s="1" t="s">
+      <c r="G19" s="0"/>
+      <c r="H19" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="H19" s="1" t="n">
+      <c r="I19" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I19" s="8" t="n">
+      <c r="J19" s="8" t="n">
         <v>0.0013</v>
       </c>
-      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
@@ -2758,17 +2849,21 @@
       <c r="C20" s="9" t="n">
         <v>0.000151</v>
       </c>
-      <c r="D20" s="0"/>
+      <c r="D20" s="0" t="n">
+        <f aca="false">ABS(F5-C20)</f>
+        <v>7.99999999999992E-007</v>
+      </c>
       <c r="E20" s="0"/>
       <c r="F20" s="0"/>
       <c r="G20" s="0"/>
-      <c r="H20" s="1" t="n">
+      <c r="H20" s="0"/>
+      <c r="I20" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="I20" s="8" t="n">
+      <c r="J20" s="8" t="n">
         <v>0.00144</v>
       </c>
-      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
@@ -2780,17 +2875,21 @@
       <c r="C21" s="9" t="n">
         <v>7.1E-005</v>
       </c>
-      <c r="D21" s="0"/>
+      <c r="D21" s="0" t="n">
+        <f aca="false">ABS(F6-C21)</f>
+        <v>7.8E-006</v>
+      </c>
       <c r="E21" s="0"/>
       <c r="F21" s="0"/>
       <c r="G21" s="0"/>
-      <c r="H21" s="1" t="n">
+      <c r="H21" s="0"/>
+      <c r="I21" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="I21" s="8" t="n">
+      <c r="J21" s="8" t="n">
         <v>0.00167</v>
       </c>
-      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
@@ -2802,17 +2901,21 @@
       <c r="C22" s="9" t="n">
         <v>0.000139</v>
       </c>
-      <c r="D22" s="0"/>
+      <c r="D22" s="0" t="n">
+        <f aca="false">ABS(F7-C22)</f>
+        <v>4.0000000000001E-007</v>
+      </c>
       <c r="E22" s="0"/>
       <c r="F22" s="0"/>
       <c r="G22" s="0"/>
-      <c r="H22" s="1" t="n">
+      <c r="H22" s="0"/>
+      <c r="I22" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="I22" s="8" t="n">
+      <c r="J22" s="8" t="n">
         <v>0.00196</v>
       </c>
-      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
@@ -2824,17 +2927,21 @@
       <c r="C23" s="9" t="n">
         <v>0.000129</v>
       </c>
-      <c r="D23" s="0"/>
+      <c r="D23" s="0" t="n">
+        <f aca="false">ABS(F8-C23)</f>
+        <v>4.0000000000001E-007</v>
+      </c>
       <c r="E23" s="0"/>
       <c r="F23" s="0"/>
       <c r="G23" s="0"/>
-      <c r="H23" s="1" t="n">
+      <c r="H23" s="0"/>
+      <c r="I23" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="I23" s="8" t="n">
+      <c r="J23" s="8" t="n">
         <v>0.00134</v>
       </c>
-      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
@@ -2846,11 +2953,15 @@
       <c r="C24" s="9" t="n">
         <v>0.000156</v>
       </c>
-      <c r="D24" s="0"/>
+      <c r="D24" s="0" t="n">
+        <f aca="false">ABS(F9-C24)</f>
+        <v>9.99999999999997E-007</v>
+      </c>
       <c r="E24" s="0"/>
       <c r="F24" s="0"/>
       <c r="G24" s="0"/>
       <c r="H24" s="0"/>
+      <c r="I24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
@@ -2862,11 +2973,15 @@
       <c r="C25" s="9" t="n">
         <v>0.000154</v>
       </c>
-      <c r="D25" s="0"/>
+      <c r="D25" s="0" t="n">
+        <f aca="false">ABS(F5-C25)</f>
+        <v>2.20000000000003E-006</v>
+      </c>
       <c r="E25" s="0"/>
       <c r="F25" s="0"/>
       <c r="G25" s="0"/>
       <c r="H25" s="0"/>
+      <c r="I25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
@@ -2878,11 +2993,15 @@
       <c r="C26" s="9" t="n">
         <v>8E-005</v>
       </c>
-      <c r="D26" s="0"/>
+      <c r="D26" s="0" t="n">
+        <f aca="false">ABS(F6-C26)</f>
+        <v>1.2E-006</v>
+      </c>
       <c r="E26" s="0"/>
       <c r="F26" s="0"/>
       <c r="G26" s="0"/>
       <c r="H26" s="0"/>
+      <c r="AMJ26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
@@ -2894,11 +3013,15 @@
       <c r="C27" s="9" t="n">
         <v>0.000143</v>
       </c>
-      <c r="D27" s="0"/>
+      <c r="D27" s="0" t="n">
+        <f aca="false">ABS(F7-C27)</f>
+        <v>4.40000000000003E-006</v>
+      </c>
       <c r="E27" s="0"/>
       <c r="F27" s="0"/>
       <c r="G27" s="0"/>
       <c r="H27" s="0"/>
+      <c r="AMJ27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
@@ -2910,11 +3033,15 @@
       <c r="C28" s="9" t="n">
         <v>0.000126</v>
       </c>
-      <c r="D28" s="0"/>
+      <c r="D28" s="0" t="n">
+        <f aca="false">ABS(F8-C28)</f>
+        <v>3.4E-006</v>
+      </c>
       <c r="E28" s="0"/>
       <c r="F28" s="0"/>
       <c r="G28" s="0"/>
       <c r="H28" s="0"/>
+      <c r="AMJ28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
@@ -2926,11 +3053,15 @@
       <c r="C29" s="9" t="n">
         <v>0.000155</v>
       </c>
-      <c r="D29" s="0"/>
+      <c r="D29" s="0" t="n">
+        <f aca="false">ABS(F9-C29)</f>
+        <v>0</v>
+      </c>
       <c r="E29" s="0"/>
       <c r="F29" s="0"/>
       <c r="G29" s="0"/>
       <c r="H29" s="0"/>
+      <c r="AMJ29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0"/>
@@ -3508,4 +3639,429 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B2:D37"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="11" width="28.5663265306122"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D3" s="11" t="n">
+        <v>0.000123610152514</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="D4" s="11" t="n">
+        <v>8.8636610599E-005</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D5" s="11" t="n">
+        <v>7.4069997936E-005</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="D6" s="11" t="n">
+        <v>6.9892732427E-005</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="D7" s="11" t="n">
+        <v>6.9483772677E-005</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>5E-005</v>
+      </c>
+      <c r="D8" s="12" t="n">
+        <v>6.8885761721E-005</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>1E-005</v>
+      </c>
+      <c r="D9" s="11" t="n">
+        <v>9.256733756E-005</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D10" s="11" t="n">
+        <v>0.000144385485328</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="D11" s="11" t="n">
+        <v>9.5978211903E-005</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D12" s="11" t="n">
+        <v>8.9935885626E-005</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="D13" s="11" t="n">
+        <v>8.4039427747E-005</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="D14" s="11" t="n">
+        <v>8.1295489508E-005</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>5E-005</v>
+      </c>
+      <c r="D15" s="11" t="n">
+        <v>8.0391145184E-005</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>1E-005</v>
+      </c>
+      <c r="D16" s="11" t="n">
+        <v>0.000102245641756</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D17" s="11" t="n">
+        <v>0.00012816459639</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="D18" s="11" t="n">
+        <v>9.1854228231E-005</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B19" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D19" s="11" t="n">
+        <v>7.8748293163E-005</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B20" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="D20" s="11" t="n">
+        <v>7.6260628703E-005</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="D21" s="11" t="n">
+        <v>7.5951844337E-005</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B22" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>5E-005</v>
+      </c>
+      <c r="D22" s="11" t="n">
+        <v>7.6219243056E-005</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B23" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>1E-005</v>
+      </c>
+      <c r="D23" s="11" t="n">
+        <v>0.000102635014628</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B24" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D24" s="11" t="n">
+        <v>0.000134039801196</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B25" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="D25" s="11" t="n">
+        <v>9.2438262072E-005</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D26" s="11" t="n">
+        <v>7.0732487075E-005</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B27" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="D27" s="11" t="n">
+        <v>7.0459493145E-005</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B28" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="D28" s="11" t="n">
+        <v>7.0160800533E-005</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B29" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>5E-005</v>
+      </c>
+      <c r="D29" s="11" t="n">
+        <v>7.0123423939E-005</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B30" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>1E-005</v>
+      </c>
+      <c r="D30" s="11" t="n">
+        <v>0.000106777326437</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B31" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>0.01</v>
+      </c>
+      <c r="D31" s="11" t="n">
+        <v>0.000113149704703</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B32" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>0.005</v>
+      </c>
+      <c r="D32" s="11" t="n">
+        <v>8.4696828455E-005</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B33" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>0.001</v>
+      </c>
+      <c r="D33" s="11" t="n">
+        <v>7.983539399E-005</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B34" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>0.0005</v>
+      </c>
+      <c r="D34" s="11" t="n">
+        <v>7.6452655776E-005</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B35" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="D35" s="11" t="n">
+        <v>7.5728094089E-005</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B36" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>5E-005</v>
+      </c>
+      <c r="D36" s="11" t="n">
+        <v>7.6094336691E-005</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B37" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>1E-005</v>
+      </c>
+      <c r="D37" s="11" t="n">
+        <v>9.8175973108E-005</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
tested more randomly distributed rewards for the baseline, writing optimizing reward section
</commit_message>
<xml_diff>
--- a/stats/stats_compilation.xlsx
+++ b/stats/stats_compilation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="weights" sheetId="1" state="visible" r:id="rId2"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="41">
   <si>
     <t xml:space="preserve">stats</t>
   </si>
@@ -144,7 +144,7 @@
     <t xml:space="preserve">BASELINES</t>
   </si>
   <si>
-    <t xml:space="preserve">weights_seed</t>
+    <t xml:space="preserve">loss</t>
   </si>
   <si>
     <t xml:space="preserve">weight_file_seed</t>
@@ -162,13 +162,7 @@
     <t xml:space="preserve">proport</t>
   </si>
   <si>
-    <t xml:space="preserve">rand1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rand2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rand3</t>
+    <t xml:space="preserve">rand</t>
   </si>
   <si>
     <t xml:space="preserve">total_time</t>
@@ -193,12 +187,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="5">
+  <numFmts count="7">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
-    <numFmt numFmtId="166" formatCode="0.00000"/>
-    <numFmt numFmtId="167" formatCode="0.000000"/>
-    <numFmt numFmtId="168" formatCode="0.000000000000000"/>
+    <numFmt numFmtId="166" formatCode="0.00000000000"/>
+    <numFmt numFmtId="167" formatCode="0.00000"/>
+    <numFmt numFmtId="168" formatCode="0.000000"/>
+    <numFmt numFmtId="169" formatCode="0.0000000"/>
+    <numFmt numFmtId="170" formatCode="0.000000000000000"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -296,7 +292,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -337,15 +333,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="168" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="170" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2277,8 +2281,8 @@
   </sheetPr>
   <dimension ref="1:52"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G18" activeCellId="0" sqref="G18"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J10" activeCellId="0" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2288,7 +2292,7 @@
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.5255102040816"/>
     <col collapsed="false" hidden="false" max="8" min="6" style="1" width="13.3622448979592"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="14.5612244897959"/>
     <col collapsed="false" hidden="false" max="1025" min="11" style="1" width="11.0714285714286"/>
   </cols>
   <sheetData>
@@ -2319,6 +2323,7 @@
       <c r="H2" s="0"/>
       <c r="I2" s="0"/>
       <c r="J2" s="0"/>
+      <c r="K2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
@@ -2332,14 +2337,15 @@
       <c r="E3" s="0"/>
       <c r="F3" s="0"/>
       <c r="G3" s="0"/>
-      <c r="H3" s="1" t="s">
+      <c r="H3" s="0"/>
+      <c r="I3" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="0"/>
       <c r="K3" s="0"/>
+      <c r="L3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -2358,19 +2364,14 @@
       <c r="F4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="I4" s="1" t="n">
-        <v>1</v>
-      </c>
       <c r="J4" s="8" t="n">
-        <v>0.00139</v>
-      </c>
-      <c r="K4" s="8" t="n">
-        <f aca="false">AVERAGE(J4:J8)</f>
-        <v>0.00161</v>
-      </c>
+        <v>0.000234784733038</v>
+      </c>
+      <c r="K4" s="9"/>
+      <c r="L4" s="9"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
@@ -2379,7 +2380,7 @@
       <c r="B5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C5" s="9" t="n">
+      <c r="C5" s="10" t="n">
         <v>0.000152</v>
       </c>
       <c r="D5" s="0" t="n">
@@ -2389,22 +2390,23 @@
       <c r="E5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F5" s="9" t="n">
+      <c r="F5" s="10" t="n">
         <f aca="false">AVERAGE(C5,C10,C15,C20,C25)</f>
         <v>0.0001518</v>
       </c>
-      <c r="G5" s="9" t="n">
+      <c r="G5" s="10" t="n">
         <f aca="false">AVERAGE(D5,D10,D15,D20,D25)</f>
         <v>9.60000000000002E-007</v>
       </c>
-      <c r="H5" s="0"/>
-      <c r="I5" s="1" t="n">
-        <v>2</v>
+      <c r="H5" s="10"/>
+      <c r="I5" s="0" t="s">
+        <v>34</v>
       </c>
       <c r="J5" s="8" t="n">
-        <v>0.00167</v>
-      </c>
-      <c r="K5" s="8"/>
+        <v>0.000400919205276</v>
+      </c>
+      <c r="K5" s="9"/>
+      <c r="L5" s="9"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
@@ -2413,7 +2415,7 @@
       <c r="B6" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C6" s="9" t="n">
+      <c r="C6" s="10" t="n">
         <v>7.4E-005</v>
       </c>
       <c r="D6" s="0" t="n">
@@ -2423,22 +2425,21 @@
       <c r="E6" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F6" s="9" t="n">
+      <c r="F6" s="10" t="n">
         <f aca="false">AVERAGE(C6,C11,C16,C21,C26)</f>
         <v>7.88E-005</v>
       </c>
-      <c r="G6" s="9" t="n">
+      <c r="G6" s="10" t="n">
         <f aca="false">AVERAGE(D6,D11,D16,D21,D26)</f>
         <v>5.04E-006</v>
       </c>
-      <c r="H6" s="0"/>
-      <c r="I6" s="1" t="n">
-        <v>3</v>
-      </c>
+      <c r="H6" s="10"/>
+      <c r="I6" s="0"/>
       <c r="J6" s="8" t="n">
-        <v>0.00155</v>
-      </c>
-      <c r="K6" s="8"/>
+        <v>0.000415126851294</v>
+      </c>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
@@ -2447,7 +2448,7 @@
       <c r="B7" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C7" s="9" t="n">
+      <c r="C7" s="10" t="n">
         <v>0.000137</v>
       </c>
       <c r="D7" s="0" t="n">
@@ -2457,22 +2458,21 @@
       <c r="E7" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F7" s="9" t="n">
+      <c r="F7" s="10" t="n">
         <f aca="false">AVERAGE(C7,C12,C17,C22,C27)</f>
         <v>0.0001386</v>
       </c>
-      <c r="G7" s="9" t="n">
+      <c r="G7" s="10" t="n">
         <f aca="false">AVERAGE(D7,D12,D17,D22,D27)</f>
         <v>2.88E-006</v>
       </c>
-      <c r="H7" s="0"/>
-      <c r="I7" s="1" t="n">
-        <v>4</v>
-      </c>
+      <c r="H7" s="10"/>
+      <c r="I7" s="0"/>
       <c r="J7" s="8" t="n">
-        <v>0.00195</v>
-      </c>
-      <c r="K7" s="8"/>
+        <v>0.000241408168222</v>
+      </c>
+      <c r="K7" s="11"/>
+      <c r="L7" s="9"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
@@ -2481,7 +2481,7 @@
       <c r="B8" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C8" s="9" t="n">
+      <c r="C8" s="10" t="n">
         <v>0.000133</v>
       </c>
       <c r="D8" s="0" t="n">
@@ -2491,22 +2491,21 @@
       <c r="E8" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="F8" s="9" t="n">
+      <c r="F8" s="10" t="n">
         <f aca="false">AVERAGE(C8,C13,C18,C23,C28)</f>
         <v>0.0001294</v>
       </c>
-      <c r="G8" s="9" t="n">
+      <c r="G8" s="10" t="n">
         <f aca="false">AVERAGE(D8,D13,D18,D23,D28)</f>
         <v>2.08E-006</v>
       </c>
-      <c r="H8" s="0"/>
-      <c r="I8" s="1" t="n">
-        <v>5</v>
-      </c>
+      <c r="H8" s="10"/>
+      <c r="I8" s="0"/>
       <c r="J8" s="8" t="n">
-        <v>0.00149</v>
-      </c>
-      <c r="K8" s="8"/>
+        <v>0.000355125812348</v>
+      </c>
+      <c r="K8" s="9"/>
+      <c r="L8" s="9"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
@@ -2515,7 +2514,7 @@
       <c r="B9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C9" s="9" t="n">
+      <c r="C9" s="10" t="n">
         <v>0.000156</v>
       </c>
       <c r="D9" s="0" t="n">
@@ -2525,27 +2524,23 @@
       <c r="E9" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F9" s="9" t="n">
+      <c r="F9" s="10" t="n">
         <f aca="false">AVERAGE(C9,C14,C19,C24,C29)</f>
         <v>0.000155</v>
       </c>
-      <c r="G9" s="9" t="n">
+      <c r="G9" s="10" t="n">
         <f aca="false">AVERAGE(D9,D14,D19,D24,D29)</f>
         <v>1.6E-006</v>
       </c>
-      <c r="H9" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="I9" s="1" t="n">
-        <v>1</v>
-      </c>
+      <c r="H9" s="10"/>
       <c r="J9" s="8" t="n">
-        <v>0.0013</v>
-      </c>
-      <c r="K9" s="8" t="n">
-        <f aca="false">AVERAGE(J9:J23)</f>
-        <v>0.001602</v>
-      </c>
+        <v>0.000243959832005</v>
+      </c>
+      <c r="K9" s="10" t="n">
+        <f aca="false">AVERAGE(J5:J9)</f>
+        <v>0.000331307973829</v>
+      </c>
+      <c r="L9" s="9"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
@@ -2554,7 +2549,7 @@
       <c r="B10" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C10" s="9" t="n">
+      <c r="C10" s="10" t="n">
         <v>0.000151</v>
       </c>
       <c r="D10" s="0" t="n">
@@ -2565,13 +2560,9 @@
       <c r="F10" s="0"/>
       <c r="G10" s="0"/>
       <c r="H10" s="0"/>
-      <c r="I10" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="J10" s="8" t="n">
-        <v>0.00149</v>
-      </c>
-      <c r="K10" s="8"/>
+      <c r="I10" s="0"/>
+      <c r="K10" s="9"/>
+      <c r="L10" s="9"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
@@ -2580,7 +2571,7 @@
       <c r="B11" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C11" s="9" t="n">
+      <c r="C11" s="10" t="n">
         <v>9E-005</v>
       </c>
       <c r="D11" s="0" t="n">
@@ -2593,14 +2584,9 @@
       <c r="F11" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="H11" s="0"/>
-      <c r="I11" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="J11" s="8" t="n">
-        <v>0.00177</v>
-      </c>
-      <c r="K11" s="8"/>
+      <c r="I11" s="0"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
@@ -2609,7 +2595,7 @@
       <c r="B12" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C12" s="9" t="n">
+      <c r="C12" s="10" t="n">
         <v>0.000141</v>
       </c>
       <c r="D12" s="0" t="n">
@@ -2619,19 +2605,15 @@
       <c r="E12" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F12" s="9" t="n">
+      <c r="F12" s="10" t="n">
         <f aca="false">AVERAGE(C4:C9)</f>
         <v>0.0001304</v>
       </c>
-      <c r="G12" s="9"/>
-      <c r="H12" s="0"/>
-      <c r="I12" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="J12" s="8" t="n">
-        <v>0.00219</v>
-      </c>
-      <c r="K12" s="8"/>
+      <c r="G12" s="10"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="0"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
@@ -2640,7 +2622,7 @@
       <c r="B13" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C13" s="9" t="n">
+      <c r="C13" s="10" t="n">
         <v>0.000131</v>
       </c>
       <c r="D13" s="0" t="n">
@@ -2650,19 +2632,15 @@
       <c r="E13" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F13" s="9" t="n">
+      <c r="F13" s="10" t="n">
         <f aca="false">AVERAGE(C10:C14)</f>
         <v>0.000134</v>
       </c>
-      <c r="G13" s="9"/>
-      <c r="H13" s="0"/>
-      <c r="I13" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="J13" s="8" t="n">
-        <v>0.00145</v>
-      </c>
-      <c r="K13" s="8"/>
+      <c r="G13" s="10"/>
+      <c r="H13" s="10"/>
+      <c r="I13" s="0"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="9"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
@@ -2671,7 +2649,7 @@
       <c r="B14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C14" s="9" t="n">
+      <c r="C14" s="10" t="n">
         <v>0.000157</v>
       </c>
       <c r="D14" s="0" t="n">
@@ -2681,21 +2659,14 @@
       <c r="E14" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F14" s="9" t="n">
+      <c r="F14" s="10" t="n">
         <f aca="false">AVERAGE(C15:C19)</f>
         <v>0.0001284</v>
       </c>
-      <c r="G14" s="9"/>
-      <c r="H14" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I14" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J14" s="8" t="n">
-        <v>0.00132</v>
-      </c>
-      <c r="K14" s="8"/>
+      <c r="G14" s="10"/>
+      <c r="H14" s="10"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
@@ -2704,7 +2675,7 @@
       <c r="B15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C15" s="9" t="n">
+      <c r="C15" s="10" t="n">
         <v>0.000151</v>
       </c>
       <c r="D15" s="0" t="n">
@@ -2714,19 +2685,15 @@
       <c r="E15" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="F15" s="9" t="n">
+      <c r="F15" s="10" t="n">
         <f aca="false">AVERAGE(C20:C24)</f>
         <v>0.0001292</v>
       </c>
-      <c r="G15" s="9"/>
-      <c r="H15" s="0"/>
-      <c r="I15" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="J15" s="8" t="n">
-        <v>0.0015</v>
-      </c>
-      <c r="K15" s="8"/>
+      <c r="G15" s="10"/>
+      <c r="H15" s="10"/>
+      <c r="I15" s="0"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
@@ -2735,7 +2702,7 @@
       <c r="B16" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C16" s="9" t="n">
+      <c r="C16" s="10" t="n">
         <v>7.9E-005</v>
       </c>
       <c r="D16" s="0" t="n">
@@ -2745,19 +2712,15 @@
       <c r="E16" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F16" s="9" t="n">
+      <c r="F16" s="10" t="n">
         <f aca="false">AVERAGE(C25:C29)</f>
         <v>0.0001316</v>
       </c>
-      <c r="G16" s="9"/>
-      <c r="H16" s="0"/>
-      <c r="I16" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="J16" s="8" t="n">
-        <v>0.00166</v>
-      </c>
-      <c r="K16" s="8"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="0"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="9"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
@@ -2766,7 +2729,7 @@
       <c r="B17" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C17" s="9" t="n">
+      <c r="C17" s="10" t="n">
         <v>0.000133</v>
       </c>
       <c r="D17" s="0" t="n">
@@ -2777,13 +2740,8 @@
       <c r="F17" s="0"/>
       <c r="G17" s="0"/>
       <c r="H17" s="0"/>
-      <c r="I17" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="J17" s="8" t="n">
-        <v>0.00219</v>
-      </c>
-      <c r="K17" s="8"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
@@ -2792,7 +2750,7 @@
       <c r="B18" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C18" s="9" t="n">
+      <c r="C18" s="10" t="n">
         <v>0.000128</v>
       </c>
       <c r="D18" s="0" t="n">
@@ -2803,13 +2761,8 @@
       <c r="F18" s="0"/>
       <c r="G18" s="0"/>
       <c r="H18" s="0"/>
-      <c r="I18" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="J18" s="8" t="n">
-        <v>0.00145</v>
-      </c>
-      <c r="K18" s="8"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
@@ -2818,7 +2771,7 @@
       <c r="B19" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C19" s="9" t="n">
+      <c r="C19" s="10" t="n">
         <v>0.000151</v>
       </c>
       <c r="D19" s="0" t="n">
@@ -2828,16 +2781,8 @@
       <c r="E19" s="0"/>
       <c r="F19" s="0"/>
       <c r="G19" s="0"/>
-      <c r="H19" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="I19" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J19" s="8" t="n">
-        <v>0.0013</v>
-      </c>
-      <c r="K19" s="8"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
@@ -2846,7 +2791,7 @@
       <c r="B20" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C20" s="9" t="n">
+      <c r="C20" s="10" t="n">
         <v>0.000151</v>
       </c>
       <c r="D20" s="0" t="n">
@@ -2857,13 +2802,8 @@
       <c r="F20" s="0"/>
       <c r="G20" s="0"/>
       <c r="H20" s="0"/>
-      <c r="I20" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="J20" s="8" t="n">
-        <v>0.00144</v>
-      </c>
-      <c r="K20" s="8"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
@@ -2872,7 +2812,7 @@
       <c r="B21" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C21" s="9" t="n">
+      <c r="C21" s="10" t="n">
         <v>7.1E-005</v>
       </c>
       <c r="D21" s="0" t="n">
@@ -2883,13 +2823,8 @@
       <c r="F21" s="0"/>
       <c r="G21" s="0"/>
       <c r="H21" s="0"/>
-      <c r="I21" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="J21" s="8" t="n">
-        <v>0.00167</v>
-      </c>
-      <c r="K21" s="8"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
@@ -2898,7 +2833,7 @@
       <c r="B22" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C22" s="9" t="n">
+      <c r="C22" s="10" t="n">
         <v>0.000139</v>
       </c>
       <c r="D22" s="0" t="n">
@@ -2909,13 +2844,8 @@
       <c r="F22" s="0"/>
       <c r="G22" s="0"/>
       <c r="H22" s="0"/>
-      <c r="I22" s="1" t="n">
-        <v>4</v>
-      </c>
-      <c r="J22" s="8" t="n">
-        <v>0.00196</v>
-      </c>
-      <c r="K22" s="8"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
@@ -2924,7 +2854,7 @@
       <c r="B23" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C23" s="9" t="n">
+      <c r="C23" s="10" t="n">
         <v>0.000129</v>
       </c>
       <c r="D23" s="0" t="n">
@@ -2935,13 +2865,8 @@
       <c r="F23" s="0"/>
       <c r="G23" s="0"/>
       <c r="H23" s="0"/>
-      <c r="I23" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="J23" s="8" t="n">
-        <v>0.00134</v>
-      </c>
-      <c r="K23" s="8"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
@@ -2950,7 +2875,7 @@
       <c r="B24" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C24" s="9" t="n">
+      <c r="C24" s="10" t="n">
         <v>0.000156</v>
       </c>
       <c r="D24" s="0" t="n">
@@ -2970,7 +2895,7 @@
       <c r="B25" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C25" s="9" t="n">
+      <c r="C25" s="10" t="n">
         <v>0.000154</v>
       </c>
       <c r="D25" s="0" t="n">
@@ -2990,7 +2915,7 @@
       <c r="B26" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C26" s="9" t="n">
+      <c r="C26" s="10" t="n">
         <v>8E-005</v>
       </c>
       <c r="D26" s="0" t="n">
@@ -3010,7 +2935,7 @@
       <c r="B27" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C27" s="9" t="n">
+      <c r="C27" s="10" t="n">
         <v>0.000143</v>
       </c>
       <c r="D27" s="0" t="n">
@@ -3030,7 +2955,7 @@
       <c r="B28" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C28" s="9" t="n">
+      <c r="C28" s="10" t="n">
         <v>0.000126</v>
       </c>
       <c r="D28" s="0" t="n">
@@ -3050,7 +2975,7 @@
       <c r="B29" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C29" s="9" t="n">
+      <c r="C29" s="10" t="n">
         <v>0.000155</v>
       </c>
       <c r="D29" s="0" t="n">
@@ -3066,7 +2991,7 @@
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0"/>
       <c r="B30" s="0"/>
-      <c r="C30" s="9" t="n">
+      <c r="C30" s="10" t="n">
         <f aca="false">MIN(C5:C29)</f>
         <v>7.1E-005</v>
       </c>
@@ -3091,22 +3016,22 @@
         <v>13</v>
       </c>
       <c r="B32" s="2"/>
-      <c r="C32" s="10" t="s">
+      <c r="C32" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" s="12"/>
+      <c r="E32" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="F32" s="12"/>
+      <c r="G32" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="F32" s="10"/>
-      <c r="G32" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="H32" s="10"/>
+      <c r="H32" s="12"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>4</v>
@@ -3406,7 +3331,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B45" s="0"/>
       <c r="C45" s="1" t="s">
@@ -3582,7 +3507,7 @@
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B52" s="7"/>
       <c r="C52" s="7"/>
@@ -3648,14 +3573,14 @@
   </sheetPr>
   <dimension ref="B2:D37"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D8" activeCellId="0" sqref="D8"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
     <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="11" width="28.5663265306122"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="28.5663265306122"/>
     <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
@@ -3666,7 +3591,7 @@
       <c r="C2" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="13" t="s">
         <v>31</v>
       </c>
     </row>
@@ -3677,7 +3602,7 @@
       <c r="C3" s="0" t="n">
         <v>0.01</v>
       </c>
-      <c r="D3" s="11" t="n">
+      <c r="D3" s="13" t="n">
         <v>0.000123610152514</v>
       </c>
     </row>
@@ -3688,7 +3613,7 @@
       <c r="C4" s="0" t="n">
         <v>0.005</v>
       </c>
-      <c r="D4" s="11" t="n">
+      <c r="D4" s="13" t="n">
         <v>8.8636610599E-005</v>
       </c>
     </row>
@@ -3699,7 +3624,7 @@
       <c r="C5" s="0" t="n">
         <v>0.001</v>
       </c>
-      <c r="D5" s="11" t="n">
+      <c r="D5" s="13" t="n">
         <v>7.4069997936E-005</v>
       </c>
     </row>
@@ -3710,7 +3635,7 @@
       <c r="C6" s="0" t="n">
         <v>0.0005</v>
       </c>
-      <c r="D6" s="11" t="n">
+      <c r="D6" s="13" t="n">
         <v>6.9892732427E-005</v>
       </c>
     </row>
@@ -3721,7 +3646,7 @@
       <c r="C7" s="0" t="n">
         <v>0.0001</v>
       </c>
-      <c r="D7" s="11" t="n">
+      <c r="D7" s="13" t="n">
         <v>6.9483772677E-005</v>
       </c>
     </row>
@@ -3732,7 +3657,7 @@
       <c r="C8" s="0" t="n">
         <v>5E-005</v>
       </c>
-      <c r="D8" s="12" t="n">
+      <c r="D8" s="14" t="n">
         <v>6.8885761721E-005</v>
       </c>
     </row>
@@ -3743,7 +3668,7 @@
       <c r="C9" s="0" t="n">
         <v>1E-005</v>
       </c>
-      <c r="D9" s="11" t="n">
+      <c r="D9" s="13" t="n">
         <v>9.256733756E-005</v>
       </c>
     </row>
@@ -3754,7 +3679,7 @@
       <c r="C10" s="0" t="n">
         <v>0.01</v>
       </c>
-      <c r="D10" s="11" t="n">
+      <c r="D10" s="13" t="n">
         <v>0.000144385485328</v>
       </c>
     </row>
@@ -3765,7 +3690,7 @@
       <c r="C11" s="0" t="n">
         <v>0.005</v>
       </c>
-      <c r="D11" s="11" t="n">
+      <c r="D11" s="13" t="n">
         <v>9.5978211903E-005</v>
       </c>
     </row>
@@ -3776,7 +3701,7 @@
       <c r="C12" s="0" t="n">
         <v>0.001</v>
       </c>
-      <c r="D12" s="11" t="n">
+      <c r="D12" s="13" t="n">
         <v>8.9935885626E-005</v>
       </c>
     </row>
@@ -3787,7 +3712,7 @@
       <c r="C13" s="0" t="n">
         <v>0.0005</v>
       </c>
-      <c r="D13" s="11" t="n">
+      <c r="D13" s="13" t="n">
         <v>8.4039427747E-005</v>
       </c>
     </row>
@@ -3798,7 +3723,7 @@
       <c r="C14" s="0" t="n">
         <v>0.0001</v>
       </c>
-      <c r="D14" s="11" t="n">
+      <c r="D14" s="13" t="n">
         <v>8.1295489508E-005</v>
       </c>
     </row>
@@ -3809,7 +3734,7 @@
       <c r="C15" s="0" t="n">
         <v>5E-005</v>
       </c>
-      <c r="D15" s="11" t="n">
+      <c r="D15" s="13" t="n">
         <v>8.0391145184E-005</v>
       </c>
     </row>
@@ -3820,7 +3745,7 @@
       <c r="C16" s="0" t="n">
         <v>1E-005</v>
       </c>
-      <c r="D16" s="11" t="n">
+      <c r="D16" s="13" t="n">
         <v>0.000102245641756</v>
       </c>
     </row>
@@ -3831,7 +3756,7 @@
       <c r="C17" s="0" t="n">
         <v>0.01</v>
       </c>
-      <c r="D17" s="11" t="n">
+      <c r="D17" s="13" t="n">
         <v>0.00012816459639</v>
       </c>
     </row>
@@ -3842,7 +3767,7 @@
       <c r="C18" s="0" t="n">
         <v>0.005</v>
       </c>
-      <c r="D18" s="11" t="n">
+      <c r="D18" s="13" t="n">
         <v>9.1854228231E-005</v>
       </c>
     </row>
@@ -3853,7 +3778,7 @@
       <c r="C19" s="0" t="n">
         <v>0.001</v>
       </c>
-      <c r="D19" s="11" t="n">
+      <c r="D19" s="13" t="n">
         <v>7.8748293163E-005</v>
       </c>
     </row>
@@ -3864,7 +3789,7 @@
       <c r="C20" s="0" t="n">
         <v>0.0005</v>
       </c>
-      <c r="D20" s="11" t="n">
+      <c r="D20" s="13" t="n">
         <v>7.6260628703E-005</v>
       </c>
     </row>
@@ -3875,7 +3800,7 @@
       <c r="C21" s="0" t="n">
         <v>0.0001</v>
       </c>
-      <c r="D21" s="11" t="n">
+      <c r="D21" s="13" t="n">
         <v>7.5951844337E-005</v>
       </c>
     </row>
@@ -3886,7 +3811,7 @@
       <c r="C22" s="0" t="n">
         <v>5E-005</v>
       </c>
-      <c r="D22" s="11" t="n">
+      <c r="D22" s="13" t="n">
         <v>7.6219243056E-005</v>
       </c>
     </row>
@@ -3897,7 +3822,7 @@
       <c r="C23" s="0" t="n">
         <v>1E-005</v>
       </c>
-      <c r="D23" s="11" t="n">
+      <c r="D23" s="13" t="n">
         <v>0.000102635014628</v>
       </c>
     </row>
@@ -3908,7 +3833,7 @@
       <c r="C24" s="0" t="n">
         <v>0.01</v>
       </c>
-      <c r="D24" s="11" t="n">
+      <c r="D24" s="13" t="n">
         <v>0.000134039801196</v>
       </c>
     </row>
@@ -3919,7 +3844,7 @@
       <c r="C25" s="0" t="n">
         <v>0.005</v>
       </c>
-      <c r="D25" s="11" t="n">
+      <c r="D25" s="13" t="n">
         <v>9.2438262072E-005</v>
       </c>
     </row>
@@ -3930,7 +3855,7 @@
       <c r="C26" s="0" t="n">
         <v>0.001</v>
       </c>
-      <c r="D26" s="11" t="n">
+      <c r="D26" s="13" t="n">
         <v>7.0732487075E-005</v>
       </c>
     </row>
@@ -3941,7 +3866,7 @@
       <c r="C27" s="0" t="n">
         <v>0.0005</v>
       </c>
-      <c r="D27" s="11" t="n">
+      <c r="D27" s="13" t="n">
         <v>7.0459493145E-005</v>
       </c>
     </row>
@@ -3952,7 +3877,7 @@
       <c r="C28" s="0" t="n">
         <v>0.0001</v>
       </c>
-      <c r="D28" s="11" t="n">
+      <c r="D28" s="13" t="n">
         <v>7.0160800533E-005</v>
       </c>
     </row>
@@ -3963,7 +3888,7 @@
       <c r="C29" s="0" t="n">
         <v>5E-005</v>
       </c>
-      <c r="D29" s="11" t="n">
+      <c r="D29" s="13" t="n">
         <v>7.0123423939E-005</v>
       </c>
     </row>
@@ -3974,7 +3899,7 @@
       <c r="C30" s="0" t="n">
         <v>1E-005</v>
       </c>
-      <c r="D30" s="11" t="n">
+      <c r="D30" s="13" t="n">
         <v>0.000106777326437</v>
       </c>
     </row>
@@ -3985,7 +3910,7 @@
       <c r="C31" s="0" t="n">
         <v>0.01</v>
       </c>
-      <c r="D31" s="11" t="n">
+      <c r="D31" s="13" t="n">
         <v>0.000113149704703</v>
       </c>
     </row>
@@ -3996,7 +3921,7 @@
       <c r="C32" s="0" t="n">
         <v>0.005</v>
       </c>
-      <c r="D32" s="11" t="n">
+      <c r="D32" s="13" t="n">
         <v>8.4696828455E-005</v>
       </c>
     </row>
@@ -4007,7 +3932,7 @@
       <c r="C33" s="0" t="n">
         <v>0.001</v>
       </c>
-      <c r="D33" s="11" t="n">
+      <c r="D33" s="13" t="n">
         <v>7.983539399E-005</v>
       </c>
     </row>
@@ -4018,7 +3943,7 @@
       <c r="C34" s="0" t="n">
         <v>0.0005</v>
       </c>
-      <c r="D34" s="11" t="n">
+      <c r="D34" s="13" t="n">
         <v>7.6452655776E-005</v>
       </c>
     </row>
@@ -4029,7 +3954,7 @@
       <c r="C35" s="0" t="n">
         <v>0.0001</v>
       </c>
-      <c r="D35" s="11" t="n">
+      <c r="D35" s="13" t="n">
         <v>7.5728094089E-005</v>
       </c>
     </row>
@@ -4040,7 +3965,7 @@
       <c r="C36" s="0" t="n">
         <v>5E-005</v>
       </c>
-      <c r="D36" s="11" t="n">
+      <c r="D36" s="13" t="n">
         <v>7.6094336691E-005</v>
       </c>
     </row>
@@ -4051,7 +3976,7 @@
       <c r="C37" s="0" t="n">
         <v>1E-005</v>
       </c>
-      <c r="D37" s="11" t="n">
+      <c r="D37" s="13" t="n">
         <v>9.8175973108E-005</v>
       </c>
     </row>

</xml_diff>

<commit_message>
deleted old data (results of 1weight nn), updated weights folder - organizing and logging stats
</commit_message>
<xml_diff>
--- a/stats/stats_compilation.xlsx
+++ b/stats/stats_compilation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="weights" sheetId="1" state="visible" r:id="rId2"/>
@@ -430,30 +430,30 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:P53"/>
+  <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C40" activeCellId="0" sqref="C40"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N12" activeCellId="0" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.5"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="9.4234693877551"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.9336734693878"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="13.5"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="9.4234693877551"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="7.1530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="9.31632653061224"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="7.02040816326531"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="1" width="10.8010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -934,7 +934,7 @@
         <v>0.02312</v>
       </c>
       <c r="K12" s="1" t="n">
-        <v>1685.7548</v>
+        <v>1618.1636</v>
       </c>
       <c r="L12" s="1" t="n">
         <v>0.0601</v>
@@ -987,7 +987,7 @@
         <v>0.00481999999999999</v>
       </c>
       <c r="K13" s="1" t="n">
-        <v>1623.1623</v>
+        <v>1669.5344</v>
       </c>
       <c r="L13" s="1" t="n">
         <v>0.0918</v>
@@ -1040,7 +1040,7 @@
         <v>0.03838</v>
       </c>
       <c r="K14" s="1" t="n">
-        <v>1615.3793</v>
+        <v>1619.9287</v>
       </c>
       <c r="L14" s="1" t="n">
         <v>0.0572</v>
@@ -1093,7 +1093,7 @@
         <v>0.01182</v>
       </c>
       <c r="K15" s="1" t="n">
-        <v>1618.4652</v>
+        <v>1621.1855</v>
       </c>
       <c r="L15" s="1" t="n">
         <v>0.039</v>
@@ -1146,7 +1146,7 @@
         <v>0.00137999999999999</v>
       </c>
       <c r="K16" s="1" t="n">
-        <v>1653.7931</v>
+        <v>1690.6036</v>
       </c>
       <c r="L16" s="1" t="n">
         <v>0.0525</v>
@@ -1197,7 +1197,7 @@
       </c>
       <c r="K17" s="1" t="n">
         <f aca="false">AVERAGE(K12:K16)</f>
-        <v>1639.31094</v>
+        <v>1643.88316</v>
       </c>
       <c r="L17" s="5" t="n">
         <f aca="false">AVERAGE(L12:L16)</f>
@@ -1898,6 +1898,8 @@
         <f aca="false">AVERAGE(D10,D17,D24,D31)</f>
         <v>1232.560875</v>
       </c>
+      <c r="E32" s="0"/>
+      <c r="F32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
@@ -1906,6 +1908,8 @@
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
+      <c r="E33" s="0"/>
+      <c r="F33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
@@ -1941,11 +1945,11 @@
         <v>9.945</v>
       </c>
       <c r="E35" s="1" t="n">
-        <f aca="false">ABS(C$47-C35)</f>
-        <v>0.00363333333331184</v>
+        <f aca="false">ABS(C$53-C35)</f>
+        <v>0.0036333333329992</v>
       </c>
       <c r="F35" s="1" t="n">
-        <f aca="false">ABS(D$47-D35)</f>
+        <f aca="false">ABS(D$53-D35)</f>
         <v>0.0260999999999996</v>
       </c>
     </row>
@@ -1963,11 +1967,11 @@
         <v>10.0032</v>
       </c>
       <c r="E36" s="1" t="n">
-        <f aca="false">ABS(C$47-C36)</f>
-        <v>4.36783333333332</v>
+        <f aca="false">ABS(C$53-C36)</f>
+        <v>4.36783333333301</v>
       </c>
       <c r="F36" s="1" t="n">
-        <f aca="false">ABS(D$47-D36)</f>
+        <f aca="false">ABS(D$53-D36)</f>
         <v>0.0320999999999998</v>
       </c>
     </row>
@@ -1985,242 +1989,276 @@
         <v>9.9651</v>
       </c>
       <c r="E37" s="1" t="n">
-        <f aca="false">ABS(C$47-C37)</f>
-        <v>4.37146666666669</v>
+        <f aca="false">ABS(C$53-C37)</f>
+        <v>4.371466666667</v>
       </c>
       <c r="F37" s="1" t="n">
-        <f aca="false">ABS(D$47-D37)</f>
+        <f aca="false">ABS(D$53-D37)</f>
         <v>0.00600000000000023</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="n">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="B38" s="1" t="n">
         <v>1</v>
       </c>
       <c r="C38" s="1" t="n">
-        <v>544.7114</v>
+        <v>440.3404</v>
       </c>
       <c r="D38" s="1" t="n">
-        <v>61.2416</v>
+        <v>40.767</v>
       </c>
       <c r="E38" s="1" t="n">
-        <f aca="false">ABS(C$48-C38)</f>
-        <v>4.60553333333326</v>
+        <f aca="false">ABS(C$54-C38)</f>
+        <v>10.3753666666667</v>
       </c>
       <c r="F38" s="1" t="n">
-        <f aca="false">ABS(D$48-D38)</f>
-        <v>0.216233333333335</v>
+        <f aca="false">ABS(D$54-D38)</f>
+        <v>0.16706666666667</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="B39" s="1" t="n">
         <v>2</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>538.4962</v>
+        <v>426.5965</v>
       </c>
       <c r="D39" s="1" t="n">
-        <v>60.9564</v>
+        <v>40.5242</v>
       </c>
       <c r="E39" s="1" t="n">
-        <f aca="false">ABS(C$48-C39)</f>
-        <v>1.60966666666673</v>
+        <f aca="false">ABS(C$54-C39)</f>
+        <v>3.36853333333335</v>
       </c>
       <c r="F39" s="1" t="n">
-        <f aca="false">ABS(D$48-D39)</f>
-        <v>0.0689666666666611</v>
+        <f aca="false">ABS(D$54-D39)</f>
+        <v>0.0757333333333321</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="n">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="B40" s="1" t="n">
         <v>3</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>537.11</v>
+        <v>422.9582</v>
       </c>
       <c r="D40" s="1" t="n">
-        <v>60.8781</v>
+        <v>40.5086</v>
       </c>
       <c r="E40" s="1" t="n">
-        <f aca="false">ABS(C$48-C40)</f>
-        <v>2.99586666666676</v>
+        <f aca="false">ABS(C$54-C40)</f>
+        <v>7.00683333333336</v>
       </c>
       <c r="F40" s="1" t="n">
-        <f aca="false">ABS(D$48-D40)</f>
-        <v>0.14726666666666</v>
+        <f aca="false">ABS(D$54-D40)</f>
+        <v>0.0913333333333313</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="n">
-        <v>173</v>
+        <v>85</v>
       </c>
       <c r="B41" s="1" t="n">
         <v>1</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>899.8638</v>
+        <v>544.7114</v>
       </c>
       <c r="D41" s="1" t="n">
-        <v>126.035</v>
+        <v>61.2416</v>
       </c>
       <c r="E41" s="1" t="n">
-        <f aca="false">ABS(C$49-C41)</f>
-        <v>1.37840000000006</v>
+        <f aca="false">ABS(C$55-C41)</f>
+        <v>4.60553333333326</v>
       </c>
       <c r="F41" s="1" t="n">
-        <f aca="false">ABS(D$49-D41)</f>
-        <v>0.295199999999994</v>
+        <f aca="false">ABS(D$55-D41)</f>
+        <v>0.216233333333335</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
-        <v>173</v>
+        <v>85</v>
       </c>
       <c r="B42" s="1" t="n">
         <v>2</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>907.0222</v>
+        <v>538.4962</v>
       </c>
       <c r="D42" s="1" t="n">
-        <v>126.388</v>
+        <v>60.9564</v>
       </c>
       <c r="E42" s="1" t="n">
-        <f aca="false">ABS(C$49-C42)</f>
-        <v>5.77999999999997</v>
+        <f aca="false">ABS(C$55-C42)</f>
+        <v>1.60966666666673</v>
       </c>
       <c r="F42" s="1" t="n">
-        <f aca="false">ABS(D$49-D42)</f>
-        <v>0.0578000000000145</v>
+        <f aca="false">ABS(D$55-D42)</f>
+        <v>0.0689666666666611</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="n">
-        <v>173</v>
+        <v>85</v>
       </c>
       <c r="B43" s="1" t="n">
         <v>3</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>896.8406</v>
+        <v>537.11</v>
       </c>
       <c r="D43" s="1" t="n">
-        <v>126.5676</v>
+        <v>60.8781</v>
       </c>
       <c r="E43" s="1" t="n">
-        <f aca="false">ABS(C$49-C43)</f>
-        <v>4.40160000000003</v>
+        <f aca="false">ABS(C$55-C43)</f>
+        <v>2.99586666666676</v>
       </c>
       <c r="F43" s="1" t="n">
-        <f aca="false">ABS(D$49-D43)</f>
-        <v>0.237400000000008</v>
+        <f aca="false">ABS(D$55-D43)</f>
+        <v>0.14726666666666</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0"/>
-      <c r="B44" s="0"/>
-      <c r="C44" s="0"/>
-      <c r="D44" s="0"/>
+      <c r="A44" s="1" t="n">
+        <v>129</v>
+      </c>
+      <c r="B44" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C44" s="1" t="n">
+        <v>865.2712</v>
+      </c>
+      <c r="D44" s="1" t="n">
+        <v>92.3451</v>
+      </c>
+      <c r="E44" s="1" t="n">
+        <f aca="false">ABS(C$56-C44)</f>
+        <v>4.72036666666668</v>
+      </c>
+      <c r="F44" s="1" t="n">
+        <f aca="false">ABS(D$56-D44)</f>
+        <v>3.78783333333332</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B45" s="0"/>
-      <c r="C45" s="0"/>
-      <c r="D45" s="0"/>
+      <c r="A45" s="1" t="n">
+        <v>129</v>
+      </c>
+      <c r="B45" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C45" s="1" t="n">
+        <v>849.1726</v>
+      </c>
+      <c r="D45" s="1" t="n">
+        <v>86.5314</v>
+      </c>
+      <c r="E45" s="1" t="n">
+        <f aca="false">ABS(C$56-C45)</f>
+        <v>11.3782333333334</v>
+      </c>
+      <c r="F45" s="1" t="n">
+        <f aca="false">ABS(D$56-D45)</f>
+        <v>2.02586666666667</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B46" s="0"/>
-      <c r="C46" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="F46" s="1" t="s">
-        <v>21</v>
+      <c r="A46" s="1" t="n">
+        <v>129</v>
+      </c>
+      <c r="B46" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C46" s="1" t="n">
+        <v>867.2087</v>
+      </c>
+      <c r="D46" s="1" t="n">
+        <v>86.7953</v>
+      </c>
+      <c r="E46" s="1" t="n">
+        <f aca="false">ABS(C$56-C46)</f>
+        <v>6.65786666666668</v>
+      </c>
+      <c r="F46" s="1" t="n">
+        <f aca="false">ABS(D$56-D46)</f>
+        <v>1.76196666666668</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="n">
-        <v>17</v>
-      </c>
-      <c r="B47" s="0"/>
+        <v>173</v>
+      </c>
+      <c r="B47" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="C47" s="1" t="n">
-        <f aca="false">AVERAGE(C35:C37)</f>
-        <v>173.567266666667</v>
+        <v>899.8638</v>
       </c>
       <c r="D47" s="1" t="n">
-        <f aca="false">AVERAGE(D35:D37)</f>
-        <v>9.9711</v>
+        <v>126.035</v>
       </c>
       <c r="E47" s="1" t="n">
-        <f aca="false">AVERAGE(E35:E37)</f>
-        <v>2.91431111111111</v>
+        <f aca="false">ABS(C$57-C47)</f>
+        <v>1.37840000000006</v>
       </c>
       <c r="F47" s="1" t="n">
-        <f aca="false">AVERAGE(F35:F37)</f>
-        <v>0.0213999999999999</v>
+        <f aca="false">ABS(D$57-D47)</f>
+        <v>0.295200000000008</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="n">
-        <v>85</v>
-      </c>
-      <c r="B48" s="0"/>
+        <v>173</v>
+      </c>
+      <c r="B48" s="1" t="n">
+        <v>2</v>
+      </c>
       <c r="C48" s="1" t="n">
-        <f aca="false">AVERAGE(C38:C40)</f>
-        <v>540.105866666667</v>
+        <v>907.0222</v>
       </c>
       <c r="D48" s="1" t="n">
-        <f aca="false">AVERAGE(D38:D40)</f>
-        <v>61.0253666666667</v>
+        <v>126.388</v>
       </c>
       <c r="E48" s="1" t="n">
-        <f aca="false">AVERAGE(E36:E38)</f>
-        <v>4.44827777777776</v>
+        <f aca="false">ABS(C$57-C48)</f>
+        <v>5.77999999999997</v>
       </c>
       <c r="F48" s="1" t="n">
-        <f aca="false">AVERAGE(F36:F38)</f>
-        <v>0.0847777777777784</v>
+        <f aca="false">ABS(D$57-D48)</f>
+        <v>0.0578000000000003</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="n">
         <v>173</v>
       </c>
-      <c r="B49" s="0"/>
+      <c r="B49" s="1" t="n">
+        <v>3</v>
+      </c>
       <c r="C49" s="1" t="n">
-        <f aca="false">AVERAGE(C41:C43)</f>
-        <v>901.2422</v>
+        <v>896.8406</v>
       </c>
       <c r="D49" s="1" t="n">
-        <f aca="false">AVERAGE(D41:D43)</f>
-        <v>126.3302</v>
+        <v>126.5676</v>
       </c>
       <c r="E49" s="1" t="n">
-        <f aca="false">AVERAGE(E37:E39)</f>
-        <v>3.52888888888889</v>
+        <f aca="false">ABS(C$57-C49)</f>
+        <v>4.40160000000003</v>
       </c>
       <c r="F49" s="1" t="n">
-        <f aca="false">AVERAGE(F37:F39)</f>
-        <v>0.0970666666666654</v>
+        <f aca="false">ABS(D$57-D49)</f>
+        <v>0.237399999999994</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2228,38 +2266,184 @@
       <c r="B50" s="0"/>
       <c r="C50" s="0"/>
       <c r="D50" s="0"/>
+      <c r="E50" s="0"/>
+      <c r="F50" s="0"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="0"/>
+      <c r="A51" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="B51" s="0"/>
-      <c r="C51" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="C51" s="0"/>
+      <c r="D51" s="0"/>
+      <c r="E51" s="0"/>
+      <c r="F51" s="0"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B52" s="0"/>
+      <c r="C52" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B53" s="0"/>
+      <c r="C53" s="1" t="n">
+        <f aca="false">AVERAGE(C35:C37)</f>
+        <v>173.567266666667</v>
+      </c>
+      <c r="D53" s="1" t="n">
+        <f aca="false">AVERAGE(D35:D37)</f>
+        <v>9.9711</v>
+      </c>
+      <c r="E53" s="1" t="n">
+        <f aca="false">AVERAGE(E35:E37)</f>
+        <v>2.914311111111</v>
+      </c>
+      <c r="F53" s="1" t="n">
+        <f aca="false">AVERAGE(F35:F37)</f>
+        <v>0.0213999999999999</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="n">
+        <v>61</v>
+      </c>
+      <c r="B54" s="0"/>
+      <c r="C54" s="1" t="n">
+        <f aca="false">AVERAGE(C38:C40)</f>
+        <v>429.965033333333</v>
+      </c>
+      <c r="D54" s="1" t="n">
+        <f aca="false">AVERAGE(D38:D40)</f>
+        <v>40.5999333333333</v>
+      </c>
+      <c r="E54" s="1" t="n">
+        <f aca="false">AVERAGE(E38:E40)</f>
+        <v>6.91691111111112</v>
+      </c>
+      <c r="F54" s="1" t="n">
+        <f aca="false">AVERAGE(F38:F40)</f>
+        <v>0.111377777777778</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="B55" s="0"/>
+      <c r="C55" s="1" t="n">
+        <f aca="false">AVERAGE(C41:C43)</f>
+        <v>540.105866666667</v>
+      </c>
+      <c r="D55" s="1" t="n">
+        <f aca="false">AVERAGE(D41:D43)</f>
+        <v>61.0253666666667</v>
+      </c>
+      <c r="E55" s="1" t="n">
+        <f aca="false">AVERAGE(E36:E41)</f>
+        <v>5.68259444444444</v>
+      </c>
+      <c r="F55" s="1" t="n">
+        <f aca="false">AVERAGE(F36:F41)</f>
+        <v>0.0980777777777782</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="n">
+        <v>129</v>
+      </c>
+      <c r="B56" s="0"/>
+      <c r="C56" s="1" t="n">
+        <f aca="false">AVERAGE(C44:C46)</f>
+        <v>860.550833333333</v>
+      </c>
+      <c r="D56" s="1" t="n">
+        <f aca="false">AVERAGE(D44:D46)</f>
+        <v>88.5572666666667</v>
+      </c>
+      <c r="E56" s="1" t="n">
+        <f aca="false">AVERAGE(E44:E46)</f>
+        <v>7.5854888888889</v>
+      </c>
+      <c r="F56" s="1" t="n">
+        <f aca="false">AVERAGE(F44:F46)</f>
+        <v>2.52522222222223</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="1" t="n">
+        <v>173</v>
+      </c>
+      <c r="B57" s="0"/>
+      <c r="C57" s="1" t="n">
+        <f aca="false">AVERAGE(C47:C49)</f>
+        <v>901.2422</v>
+      </c>
+      <c r="D57" s="1" t="n">
+        <f aca="false">AVERAGE(D47:D49)</f>
+        <v>126.3302</v>
+      </c>
+      <c r="E57" s="1" t="n">
+        <f aca="false">AVERAGE(E37:E42)</f>
+        <v>3.52888888888899</v>
+      </c>
+      <c r="F57" s="1" t="n">
+        <f aca="false">AVERAGE(F37:F42)</f>
+        <v>0.0970666666666654</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0"/>
+      <c r="B58" s="0"/>
+      <c r="C58" s="0"/>
+      <c r="D58" s="0"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0"/>
+      <c r="B59" s="0"/>
+      <c r="C59" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B52" s="0"/>
-      <c r="C52" s="1" t="n">
-        <f aca="false">SLOPE(C47:C49,$A$47:$A$49)</f>
-        <v>4.63769375908166</v>
-      </c>
-      <c r="D52" s="1" t="n">
-        <f aca="false">SLOPE(D47:D49,$A$47:$A$49)</f>
-        <v>0.745709869950596</v>
-      </c>
-    </row>
-    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="7"/>
-      <c r="B53" s="7"/>
-      <c r="C53" s="7"/>
-      <c r="D53" s="7" t="n">
-        <f aca="false">C52/D52</f>
-        <v>6.21916638891868</v>
+      <c r="B60" s="0"/>
+      <c r="C60" s="1" t="n">
+        <f aca="false">SLOPE(C53:C57,$A$53:$A$57)</f>
+        <v>4.93189325091575</v>
+      </c>
+      <c r="D60" s="1" t="n">
+        <f aca="false">SLOPE(D53:D57,$A$53:$A$57)</f>
+        <v>0.738274258241758</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="7"/>
+      <c r="B61" s="7"/>
+      <c r="C61" s="7"/>
+      <c r="D61" s="7" t="n">
+        <f aca="false">C60/D60</f>
+        <v>6.68029962559081</v>
       </c>
     </row>
   </sheetData>
@@ -2281,19 +2465,19 @@
   </sheetPr>
   <dimension ref="1:52"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J10" activeCellId="0" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="1" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="1" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="14.5612244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="1" width="11.0714285714286"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="1" width="13.2295918367347"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="14.3112244897959"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="1" width="10.8010204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2309,6 +2493,9 @@
       <c r="H1" s="0"/>
       <c r="I1" s="0"/>
       <c r="J1" s="0"/>
+      <c r="K1" s="0"/>
+      <c r="L1" s="0"/>
+      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -2324,6 +2511,8 @@
       <c r="I2" s="0"/>
       <c r="J2" s="0"/>
       <c r="K2" s="0"/>
+      <c r="L2" s="0"/>
+      <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
@@ -2346,6 +2535,7 @@
       </c>
       <c r="K3" s="0"/>
       <c r="L3" s="0"/>
+      <c r="AMJ3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -2364,6 +2554,8 @@
       <c r="F4" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="G4" s="0"/>
+      <c r="H4" s="0"/>
       <c r="I4" s="1" t="s">
         <v>33</v>
       </c>
@@ -2372,6 +2564,7 @@
       </c>
       <c r="K4" s="9"/>
       <c r="L4" s="9"/>
+      <c r="AMJ4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
@@ -2407,6 +2600,7 @@
       </c>
       <c r="K5" s="9"/>
       <c r="L5" s="9"/>
+      <c r="AMJ5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
@@ -2440,6 +2634,7 @@
       </c>
       <c r="K6" s="9"/>
       <c r="L6" s="9"/>
+      <c r="AMJ6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
@@ -2473,6 +2668,7 @@
       </c>
       <c r="K7" s="11"/>
       <c r="L7" s="9"/>
+      <c r="AMJ7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
@@ -2506,6 +2702,7 @@
       </c>
       <c r="K8" s="9"/>
       <c r="L8" s="9"/>
+      <c r="AMJ8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
@@ -2533,6 +2730,7 @@
         <v>1.6E-006</v>
       </c>
       <c r="H9" s="10"/>
+      <c r="I9" s="0"/>
       <c r="J9" s="8" t="n">
         <v>0.000243959832005</v>
       </c>
@@ -2541,6 +2739,7 @@
         <v>0.000331307973829</v>
       </c>
       <c r="L9" s="9"/>
+      <c r="AMJ9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
@@ -2561,8 +2760,10 @@
       <c r="G10" s="0"/>
       <c r="H10" s="0"/>
       <c r="I10" s="0"/>
+      <c r="J10" s="0"/>
       <c r="K10" s="9"/>
       <c r="L10" s="9"/>
+      <c r="AMJ10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
@@ -2584,9 +2785,13 @@
       <c r="F11" s="1" t="s">
         <v>32</v>
       </c>
+      <c r="G11" s="0"/>
+      <c r="H11" s="0"/>
       <c r="I11" s="0"/>
+      <c r="J11" s="0"/>
       <c r="K11" s="9"/>
       <c r="L11" s="9"/>
+      <c r="AMJ11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
@@ -2612,8 +2817,10 @@
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
       <c r="I12" s="0"/>
+      <c r="J12" s="0"/>
       <c r="K12" s="9"/>
       <c r="L12" s="9"/>
+      <c r="AMJ12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
@@ -2639,8 +2846,10 @@
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
       <c r="I13" s="0"/>
+      <c r="J13" s="0"/>
       <c r="K13" s="9"/>
       <c r="L13" s="9"/>
+      <c r="AMJ13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
@@ -2665,8 +2874,11 @@
       </c>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
+      <c r="I14" s="0"/>
+      <c r="J14" s="0"/>
       <c r="K14" s="9"/>
       <c r="L14" s="9"/>
+      <c r="AMJ14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
@@ -2692,8 +2904,10 @@
       <c r="G15" s="10"/>
       <c r="H15" s="10"/>
       <c r="I15" s="0"/>
+      <c r="J15" s="0"/>
       <c r="K15" s="9"/>
       <c r="L15" s="9"/>
+      <c r="AMJ15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
@@ -2719,8 +2933,10 @@
       <c r="G16" s="10"/>
       <c r="H16" s="10"/>
       <c r="I16" s="0"/>
+      <c r="J16" s="0"/>
       <c r="K16" s="9"/>
       <c r="L16" s="9"/>
+      <c r="AMJ16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
@@ -2740,8 +2956,10 @@
       <c r="F17" s="0"/>
       <c r="G17" s="0"/>
       <c r="H17" s="0"/>
+      <c r="I17" s="0"/>
       <c r="J17" s="9"/>
       <c r="K17" s="9"/>
+      <c r="AMJ17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
@@ -2761,8 +2979,10 @@
       <c r="F18" s="0"/>
       <c r="G18" s="0"/>
       <c r="H18" s="0"/>
+      <c r="I18" s="0"/>
       <c r="J18" s="9"/>
       <c r="K18" s="9"/>
+      <c r="AMJ18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
@@ -2781,8 +3001,11 @@
       <c r="E19" s="0"/>
       <c r="F19" s="0"/>
       <c r="G19" s="0"/>
+      <c r="H19" s="0"/>
+      <c r="I19" s="0"/>
       <c r="J19" s="9"/>
       <c r="K19" s="9"/>
+      <c r="AMJ19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
@@ -2802,8 +3025,10 @@
       <c r="F20" s="0"/>
       <c r="G20" s="0"/>
       <c r="H20" s="0"/>
+      <c r="I20" s="0"/>
       <c r="J20" s="9"/>
       <c r="K20" s="9"/>
+      <c r="AMJ20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
@@ -2823,8 +3048,10 @@
       <c r="F21" s="0"/>
       <c r="G21" s="0"/>
       <c r="H21" s="0"/>
+      <c r="I21" s="0"/>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
+      <c r="AMJ21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
@@ -2844,8 +3071,10 @@
       <c r="F22" s="0"/>
       <c r="G22" s="0"/>
       <c r="H22" s="0"/>
+      <c r="I22" s="0"/>
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
+      <c r="AMJ22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
@@ -2865,8 +3094,10 @@
       <c r="F23" s="0"/>
       <c r="G23" s="0"/>
       <c r="H23" s="0"/>
+      <c r="I23" s="0"/>
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
+      <c r="AMJ23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
@@ -2887,6 +3118,7 @@
       <c r="G24" s="0"/>
       <c r="H24" s="0"/>
       <c r="I24" s="0"/>
+      <c r="AMJ24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
@@ -2907,6 +3139,7 @@
       <c r="G25" s="0"/>
       <c r="H25" s="0"/>
       <c r="I25" s="0"/>
+      <c r="AMJ25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
@@ -3571,7 +3804,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B2:D37"/>
+  <dimension ref="B1:D37"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D21" activeCellId="0" sqref="D21"/>
@@ -3579,11 +3812,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.5204081632653"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="28.5663265306122"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="28.2142857142857"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D1" s="0"/>
+    </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="0" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
organized reward results, changed tex files
</commit_message>
<xml_diff>
--- a/stats/stats_compilation.xlsx
+++ b/stats/stats_compilation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="weights" sheetId="1" state="visible" r:id="rId2"/>
@@ -432,8 +432,8 @@
   </sheetPr>
   <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N12" activeCellId="0" sqref="N12"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C31" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N22" activeCellId="0" sqref="N22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2463,10 +2463,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:52"/>
+  <dimension ref="1:60"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J10" activeCellId="0" sqref="J10"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G53" activeCellId="0" sqref="G53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3374,306 +3374,338 @@
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="n">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="B37" s="1" t="n">
         <v>1</v>
       </c>
       <c r="C37" s="1" t="n">
-        <v>80.3965</v>
+        <v>41.161</v>
       </c>
       <c r="D37" s="1" t="n">
-        <v>48.0494</v>
+        <v>25.7084</v>
       </c>
       <c r="E37" s="1" t="n">
-        <v>77.837</v>
+        <v>39.3326</v>
       </c>
       <c r="F37" s="1" t="n">
-        <v>45.9833</v>
+        <v>23.9268</v>
       </c>
       <c r="G37" s="1" t="n">
         <f aca="false">C37-E37</f>
-        <v>2.5595</v>
+        <v>1.8284</v>
       </c>
       <c r="H37" s="1" t="n">
         <f aca="false">D37-F37</f>
-        <v>2.0661</v>
+        <v>1.7816</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="n">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="B38" s="1" t="n">
         <v>2</v>
       </c>
       <c r="C38" s="1" t="n">
-        <v>82.2621</v>
+        <v>43.3183</v>
       </c>
       <c r="D38" s="1" t="n">
-        <v>47.99</v>
+        <v>26.524</v>
       </c>
       <c r="E38" s="1" t="n">
-        <v>79.559</v>
+        <v>41.464</v>
       </c>
       <c r="F38" s="1" t="n">
-        <v>45.9413</v>
+        <v>24.7341</v>
       </c>
       <c r="G38" s="1" t="n">
         <f aca="false">C38-E38</f>
-        <v>2.70310000000001</v>
+        <v>1.8543</v>
       </c>
       <c r="H38" s="1" t="n">
         <f aca="false">D38-F38</f>
-        <v>2.0487</v>
+        <v>1.7899</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="B39" s="1" t="n">
         <v>3</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>77.5451</v>
+        <v>40.7954</v>
       </c>
       <c r="D39" s="1" t="n">
-        <v>49.4514</v>
+        <v>25.4616</v>
       </c>
       <c r="E39" s="1" t="n">
-        <v>75.0593</v>
+        <v>39.0132</v>
       </c>
       <c r="F39" s="1" t="n">
-        <v>47.4115</v>
+        <v>23.7196</v>
       </c>
       <c r="G39" s="1" t="n">
         <f aca="false">C39-E39</f>
-        <v>2.48580000000001</v>
+        <v>1.7822</v>
       </c>
       <c r="H39" s="1" t="n">
         <f aca="false">D39-F39</f>
-        <v>2.0399</v>
+        <v>1.742</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="n">
-        <v>116</v>
+        <v>55</v>
       </c>
       <c r="B40" s="1" t="n">
         <v>1</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>299.8727</v>
+        <v>80.3965</v>
       </c>
       <c r="D40" s="1" t="n">
-        <v>163.6952</v>
+        <v>48.0494</v>
       </c>
       <c r="E40" s="1" t="n">
-        <v>290.2085</v>
+        <v>77.837</v>
       </c>
       <c r="F40" s="1" t="n">
-        <v>160.7069</v>
+        <v>45.9833</v>
       </c>
       <c r="G40" s="1" t="n">
         <f aca="false">C40-E40</f>
-        <v>9.66419999999999</v>
+        <v>2.5595</v>
       </c>
       <c r="H40" s="1" t="n">
         <f aca="false">D40-F40</f>
-        <v>2.98830000000001</v>
+        <v>2.0661</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="n">
-        <v>116</v>
+        <v>55</v>
       </c>
       <c r="B41" s="1" t="n">
         <v>2</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>314.5035</v>
+        <v>82.2621</v>
       </c>
       <c r="D41" s="1" t="n">
-        <v>158.9194</v>
+        <v>47.99</v>
       </c>
       <c r="E41" s="1" t="n">
-        <v>304.5913</v>
+        <v>79.559</v>
       </c>
       <c r="F41" s="1" t="n">
-        <v>155.9664</v>
+        <v>45.9413</v>
       </c>
       <c r="G41" s="1" t="n">
         <f aca="false">C41-E41</f>
-        <v>9.91219999999998</v>
+        <v>2.70310000000001</v>
       </c>
       <c r="H41" s="1" t="n">
         <f aca="false">D41-F41</f>
-        <v>2.953</v>
+        <v>2.0487</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
-        <v>116</v>
+        <v>55</v>
       </c>
       <c r="B42" s="1" t="n">
         <v>3</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>317.9456</v>
+        <v>77.5451</v>
       </c>
       <c r="D42" s="1" t="n">
-        <v>166.705</v>
+        <v>49.4514</v>
       </c>
       <c r="E42" s="1" t="n">
-        <v>307.8481</v>
+        <v>75.0593</v>
       </c>
       <c r="F42" s="1" t="n">
-        <v>163.6936</v>
+        <v>47.4115</v>
       </c>
       <c r="G42" s="1" t="n">
         <f aca="false">C42-E42</f>
-        <v>10.0975</v>
+        <v>2.48580000000001</v>
       </c>
       <c r="H42" s="1" t="n">
         <f aca="false">D42-F42</f>
-        <v>3.01140000000001</v>
+        <v>2.0399</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0"/>
-      <c r="B43" s="0"/>
-      <c r="C43" s="0"/>
-      <c r="D43" s="0"/>
-      <c r="E43" s="0"/>
-      <c r="F43" s="0"/>
-      <c r="G43" s="0"/>
-      <c r="H43" s="0"/>
+      <c r="A43" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="B43" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C43" s="1" t="n">
+        <v>163.09</v>
+      </c>
+      <c r="D43" s="1" t="n">
+        <v>103.1971</v>
+      </c>
+      <c r="E43" s="1" t="n">
+        <v>158.4996</v>
+      </c>
+      <c r="F43" s="1" t="n">
+        <v>100.6963</v>
+      </c>
+      <c r="G43" s="1" t="n">
+        <f aca="false">C43-E43</f>
+        <v>4.59040000000002</v>
+      </c>
+      <c r="H43" s="1" t="n">
+        <f aca="false">D43-F43</f>
+        <v>2.50080000000001</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B44" s="0"/>
-      <c r="C44" s="0"/>
-      <c r="D44" s="0"/>
-      <c r="E44" s="0"/>
-      <c r="F44" s="0"/>
-      <c r="G44" s="0"/>
-      <c r="H44" s="0"/>
+      <c r="A44" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="B44" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C44" s="1" t="n">
+        <v>163.909</v>
+      </c>
+      <c r="D44" s="1" t="n">
+        <v>100.0818</v>
+      </c>
+      <c r="E44" s="1" t="n">
+        <v>159.2891</v>
+      </c>
+      <c r="F44" s="1" t="n">
+        <v>97.5565</v>
+      </c>
+      <c r="G44" s="1" t="n">
+        <f aca="false">C44-E44</f>
+        <v>4.6199</v>
+      </c>
+      <c r="H44" s="1" t="n">
+        <f aca="false">D44-F44</f>
+        <v>2.5253</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="B45" s="0"/>
-      <c r="C45" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D45" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="E45" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F45" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G45" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="H45" s="1" t="s">
-        <v>16</v>
+      <c r="A45" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="B45" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C45" s="1" t="n">
+        <v>159.2058</v>
+      </c>
+      <c r="D45" s="1" t="n">
+        <v>99.6557</v>
+      </c>
+      <c r="E45" s="1" t="n">
+        <v>154.9584</v>
+      </c>
+      <c r="F45" s="1" t="n">
+        <v>97.157</v>
+      </c>
+      <c r="G45" s="1" t="n">
+        <f aca="false">C45-E45</f>
+        <v>4.2474</v>
+      </c>
+      <c r="H45" s="1" t="n">
+        <f aca="false">D45-F45</f>
+        <v>2.4987</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="n">
-        <v>11</v>
-      </c>
-      <c r="B46" s="0"/>
+        <v>116</v>
+      </c>
+      <c r="B46" s="1" t="n">
+        <v>1</v>
+      </c>
       <c r="C46" s="1" t="n">
-        <f aca="false">AVERAGE(C34:C36)</f>
-        <v>14.2092333333333</v>
+        <v>299.8727</v>
       </c>
       <c r="D46" s="1" t="n">
-        <f aca="false">AVERAGE(D34:D36)</f>
-        <v>8.13406666666667</v>
+        <v>163.6952</v>
       </c>
       <c r="E46" s="1" t="n">
-        <f aca="false">AVERAGE(E34:E36)</f>
-        <v>12.9574666666667</v>
+        <v>290.2085</v>
       </c>
       <c r="F46" s="1" t="n">
-        <f aca="false">AVERAGE(F34:F36)</f>
-        <v>6.70373333333333</v>
+        <v>160.7069</v>
       </c>
       <c r="G46" s="1" t="n">
-        <f aca="false">AVERAGE(G34:G36)</f>
-        <v>1.25176666666667</v>
+        <f aca="false">C46-E46</f>
+        <v>9.66419999999999</v>
       </c>
       <c r="H46" s="1" t="n">
-        <f aca="false">AVERAGE(H34:H36)</f>
-        <v>1.43033333333333</v>
+        <f aca="false">D46-F46</f>
+        <v>2.98830000000001</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="n">
-        <v>55</v>
-      </c>
-      <c r="B47" s="0"/>
+        <v>116</v>
+      </c>
+      <c r="B47" s="1" t="n">
+        <v>2</v>
+      </c>
       <c r="C47" s="1" t="n">
-        <f aca="false">AVERAGE(C37:C39)</f>
-        <v>80.0679</v>
+        <v>314.5035</v>
       </c>
       <c r="D47" s="1" t="n">
-        <f aca="false">AVERAGE(D37:D39)</f>
-        <v>48.4969333333333</v>
+        <v>158.9194</v>
       </c>
       <c r="E47" s="1" t="n">
-        <f aca="false">AVERAGE(E37:E39)</f>
-        <v>77.4851</v>
+        <v>304.5913</v>
       </c>
       <c r="F47" s="1" t="n">
-        <f aca="false">AVERAGE(F37:F39)</f>
-        <v>46.4453666666667</v>
+        <v>155.9664</v>
       </c>
       <c r="G47" s="1" t="n">
-        <f aca="false">AVERAGE(G37:G39)</f>
-        <v>2.58280000000001</v>
+        <f aca="false">C47-E47</f>
+        <v>9.91219999999998</v>
       </c>
       <c r="H47" s="1" t="n">
-        <f aca="false">AVERAGE(H37:H39)</f>
-        <v>2.05156666666667</v>
+        <f aca="false">D47-F47</f>
+        <v>2.953</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="n">
         <v>116</v>
       </c>
-      <c r="B48" s="0"/>
+      <c r="B48" s="1" t="n">
+        <v>3</v>
+      </c>
       <c r="C48" s="1" t="n">
-        <f aca="false">AVERAGE(C40:C42)</f>
-        <v>310.773933333333</v>
+        <v>317.9456</v>
       </c>
       <c r="D48" s="1" t="n">
-        <f aca="false">AVERAGE(D40:D42)</f>
-        <v>163.106533333333</v>
+        <v>166.705</v>
       </c>
       <c r="E48" s="1" t="n">
-        <f aca="false">AVERAGE(E40:E42)</f>
-        <v>300.882633333333</v>
+        <v>307.8481</v>
       </c>
       <c r="F48" s="1" t="n">
-        <f aca="false">AVERAGE(F40:F42)</f>
-        <v>160.1223</v>
+        <v>163.6936</v>
       </c>
       <c r="G48" s="1" t="n">
-        <f aca="false">AVERAGE(G40:G42)</f>
-        <v>9.8913</v>
+        <f aca="false">C48-E48</f>
+        <v>10.0975</v>
       </c>
       <c r="H48" s="1" t="n">
-        <f aca="false">AVERAGE(H40:H42)</f>
-        <v>2.98423333333334</v>
+        <f aca="false">D48-F48</f>
+        <v>3.01140000000001</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3687,76 +3719,272 @@
       <c r="H49" s="0"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0"/>
+      <c r="A50" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="B50" s="0"/>
-      <c r="C50" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E50" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="F50" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G50" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="H50" s="1" t="s">
-        <v>23</v>
-      </c>
+      <c r="C50" s="0"/>
+      <c r="D50" s="0"/>
+      <c r="E50" s="0"/>
+      <c r="F50" s="0"/>
+      <c r="G50" s="0"/>
+      <c r="H50" s="0"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B51" s="0"/>
+      <c r="C51" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F51" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G51" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H51" s="1" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B52" s="0"/>
+      <c r="C52" s="1" t="n">
+        <f aca="false">AVERAGE(C34:C36)</f>
+        <v>14.2092333333333</v>
+      </c>
+      <c r="D52" s="1" t="n">
+        <f aca="false">AVERAGE(D34:D36)</f>
+        <v>8.13406666666667</v>
+      </c>
+      <c r="E52" s="1" t="n">
+        <f aca="false">AVERAGE(E34:E36)</f>
+        <v>12.9574666666667</v>
+      </c>
+      <c r="F52" s="1" t="n">
+        <f aca="false">AVERAGE(F34:F36)</f>
+        <v>6.70373333333333</v>
+      </c>
+      <c r="G52" s="1" t="n">
+        <f aca="false">AVERAGE(G34:G36)</f>
+        <v>1.25176666666667</v>
+      </c>
+      <c r="H52" s="1" t="n">
+        <f aca="false">AVERAGE(H34:H36)</f>
+        <v>1.43033333333333</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B53" s="0"/>
+      <c r="C53" s="1" t="n">
+        <f aca="false">AVERAGE(C37:C39)</f>
+        <v>41.7582333333333</v>
+      </c>
+      <c r="D53" s="1" t="n">
+        <f aca="false">AVERAGE(D37:D39)</f>
+        <v>25.898</v>
+      </c>
+      <c r="E53" s="1" t="n">
+        <f aca="false">AVERAGE(E37:E39)</f>
+        <v>39.9366</v>
+      </c>
+      <c r="F53" s="1" t="n">
+        <f aca="false">AVERAGE(F37:F39)</f>
+        <v>24.1268333333333</v>
+      </c>
+      <c r="G53" s="1" t="n">
+        <f aca="false">AVERAGE(G37:G39)</f>
+        <v>1.82163333333334</v>
+      </c>
+      <c r="H53" s="1" t="n">
+        <f aca="false">AVERAGE(H37:H39)</f>
+        <v>1.77116666666667</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B54" s="0"/>
+      <c r="C54" s="1" t="n">
+        <f aca="false">AVERAGE(C40:C42)</f>
+        <v>80.0679</v>
+      </c>
+      <c r="D54" s="1" t="n">
+        <f aca="false">AVERAGE(D40:D42)</f>
+        <v>48.4969333333333</v>
+      </c>
+      <c r="E54" s="1" t="n">
+        <f aca="false">AVERAGE(E40:E42)</f>
+        <v>77.4851</v>
+      </c>
+      <c r="F54" s="1" t="n">
+        <f aca="false">AVERAGE(F40:F42)</f>
+        <v>46.4453666666667</v>
+      </c>
+      <c r="G54" s="1" t="n">
+        <f aca="false">AVERAGE(G40:G42)</f>
+        <v>2.58280000000001</v>
+      </c>
+      <c r="H54" s="1" t="n">
+        <f aca="false">AVERAGE(H40:H42)</f>
+        <v>2.05156666666667</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="B55" s="0"/>
+      <c r="C55" s="1" t="n">
+        <f aca="false">AVERAGE(C43:C45)</f>
+        <v>162.068266666667</v>
+      </c>
+      <c r="D55" s="1" t="n">
+        <f aca="false">AVERAGE(D43:D45)</f>
+        <v>100.9782</v>
+      </c>
+      <c r="E55" s="1" t="n">
+        <f aca="false">AVERAGE(E43:E45)</f>
+        <v>157.582366666667</v>
+      </c>
+      <c r="F55" s="1" t="n">
+        <f aca="false">AVERAGE(F43:F45)</f>
+        <v>98.4699333333333</v>
+      </c>
+      <c r="G55" s="1" t="n">
+        <f aca="false">AVERAGE(G43:G45)</f>
+        <v>4.48590000000001</v>
+      </c>
+      <c r="H55" s="1" t="n">
+        <f aca="false">AVERAGE(H43:H45)</f>
+        <v>2.50826666666667</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="1" t="n">
+        <v>116</v>
+      </c>
+      <c r="B56" s="0"/>
+      <c r="C56" s="1" t="n">
+        <f aca="false">AVERAGE(C46:C48)</f>
+        <v>310.773933333333</v>
+      </c>
+      <c r="D56" s="1" t="n">
+        <f aca="false">AVERAGE(D46:D48)</f>
+        <v>163.106533333333</v>
+      </c>
+      <c r="E56" s="1" t="n">
+        <f aca="false">AVERAGE(E46:E48)</f>
+        <v>300.882633333333</v>
+      </c>
+      <c r="F56" s="1" t="n">
+        <f aca="false">AVERAGE(F46:F48)</f>
+        <v>160.1223</v>
+      </c>
+      <c r="G56" s="1" t="n">
+        <f aca="false">AVERAGE(G46:G48)</f>
+        <v>9.8913</v>
+      </c>
+      <c r="H56" s="1" t="n">
+        <f aca="false">AVERAGE(H46:H48)</f>
+        <v>2.98423333333334</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0"/>
+      <c r="B57" s="0"/>
+      <c r="C57" s="0"/>
+      <c r="D57" s="0"/>
+      <c r="E57" s="0"/>
+      <c r="F57" s="0"/>
+      <c r="G57" s="0"/>
+      <c r="H57" s="0"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0"/>
+      <c r="B58" s="0"/>
+      <c r="C58" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F58" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G58" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H58" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B51" s="0"/>
-      <c r="C51" s="1" t="n">
-        <f aca="false">SLOPE(C46:C48,$A$46:$A$48)</f>
-        <v>2.88395533309355</v>
-      </c>
-      <c r="D51" s="1" t="n">
-        <f aca="false">SLOPE(D46:D48,$A$46:$A$48)</f>
-        <v>1.50097474723255</v>
-      </c>
-      <c r="E51" s="1" t="n">
-        <f aca="false">SLOPE(E46:E48,$A$46:$A$48)</f>
-        <v>2.79934108020621</v>
-      </c>
-      <c r="F51" s="1" t="n">
-        <f aca="false">SLOPE(F46:F48,$A$46:$A$48)</f>
-        <v>1.48614520441194</v>
-      </c>
-      <c r="G51" s="1" t="n">
-        <f aca="false">SLOPE(G46:G48,$A$46:$A$48)</f>
-        <v>0.0846142528873437</v>
-      </c>
-      <c r="H51" s="1" t="n">
-        <f aca="false">SLOPE(H46:H48,$A$46:$A$48)</f>
-        <v>0.0148295428206051</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="7" t="s">
+      <c r="B59" s="0"/>
+      <c r="C59" s="1" t="n">
+        <f aca="false">SLOPE(C52:C56,$A$52:$A$56)</f>
+        <v>2.79993953194738</v>
+      </c>
+      <c r="D59" s="1" t="n">
+        <f aca="false">SLOPE(D52:D56,$A$52:$A$56)</f>
+        <v>1.50212465351186</v>
+      </c>
+      <c r="E59" s="1" t="n">
+        <f aca="false">SLOPE(E52:E56,$A$52:$A$56)</f>
+        <v>2.72091446441155</v>
+      </c>
+      <c r="F59" s="1" t="n">
+        <f aca="false">SLOPE(F52:F56,$A$52:$A$56)</f>
+        <v>1.4873104983948</v>
+      </c>
+      <c r="G59" s="1" t="n">
+        <f aca="false">SLOPE(G52:G56,$A$52:$A$56)</f>
+        <v>0.0790250675358234</v>
+      </c>
+      <c r="H59" s="1" t="n">
+        <f aca="false">SLOPE(H52:H56,$A$52:$A$56)</f>
+        <v>0.0148141551170622</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="B52" s="7"/>
-      <c r="C52" s="7"/>
-      <c r="D52" s="7" t="n">
-        <f aca="false">C51/D51</f>
-        <v>1.92138831010376</v>
-      </c>
-      <c r="E52" s="7"/>
-      <c r="F52" s="7" t="n">
-        <f aca="false">E51/F51</f>
-        <v>1.8836255514574</v>
-      </c>
-      <c r="G52" s="7"/>
-      <c r="H52" s="7" t="n">
-        <f aca="false">G51/H51</f>
-        <v>5.70578971387946</v>
+      <c r="B60" s="7"/>
+      <c r="C60" s="7"/>
+      <c r="D60" s="7" t="n">
+        <f aca="false">C59/D59</f>
+        <v>1.86398613816857</v>
+      </c>
+      <c r="E60" s="7"/>
+      <c r="F60" s="7" t="n">
+        <f aca="false">E59/F59</f>
+        <v>1.82941925532573</v>
+      </c>
+      <c r="G60" s="7"/>
+      <c r="H60" s="7" t="n">
+        <f aca="false">G59/H59</f>
+        <v>5.33442959867528</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
revised language and updated gpu weights results
</commit_message>
<xml_diff>
--- a/stats/stats_compilation.xlsx
+++ b/stats/stats_compilation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="weights" sheetId="1" state="visible" r:id="rId2"/>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="42">
   <si>
     <t xml:space="preserve">stats</t>
   </si>
@@ -126,6 +126,12 @@
     <t xml:space="preserve">+-gpu</t>
   </si>
   <si>
+    <t xml:space="preserve">speedup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">speedup+-</t>
+  </si>
+  <si>
     <t xml:space="preserve">scaling on cpu</t>
   </si>
   <si>
@@ -178,9 +184,6 @@
   </si>
   <si>
     <t xml:space="preserve">batch_size (J)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">speedup</t>
   </si>
 </sst>
 </file>
@@ -432,28 +435,28 @@
   </sheetPr>
   <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C31" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="N22" activeCellId="0" sqref="N22"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A29" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I57" activeCellId="0" sqref="I57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="9.31632653061224"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="7.02040816326531"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="9.98979591836735"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="9.17857142857143"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="6.88265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="1" width="10.6632653061225"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1932,25 +1935,25 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="1" t="n">
+      <c r="A35" s="2" t="n">
         <v>17</v>
       </c>
       <c r="B35" s="1" t="n">
         <v>1</v>
       </c>
       <c r="C35" s="1" t="n">
-        <v>173.5709</v>
+        <v>120.3339</v>
       </c>
       <c r="D35" s="1" t="n">
-        <v>9.945</v>
+        <v>12.5933</v>
       </c>
       <c r="E35" s="1" t="n">
         <f aca="false">ABS(C$53-C35)</f>
-        <v>0.0036333333329992</v>
+        <v>2.0993</v>
       </c>
       <c r="F35" s="1" t="n">
         <f aca="false">ABS(D$53-D35)</f>
-        <v>0.0260999999999996</v>
+        <v>0.0324333333333318</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1961,18 +1964,18 @@
         <v>2</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>177.9351</v>
+        <v>118.7848</v>
       </c>
       <c r="D36" s="1" t="n">
-        <v>10.0032</v>
+        <v>12.5573</v>
       </c>
       <c r="E36" s="1" t="n">
         <f aca="false">ABS(C$53-C36)</f>
-        <v>4.36783333333301</v>
+        <v>0.550200000000004</v>
       </c>
       <c r="F36" s="1" t="n">
         <f aca="false">ABS(D$53-D36)</f>
-        <v>0.0320999999999998</v>
+        <v>0.00356666666666783</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1983,106 +1986,106 @@
         <v>3</v>
       </c>
       <c r="C37" s="1" t="n">
-        <v>169.1958</v>
+        <v>115.5851</v>
       </c>
       <c r="D37" s="1" t="n">
-        <v>9.9651</v>
+        <v>12.532</v>
       </c>
       <c r="E37" s="1" t="n">
         <f aca="false">ABS(C$53-C37)</f>
-        <v>4.371466666667</v>
+        <v>2.6495</v>
       </c>
       <c r="F37" s="1" t="n">
         <f aca="false">ABS(D$53-D37)</f>
-        <v>0.00600000000000023</v>
+        <v>0.0288666666666675</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="1" t="n">
-        <v>61</v>
+      <c r="A38" s="2" t="n">
+        <v>51</v>
       </c>
       <c r="B38" s="1" t="n">
         <v>1</v>
       </c>
       <c r="C38" s="1" t="n">
-        <v>440.3404</v>
+        <v>342.3194</v>
       </c>
       <c r="D38" s="1" t="n">
-        <v>40.767</v>
+        <v>35.7989</v>
       </c>
       <c r="E38" s="1" t="n">
         <f aca="false">ABS(C$54-C38)</f>
-        <v>10.3753666666667</v>
+        <v>3.00706666666667</v>
       </c>
       <c r="F38" s="1" t="n">
         <f aca="false">ABS(D$54-D38)</f>
-        <v>0.16706666666667</v>
+        <v>0.0536666666666648</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B39" s="1" t="n">
         <v>2</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>426.5965</v>
+        <v>347.6656</v>
       </c>
       <c r="D39" s="1" t="n">
-        <v>40.5242</v>
+        <v>35.5587</v>
       </c>
       <c r="E39" s="1" t="n">
         <f aca="false">ABS(C$54-C39)</f>
-        <v>3.36853333333335</v>
+        <v>2.33913333333334</v>
       </c>
       <c r="F39" s="1" t="n">
         <f aca="false">ABS(D$54-D39)</f>
-        <v>0.0757333333333321</v>
+        <v>0.293866666666666</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="n">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B40" s="1" t="n">
         <v>3</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>422.9582</v>
+        <v>345.9944</v>
       </c>
       <c r="D40" s="1" t="n">
-        <v>40.5086</v>
+        <v>36.2001</v>
       </c>
       <c r="E40" s="1" t="n">
         <f aca="false">ABS(C$54-C40)</f>
-        <v>7.00683333333336</v>
+        <v>0.667933333333338</v>
       </c>
       <c r="F40" s="1" t="n">
         <f aca="false">ABS(D$54-D40)</f>
-        <v>0.0913333333333313</v>
+        <v>0.347533333333331</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="1" t="n">
+      <c r="A41" s="2" t="n">
         <v>85</v>
       </c>
       <c r="B41" s="1" t="n">
         <v>1</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>544.7114</v>
+        <v>546.23</v>
       </c>
       <c r="D41" s="1" t="n">
-        <v>61.2416</v>
+        <v>59.0627</v>
       </c>
       <c r="E41" s="1" t="n">
         <f aca="false">ABS(C$55-C41)</f>
-        <v>4.60553333333326</v>
+        <v>1.35759999999993</v>
       </c>
       <c r="F41" s="1" t="n">
         <f aca="false">ABS(D$55-D41)</f>
-        <v>0.216233333333335</v>
+        <v>0.0576666666666625</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2093,18 +2096,18 @@
         <v>2</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>538.4962</v>
+        <v>547.8033</v>
       </c>
       <c r="D42" s="1" t="n">
-        <v>60.9564</v>
+        <v>59.3535</v>
       </c>
       <c r="E42" s="1" t="n">
         <f aca="false">ABS(C$55-C42)</f>
-        <v>1.60966666666673</v>
+        <v>0.215700000000083</v>
       </c>
       <c r="F42" s="1" t="n">
         <f aca="false">ABS(D$55-D42)</f>
-        <v>0.0689666666666611</v>
+        <v>0.233133333333335</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2115,40 +2118,40 @@
         <v>3</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>537.11</v>
+        <v>548.7295</v>
       </c>
       <c r="D43" s="1" t="n">
-        <v>60.8781</v>
+        <v>58.9449</v>
       </c>
       <c r="E43" s="1" t="n">
         <f aca="false">ABS(C$55-C43)</f>
-        <v>2.99586666666676</v>
+        <v>1.14190000000008</v>
       </c>
       <c r="F43" s="1" t="n">
         <f aca="false">ABS(D$55-D43)</f>
-        <v>0.14726666666666</v>
+        <v>0.175466666666665</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="1" t="n">
+      <c r="A44" s="2" t="n">
         <v>129</v>
       </c>
       <c r="B44" s="1" t="n">
         <v>1</v>
       </c>
       <c r="C44" s="1" t="n">
-        <v>865.2712</v>
+        <v>868.9906</v>
       </c>
       <c r="D44" s="1" t="n">
-        <v>92.3451</v>
+        <v>111.4689</v>
       </c>
       <c r="E44" s="1" t="n">
         <f aca="false">ABS(C$56-C44)</f>
-        <v>4.72036666666668</v>
+        <v>2.01636666666673</v>
       </c>
       <c r="F44" s="1" t="n">
         <f aca="false">ABS(D$56-D44)</f>
-        <v>3.78783333333332</v>
+        <v>3.51679999999999</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2159,18 +2162,18 @@
         <v>2</v>
       </c>
       <c r="C45" s="1" t="n">
-        <v>849.1726</v>
+        <v>868.381</v>
       </c>
       <c r="D45" s="1" t="n">
-        <v>86.5314</v>
+        <v>123.6168</v>
       </c>
       <c r="E45" s="1" t="n">
         <f aca="false">ABS(C$56-C45)</f>
-        <v>11.3782333333334</v>
+        <v>2.62596666666673</v>
       </c>
       <c r="F45" s="1" t="n">
         <f aca="false">ABS(D$56-D45)</f>
-        <v>2.02586666666667</v>
+        <v>15.6647</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2181,40 +2184,40 @@
         <v>3</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>867.2087</v>
+        <v>875.6493</v>
       </c>
       <c r="D46" s="1" t="n">
-        <v>86.7953</v>
+        <v>88.7706</v>
       </c>
       <c r="E46" s="1" t="n">
         <f aca="false">ABS(C$56-C46)</f>
-        <v>6.65786666666668</v>
+        <v>4.64233333333334</v>
       </c>
       <c r="F46" s="1" t="n">
         <f aca="false">ABS(D$56-D46)</f>
-        <v>1.76196666666668</v>
+        <v>19.1815</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="1" t="n">
+      <c r="A47" s="2" t="n">
         <v>173</v>
       </c>
       <c r="B47" s="1" t="n">
         <v>1</v>
       </c>
       <c r="C47" s="1" t="n">
-        <v>899.8638</v>
+        <v>1068.876</v>
       </c>
       <c r="D47" s="1" t="n">
-        <v>126.035</v>
+        <v>119.2222</v>
       </c>
       <c r="E47" s="1" t="n">
         <f aca="false">ABS(C$57-C47)</f>
-        <v>1.37840000000006</v>
+        <v>26.3657333333333</v>
       </c>
       <c r="F47" s="1" t="n">
         <f aca="false">ABS(D$57-D47)</f>
-        <v>0.295200000000008</v>
+        <v>3.49953333333332</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2225,18 +2228,18 @@
         <v>2</v>
       </c>
       <c r="C48" s="1" t="n">
-        <v>907.0222</v>
+        <v>1152.8102</v>
       </c>
       <c r="D48" s="1" t="n">
-        <v>126.388</v>
+        <v>129.2446</v>
       </c>
       <c r="E48" s="1" t="n">
         <f aca="false">ABS(C$57-C48)</f>
-        <v>5.77999999999997</v>
+        <v>57.5684666666666</v>
       </c>
       <c r="F48" s="1" t="n">
         <f aca="false">ABS(D$57-D48)</f>
-        <v>0.0578000000000003</v>
+        <v>6.52286666666667</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2247,18 +2250,18 @@
         <v>3</v>
       </c>
       <c r="C49" s="1" t="n">
-        <v>896.8406</v>
+        <v>1064.039</v>
       </c>
       <c r="D49" s="1" t="n">
-        <v>126.5676</v>
+        <v>119.6984</v>
       </c>
       <c r="E49" s="1" t="n">
         <f aca="false">ABS(C$57-C49)</f>
-        <v>4.40160000000003</v>
+        <v>31.2027333333333</v>
       </c>
       <c r="F49" s="1" t="n">
         <f aca="false">ABS(D$57-D49)</f>
-        <v>0.237399999999994</v>
+        <v>3.02333333333331</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2296,6 +2299,12 @@
       <c r="F52" s="1" t="s">
         <v>21</v>
       </c>
+      <c r="G52" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>23</v>
+      </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="n">
@@ -2304,41 +2313,57 @@
       <c r="B53" s="0"/>
       <c r="C53" s="1" t="n">
         <f aca="false">AVERAGE(C35:C37)</f>
-        <v>173.567266666667</v>
+        <v>118.2346</v>
       </c>
       <c r="D53" s="1" t="n">
         <f aca="false">AVERAGE(D35:D37)</f>
-        <v>9.9711</v>
+        <v>12.5608666666667</v>
       </c>
       <c r="E53" s="1" t="n">
         <f aca="false">AVERAGE(E35:E37)</f>
-        <v>2.914311111111</v>
+        <v>1.76633333333334</v>
       </c>
       <c r="F53" s="1" t="n">
         <f aca="false">AVERAGE(F35:F37)</f>
-        <v>0.0213999999999999</v>
+        <v>0.0216222222222224</v>
+      </c>
+      <c r="G53" s="1" t="n">
+        <f aca="false">C53/D53</f>
+        <v>9.41293329016575</v>
+      </c>
+      <c r="H53" s="1" t="n">
+        <f aca="false">ABS($G$58-G53)</f>
+        <v>0.352916609290604</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="n">
-        <v>61</v>
+        <v>51</v>
       </c>
       <c r="B54" s="0"/>
       <c r="C54" s="1" t="n">
         <f aca="false">AVERAGE(C38:C40)</f>
-        <v>429.965033333333</v>
+        <v>345.326466666667</v>
       </c>
       <c r="D54" s="1" t="n">
         <f aca="false">AVERAGE(D38:D40)</f>
-        <v>40.5999333333333</v>
+        <v>35.8525666666667</v>
       </c>
       <c r="E54" s="1" t="n">
         <f aca="false">AVERAGE(E38:E40)</f>
-        <v>6.91691111111112</v>
+        <v>2.00471111111112</v>
       </c>
       <c r="F54" s="1" t="n">
         <f aca="false">AVERAGE(F38:F40)</f>
-        <v>0.111377777777778</v>
+        <v>0.231688888888887</v>
+      </c>
+      <c r="G54" s="1" t="n">
+        <f aca="false">C54/D54</f>
+        <v>9.6318478360917</v>
+      </c>
+      <c r="H54" s="1" t="n">
+        <f aca="false">ABS($G$58-G54)</f>
+        <v>0.57183115521655</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2348,19 +2373,27 @@
       <c r="B55" s="0"/>
       <c r="C55" s="1" t="n">
         <f aca="false">AVERAGE(C41:C43)</f>
-        <v>540.105866666667</v>
+        <v>547.5876</v>
       </c>
       <c r="D55" s="1" t="n">
         <f aca="false">AVERAGE(D41:D43)</f>
-        <v>61.0253666666667</v>
+        <v>59.1203666666667</v>
       </c>
       <c r="E55" s="1" t="n">
         <f aca="false">AVERAGE(E36:E41)</f>
-        <v>5.68259444444444</v>
+        <v>1.76190555555555</v>
       </c>
       <c r="F55" s="1" t="n">
         <f aca="false">AVERAGE(F36:F41)</f>
-        <v>0.0980777777777782</v>
+        <v>0.13086111111111</v>
+      </c>
+      <c r="G55" s="1" t="n">
+        <f aca="false">C55/D55</f>
+        <v>9.26224972668753</v>
+      </c>
+      <c r="H55" s="1" t="n">
+        <f aca="false">ABS($G$58-G55)</f>
+        <v>0.202233045812385</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2370,19 +2403,27 @@
       <c r="B56" s="0"/>
       <c r="C56" s="1" t="n">
         <f aca="false">AVERAGE(C44:C46)</f>
-        <v>860.550833333333</v>
+        <v>871.006966666667</v>
       </c>
       <c r="D56" s="1" t="n">
         <f aca="false">AVERAGE(D44:D46)</f>
-        <v>88.5572666666667</v>
+        <v>107.9521</v>
       </c>
       <c r="E56" s="1" t="n">
         <f aca="false">AVERAGE(E44:E46)</f>
-        <v>7.5854888888889</v>
+        <v>3.09488888888893</v>
       </c>
       <c r="F56" s="1" t="n">
         <f aca="false">AVERAGE(F44:F46)</f>
-        <v>2.52522222222223</v>
+        <v>12.7876666666667</v>
+      </c>
+      <c r="G56" s="1" t="n">
+        <f aca="false">C56/D56</f>
+        <v>8.06845783145179</v>
+      </c>
+      <c r="H56" s="1" t="n">
+        <f aca="false">ABS($G$58-G56)</f>
+        <v>0.99155884942336</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2392,19 +2433,27 @@
       <c r="B57" s="0"/>
       <c r="C57" s="1" t="n">
         <f aca="false">AVERAGE(C47:C49)</f>
-        <v>901.2422</v>
+        <v>1095.24173333333</v>
       </c>
       <c r="D57" s="1" t="n">
         <f aca="false">AVERAGE(D47:D49)</f>
-        <v>126.3302</v>
+        <v>122.721733333333</v>
       </c>
       <c r="E57" s="1" t="n">
         <f aca="false">AVERAGE(E37:E42)</f>
-        <v>3.52888888888899</v>
+        <v>1.70615555555556</v>
       </c>
       <c r="F57" s="1" t="n">
         <f aca="false">AVERAGE(F37:F42)</f>
-        <v>0.0970666666666654</v>
+        <v>0.169122222222221</v>
+      </c>
+      <c r="G57" s="1" t="n">
+        <f aca="false">C57/D57</f>
+        <v>8.92459471997897</v>
+      </c>
+      <c r="H57" s="1" t="n">
+        <f aca="false">ABS($G$58-G57)</f>
+        <v>0.135421960896181</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2412,29 +2461,37 @@
       <c r="B58" s="0"/>
       <c r="C58" s="0"/>
       <c r="D58" s="0"/>
+      <c r="G58" s="1" t="n">
+        <f aca="false">AVERAGE(G53:G57)</f>
+        <v>9.06001668087515</v>
+      </c>
+      <c r="H58" s="1" t="n">
+        <f aca="false">AVERAGE(H53:H57)</f>
+        <v>0.450792324127816</v>
+      </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0"/>
       <c r="B59" s="0"/>
       <c r="C59" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B60" s="0"/>
       <c r="C60" s="1" t="n">
         <f aca="false">SLOPE(C53:C57,$A$53:$A$57)</f>
-        <v>4.93189325091575</v>
+        <v>6.35210354712042</v>
       </c>
       <c r="D60" s="1" t="n">
         <f aca="false">SLOPE(D53:D57,$A$53:$A$57)</f>
-        <v>0.738274258241758</v>
+        <v>0.749151369982548</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2443,7 +2500,7 @@
       <c r="C61" s="7"/>
       <c r="D61" s="7" t="n">
         <f aca="false">C60/D60</f>
-        <v>6.68029962559081</v>
+        <v>8.47906551551577</v>
       </c>
     </row>
   </sheetData>
@@ -2465,19 +2522,19 @@
   </sheetPr>
   <dimension ref="1:60"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G53" activeCellId="0" sqref="G53"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H49" activeCellId="0" sqref="H49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.3877551020408"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="1" width="13.2295918367347"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="14.3112244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="1" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.2551020408163"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="1" width="13.0918367346939"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="7.83163265306122"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="14.0408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="1" width="10.6632653061225"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2499,7 +2556,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B2" s="0"/>
       <c r="C2" s="0"/>
@@ -2519,7 +2576,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C3" s="0"/>
       <c r="D3" s="0"/>
@@ -2528,10 +2585,10 @@
       <c r="G3" s="0"/>
       <c r="H3" s="0"/>
       <c r="I3" s="1" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="K3" s="0"/>
       <c r="L3" s="0"/>
@@ -2539,25 +2596,25 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D4" s="0"/>
       <c r="E4" s="1" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G4" s="0"/>
       <c r="H4" s="0"/>
       <c r="I4" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="J4" s="8" t="n">
         <v>0.000234784733038</v>
@@ -2593,7 +2650,7 @@
       </c>
       <c r="H5" s="10"/>
       <c r="I5" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="J5" s="8" t="n">
         <v>0.000400919205276</v>
@@ -2780,10 +2837,10 @@
         <v>1.12E-005</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G11" s="0"/>
       <c r="H11" s="0"/>
@@ -3250,21 +3307,21 @@
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="12" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="D32" s="12"/>
       <c r="E32" s="12" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="F32" s="12"/>
       <c r="G32" s="12" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="H32" s="12"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>4</v>
@@ -3732,7 +3789,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B51" s="0"/>
       <c r="C51" s="1" t="s">
@@ -3918,27 +3975,27 @@
       <c r="A58" s="0"/>
       <c r="B58" s="0"/>
       <c r="C58" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B59" s="0"/>
       <c r="C59" s="1" t="n">
@@ -3968,7 +4025,7 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="7" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="B60" s="7"/>
       <c r="C60" s="7"/>
@@ -4040,9 +4097,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="28.2142857142857"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="27.8061224489796"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4056,7 +4111,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="13" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
added rewards results, strange lp speedup. writing conclusion and appendix now
</commit_message>
<xml_diff>
--- a/stats/stats_compilation.xlsx
+++ b/stats/stats_compilation.xlsx
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="46">
   <si>
     <t xml:space="preserve">stats</t>
   </si>
@@ -183,21 +183,29 @@
     <t xml:space="preserve">batch_size(J)</t>
   </si>
   <si>
+    <t xml:space="preserve">cpu+-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gpu+-</t>
+  </si>
+  <si>
     <t xml:space="preserve">batch_size (J)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">congpu+-</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contribution</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="7">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.0000"/>
-    <numFmt numFmtId="166" formatCode="0.00000000000"/>
-    <numFmt numFmtId="167" formatCode="0.00000"/>
-    <numFmt numFmtId="168" formatCode="0.000000"/>
-    <numFmt numFmtId="169" formatCode="0.0000000"/>
-    <numFmt numFmtId="170" formatCode="0.000000000000000"/>
+    <numFmt numFmtId="166" formatCode="0.000000000000000"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -295,7 +303,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -328,31 +336,15 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="170" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -435,28 +427,28 @@
   </sheetPr>
   <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E61" activeCellId="0" sqref="E61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="9.98979591836735"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="9.17857142857143"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="6.75"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="9.85204081632653"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="6.75"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="1" width="10.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1903,6 +1895,8 @@
       </c>
       <c r="E32" s="0"/>
       <c r="F32" s="0"/>
+      <c r="G32" s="0"/>
+      <c r="H32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
@@ -1913,6 +1907,8 @@
       <c r="D33" s="2"/>
       <c r="E33" s="0"/>
       <c r="F33" s="0"/>
+      <c r="G33" s="0"/>
+      <c r="H33" s="0"/>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
@@ -1933,6 +1929,8 @@
       <c r="F34" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="G34" s="0"/>
+      <c r="H34" s="0"/>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="2" t="n">
@@ -1955,6 +1953,8 @@
         <f aca="false">ABS(D$53-D35)</f>
         <v>0.0324333333333318</v>
       </c>
+      <c r="G35" s="0"/>
+      <c r="H35" s="0"/>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="n">
@@ -1977,6 +1977,8 @@
         <f aca="false">ABS(D$53-D36)</f>
         <v>0.00356666666666783</v>
       </c>
+      <c r="G36" s="0"/>
+      <c r="H36" s="0"/>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="n">
@@ -1999,6 +2001,8 @@
         <f aca="false">ABS(D$53-D37)</f>
         <v>0.0288666666666675</v>
       </c>
+      <c r="G37" s="0"/>
+      <c r="H37" s="0"/>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="2" t="n">
@@ -2021,6 +2025,8 @@
         <f aca="false">ABS(D$54-D38)</f>
         <v>0.0536666666666648</v>
       </c>
+      <c r="G38" s="0"/>
+      <c r="H38" s="0"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="n">
@@ -2043,6 +2049,8 @@
         <f aca="false">ABS(D$54-D39)</f>
         <v>0.293866666666666</v>
       </c>
+      <c r="G39" s="0"/>
+      <c r="H39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="n">
@@ -2065,6 +2073,8 @@
         <f aca="false">ABS(D$54-D40)</f>
         <v>0.347533333333331</v>
       </c>
+      <c r="G40" s="0"/>
+      <c r="H40" s="0"/>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="2" t="n">
@@ -2087,6 +2097,8 @@
         <f aca="false">ABS(D$55-D41)</f>
         <v>0.0576666666666625</v>
       </c>
+      <c r="G41" s="0"/>
+      <c r="H41" s="0"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="n">
@@ -2109,6 +2121,8 @@
         <f aca="false">ABS(D$55-D42)</f>
         <v>0.233133333333335</v>
       </c>
+      <c r="G42" s="0"/>
+      <c r="H42" s="0"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="n">
@@ -2131,6 +2145,8 @@
         <f aca="false">ABS(D$55-D43)</f>
         <v>0.175466666666665</v>
       </c>
+      <c r="G43" s="0"/>
+      <c r="H43" s="0"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="2" t="n">
@@ -2153,6 +2169,8 @@
         <f aca="false">ABS(D$56-D44)</f>
         <v>3.51679999999999</v>
       </c>
+      <c r="G44" s="0"/>
+      <c r="H44" s="0"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="n">
@@ -2175,6 +2193,8 @@
         <f aca="false">ABS(D$56-D45)</f>
         <v>15.6647</v>
       </c>
+      <c r="G45" s="0"/>
+      <c r="H45" s="0"/>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="n">
@@ -2197,6 +2217,8 @@
         <f aca="false">ABS(D$56-D46)</f>
         <v>19.1815</v>
       </c>
+      <c r="G46" s="0"/>
+      <c r="H46" s="0"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="2" t="n">
@@ -2219,6 +2241,8 @@
         <f aca="false">ABS(D$57-D47)</f>
         <v>3.49953333333332</v>
       </c>
+      <c r="G47" s="0"/>
+      <c r="H47" s="0"/>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="n">
@@ -2241,6 +2265,8 @@
         <f aca="false">ABS(D$57-D48)</f>
         <v>6.52286666666667</v>
       </c>
+      <c r="G48" s="0"/>
+      <c r="H48" s="0"/>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="n">
@@ -2263,6 +2289,8 @@
         <f aca="false">ABS(D$57-D49)</f>
         <v>3.02333333333331</v>
       </c>
+      <c r="G49" s="0"/>
+      <c r="H49" s="0"/>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="0"/>
@@ -2271,6 +2299,8 @@
       <c r="D50" s="0"/>
       <c r="E50" s="0"/>
       <c r="F50" s="0"/>
+      <c r="G50" s="0"/>
+      <c r="H50" s="0"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
@@ -2281,6 +2311,8 @@
       <c r="D51" s="0"/>
       <c r="E51" s="0"/>
       <c r="F51" s="0"/>
+      <c r="G51" s="0"/>
+      <c r="H51" s="0"/>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
@@ -2520,79 +2552,46 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:60"/>
+  <dimension ref="A1:N74"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A28" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H34" activeCellId="0" sqref="H34"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C45" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L64" activeCellId="0" sqref="L64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="1" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="1" width="13.0918367346939"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="14.0408163265306"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="1" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="13.7704081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="1" width="10.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0"/>
-      <c r="C1" s="0"/>
-      <c r="D1" s="0"/>
-      <c r="E1" s="0"/>
-      <c r="F1" s="0"/>
-      <c r="G1" s="0"/>
-      <c r="H1" s="0"/>
-      <c r="I1" s="0"/>
-      <c r="J1" s="0"/>
-      <c r="K1" s="0"/>
-      <c r="L1" s="0"/>
-      <c r="AMJ1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="B2" s="0"/>
-      <c r="C2" s="0"/>
-      <c r="D2" s="0"/>
-      <c r="E2" s="0"/>
-      <c r="F2" s="0"/>
-      <c r="G2" s="0"/>
-      <c r="H2" s="0"/>
-      <c r="I2" s="0"/>
-      <c r="J2" s="0"/>
-      <c r="K2" s="0"/>
-      <c r="L2" s="0"/>
-      <c r="AMJ2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C3" s="0"/>
-      <c r="D3" s="0"/>
-      <c r="E3" s="0"/>
-      <c r="F3" s="0"/>
-      <c r="G3" s="0"/>
-      <c r="H3" s="0"/>
       <c r="I3" s="1" t="s">
         <v>29</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="K3" s="0"/>
-      <c r="L3" s="0"/>
-      <c r="AMJ3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -2604,24 +2603,18 @@
       <c r="C4" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D4" s="0"/>
       <c r="E4" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G4" s="0"/>
-      <c r="H4" s="0"/>
       <c r="I4" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="J4" s="8" t="n">
+      <c r="J4" s="1" t="n">
         <v>0.000234784733038</v>
       </c>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="AMJ4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
@@ -2630,34 +2623,30 @@
       <c r="B5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C5" s="10" t="n">
+      <c r="C5" s="1" t="n">
         <v>0.000152</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="D5" s="1" t="n">
         <f aca="false">ABS(F5-C5)</f>
         <v>2.00000000000005E-007</v>
       </c>
       <c r="E5" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F5" s="10" t="n">
+      <c r="F5" s="1" t="n">
         <f aca="false">AVERAGE(C5,C10,C15,C20,C25)</f>
         <v>0.0001518</v>
       </c>
-      <c r="G5" s="10" t="n">
+      <c r="G5" s="1" t="n">
         <f aca="false">AVERAGE(D5,D10,D15,D20,D25)</f>
         <v>9.60000000000002E-007</v>
       </c>
-      <c r="H5" s="10"/>
-      <c r="I5" s="0" t="s">
+      <c r="I5" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="J5" s="8" t="n">
+      <c r="J5" s="1" t="n">
         <v>0.000400919205276</v>
       </c>
-      <c r="K5" s="9"/>
-      <c r="L5" s="9"/>
-      <c r="AMJ5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
@@ -2666,32 +2655,27 @@
       <c r="B6" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C6" s="10" t="n">
+      <c r="C6" s="1" t="n">
         <v>7.4E-005</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="D6" s="1" t="n">
         <f aca="false">ABS(F6-C6)</f>
         <v>4.79999999999999E-006</v>
       </c>
       <c r="E6" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F6" s="10" t="n">
+      <c r="F6" s="1" t="n">
         <f aca="false">AVERAGE(C6,C11,C16,C21,C26)</f>
         <v>7.88E-005</v>
       </c>
-      <c r="G6" s="10" t="n">
+      <c r="G6" s="1" t="n">
         <f aca="false">AVERAGE(D6,D11,D16,D21,D26)</f>
         <v>5.04E-006</v>
       </c>
-      <c r="H6" s="10"/>
-      <c r="I6" s="0"/>
-      <c r="J6" s="8" t="n">
+      <c r="J6" s="1" t="n">
         <v>0.000415126851294</v>
       </c>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="AMJ6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
@@ -2700,32 +2684,27 @@
       <c r="B7" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C7" s="10" t="n">
+      <c r="C7" s="1" t="n">
         <v>0.000137</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="D7" s="1" t="n">
         <f aca="false">ABS(F7-C7)</f>
         <v>1.59999999999998E-006</v>
       </c>
       <c r="E7" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F7" s="10" t="n">
+      <c r="F7" s="1" t="n">
         <f aca="false">AVERAGE(C7,C12,C17,C22,C27)</f>
         <v>0.0001386</v>
       </c>
-      <c r="G7" s="10" t="n">
+      <c r="G7" s="1" t="n">
         <f aca="false">AVERAGE(D7,D12,D17,D22,D27)</f>
         <v>2.88E-006</v>
       </c>
-      <c r="H7" s="10"/>
-      <c r="I7" s="0"/>
-      <c r="J7" s="8" t="n">
+      <c r="J7" s="1" t="n">
         <v>0.000241408168222</v>
       </c>
-      <c r="K7" s="11"/>
-      <c r="L7" s="9"/>
-      <c r="AMJ7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
@@ -2734,32 +2713,27 @@
       <c r="B8" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C8" s="10" t="n">
+      <c r="C8" s="1" t="n">
         <v>0.000133</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="D8" s="1" t="n">
         <f aca="false">ABS(F8-C8)</f>
         <v>3.60000000000001E-006</v>
       </c>
       <c r="E8" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="F8" s="10" t="n">
+      <c r="F8" s="1" t="n">
         <f aca="false">AVERAGE(C8,C13,C18,C23,C28)</f>
         <v>0.0001294</v>
       </c>
-      <c r="G8" s="10" t="n">
+      <c r="G8" s="1" t="n">
         <f aca="false">AVERAGE(D8,D13,D18,D23,D28)</f>
         <v>2.08E-006</v>
       </c>
-      <c r="H8" s="10"/>
-      <c r="I8" s="0"/>
-      <c r="J8" s="8" t="n">
+      <c r="J8" s="1" t="n">
         <v>0.000355125812348</v>
       </c>
-      <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
-      <c r="AMJ8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
@@ -2768,35 +2742,31 @@
       <c r="B9" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C9" s="10" t="n">
+      <c r="C9" s="1" t="n">
         <v>0.000156</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="D9" s="1" t="n">
         <f aca="false">ABS(F9-C9)</f>
         <v>9.99999999999997E-007</v>
       </c>
       <c r="E9" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F9" s="10" t="n">
+      <c r="F9" s="1" t="n">
         <f aca="false">AVERAGE(C9,C14,C19,C24,C29)</f>
         <v>0.000155</v>
       </c>
-      <c r="G9" s="10" t="n">
+      <c r="G9" s="1" t="n">
         <f aca="false">AVERAGE(D9,D14,D19,D24,D29)</f>
         <v>1.6E-006</v>
       </c>
-      <c r="H9" s="10"/>
-      <c r="I9" s="0"/>
-      <c r="J9" s="8" t="n">
+      <c r="J9" s="1" t="n">
         <v>0.000243959832005</v>
       </c>
-      <c r="K9" s="10" t="n">
+      <c r="K9" s="1" t="n">
         <f aca="false">AVERAGE(J5:J9)</f>
         <v>0.000331307973829</v>
       </c>
-      <c r="L9" s="9"/>
-      <c r="AMJ9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
@@ -2805,22 +2775,13 @@
       <c r="B10" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C10" s="10" t="n">
+      <c r="C10" s="1" t="n">
         <v>0.000151</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="D10" s="1" t="n">
         <f aca="false">ABS(F5-C10)</f>
         <v>7.99999999999992E-007</v>
       </c>
-      <c r="E10" s="0"/>
-      <c r="F10" s="0"/>
-      <c r="G10" s="0"/>
-      <c r="H10" s="0"/>
-      <c r="I10" s="0"/>
-      <c r="J10" s="0"/>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
-      <c r="AMJ10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
@@ -2829,10 +2790,10 @@
       <c r="B11" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C11" s="10" t="n">
+      <c r="C11" s="1" t="n">
         <v>9E-005</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="D11" s="1" t="n">
         <f aca="false">ABS(F6-C11)</f>
         <v>1.12E-005</v>
       </c>
@@ -2842,13 +2803,6 @@
       <c r="F11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G11" s="0"/>
-      <c r="H11" s="0"/>
-      <c r="I11" s="0"/>
-      <c r="J11" s="0"/>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
-      <c r="AMJ11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
@@ -2857,27 +2811,20 @@
       <c r="B12" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C12" s="10" t="n">
+      <c r="C12" s="1" t="n">
         <v>0.000141</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="D12" s="1" t="n">
         <f aca="false">ABS(F7-C12)</f>
         <v>2.4E-006</v>
       </c>
       <c r="E12" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="F12" s="10" t="n">
+      <c r="F12" s="1" t="n">
         <f aca="false">AVERAGE(C4:C9)</f>
         <v>0.0001304</v>
       </c>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="0"/>
-      <c r="J12" s="0"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="AMJ12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
@@ -2886,27 +2833,20 @@
       <c r="B13" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C13" s="10" t="n">
+      <c r="C13" s="1" t="n">
         <v>0.000131</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="D13" s="1" t="n">
         <f aca="false">ABS(F8-C13)</f>
         <v>1.59999999999998E-006</v>
       </c>
       <c r="E13" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="F13" s="10" t="n">
+      <c r="F13" s="1" t="n">
         <f aca="false">AVERAGE(C10:C14)</f>
         <v>0.000134</v>
       </c>
-      <c r="G13" s="10"/>
-      <c r="H13" s="10"/>
-      <c r="I13" s="0"/>
-      <c r="J13" s="0"/>
-      <c r="K13" s="9"/>
-      <c r="L13" s="9"/>
-      <c r="AMJ13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
@@ -2915,27 +2855,20 @@
       <c r="B14" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="C14" s="10" t="n">
+      <c r="C14" s="1" t="n">
         <v>0.000157</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="D14" s="1" t="n">
         <f aca="false">ABS(F9-C14)</f>
         <v>2E-006</v>
       </c>
       <c r="E14" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="F14" s="10" t="n">
+      <c r="F14" s="1" t="n">
         <f aca="false">AVERAGE(C15:C19)</f>
         <v>0.0001284</v>
       </c>
-      <c r="G14" s="10"/>
-      <c r="H14" s="10"/>
-      <c r="I14" s="0"/>
-      <c r="J14" s="0"/>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
-      <c r="AMJ14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
@@ -2944,27 +2877,20 @@
       <c r="B15" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C15" s="10" t="n">
+      <c r="C15" s="1" t="n">
         <v>0.000151</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="D15" s="1" t="n">
         <f aca="false">ABS(F5-C15)</f>
         <v>7.99999999999992E-007</v>
       </c>
       <c r="E15" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="F15" s="10" t="n">
+      <c r="F15" s="1" t="n">
         <f aca="false">AVERAGE(C20:C24)</f>
         <v>0.0001292</v>
       </c>
-      <c r="G15" s="10"/>
-      <c r="H15" s="10"/>
-      <c r="I15" s="0"/>
-      <c r="J15" s="0"/>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
-      <c r="AMJ15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
@@ -2973,27 +2899,20 @@
       <c r="B16" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C16" s="10" t="n">
+      <c r="C16" s="1" t="n">
         <v>7.9E-005</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="D16" s="1" t="n">
         <f aca="false">ABS(F6-C16)</f>
         <v>2.00000000000005E-007</v>
       </c>
       <c r="E16" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="F16" s="10" t="n">
+      <c r="F16" s="1" t="n">
         <f aca="false">AVERAGE(C25:C29)</f>
         <v>0.0001316</v>
       </c>
-      <c r="G16" s="10"/>
-      <c r="H16" s="10"/>
-      <c r="I16" s="0"/>
-      <c r="J16" s="0"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
-      <c r="AMJ16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
@@ -3002,21 +2921,13 @@
       <c r="B17" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C17" s="10" t="n">
+      <c r="C17" s="1" t="n">
         <v>0.000133</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="D17" s="1" t="n">
         <f aca="false">ABS(F7-C17)</f>
         <v>5.59999999999997E-006</v>
       </c>
-      <c r="E17" s="0"/>
-      <c r="F17" s="0"/>
-      <c r="G17" s="0"/>
-      <c r="H17" s="0"/>
-      <c r="I17" s="0"/>
-      <c r="J17" s="9"/>
-      <c r="K17" s="9"/>
-      <c r="AMJ17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
@@ -3025,21 +2936,13 @@
       <c r="B18" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C18" s="10" t="n">
+      <c r="C18" s="1" t="n">
         <v>0.000128</v>
       </c>
-      <c r="D18" s="0" t="n">
+      <c r="D18" s="1" t="n">
         <f aca="false">ABS(F8-C18)</f>
         <v>1.40000000000001E-006</v>
       </c>
-      <c r="E18" s="0"/>
-      <c r="F18" s="0"/>
-      <c r="G18" s="0"/>
-      <c r="H18" s="0"/>
-      <c r="I18" s="0"/>
-      <c r="J18" s="9"/>
-      <c r="K18" s="9"/>
-      <c r="AMJ18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
@@ -3048,21 +2951,13 @@
       <c r="B19" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="C19" s="10" t="n">
+      <c r="C19" s="1" t="n">
         <v>0.000151</v>
       </c>
-      <c r="D19" s="0" t="n">
+      <c r="D19" s="1" t="n">
         <f aca="false">ABS(F9-C19)</f>
         <v>4.00000000000002E-006</v>
       </c>
-      <c r="E19" s="0"/>
-      <c r="F19" s="0"/>
-      <c r="G19" s="0"/>
-      <c r="H19" s="0"/>
-      <c r="I19" s="0"/>
-      <c r="J19" s="9"/>
-      <c r="K19" s="9"/>
-      <c r="AMJ19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
@@ -3071,21 +2966,13 @@
       <c r="B20" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C20" s="10" t="n">
+      <c r="C20" s="1" t="n">
         <v>0.000151</v>
       </c>
-      <c r="D20" s="0" t="n">
+      <c r="D20" s="1" t="n">
         <f aca="false">ABS(F5-C20)</f>
         <v>7.99999999999992E-007</v>
       </c>
-      <c r="E20" s="0"/>
-      <c r="F20" s="0"/>
-      <c r="G20" s="0"/>
-      <c r="H20" s="0"/>
-      <c r="I20" s="0"/>
-      <c r="J20" s="9"/>
-      <c r="K20" s="9"/>
-      <c r="AMJ20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
@@ -3094,21 +2981,13 @@
       <c r="B21" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C21" s="10" t="n">
+      <c r="C21" s="1" t="n">
         <v>7.1E-005</v>
       </c>
-      <c r="D21" s="0" t="n">
+      <c r="D21" s="1" t="n">
         <f aca="false">ABS(F6-C21)</f>
         <v>7.8E-006</v>
       </c>
-      <c r="E21" s="0"/>
-      <c r="F21" s="0"/>
-      <c r="G21" s="0"/>
-      <c r="H21" s="0"/>
-      <c r="I21" s="0"/>
-      <c r="J21" s="9"/>
-      <c r="K21" s="9"/>
-      <c r="AMJ21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
@@ -3117,21 +2996,13 @@
       <c r="B22" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C22" s="10" t="n">
+      <c r="C22" s="1" t="n">
         <v>0.000139</v>
       </c>
-      <c r="D22" s="0" t="n">
+      <c r="D22" s="1" t="n">
         <f aca="false">ABS(F7-C22)</f>
         <v>4.0000000000001E-007</v>
       </c>
-      <c r="E22" s="0"/>
-      <c r="F22" s="0"/>
-      <c r="G22" s="0"/>
-      <c r="H22" s="0"/>
-      <c r="I22" s="0"/>
-      <c r="J22" s="9"/>
-      <c r="K22" s="9"/>
-      <c r="AMJ22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
@@ -3140,21 +3011,13 @@
       <c r="B23" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C23" s="10" t="n">
+      <c r="C23" s="1" t="n">
         <v>0.000129</v>
       </c>
-      <c r="D23" s="0" t="n">
+      <c r="D23" s="1" t="n">
         <f aca="false">ABS(F8-C23)</f>
         <v>4.0000000000001E-007</v>
       </c>
-      <c r="E23" s="0"/>
-      <c r="F23" s="0"/>
-      <c r="G23" s="0"/>
-      <c r="H23" s="0"/>
-      <c r="I23" s="0"/>
-      <c r="J23" s="9"/>
-      <c r="K23" s="9"/>
-      <c r="AMJ23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
@@ -3163,19 +3026,13 @@
       <c r="B24" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="C24" s="10" t="n">
+      <c r="C24" s="1" t="n">
         <v>0.000156</v>
       </c>
-      <c r="D24" s="0" t="n">
+      <c r="D24" s="1" t="n">
         <f aca="false">ABS(F9-C24)</f>
         <v>9.99999999999997E-007</v>
       </c>
-      <c r="E24" s="0"/>
-      <c r="F24" s="0"/>
-      <c r="G24" s="0"/>
-      <c r="H24" s="0"/>
-      <c r="I24" s="0"/>
-      <c r="AMJ24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
@@ -3184,19 +3041,13 @@
       <c r="B25" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C25" s="10" t="n">
+      <c r="C25" s="1" t="n">
         <v>0.000154</v>
       </c>
-      <c r="D25" s="0" t="n">
+      <c r="D25" s="1" t="n">
         <f aca="false">ABS(F5-C25)</f>
         <v>2.20000000000003E-006</v>
       </c>
-      <c r="E25" s="0"/>
-      <c r="F25" s="0"/>
-      <c r="G25" s="0"/>
-      <c r="H25" s="0"/>
-      <c r="I25" s="0"/>
-      <c r="AMJ25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
@@ -3205,18 +3056,13 @@
       <c r="B26" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C26" s="10" t="n">
+      <c r="C26" s="1" t="n">
         <v>8E-005</v>
       </c>
-      <c r="D26" s="0" t="n">
+      <c r="D26" s="1" t="n">
         <f aca="false">ABS(F6-C26)</f>
         <v>1.2E-006</v>
       </c>
-      <c r="E26" s="0"/>
-      <c r="F26" s="0"/>
-      <c r="G26" s="0"/>
-      <c r="H26" s="0"/>
-      <c r="AMJ26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
@@ -3225,18 +3071,13 @@
       <c r="B27" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C27" s="10" t="n">
+      <c r="C27" s="1" t="n">
         <v>0.000143</v>
       </c>
-      <c r="D27" s="0" t="n">
+      <c r="D27" s="1" t="n">
         <f aca="false">ABS(F7-C27)</f>
         <v>4.40000000000003E-006</v>
       </c>
-      <c r="E27" s="0"/>
-      <c r="F27" s="0"/>
-      <c r="G27" s="0"/>
-      <c r="H27" s="0"/>
-      <c r="AMJ27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
@@ -3245,18 +3086,13 @@
       <c r="B28" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C28" s="10" t="n">
+      <c r="C28" s="1" t="n">
         <v>0.000126</v>
       </c>
-      <c r="D28" s="0" t="n">
+      <c r="D28" s="1" t="n">
         <f aca="false">ABS(F8-C28)</f>
         <v>3.4E-006</v>
       </c>
-      <c r="E28" s="0"/>
-      <c r="F28" s="0"/>
-      <c r="G28" s="0"/>
-      <c r="H28" s="0"/>
-      <c r="AMJ28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
@@ -3265,59 +3101,41 @@
       <c r="B29" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="C29" s="10" t="n">
+      <c r="C29" s="1" t="n">
         <v>0.000155</v>
       </c>
-      <c r="D29" s="0" t="n">
+      <c r="D29" s="1" t="n">
         <f aca="false">ABS(F9-C29)</f>
         <v>0</v>
       </c>
-      <c r="E29" s="0"/>
-      <c r="F29" s="0"/>
-      <c r="G29" s="0"/>
-      <c r="H29" s="0"/>
-      <c r="AMJ29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0"/>
-      <c r="B30" s="0"/>
-      <c r="C30" s="10" t="n">
+      <c r="C30" s="1" t="n">
         <f aca="false">MIN(C5:C29)</f>
         <v>7.1E-005</v>
       </c>
-      <c r="D30" s="0"/>
-      <c r="E30" s="0"/>
-      <c r="F30" s="0"/>
-      <c r="G30" s="0"/>
-      <c r="H30" s="0"/>
-    </row>
-    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0"/>
-      <c r="B31" s="0"/>
-      <c r="C31" s="0"/>
-      <c r="D31" s="0"/>
-      <c r="E31" s="0"/>
-      <c r="F31" s="0"/>
-      <c r="G31" s="0"/>
-      <c r="H31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B32" s="2"/>
-      <c r="C32" s="12" t="s">
+      <c r="C32" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12" t="s">
+      <c r="D32" s="8"/>
+      <c r="E32" s="8"/>
+      <c r="F32" s="8"/>
+      <c r="G32" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="F32" s="12"/>
-      <c r="G32" s="12" t="s">
+      <c r="H32" s="8"/>
+      <c r="I32" s="8"/>
+      <c r="J32" s="8"/>
+      <c r="K32" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="H32" s="12"/>
+      <c r="L32" s="8"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
@@ -3333,16 +3151,34 @@
         <v>16</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="G33" s="1" t="s">
         <v>15</v>
       </c>
       <c r="H33" s="1" t="s">
         <v>16</v>
+      </c>
+      <c r="I33" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J33" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L33" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M33" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N33" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3353,24 +3189,48 @@
         <v>1</v>
       </c>
       <c r="C34" s="1" t="n">
-        <v>13.241</v>
+        <v>11.5217</v>
       </c>
       <c r="D34" s="1" t="n">
-        <v>9.759</v>
+        <v>9.8314</v>
       </c>
       <c r="E34" s="1" t="n">
-        <v>12.074</v>
+        <f aca="false">ABS(C$52-C34)</f>
+        <v>1.55516666666667</v>
       </c>
       <c r="F34" s="1" t="n">
-        <v>7.1731</v>
+        <f aca="false">ABS(D$52-D34)</f>
+        <v>0.113933333333334</v>
       </c>
       <c r="G34" s="1" t="n">
-        <f aca="false">C34-E34</f>
-        <v>1.167</v>
+        <v>10.5199</v>
       </c>
       <c r="H34" s="1" t="n">
-        <f aca="false">D34-F34</f>
-        <v>2.5859</v>
+        <v>7.2581</v>
+      </c>
+      <c r="I34" s="1" t="n">
+        <f aca="false">ABS(G$52-G34)</f>
+        <v>1.411</v>
+      </c>
+      <c r="J34" s="1" t="n">
+        <f aca="false">ABS(H$52-H34)</f>
+        <v>0.114766666666666</v>
+      </c>
+      <c r="K34" s="1" t="n">
+        <f aca="false">C34-G34</f>
+        <v>1.0018</v>
+      </c>
+      <c r="L34" s="1" t="n">
+        <f aca="false">D34-H34</f>
+        <v>2.5733</v>
+      </c>
+      <c r="M34" s="1" t="n">
+        <f aca="false">ABS(K$52-K34)</f>
+        <v>0.144166666666667</v>
+      </c>
+      <c r="N34" s="1" t="n">
+        <f aca="false">ABS(L$52-L34)</f>
+        <v>0.000833333333333464</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3381,24 +3241,48 @@
         <v>2</v>
       </c>
       <c r="C35" s="1" t="n">
-        <v>12.7705</v>
+        <v>14.4238</v>
       </c>
       <c r="D35" s="1" t="n">
-        <v>8.1344</v>
+        <v>9.659</v>
       </c>
       <c r="E35" s="1" t="n">
-        <v>11.6554</v>
+        <f aca="false">ABS(C$52-C35)</f>
+        <v>1.34693333333333</v>
       </c>
       <c r="F35" s="1" t="n">
-        <v>6.6935</v>
+        <f aca="false">ABS(D$52-D35)</f>
+        <v>0.058466666666666</v>
       </c>
       <c r="G35" s="1" t="n">
-        <f aca="false">C35-E35</f>
-        <v>1.1151</v>
+        <v>13.1362</v>
       </c>
       <c r="H35" s="1" t="n">
-        <f aca="false">D35-F35</f>
-        <v>1.4409</v>
+        <v>7.0731</v>
+      </c>
+      <c r="I35" s="1" t="n">
+        <f aca="false">ABS(G$52-G35)</f>
+        <v>1.2053</v>
+      </c>
+      <c r="J35" s="1" t="n">
+        <f aca="false">ABS(H$52-H35)</f>
+        <v>0.0702333333333334</v>
+      </c>
+      <c r="K35" s="1" t="n">
+        <f aca="false">C35-G35</f>
+        <v>1.2876</v>
+      </c>
+      <c r="L35" s="1" t="n">
+        <f aca="false">D35-H35</f>
+        <v>2.5859</v>
+      </c>
+      <c r="M35" s="1" t="n">
+        <f aca="false">ABS(K$52-K35)</f>
+        <v>0.141633333333333</v>
+      </c>
+      <c r="N35" s="1" t="n">
+        <f aca="false">ABS(L$52-L35)</f>
+        <v>0.0117666666666665</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3409,24 +3293,48 @@
         <v>3</v>
       </c>
       <c r="C36" s="1" t="n">
-        <v>13.5348</v>
+        <v>13.2851</v>
       </c>
       <c r="D36" s="1" t="n">
-        <v>8.1168</v>
+        <v>9.662</v>
       </c>
       <c r="E36" s="1" t="n">
-        <v>12.3499</v>
+        <f aca="false">ABS(C$52-C36)</f>
+        <v>0.208233333333334</v>
       </c>
       <c r="F36" s="1" t="n">
-        <v>6.6934</v>
+        <f aca="false">ABS(D$52-D36)</f>
+        <v>0.0554666666666659</v>
       </c>
       <c r="G36" s="1" t="n">
-        <f aca="false">C36-E36</f>
-        <v>1.1849</v>
+        <v>12.1366</v>
       </c>
       <c r="H36" s="1" t="n">
-        <f aca="false">D36-F36</f>
-        <v>1.4234</v>
+        <v>7.0988</v>
+      </c>
+      <c r="I36" s="1" t="n">
+        <f aca="false">ABS(G$52-G36)</f>
+        <v>0.2057</v>
+      </c>
+      <c r="J36" s="1" t="n">
+        <f aca="false">ABS(H$52-H36)</f>
+        <v>0.0445333333333338</v>
+      </c>
+      <c r="K36" s="1" t="n">
+        <f aca="false">C36-G36</f>
+        <v>1.1485</v>
+      </c>
+      <c r="L36" s="1" t="n">
+        <f aca="false">D36-H36</f>
+        <v>2.5632</v>
+      </c>
+      <c r="M36" s="1" t="n">
+        <f aca="false">ABS(K$52-K36)</f>
+        <v>0.00253333333333394</v>
+      </c>
+      <c r="N36" s="1" t="n">
+        <f aca="false">ABS(L$52-L36)</f>
+        <v>0.010933333333333</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3437,24 +3345,48 @@
         <v>1</v>
       </c>
       <c r="C37" s="1" t="n">
-        <v>50.3415</v>
+        <v>53.1111</v>
       </c>
       <c r="D37" s="1" t="n">
-        <v>33.6828</v>
+        <v>34.3539</v>
       </c>
       <c r="E37" s="1" t="n">
-        <v>48.6051</v>
+        <f aca="false">ABS(C$53-C37)</f>
+        <v>2.5963</v>
       </c>
       <c r="F37" s="1" t="n">
-        <v>30.8083</v>
+        <f aca="false">ABS(D$53-D37)</f>
+        <v>0.384933333333336</v>
       </c>
       <c r="G37" s="1" t="n">
-        <f aca="false">C37-E37</f>
-        <v>1.7364</v>
+        <v>51.2869</v>
       </c>
       <c r="H37" s="1" t="n">
-        <f aca="false">D37-F37</f>
-        <v>2.8745</v>
+        <v>31.4538</v>
+      </c>
+      <c r="I37" s="1" t="n">
+        <f aca="false">ABS(G$53-G37)</f>
+        <v>2.52406666666667</v>
+      </c>
+      <c r="J37" s="1" t="n">
+        <f aca="false">ABS(H$53-H37)</f>
+        <v>0.390900000000002</v>
+      </c>
+      <c r="K37" s="1" t="n">
+        <f aca="false">C37-G37</f>
+        <v>1.8242</v>
+      </c>
+      <c r="L37" s="1" t="n">
+        <f aca="false">D37-H37</f>
+        <v>2.9001</v>
+      </c>
+      <c r="M37" s="1" t="n">
+        <f aca="false">ABS(K$53-K37)</f>
+        <v>0.072233333333332</v>
+      </c>
+      <c r="N37" s="1" t="n">
+        <f aca="false">ABS(L$53-L37)</f>
+        <v>0.00596666666666446</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3465,24 +3397,48 @@
         <v>2</v>
       </c>
       <c r="C38" s="1" t="n">
-        <v>50.5889</v>
+        <v>49.4526</v>
       </c>
       <c r="D38" s="1" t="n">
-        <v>26.524</v>
+        <v>33.8754</v>
       </c>
       <c r="E38" s="1" t="n">
-        <v>48.8557</v>
+        <f aca="false">ABS(C$53-C38)</f>
+        <v>1.0622</v>
       </c>
       <c r="F38" s="1" t="n">
-        <v>24.7341</v>
+        <f aca="false">ABS(D$53-D38)</f>
+        <v>0.0935666666666677</v>
       </c>
       <c r="G38" s="1" t="n">
-        <f aca="false">C38-E38</f>
-        <v>1.7332</v>
+        <v>47.7151</v>
       </c>
       <c r="H38" s="1" t="n">
-        <f aca="false">D38-F38</f>
-        <v>1.7899</v>
+        <v>30.9728</v>
+      </c>
+      <c r="I38" s="1" t="n">
+        <f aca="false">ABS(G$53-G38)</f>
+        <v>1.04773333333333</v>
+      </c>
+      <c r="J38" s="1" t="n">
+        <f aca="false">ABS(H$53-H38)</f>
+        <v>0.0900999999999996</v>
+      </c>
+      <c r="K38" s="1" t="n">
+        <f aca="false">C38-G38</f>
+        <v>1.7375</v>
+      </c>
+      <c r="L38" s="1" t="n">
+        <f aca="false">D38-H38</f>
+        <v>2.9026</v>
+      </c>
+      <c r="M38" s="1" t="n">
+        <f aca="false">ABS(K$53-K38)</f>
+        <v>0.0144666666666684</v>
+      </c>
+      <c r="N38" s="1" t="n">
+        <f aca="false">ABS(L$53-L38)</f>
+        <v>0.00346666666666673</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3493,24 +3449,48 @@
         <v>3</v>
       </c>
       <c r="C39" s="1" t="n">
-        <v>48.7033</v>
+        <v>48.9807</v>
       </c>
       <c r="D39" s="1" t="n">
-        <v>25.4616</v>
+        <v>33.6776</v>
       </c>
       <c r="E39" s="1" t="n">
-        <v>46.9841</v>
+        <f aca="false">ABS(C$53-C39)</f>
+        <v>1.5341</v>
       </c>
       <c r="F39" s="1" t="n">
-        <v>23.7196</v>
+        <f aca="false">ABS(D$53-D39)</f>
+        <v>0.291366666666669</v>
       </c>
       <c r="G39" s="1" t="n">
-        <f aca="false">C39-E39</f>
-        <v>1.7192</v>
+        <v>47.2865</v>
       </c>
       <c r="H39" s="1" t="n">
-        <f aca="false">D39-F39</f>
-        <v>1.742</v>
+        <v>30.7621</v>
+      </c>
+      <c r="I39" s="1" t="n">
+        <f aca="false">ABS(G$53-G39)</f>
+        <v>1.47633333333334</v>
+      </c>
+      <c r="J39" s="1" t="n">
+        <f aca="false">ABS(H$53-H39)</f>
+        <v>0.300799999999999</v>
+      </c>
+      <c r="K39" s="1" t="n">
+        <f aca="false">C39-G39</f>
+        <v>1.6942</v>
+      </c>
+      <c r="L39" s="1" t="n">
+        <f aca="false">D39-H39</f>
+        <v>2.9155</v>
+      </c>
+      <c r="M39" s="1" t="n">
+        <f aca="false">ABS(K$53-K39)</f>
+        <v>0.0577666666666634</v>
+      </c>
+      <c r="N39" s="1" t="n">
+        <f aca="false">ABS(L$53-L39)</f>
+        <v>0.00943333333333163</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3521,24 +3501,48 @@
         <v>1</v>
       </c>
       <c r="C40" s="1" t="n">
-        <v>89.2566</v>
+        <v>88.6947</v>
       </c>
       <c r="D40" s="1" t="n">
-        <v>62.564</v>
+        <v>58.6917</v>
       </c>
       <c r="E40" s="1" t="n">
-        <v>86.7909</v>
+        <f aca="false">ABS(C$54-C40)</f>
+        <v>0.260166666666663</v>
       </c>
       <c r="F40" s="1" t="n">
-        <v>59.2958</v>
+        <f aca="false">ABS(D$54-D40)</f>
+        <v>0.282566666666668</v>
       </c>
       <c r="G40" s="1" t="n">
-        <f aca="false">C40-E40</f>
-        <v>2.46570000000001</v>
+        <v>86.2185</v>
       </c>
       <c r="H40" s="1" t="n">
-        <f aca="false">D40-F40</f>
-        <v>3.2682</v>
+        <v>55.5258</v>
+      </c>
+      <c r="I40" s="1" t="n">
+        <f aca="false">ABS(G$54-G40)</f>
+        <v>0.276333333333341</v>
+      </c>
+      <c r="J40" s="1" t="n">
+        <f aca="false">ABS(H$54-H40)</f>
+        <v>0.284366666666671</v>
+      </c>
+      <c r="K40" s="1" t="n">
+        <f aca="false">C40-G40</f>
+        <v>2.47619999999999</v>
+      </c>
+      <c r="L40" s="1" t="n">
+        <f aca="false">D40-H40</f>
+        <v>3.1659</v>
+      </c>
+      <c r="M40" s="1" t="n">
+        <f aca="false">ABS(K$54-K40)</f>
+        <v>0.0161666666666633</v>
+      </c>
+      <c r="N40" s="1" t="n">
+        <f aca="false">ABS(L$54-L40)</f>
+        <v>0.00179999999999803</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3549,24 +3553,48 @@
         <v>2</v>
       </c>
       <c r="C41" s="1" t="n">
-        <v>90.1395</v>
+        <v>89.4783</v>
       </c>
       <c r="D41" s="1" t="n">
-        <v>47.99</v>
+        <v>59.258</v>
       </c>
       <c r="E41" s="1" t="n">
-        <v>87.6366</v>
+        <f aca="false">ABS(C$54-C41)</f>
+        <v>0.523433333333344</v>
       </c>
       <c r="F41" s="1" t="n">
-        <v>45.9413</v>
+        <f aca="false">ABS(D$54-D41)</f>
+        <v>0.283733333333338</v>
       </c>
       <c r="G41" s="1" t="n">
-        <f aca="false">C41-E41</f>
-        <v>2.5029</v>
+        <v>87.0313</v>
       </c>
       <c r="H41" s="1" t="n">
-        <f aca="false">D41-F41</f>
-        <v>2.0487</v>
+        <v>56.0749</v>
+      </c>
+      <c r="I41" s="1" t="n">
+        <f aca="false">ABS(G$54-G41)</f>
+        <v>0.536466666666655</v>
+      </c>
+      <c r="J41" s="1" t="n">
+        <f aca="false">ABS(H$54-H41)</f>
+        <v>0.264733333333332</v>
+      </c>
+      <c r="K41" s="1" t="n">
+        <f aca="false">C41-G41</f>
+        <v>2.447</v>
+      </c>
+      <c r="L41" s="1" t="n">
+        <f aca="false">D41-H41</f>
+        <v>3.1831</v>
+      </c>
+      <c r="M41" s="1" t="n">
+        <f aca="false">ABS(K$54-K41)</f>
+        <v>0.0130333333333255</v>
+      </c>
+      <c r="N41" s="1" t="n">
+        <f aca="false">ABS(L$54-L41)</f>
+        <v>0.0190000000000006</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3577,24 +3605,48 @@
         <v>3</v>
       </c>
       <c r="C42" s="1" t="n">
-        <v>91.3239</v>
+        <v>88.6916</v>
       </c>
       <c r="D42" s="1" t="n">
-        <v>49.4514</v>
+        <v>58.9731</v>
       </c>
       <c r="E42" s="1" t="n">
-        <v>88.8192</v>
+        <f aca="false">ABS(C$54-C42)</f>
+        <v>0.263266666666667</v>
       </c>
       <c r="F42" s="1" t="n">
-        <v>47.4115</v>
+        <f aca="false">ABS(D$54-D42)</f>
+        <v>0.00116666666666276</v>
       </c>
       <c r="G42" s="1" t="n">
-        <f aca="false">C42-E42</f>
-        <v>2.5047</v>
+        <v>86.2347</v>
       </c>
       <c r="H42" s="1" t="n">
-        <f aca="false">D42-F42</f>
-        <v>2.0399</v>
+        <v>55.8298</v>
+      </c>
+      <c r="I42" s="1" t="n">
+        <f aca="false">ABS(G$54-G42)</f>
+        <v>0.260133333333343</v>
+      </c>
+      <c r="J42" s="1" t="n">
+        <f aca="false">ABS(H$54-H42)</f>
+        <v>0.0196333333333314</v>
+      </c>
+      <c r="K42" s="1" t="n">
+        <f aca="false">C42-G42</f>
+        <v>2.45689999999999</v>
+      </c>
+      <c r="L42" s="1" t="n">
+        <f aca="false">D42-H42</f>
+        <v>3.1433</v>
+      </c>
+      <c r="M42" s="1" t="n">
+        <f aca="false">ABS(K$54-K42)</f>
+        <v>0.00313333333333787</v>
+      </c>
+      <c r="N42" s="1" t="n">
+        <f aca="false">ABS(L$54-L42)</f>
+        <v>0.020799999999999</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3605,24 +3657,48 @@
         <v>1</v>
       </c>
       <c r="C43" s="1" t="n">
-        <v>186.2137</v>
+        <v>184.4679</v>
       </c>
       <c r="D43" s="1" t="n">
-        <v>118.6899</v>
+        <v>119.2639</v>
       </c>
       <c r="E43" s="1" t="n">
-        <v>181.4767</v>
+        <f aca="false">ABS(C$55-C43)</f>
+        <v>0.87136666666666</v>
       </c>
       <c r="F43" s="1" t="n">
-        <v>114.9413</v>
+        <f aca="false">ABS(D$55-D43)</f>
+        <v>0.237899999999996</v>
       </c>
       <c r="G43" s="1" t="n">
-        <f aca="false">C43-E43</f>
-        <v>4.737</v>
+        <v>179.7512</v>
       </c>
       <c r="H43" s="1" t="n">
-        <f aca="false">D43-F43</f>
-        <v>3.7486</v>
+        <v>115.5621</v>
+      </c>
+      <c r="I43" s="1" t="n">
+        <f aca="false">ABS(G$55-G43)</f>
+        <v>0.849799999999988</v>
+      </c>
+      <c r="J43" s="1" t="n">
+        <f aca="false">ABS(H$55-H43)</f>
+        <v>0.243466666666663</v>
+      </c>
+      <c r="K43" s="1" t="n">
+        <f aca="false">C43-G43</f>
+        <v>4.71669999999997</v>
+      </c>
+      <c r="L43" s="1" t="n">
+        <f aca="false">D43-H43</f>
+        <v>3.70180000000001</v>
+      </c>
+      <c r="M43" s="1" t="n">
+        <f aca="false">ABS(K$55-K43)</f>
+        <v>0.0215666666666818</v>
+      </c>
+      <c r="N43" s="1" t="n">
+        <f aca="false">ABS(L$55-L43)</f>
+        <v>0.00556666666666672</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3633,24 +3709,48 @@
         <v>2</v>
       </c>
       <c r="C44" s="1" t="n">
-        <v>182.3538</v>
+        <v>184.7837</v>
       </c>
       <c r="D44" s="1" t="n">
-        <v>100.0818</v>
+        <v>120.0267</v>
       </c>
       <c r="E44" s="1" t="n">
-        <v>177.653</v>
+        <f aca="false">ABS(C$55-C44)</f>
+        <v>0.555566666666635</v>
       </c>
       <c r="F44" s="1" t="n">
-        <v>97.5565</v>
+        <f aca="false">ABS(D$55-D44)</f>
+        <v>0.524900000000002</v>
       </c>
       <c r="G44" s="1" t="n">
-        <f aca="false">C44-E44</f>
-        <v>4.70080000000002</v>
+        <v>179.9944</v>
       </c>
       <c r="H44" s="1" t="n">
-        <f aca="false">D44-F44</f>
-        <v>2.5253</v>
+        <v>116.3367</v>
+      </c>
+      <c r="I44" s="1" t="n">
+        <f aca="false">ABS(G$55-G44)</f>
+        <v>0.606599999999986</v>
+      </c>
+      <c r="J44" s="1" t="n">
+        <f aca="false">ABS(H$55-H44)</f>
+        <v>0.531133333333329</v>
+      </c>
+      <c r="K44" s="1" t="n">
+        <f aca="false">C44-G44</f>
+        <v>4.7893</v>
+      </c>
+      <c r="L44" s="1" t="n">
+        <f aca="false">D44-H44</f>
+        <v>3.69000000000001</v>
+      </c>
+      <c r="M44" s="1" t="n">
+        <f aca="false">ABS(K$55-K44)</f>
+        <v>0.0510333333333408</v>
+      </c>
+      <c r="N44" s="1" t="n">
+        <f aca="false">ABS(L$55-L44)</f>
+        <v>0.0062333333333271</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3661,24 +3761,48 @@
         <v>3</v>
       </c>
       <c r="C45" s="1" t="n">
-        <v>186.6589</v>
+        <v>186.7662</v>
       </c>
       <c r="D45" s="1" t="n">
-        <v>99.6557</v>
+        <v>119.2148</v>
       </c>
       <c r="E45" s="1" t="n">
-        <v>181.7956</v>
+        <f aca="false">ABS(C$55-C45)</f>
+        <v>1.42693333333335</v>
       </c>
       <c r="F45" s="1" t="n">
-        <v>97.157</v>
+        <f aca="false">ABS(D$55-D45)</f>
+        <v>0.287000000000006</v>
       </c>
       <c r="G45" s="1" t="n">
-        <f aca="false">C45-E45</f>
-        <v>4.86329999999998</v>
+        <v>182.0574</v>
       </c>
       <c r="H45" s="1" t="n">
-        <f aca="false">D45-F45</f>
-        <v>2.4987</v>
+        <v>115.5179</v>
+      </c>
+      <c r="I45" s="1" t="n">
+        <f aca="false">ABS(G$55-G45)</f>
+        <v>1.4564</v>
+      </c>
+      <c r="J45" s="1" t="n">
+        <f aca="false">ABS(H$55-H45)</f>
+        <v>0.287666666666667</v>
+      </c>
+      <c r="K45" s="1" t="n">
+        <f aca="false">C45-G45</f>
+        <v>4.7088</v>
+      </c>
+      <c r="L45" s="1" t="n">
+        <f aca="false">D45-H45</f>
+        <v>3.6969</v>
+      </c>
+      <c r="M45" s="1" t="n">
+        <f aca="false">ABS(K$55-K45)</f>
+        <v>0.0294666666666599</v>
+      </c>
+      <c r="N45" s="1" t="n">
+        <f aca="false">ABS(L$55-L45)</f>
+        <v>0.000666666666660376</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3689,24 +3813,48 @@
         <v>1</v>
       </c>
       <c r="C46" s="1" t="n">
-        <v>359.6653</v>
+        <v>348.4523</v>
       </c>
       <c r="D46" s="1" t="n">
-        <v>199.1861</v>
+        <v>193.787</v>
       </c>
       <c r="E46" s="1" t="n">
-        <v>349.5299</v>
+        <f aca="false">ABS(C$56-C46)</f>
+        <v>2.11090000000001</v>
       </c>
       <c r="F46" s="1" t="n">
-        <v>195.0206</v>
+        <f aca="false">ABS(D$56-D46)</f>
+        <v>4.01086666666666</v>
       </c>
       <c r="G46" s="1" t="n">
-        <f aca="false">C46-E46</f>
-        <v>10.1354</v>
+        <v>337.951</v>
       </c>
       <c r="H46" s="1" t="n">
-        <f aca="false">D46-F46</f>
-        <v>4.16550000000001</v>
+        <v>189.6535</v>
+      </c>
+      <c r="I46" s="1" t="n">
+        <f aca="false">ABS(G$56-G46)</f>
+        <v>1.71866666666671</v>
+      </c>
+      <c r="J46" s="1" t="n">
+        <f aca="false">ABS(H$56-H46)</f>
+        <v>4.00956666666664</v>
+      </c>
+      <c r="K46" s="1" t="n">
+        <f aca="false">C46-G46</f>
+        <v>10.5013</v>
+      </c>
+      <c r="L46" s="1" t="n">
+        <f aca="false">D46-H46</f>
+        <v>4.1335</v>
+      </c>
+      <c r="M46" s="1" t="n">
+        <f aca="false">ABS(K$56-K46)</f>
+        <v>0.392233333333309</v>
+      </c>
+      <c r="N46" s="1" t="n">
+        <f aca="false">ABS(L$56-L46)</f>
+        <v>0.00129999999999608</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3717,24 +3865,48 @@
         <v>2</v>
       </c>
       <c r="C47" s="1" t="n">
-        <v>337.4942</v>
+        <v>346.7371</v>
       </c>
       <c r="D47" s="1" t="n">
-        <v>158.9194</v>
+        <v>203.8251</v>
       </c>
       <c r="E47" s="1" t="n">
-        <v>327.7298</v>
+        <f aca="false">ABS(C$56-C47)</f>
+        <v>0.395700000000033</v>
       </c>
       <c r="F47" s="1" t="n">
-        <v>155.9664</v>
+        <f aca="false">ABS(D$56-D47)</f>
+        <v>6.02723333333333</v>
       </c>
       <c r="G47" s="1" t="n">
-        <f aca="false">C47-E47</f>
-        <v>9.76439999999997</v>
+        <v>336.698</v>
       </c>
       <c r="H47" s="1" t="n">
-        <f aca="false">D47-F47</f>
-        <v>2.953</v>
+        <v>199.6895</v>
+      </c>
+      <c r="I47" s="1" t="n">
+        <f aca="false">ABS(G$56-G47)</f>
+        <v>0.465666666666664</v>
+      </c>
+      <c r="J47" s="1" t="n">
+        <f aca="false">ABS(H$56-H47)</f>
+        <v>6.02643333333336</v>
+      </c>
+      <c r="K47" s="1" t="n">
+        <f aca="false">C47-G47</f>
+        <v>10.0391</v>
+      </c>
+      <c r="L47" s="1" t="n">
+        <f aca="false">D47-H47</f>
+        <v>4.13559999999998</v>
+      </c>
+      <c r="M47" s="1" t="n">
+        <f aca="false">ABS(K$56-K47)</f>
+        <v>0.0699666666666303</v>
+      </c>
+      <c r="N47" s="1" t="n">
+        <f aca="false">ABS(L$56-L47)</f>
+        <v>0.000799999999988366</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3745,53 +3917,59 @@
         <v>3</v>
       </c>
       <c r="C48" s="1" t="n">
-        <v>349.4293</v>
+        <v>343.8348</v>
       </c>
       <c r="D48" s="1" t="n">
-        <v>166.705</v>
+        <v>195.7815</v>
       </c>
       <c r="E48" s="1" t="n">
-        <v>340.0153</v>
+        <f aca="false">ABS(C$56-C48)</f>
+        <v>2.50659999999999</v>
       </c>
       <c r="F48" s="1" t="n">
-        <v>163.6936</v>
+        <f aca="false">ABS(D$56-D48)</f>
+        <v>2.01636666666667</v>
       </c>
       <c r="G48" s="1" t="n">
-        <f aca="false">C48-E48</f>
-        <v>9.41399999999999</v>
+        <v>334.048</v>
       </c>
       <c r="H48" s="1" t="n">
-        <f aca="false">D48-F48</f>
-        <v>3.01140000000001</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0"/>
-      <c r="B49" s="0"/>
-      <c r="C49" s="0"/>
-      <c r="D49" s="0"/>
-      <c r="E49" s="0"/>
-      <c r="F49" s="0"/>
-      <c r="G49" s="0"/>
-      <c r="H49" s="0"/>
+        <v>191.6462</v>
+      </c>
+      <c r="I48" s="1" t="n">
+        <f aca="false">ABS(G$56-G48)</f>
+        <v>2.18433333333331</v>
+      </c>
+      <c r="J48" s="1" t="n">
+        <f aca="false">ABS(H$56-H48)</f>
+        <v>2.01686666666666</v>
+      </c>
+      <c r="K48" s="1" t="n">
+        <f aca="false">C48-G48</f>
+        <v>9.78679999999997</v>
+      </c>
+      <c r="L48" s="1" t="n">
+        <f aca="false">D48-H48</f>
+        <v>4.1353</v>
+      </c>
+      <c r="M48" s="1" t="n">
+        <f aca="false">ABS(K$56-K48)</f>
+        <v>0.322266666666678</v>
+      </c>
+      <c r="N48" s="1" t="n">
+        <f aca="false">ABS(L$56-L48)</f>
+        <v>0.000500000000006828</v>
+      </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B50" s="0"/>
-      <c r="C50" s="0"/>
-      <c r="D50" s="0"/>
-      <c r="E50" s="0"/>
-      <c r="F50" s="0"/>
-      <c r="G50" s="0"/>
-      <c r="H50" s="0"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="B51" s="0"/>
+        <v>43</v>
+      </c>
       <c r="C51" s="1" t="s">
         <v>15</v>
       </c>
@@ -3799,256 +3977,658 @@
         <v>16</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="G51" s="1" t="s">
         <v>15</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>16</v>
+      </c>
+      <c r="I51" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J51" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K51" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L51" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M51" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N51" s="1" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B52" s="0"/>
       <c r="C52" s="1" t="n">
         <f aca="false">AVERAGE(C34:C36)</f>
-        <v>13.1821</v>
+        <v>13.0768666666667</v>
       </c>
       <c r="D52" s="1" t="n">
         <f aca="false">AVERAGE(D34:D36)</f>
-        <v>8.67006666666667</v>
+        <v>9.71746666666667</v>
       </c>
       <c r="E52" s="1" t="n">
-        <f aca="false">AVERAGE(E34:E36)</f>
-        <v>12.0264333333333</v>
+        <f aca="false">C52/D52</f>
+        <v>1.34570738601282</v>
       </c>
       <c r="F52" s="1" t="n">
-        <f aca="false">AVERAGE(F34:F36)</f>
-        <v>6.85333333333333</v>
+        <f aca="false">ABS(E$57-E52)</f>
+        <v>0.1829088128598</v>
       </c>
       <c r="G52" s="1" t="n">
         <f aca="false">AVERAGE(G34:G36)</f>
-        <v>1.15566666666667</v>
+        <v>11.9309</v>
       </c>
       <c r="H52" s="1" t="n">
         <f aca="false">AVERAGE(H34:H36)</f>
-        <v>1.81673333333333</v>
+        <v>7.14333333333333</v>
+      </c>
+      <c r="I52" s="1" t="n">
+        <f aca="false">G52/H52</f>
+        <v>1.67021465235651</v>
+      </c>
+      <c r="J52" s="1" t="n">
+        <f aca="false">ABS(I$57-I52)</f>
+        <v>0.05311081703535</v>
+      </c>
+      <c r="K52" s="1" t="n">
+        <f aca="false">AVERAGE(K34:K36)</f>
+        <v>1.14596666666667</v>
+      </c>
+      <c r="L52" s="1" t="n">
+        <f aca="false">AVERAGE(L34:L36)</f>
+        <v>2.57413333333333</v>
+      </c>
+      <c r="M52" s="1" t="n">
+        <f aca="false">K52/L52</f>
+        <v>0.445185434579923</v>
+      </c>
+      <c r="N52" s="1" t="n">
+        <f aca="false">ABS(M$57-M52)</f>
+        <v>0.665279672229248</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="n">
         <v>35</v>
       </c>
-      <c r="B53" s="0"/>
       <c r="C53" s="1" t="n">
         <f aca="false">AVERAGE(C37:C39)</f>
-        <v>49.8779</v>
+        <v>50.5148</v>
       </c>
       <c r="D53" s="1" t="n">
         <f aca="false">AVERAGE(D37:D39)</f>
-        <v>28.5561333333333</v>
+        <v>33.9689666666667</v>
       </c>
       <c r="E53" s="1" t="n">
-        <f aca="false">AVERAGE(E37:E39)</f>
-        <v>48.1483</v>
+        <f aca="false">C53/D53</f>
+        <v>1.48708674289965</v>
       </c>
       <c r="F53" s="1" t="n">
-        <f aca="false">AVERAGE(F37:F39)</f>
-        <v>26.4206666666667</v>
+        <f aca="false">ABS(E$57-E53)</f>
+        <v>0.0415294559729686</v>
       </c>
       <c r="G53" s="1" t="n">
         <f aca="false">AVERAGE(G37:G39)</f>
-        <v>1.7296</v>
+        <v>48.7628333333333</v>
       </c>
       <c r="H53" s="1" t="n">
         <f aca="false">AVERAGE(H37:H39)</f>
-        <v>2.13546666666667</v>
+        <v>31.0629</v>
+      </c>
+      <c r="I53" s="1" t="n">
+        <f aca="false">G53/H53</f>
+        <v>1.56980942968407</v>
+      </c>
+      <c r="J53" s="1" t="n">
+        <f aca="false">ABS(I$57-I53)</f>
+        <v>0.0472944056370881</v>
+      </c>
+      <c r="K53" s="1" t="n">
+        <f aca="false">AVERAGE(K37:K39)</f>
+        <v>1.75196666666667</v>
+      </c>
+      <c r="L53" s="1" t="n">
+        <f aca="false">AVERAGE(L37:L39)</f>
+        <v>2.90606666666667</v>
+      </c>
+      <c r="M53" s="1" t="n">
+        <f aca="false">K53/L53</f>
+        <v>0.602865270353972</v>
+      </c>
+      <c r="N53" s="1" t="n">
+        <f aca="false">ABS(M$57-M53)</f>
+        <v>0.507599836455199</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="n">
         <v>55</v>
       </c>
-      <c r="B54" s="0"/>
       <c r="C54" s="1" t="n">
         <f aca="false">AVERAGE(C40:C42)</f>
-        <v>90.24</v>
+        <v>88.9548666666667</v>
       </c>
       <c r="D54" s="1" t="n">
         <f aca="false">AVERAGE(D40:D42)</f>
-        <v>53.3351333333333</v>
+        <v>58.9742666666667</v>
       </c>
       <c r="E54" s="1" t="n">
-        <f aca="false">AVERAGE(E40:E42)</f>
-        <v>87.7489</v>
+        <f aca="false">C54/D54</f>
+        <v>1.50836749135781</v>
       </c>
       <c r="F54" s="1" t="n">
-        <f aca="false">AVERAGE(F40:F42)</f>
-        <v>50.8828666666667</v>
+        <f aca="false">ABS(E$57-E54)</f>
+        <v>0.0202487075148028</v>
       </c>
       <c r="G54" s="1" t="n">
         <f aca="false">AVERAGE(G40:G42)</f>
-        <v>2.4911</v>
+        <v>86.4948333333333</v>
       </c>
       <c r="H54" s="1" t="n">
         <f aca="false">AVERAGE(H40:H42)</f>
-        <v>2.45226666666667</v>
+        <v>55.8101666666667</v>
+      </c>
+      <c r="I54" s="1" t="n">
+        <f aca="false">G54/H54</f>
+        <v>1.54980424713538</v>
+      </c>
+      <c r="J54" s="1" t="n">
+        <f aca="false">ABS(I$57-I54)</f>
+        <v>0.0672995881857805</v>
+      </c>
+      <c r="K54" s="1" t="n">
+        <f aca="false">AVERAGE(K40:K42)</f>
+        <v>2.46003333333333</v>
+      </c>
+      <c r="L54" s="1" t="n">
+        <f aca="false">AVERAGE(L40:L42)</f>
+        <v>3.1641</v>
+      </c>
+      <c r="M54" s="1" t="n">
+        <f aca="false">K54/L54</f>
+        <v>0.777482801849918</v>
+      </c>
+      <c r="N54" s="1" t="n">
+        <f aca="false">ABS(M$57-M54)</f>
+        <v>0.332982304959253</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="n">
         <v>85</v>
       </c>
-      <c r="B55" s="0"/>
       <c r="C55" s="1" t="n">
         <f aca="false">AVERAGE(C43:C45)</f>
-        <v>185.075466666667</v>
+        <v>185.339266666667</v>
       </c>
       <c r="D55" s="1" t="n">
         <f aca="false">AVERAGE(D43:D45)</f>
-        <v>106.142466666667</v>
+        <v>119.5018</v>
       </c>
       <c r="E55" s="1" t="n">
-        <f aca="false">AVERAGE(E43:E45)</f>
-        <v>180.308433333333</v>
+        <f aca="false">C55/D55</f>
+        <v>1.55093284508406</v>
       </c>
       <c r="F55" s="1" t="n">
-        <f aca="false">AVERAGE(F43:F45)</f>
-        <v>103.218266666667</v>
+        <f aca="false">ABS(E$57-E55)</f>
+        <v>0.0223166462114475</v>
       </c>
       <c r="G55" s="1" t="n">
         <f aca="false">AVERAGE(G43:G45)</f>
-        <v>4.76703333333333</v>
+        <v>180.601</v>
       </c>
       <c r="H55" s="1" t="n">
         <f aca="false">AVERAGE(H43:H45)</f>
-        <v>2.9242</v>
+        <v>115.805566666667</v>
+      </c>
+      <c r="I55" s="1" t="n">
+        <f aca="false">G55/H55</f>
+        <v>1.55951915955681</v>
+      </c>
+      <c r="J55" s="1" t="n">
+        <f aca="false">ABS(I$57-I55)</f>
+        <v>0.0575846757643503</v>
+      </c>
+      <c r="K55" s="1" t="n">
+        <f aca="false">AVERAGE(K43:K45)</f>
+        <v>4.73826666666666</v>
+      </c>
+      <c r="L55" s="1" t="n">
+        <f aca="false">AVERAGE(L43:L45)</f>
+        <v>3.69623333333334</v>
+      </c>
+      <c r="M55" s="1" t="n">
+        <f aca="false">K55/L55</f>
+        <v>1.28191762785538</v>
+      </c>
+      <c r="N55" s="1" t="n">
+        <f aca="false">ABS(M$57-M55)</f>
+        <v>0.171452521046209</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="n">
         <v>116</v>
       </c>
-      <c r="B56" s="0"/>
       <c r="C56" s="1" t="n">
         <f aca="false">AVERAGE(C46:C48)</f>
-        <v>348.862933333333</v>
+        <v>346.3414</v>
       </c>
       <c r="D56" s="1" t="n">
         <f aca="false">AVERAGE(D46:D48)</f>
-        <v>174.936833333333</v>
+        <v>197.797866666667</v>
       </c>
       <c r="E56" s="1" t="n">
-        <f aca="false">AVERAGE(E46:E48)</f>
-        <v>339.091666666667</v>
+        <f aca="false">C56/D56</f>
+        <v>1.75098652900874</v>
       </c>
       <c r="F56" s="1" t="n">
-        <f aca="false">AVERAGE(F46:F48)</f>
-        <v>171.5602</v>
+        <f aca="false">ABS(E$57-E56)</f>
+        <v>0.222370330136123</v>
       </c>
       <c r="G56" s="1" t="n">
         <f aca="false">AVERAGE(G46:G48)</f>
-        <v>9.77126666666665</v>
+        <v>336.232333333333</v>
       </c>
       <c r="H56" s="1" t="n">
         <f aca="false">AVERAGE(H46:H48)</f>
-        <v>3.37663333333334</v>
+        <v>193.663066666667</v>
+      </c>
+      <c r="I56" s="1" t="n">
+        <f aca="false">G56/H56</f>
+        <v>1.73617168787303</v>
+      </c>
+      <c r="J56" s="1" t="n">
+        <f aca="false">ABS(I$57-I56)</f>
+        <v>0.119067852551868</v>
+      </c>
+      <c r="K56" s="1" t="n">
+        <f aca="false">AVERAGE(K46:K48)</f>
+        <v>10.1090666666666</v>
+      </c>
+      <c r="L56" s="1" t="n">
+        <f aca="false">AVERAGE(L46:L48)</f>
+        <v>4.13479999999999</v>
+      </c>
+      <c r="M56" s="1" t="n">
+        <f aca="false">K56/L56</f>
+        <v>2.44487439940666</v>
+      </c>
+      <c r="N56" s="1" t="n">
+        <f aca="false">ABS(M$57-M56)</f>
+        <v>1.33440929259749</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0"/>
-      <c r="B57" s="0"/>
-      <c r="C57" s="0"/>
-      <c r="D57" s="0"/>
-      <c r="E57" s="0"/>
-      <c r="F57" s="0"/>
-      <c r="G57" s="0"/>
-      <c r="H57" s="0"/>
-    </row>
-    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0"/>
-      <c r="B58" s="0"/>
-      <c r="C58" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E58" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="H58" s="1" t="s">
-        <v>25</v>
+      <c r="E57" s="1" t="n">
+        <f aca="false">AVERAGE(E52:E56)</f>
+        <v>1.52861619887262</v>
+      </c>
+      <c r="F57" s="1" t="n">
+        <f aca="false">AVERAGE(F52:F56)</f>
+        <v>0.0978747905390285</v>
+      </c>
+      <c r="I57" s="1" t="n">
+        <f aca="false">AVERAGE(I52:I56)</f>
+        <v>1.61710383532116</v>
+      </c>
+      <c r="J57" s="1" t="n">
+        <f aca="false">AVERAGE(J52:J56)</f>
+        <v>0.0688714678348874</v>
+      </c>
+      <c r="M57" s="1" t="n">
+        <f aca="false">AVERAGE(M52:M56)</f>
+        <v>1.11046510680917</v>
+      </c>
+      <c r="N57" s="1" t="n">
+        <f aca="false">AVERAGE(N52:N56)</f>
+        <v>0.60234472545748</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C59" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G59" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H59" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K59" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L59" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="C60" s="1" t="n">
+        <f aca="false">AVERAGE(E34:E36)</f>
+        <v>1.03677777777778</v>
+      </c>
+      <c r="D60" s="1" t="n">
+        <f aca="false">AVERAGE(F34:F36)</f>
+        <v>0.0759555555555552</v>
+      </c>
+      <c r="G60" s="1" t="n">
+        <f aca="false">AVERAGE(I34:I36)</f>
+        <v>0.940666666666667</v>
+      </c>
+      <c r="H60" s="1" t="n">
+        <f aca="false">AVERAGE(J34:J36)</f>
+        <v>0.0765111111111111</v>
+      </c>
+      <c r="K60" s="1" t="n">
+        <f aca="false">AVERAGE(M34:M36)</f>
+        <v>0.0961111111111113</v>
+      </c>
+      <c r="L60" s="1" t="n">
+        <f aca="false">AVERAGE(N34:N36)</f>
+        <v>0.00784444444444432</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="C61" s="1" t="n">
+        <f aca="false">AVERAGE(E37:E39)</f>
+        <v>1.73086666666667</v>
+      </c>
+      <c r="D61" s="1" t="n">
+        <f aca="false">AVERAGE(F37:F39)</f>
+        <v>0.256622222222224</v>
+      </c>
+      <c r="G61" s="1" t="n">
+        <f aca="false">AVERAGE(I37:I39)</f>
+        <v>1.68271111111111</v>
+      </c>
+      <c r="H61" s="1" t="n">
+        <f aca="false">AVERAGE(J37:J39)</f>
+        <v>0.2606</v>
+      </c>
+      <c r="K61" s="1" t="n">
+        <f aca="false">AVERAGE(M37:M39)</f>
+        <v>0.0481555555555546</v>
+      </c>
+      <c r="L61" s="1" t="n">
+        <f aca="false">AVERAGE(N37:N39)</f>
+        <v>0.0062888888888876</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="C62" s="1" t="n">
+        <f aca="false">AVERAGE(E40:E42)</f>
+        <v>0.348955555555558</v>
+      </c>
+      <c r="D62" s="1" t="n">
+        <f aca="false">AVERAGE(F40:F42)</f>
+        <v>0.189155555555556</v>
+      </c>
+      <c r="G62" s="1" t="n">
+        <f aca="false">AVERAGE(I40:I42)</f>
+        <v>0.357644444444446</v>
+      </c>
+      <c r="H62" s="1" t="n">
+        <f aca="false">AVERAGE(J40:J42)</f>
+        <v>0.189577777777778</v>
+      </c>
+      <c r="K62" s="1" t="n">
+        <f aca="false">AVERAGE(M40:M42)</f>
+        <v>0.0107777777777756</v>
+      </c>
+      <c r="L62" s="1" t="n">
+        <f aca="false">AVERAGE(N40:N42)</f>
+        <v>0.0138666666666659</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="C63" s="1" t="n">
+        <f aca="false">AVERAGE(E43:E45)</f>
+        <v>0.951288888888882</v>
+      </c>
+      <c r="D63" s="1" t="n">
+        <f aca="false">AVERAGE(F43:F45)</f>
+        <v>0.349933333333335</v>
+      </c>
+      <c r="G63" s="1" t="n">
+        <f aca="false">AVERAGE(I43:I45)</f>
+        <v>0.970933333333325</v>
+      </c>
+      <c r="H63" s="1" t="n">
+        <f aca="false">AVERAGE(J43:J45)</f>
+        <v>0.354088888888886</v>
+      </c>
+      <c r="K63" s="1" t="n">
+        <f aca="false">AVERAGE(M43:M45)</f>
+        <v>0.0340222222222275</v>
+      </c>
+      <c r="L63" s="1" t="n">
+        <f aca="false">AVERAGE(N43:N45)</f>
+        <v>0.0041555555555514</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="1" t="n">
+        <v>116</v>
+      </c>
+      <c r="C64" s="1" t="n">
+        <f aca="false">AVERAGE(E46:E48)</f>
+        <v>1.67106666666668</v>
+      </c>
+      <c r="D64" s="1" t="n">
+        <f aca="false">AVERAGE(F46:F48)</f>
+        <v>4.01815555555555</v>
+      </c>
+      <c r="G64" s="1" t="n">
+        <f aca="false">AVERAGE(I46:I48)</f>
+        <v>1.45622222222223</v>
+      </c>
+      <c r="H64" s="1" t="n">
+        <f aca="false">AVERAGE(J46:J48)</f>
+        <v>4.01762222222222</v>
+      </c>
+      <c r="K64" s="1" t="n">
+        <f aca="false">AVERAGE(M46:M48)</f>
+        <v>0.261488888888872</v>
+      </c>
+      <c r="L64" s="1" t="n">
+        <f aca="false">AVERAGE(N46:N48)</f>
+        <v>0.000866666666663759</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E65" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C66" s="0" t="n">
+        <f aca="false">G52/C52</f>
+        <v>0.912366876876724</v>
+      </c>
+      <c r="D66" s="1" t="n">
+        <f aca="false">H52/D52</f>
+        <v>0.735102427244412</v>
+      </c>
+      <c r="E66" s="1" t="n">
+        <f aca="false">ABS(D$71-D66)</f>
+        <v>0.173710583171285</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C67" s="0" t="n">
+        <f aca="false">G53/C53</f>
+        <v>0.965317755060563</v>
+      </c>
+      <c r="D67" s="1" t="n">
+        <f aca="false">H53/D53</f>
+        <v>0.914449365057715</v>
+      </c>
+      <c r="E67" s="1" t="n">
+        <f aca="false">ABS(D$71-D67)</f>
+        <v>0.00563635464201706</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C68" s="0" t="n">
+        <f aca="false">G54/C54</f>
+        <v>0.972345151811068</v>
+      </c>
+      <c r="D68" s="1" t="n">
+        <f aca="false">H54/D54</f>
+        <v>0.946347785587838</v>
+      </c>
+      <c r="E68" s="1" t="n">
+        <f aca="false">ABS(D$71-D68)</f>
+        <v>0.037534775172141</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C69" s="0" t="n">
+        <f aca="false">G55/C55</f>
+        <v>0.974434631409282</v>
+      </c>
+      <c r="D69" s="1" t="n">
+        <f aca="false">H55/D55</f>
+        <v>0.969069643023508</v>
+      </c>
+      <c r="E69" s="1" t="n">
+        <f aca="false">ABS(D$71-D69)</f>
+        <v>0.0602566326078107</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C70" s="0" t="n">
+        <f aca="false">G56/C56</f>
+        <v>0.970811844420948</v>
+      </c>
+      <c r="D70" s="1" t="n">
+        <f aca="false">H56/D56</f>
+        <v>0.979095831165014</v>
+      </c>
+      <c r="E70" s="1" t="n">
+        <f aca="false">ABS(D$71-D70)</f>
+        <v>0.0702828207493168</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D71" s="1" t="n">
+        <f aca="false">AVERAGE(D66:D70)</f>
+        <v>0.908813010415697</v>
+      </c>
+      <c r="E71" s="1" t="n">
+        <f aca="false">AVERAGE(E66:E70)</f>
+        <v>0.0694842332685142</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C72" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F72" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G72" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H72" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B59" s="0"/>
-      <c r="C59" s="1" t="n">
+      <c r="C73" s="1" t="n">
         <f aca="false">SLOPE(C52:C56,$A$52:$A$56)</f>
-        <v>3.16306160050114</v>
-      </c>
-      <c r="D59" s="1" t="n">
+        <v>3.14283802952001</v>
+      </c>
+      <c r="D73" s="1" t="n">
         <f aca="false">SLOPE(D52:D56,$A$52:$A$56)</f>
-        <v>1.59971162399186</v>
-      </c>
-      <c r="E59" s="1" t="n">
-        <f aca="false">SLOPE(E52:E56,$A$52:$A$56)</f>
-        <v>3.08288810194973</v>
-      </c>
-      <c r="F59" s="1" t="n">
-        <f aca="false">SLOPE(F52:F56,$A$52:$A$56)</f>
-        <v>1.58467074817947</v>
-      </c>
-      <c r="G59" s="1" t="n">
+        <v>1.80232411616162</v>
+      </c>
+      <c r="E73" s="1" t="n">
         <f aca="false">SLOPE(G52:G56,$A$52:$A$56)</f>
-        <v>0.0801734985514054</v>
-      </c>
-      <c r="H59" s="1" t="n">
+        <v>3.05999938434735</v>
+      </c>
+      <c r="F73" s="1" t="n">
         <f aca="false">SLOPE(H52:H56,$A$52:$A$56)</f>
-        <v>0.0150408758123875</v>
-      </c>
-    </row>
-    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A60" s="7" t="s">
+        <v>1.78723722985671</v>
+      </c>
+      <c r="G73" s="1" t="n">
+        <f aca="false">SLOPE(K52:K56,$A$52:$A$56)</f>
+        <v>0.0828386451726566</v>
+      </c>
+      <c r="H73" s="1" t="n">
+        <f aca="false">SLOPE(L52:L56,$A$52:$A$56)</f>
+        <v>0.0150868863049095</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B60" s="7"/>
-      <c r="C60" s="7"/>
-      <c r="D60" s="7" t="n">
-        <f aca="false">C59/D59</f>
-        <v>1.97726987355893</v>
-      </c>
-      <c r="E60" s="7"/>
-      <c r="F60" s="7" t="n">
-        <f aca="false">E59/F59</f>
-        <v>1.94544393874341</v>
-      </c>
-      <c r="G60" s="7"/>
-      <c r="H60" s="7" t="n">
-        <f aca="false">G59/H59</f>
-        <v>5.33037434464923</v>
+      <c r="B74" s="7"/>
+      <c r="C74" s="7"/>
+      <c r="D74" s="7" t="n">
+        <f aca="false">C73/D73</f>
+        <v>1.74376961465359</v>
+      </c>
+      <c r="E74" s="7"/>
+      <c r="F74" s="7" t="n">
+        <f aca="false">E73/F73</f>
+        <v>1.71213945928862</v>
+      </c>
+      <c r="G74" s="7"/>
+      <c r="H74" s="7" t="n">
+        <f aca="false">G73/H73</f>
+        <v>5.49077148846144</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="C32:D32"/>
-    <mergeCell ref="E32:F32"/>
     <mergeCell ref="G32:H32"/>
+    <mergeCell ref="K32:L32"/>
   </mergeCells>
   <conditionalFormatting sqref="C5:C29">
     <cfRule type="colorScale" priority="2">
@@ -4097,7 +4677,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="4" min="4" style="13" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="9" width="27.5408163265306"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4110,7 +4692,7 @@
       <c r="C2" s="0" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="9" t="s">
         <v>33</v>
       </c>
     </row>
@@ -4121,7 +4703,7 @@
       <c r="C3" s="0" t="n">
         <v>0.01</v>
       </c>
-      <c r="D3" s="13" t="n">
+      <c r="D3" s="9" t="n">
         <v>0.000123610152514</v>
       </c>
     </row>
@@ -4132,7 +4714,7 @@
       <c r="C4" s="0" t="n">
         <v>0.005</v>
       </c>
-      <c r="D4" s="13" t="n">
+      <c r="D4" s="9" t="n">
         <v>8.8636610599E-005</v>
       </c>
     </row>
@@ -4143,7 +4725,7 @@
       <c r="C5" s="0" t="n">
         <v>0.001</v>
       </c>
-      <c r="D5" s="13" t="n">
+      <c r="D5" s="9" t="n">
         <v>7.4069997936E-005</v>
       </c>
     </row>
@@ -4154,7 +4736,7 @@
       <c r="C6" s="0" t="n">
         <v>0.0005</v>
       </c>
-      <c r="D6" s="13" t="n">
+      <c r="D6" s="9" t="n">
         <v>6.9892732427E-005</v>
       </c>
     </row>
@@ -4165,7 +4747,7 @@
       <c r="C7" s="0" t="n">
         <v>0.0001</v>
       </c>
-      <c r="D7" s="13" t="n">
+      <c r="D7" s="9" t="n">
         <v>6.9483772677E-005</v>
       </c>
     </row>
@@ -4176,7 +4758,7 @@
       <c r="C8" s="0" t="n">
         <v>5E-005</v>
       </c>
-      <c r="D8" s="14" t="n">
+      <c r="D8" s="10" t="n">
         <v>6.8885761721E-005</v>
       </c>
     </row>
@@ -4187,7 +4769,7 @@
       <c r="C9" s="0" t="n">
         <v>1E-005</v>
       </c>
-      <c r="D9" s="13" t="n">
+      <c r="D9" s="9" t="n">
         <v>9.256733756E-005</v>
       </c>
     </row>
@@ -4198,7 +4780,7 @@
       <c r="C10" s="0" t="n">
         <v>0.01</v>
       </c>
-      <c r="D10" s="13" t="n">
+      <c r="D10" s="9" t="n">
         <v>0.000144385485328</v>
       </c>
     </row>
@@ -4209,7 +4791,7 @@
       <c r="C11" s="0" t="n">
         <v>0.005</v>
       </c>
-      <c r="D11" s="13" t="n">
+      <c r="D11" s="9" t="n">
         <v>9.5978211903E-005</v>
       </c>
     </row>
@@ -4220,7 +4802,7 @@
       <c r="C12" s="0" t="n">
         <v>0.001</v>
       </c>
-      <c r="D12" s="13" t="n">
+      <c r="D12" s="9" t="n">
         <v>8.9935885626E-005</v>
       </c>
     </row>
@@ -4231,7 +4813,7 @@
       <c r="C13" s="0" t="n">
         <v>0.0005</v>
       </c>
-      <c r="D13" s="13" t="n">
+      <c r="D13" s="9" t="n">
         <v>8.4039427747E-005</v>
       </c>
     </row>
@@ -4242,7 +4824,7 @@
       <c r="C14" s="0" t="n">
         <v>0.0001</v>
       </c>
-      <c r="D14" s="13" t="n">
+      <c r="D14" s="9" t="n">
         <v>8.1295489508E-005</v>
       </c>
     </row>
@@ -4253,7 +4835,7 @@
       <c r="C15" s="0" t="n">
         <v>5E-005</v>
       </c>
-      <c r="D15" s="13" t="n">
+      <c r="D15" s="9" t="n">
         <v>8.0391145184E-005</v>
       </c>
     </row>
@@ -4264,7 +4846,7 @@
       <c r="C16" s="0" t="n">
         <v>1E-005</v>
       </c>
-      <c r="D16" s="13" t="n">
+      <c r="D16" s="9" t="n">
         <v>0.000102245641756</v>
       </c>
     </row>
@@ -4275,7 +4857,7 @@
       <c r="C17" s="0" t="n">
         <v>0.01</v>
       </c>
-      <c r="D17" s="13" t="n">
+      <c r="D17" s="9" t="n">
         <v>0.00012816459639</v>
       </c>
     </row>
@@ -4286,7 +4868,7 @@
       <c r="C18" s="0" t="n">
         <v>0.005</v>
       </c>
-      <c r="D18" s="13" t="n">
+      <c r="D18" s="9" t="n">
         <v>9.1854228231E-005</v>
       </c>
     </row>
@@ -4297,7 +4879,7 @@
       <c r="C19" s="0" t="n">
         <v>0.001</v>
       </c>
-      <c r="D19" s="13" t="n">
+      <c r="D19" s="9" t="n">
         <v>7.8748293163E-005</v>
       </c>
     </row>
@@ -4308,7 +4890,7 @@
       <c r="C20" s="0" t="n">
         <v>0.0005</v>
       </c>
-      <c r="D20" s="13" t="n">
+      <c r="D20" s="9" t="n">
         <v>7.6260628703E-005</v>
       </c>
     </row>
@@ -4319,7 +4901,7 @@
       <c r="C21" s="0" t="n">
         <v>0.0001</v>
       </c>
-      <c r="D21" s="13" t="n">
+      <c r="D21" s="9" t="n">
         <v>7.5951844337E-005</v>
       </c>
     </row>
@@ -4330,7 +4912,7 @@
       <c r="C22" s="0" t="n">
         <v>5E-005</v>
       </c>
-      <c r="D22" s="13" t="n">
+      <c r="D22" s="9" t="n">
         <v>7.6219243056E-005</v>
       </c>
     </row>
@@ -4341,7 +4923,7 @@
       <c r="C23" s="0" t="n">
         <v>1E-005</v>
       </c>
-      <c r="D23" s="13" t="n">
+      <c r="D23" s="9" t="n">
         <v>0.000102635014628</v>
       </c>
     </row>
@@ -4352,7 +4934,7 @@
       <c r="C24" s="0" t="n">
         <v>0.01</v>
       </c>
-      <c r="D24" s="13" t="n">
+      <c r="D24" s="9" t="n">
         <v>0.000134039801196</v>
       </c>
     </row>
@@ -4363,7 +4945,7 @@
       <c r="C25" s="0" t="n">
         <v>0.005</v>
       </c>
-      <c r="D25" s="13" t="n">
+      <c r="D25" s="9" t="n">
         <v>9.2438262072E-005</v>
       </c>
     </row>
@@ -4374,7 +4956,7 @@
       <c r="C26" s="0" t="n">
         <v>0.001</v>
       </c>
-      <c r="D26" s="13" t="n">
+      <c r="D26" s="9" t="n">
         <v>7.0732487075E-005</v>
       </c>
     </row>
@@ -4385,7 +4967,7 @@
       <c r="C27" s="0" t="n">
         <v>0.0005</v>
       </c>
-      <c r="D27" s="13" t="n">
+      <c r="D27" s="9" t="n">
         <v>7.0459493145E-005</v>
       </c>
     </row>
@@ -4396,7 +4978,7 @@
       <c r="C28" s="0" t="n">
         <v>0.0001</v>
       </c>
-      <c r="D28" s="13" t="n">
+      <c r="D28" s="9" t="n">
         <v>7.0160800533E-005</v>
       </c>
     </row>
@@ -4407,7 +4989,7 @@
       <c r="C29" s="0" t="n">
         <v>5E-005</v>
       </c>
-      <c r="D29" s="13" t="n">
+      <c r="D29" s="9" t="n">
         <v>7.0123423939E-005</v>
       </c>
     </row>
@@ -4418,7 +5000,7 @@
       <c r="C30" s="0" t="n">
         <v>1E-005</v>
       </c>
-      <c r="D30" s="13" t="n">
+      <c r="D30" s="9" t="n">
         <v>0.000106777326437</v>
       </c>
     </row>
@@ -4429,7 +5011,7 @@
       <c r="C31" s="0" t="n">
         <v>0.01</v>
       </c>
-      <c r="D31" s="13" t="n">
+      <c r="D31" s="9" t="n">
         <v>0.000113149704703</v>
       </c>
     </row>
@@ -4440,7 +5022,7 @@
       <c r="C32" s="0" t="n">
         <v>0.005</v>
       </c>
-      <c r="D32" s="13" t="n">
+      <c r="D32" s="9" t="n">
         <v>8.4696828455E-005</v>
       </c>
     </row>
@@ -4451,7 +5033,7 @@
       <c r="C33" s="0" t="n">
         <v>0.001</v>
       </c>
-      <c r="D33" s="13" t="n">
+      <c r="D33" s="9" t="n">
         <v>7.983539399E-005</v>
       </c>
     </row>
@@ -4462,7 +5044,7 @@
       <c r="C34" s="0" t="n">
         <v>0.0005</v>
       </c>
-      <c r="D34" s="13" t="n">
+      <c r="D34" s="9" t="n">
         <v>7.6452655776E-005</v>
       </c>
     </row>
@@ -4473,7 +5055,7 @@
       <c r="C35" s="0" t="n">
         <v>0.0001</v>
       </c>
-      <c r="D35" s="13" t="n">
+      <c r="D35" s="9" t="n">
         <v>7.5728094089E-005</v>
       </c>
     </row>
@@ -4484,7 +5066,7 @@
       <c r="C36" s="0" t="n">
         <v>5E-005</v>
       </c>
-      <c r="D36" s="13" t="n">
+      <c r="D36" s="9" t="n">
         <v>7.6094336691E-005</v>
       </c>
     </row>
@@ -4495,7 +5077,7 @@
       <c r="C37" s="0" t="n">
         <v>1E-005</v>
       </c>
-      <c r="D37" s="13" t="n">
+      <c r="D37" s="9" t="n">
         <v>9.8175973108E-005</v>
       </c>
     </row>

</xml_diff>

<commit_message>
created space for recording resulst
</commit_message>
<xml_diff>
--- a/stats/stats_compilation.xlsx
+++ b/stats/stats_compilation.xlsx
@@ -5,12 +5,14 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="weights" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="rewards" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="best_rewards" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="weights_1cpu" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="rewards_1cpu" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -58,7 +60,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="46">
   <si>
     <t xml:space="preserve">stats</t>
   </si>
@@ -427,28 +429,28 @@
   </sheetPr>
   <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A40" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E61" activeCellId="0" sqref="E61"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A33" activeCellId="0" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="6.75"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="9.85204081632653"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.6887755102041"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="6.75"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="12.5561224489796"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="6.61224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="1" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2554,30 +2556,56 @@
   </sheetPr>
   <dimension ref="A1:N74"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C45" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L64" activeCellId="0" sqref="L64"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C46" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A32" activeCellId="0" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="4" min="2" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="15.1173469387755"/>
-    <col collapsed="false" hidden="false" max="8" min="6" style="1" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="7.69387755102041"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="13.7704081632653"/>
-    <col collapsed="false" hidden="false" max="1025" min="11" style="1" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="2" style="1" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="14.8469387755102"/>
+    <col collapsed="false" hidden="false" max="8" min="6" style="1" width="12.8265306122449"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="13.5"/>
+    <col collapsed="false" hidden="false" max="1025" min="11" style="1" width="10.3928571428571"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" s="0"/>
+      <c r="C1" s="0"/>
+      <c r="D1" s="0"/>
+      <c r="E1" s="0"/>
+      <c r="F1" s="0"/>
+      <c r="G1" s="0"/>
+      <c r="H1" s="0"/>
+      <c r="I1" s="0"/>
+      <c r="J1" s="0"/>
+      <c r="K1" s="0"/>
+      <c r="L1" s="0"/>
+      <c r="M1" s="0"/>
+      <c r="N1" s="0"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
         <v>27</v>
       </c>
+      <c r="B2" s="0"/>
+      <c r="C2" s="0"/>
+      <c r="D2" s="0"/>
+      <c r="E2" s="0"/>
+      <c r="F2" s="0"/>
+      <c r="G2" s="0"/>
+      <c r="H2" s="0"/>
+      <c r="I2" s="0"/>
+      <c r="J2" s="0"/>
+      <c r="K2" s="0"/>
+      <c r="L2" s="0"/>
+      <c r="M2" s="0"/>
+      <c r="N2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
@@ -2586,12 +2614,22 @@
       <c r="B3" s="1" t="s">
         <v>28</v>
       </c>
+      <c r="C3" s="0"/>
+      <c r="D3" s="0"/>
+      <c r="E3" s="0"/>
+      <c r="F3" s="0"/>
+      <c r="G3" s="0"/>
+      <c r="H3" s="0"/>
       <c r="I3" s="1" t="s">
         <v>29</v>
       </c>
       <c r="J3" s="1" t="s">
         <v>30</v>
       </c>
+      <c r="K3" s="0"/>
+      <c r="L3" s="0"/>
+      <c r="M3" s="0"/>
+      <c r="N3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -2603,18 +2641,25 @@
       <c r="C4" s="1" t="s">
         <v>33</v>
       </c>
+      <c r="D4" s="0"/>
       <c r="E4" s="1" t="s">
         <v>31</v>
       </c>
       <c r="F4" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="G4" s="0"/>
+      <c r="H4" s="0"/>
       <c r="I4" s="1" t="s">
         <v>35</v>
       </c>
       <c r="J4" s="1" t="n">
         <v>0.000234784733038</v>
       </c>
+      <c r="K4" s="0"/>
+      <c r="L4" s="0"/>
+      <c r="M4" s="0"/>
+      <c r="N4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="n">
@@ -2641,12 +2686,17 @@
         <f aca="false">AVERAGE(D5,D10,D15,D20,D25)</f>
         <v>9.60000000000002E-007</v>
       </c>
+      <c r="H5" s="0"/>
       <c r="I5" s="1" t="s">
         <v>36</v>
       </c>
       <c r="J5" s="1" t="n">
         <v>0.000400919205276</v>
       </c>
+      <c r="K5" s="0"/>
+      <c r="L5" s="0"/>
+      <c r="M5" s="0"/>
+      <c r="N5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="n">
@@ -2673,9 +2723,15 @@
         <f aca="false">AVERAGE(D6,D11,D16,D21,D26)</f>
         <v>5.04E-006</v>
       </c>
+      <c r="H6" s="0"/>
+      <c r="I6" s="0"/>
       <c r="J6" s="1" t="n">
         <v>0.000415126851294</v>
       </c>
+      <c r="K6" s="0"/>
+      <c r="L6" s="0"/>
+      <c r="M6" s="0"/>
+      <c r="N6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="n">
@@ -2702,9 +2758,15 @@
         <f aca="false">AVERAGE(D7,D12,D17,D22,D27)</f>
         <v>2.88E-006</v>
       </c>
+      <c r="H7" s="0"/>
+      <c r="I7" s="0"/>
       <c r="J7" s="1" t="n">
         <v>0.000241408168222</v>
       </c>
+      <c r="K7" s="0"/>
+      <c r="L7" s="0"/>
+      <c r="M7" s="0"/>
+      <c r="N7" s="0"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="n">
@@ -2731,9 +2793,15 @@
         <f aca="false">AVERAGE(D8,D13,D18,D23,D28)</f>
         <v>2.08E-006</v>
       </c>
+      <c r="H8" s="0"/>
+      <c r="I8" s="0"/>
       <c r="J8" s="1" t="n">
         <v>0.000355125812348</v>
       </c>
+      <c r="K8" s="0"/>
+      <c r="L8" s="0"/>
+      <c r="M8" s="0"/>
+      <c r="N8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="n">
@@ -2760,6 +2828,8 @@
         <f aca="false">AVERAGE(D9,D14,D19,D24,D29)</f>
         <v>1.6E-006</v>
       </c>
+      <c r="H9" s="0"/>
+      <c r="I9" s="0"/>
       <c r="J9" s="1" t="n">
         <v>0.000243959832005</v>
       </c>
@@ -2767,6 +2837,9 @@
         <f aca="false">AVERAGE(J5:J9)</f>
         <v>0.000331307973829</v>
       </c>
+      <c r="L9" s="0"/>
+      <c r="M9" s="0"/>
+      <c r="N9" s="0"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="n">
@@ -2782,6 +2855,16 @@
         <f aca="false">ABS(F5-C10)</f>
         <v>7.99999999999992E-007</v>
       </c>
+      <c r="E10" s="0"/>
+      <c r="F10" s="0"/>
+      <c r="G10" s="0"/>
+      <c r="H10" s="0"/>
+      <c r="I10" s="0"/>
+      <c r="J10" s="0"/>
+      <c r="K10" s="0"/>
+      <c r="L10" s="0"/>
+      <c r="M10" s="0"/>
+      <c r="N10" s="0"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="n">
@@ -2803,6 +2886,14 @@
       <c r="F11" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="G11" s="0"/>
+      <c r="H11" s="0"/>
+      <c r="I11" s="0"/>
+      <c r="J11" s="0"/>
+      <c r="K11" s="0"/>
+      <c r="L11" s="0"/>
+      <c r="M11" s="0"/>
+      <c r="N11" s="0"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="n">
@@ -2825,6 +2916,14 @@
         <f aca="false">AVERAGE(C4:C9)</f>
         <v>0.0001304</v>
       </c>
+      <c r="G12" s="0"/>
+      <c r="H12" s="0"/>
+      <c r="I12" s="0"/>
+      <c r="J12" s="0"/>
+      <c r="K12" s="0"/>
+      <c r="L12" s="0"/>
+      <c r="M12" s="0"/>
+      <c r="N12" s="0"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="n">
@@ -2847,6 +2946,14 @@
         <f aca="false">AVERAGE(C10:C14)</f>
         <v>0.000134</v>
       </c>
+      <c r="G13" s="0"/>
+      <c r="H13" s="0"/>
+      <c r="I13" s="0"/>
+      <c r="J13" s="0"/>
+      <c r="K13" s="0"/>
+      <c r="L13" s="0"/>
+      <c r="M13" s="0"/>
+      <c r="N13" s="0"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="n">
@@ -2869,6 +2976,14 @@
         <f aca="false">AVERAGE(C15:C19)</f>
         <v>0.0001284</v>
       </c>
+      <c r="G14" s="0"/>
+      <c r="H14" s="0"/>
+      <c r="I14" s="0"/>
+      <c r="J14" s="0"/>
+      <c r="K14" s="0"/>
+      <c r="L14" s="0"/>
+      <c r="M14" s="0"/>
+      <c r="N14" s="0"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="n">
@@ -2891,6 +3006,14 @@
         <f aca="false">AVERAGE(C20:C24)</f>
         <v>0.0001292</v>
       </c>
+      <c r="G15" s="0"/>
+      <c r="H15" s="0"/>
+      <c r="I15" s="0"/>
+      <c r="J15" s="0"/>
+      <c r="K15" s="0"/>
+      <c r="L15" s="0"/>
+      <c r="M15" s="0"/>
+      <c r="N15" s="0"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="n">
@@ -2913,6 +3036,14 @@
         <f aca="false">AVERAGE(C25:C29)</f>
         <v>0.0001316</v>
       </c>
+      <c r="G16" s="0"/>
+      <c r="H16" s="0"/>
+      <c r="I16" s="0"/>
+      <c r="J16" s="0"/>
+      <c r="K16" s="0"/>
+      <c r="L16" s="0"/>
+      <c r="M16" s="0"/>
+      <c r="N16" s="0"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="n">
@@ -2928,6 +3059,16 @@
         <f aca="false">ABS(F7-C17)</f>
         <v>5.59999999999997E-006</v>
       </c>
+      <c r="E17" s="0"/>
+      <c r="F17" s="0"/>
+      <c r="G17" s="0"/>
+      <c r="H17" s="0"/>
+      <c r="I17" s="0"/>
+      <c r="J17" s="0"/>
+      <c r="K17" s="0"/>
+      <c r="L17" s="0"/>
+      <c r="M17" s="0"/>
+      <c r="N17" s="0"/>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="n">
@@ -2943,6 +3084,16 @@
         <f aca="false">ABS(F8-C18)</f>
         <v>1.40000000000001E-006</v>
       </c>
+      <c r="E18" s="0"/>
+      <c r="F18" s="0"/>
+      <c r="G18" s="0"/>
+      <c r="H18" s="0"/>
+      <c r="I18" s="0"/>
+      <c r="J18" s="0"/>
+      <c r="K18" s="0"/>
+      <c r="L18" s="0"/>
+      <c r="M18" s="0"/>
+      <c r="N18" s="0"/>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="n">
@@ -2958,6 +3109,16 @@
         <f aca="false">ABS(F9-C19)</f>
         <v>4.00000000000002E-006</v>
       </c>
+      <c r="E19" s="0"/>
+      <c r="F19" s="0"/>
+      <c r="G19" s="0"/>
+      <c r="H19" s="0"/>
+      <c r="I19" s="0"/>
+      <c r="J19" s="0"/>
+      <c r="K19" s="0"/>
+      <c r="L19" s="0"/>
+      <c r="M19" s="0"/>
+      <c r="N19" s="0"/>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="n">
@@ -2973,6 +3134,16 @@
         <f aca="false">ABS(F5-C20)</f>
         <v>7.99999999999992E-007</v>
       </c>
+      <c r="E20" s="0"/>
+      <c r="F20" s="0"/>
+      <c r="G20" s="0"/>
+      <c r="H20" s="0"/>
+      <c r="I20" s="0"/>
+      <c r="J20" s="0"/>
+      <c r="K20" s="0"/>
+      <c r="L20" s="0"/>
+      <c r="M20" s="0"/>
+      <c r="N20" s="0"/>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="n">
@@ -2988,6 +3159,16 @@
         <f aca="false">ABS(F6-C21)</f>
         <v>7.8E-006</v>
       </c>
+      <c r="E21" s="0"/>
+      <c r="F21" s="0"/>
+      <c r="G21" s="0"/>
+      <c r="H21" s="0"/>
+      <c r="I21" s="0"/>
+      <c r="J21" s="0"/>
+      <c r="K21" s="0"/>
+      <c r="L21" s="0"/>
+      <c r="M21" s="0"/>
+      <c r="N21" s="0"/>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="n">
@@ -3003,6 +3184,16 @@
         <f aca="false">ABS(F7-C22)</f>
         <v>4.0000000000001E-007</v>
       </c>
+      <c r="E22" s="0"/>
+      <c r="F22" s="0"/>
+      <c r="G22" s="0"/>
+      <c r="H22" s="0"/>
+      <c r="I22" s="0"/>
+      <c r="J22" s="0"/>
+      <c r="K22" s="0"/>
+      <c r="L22" s="0"/>
+      <c r="M22" s="0"/>
+      <c r="N22" s="0"/>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="n">
@@ -3018,6 +3209,16 @@
         <f aca="false">ABS(F8-C23)</f>
         <v>4.0000000000001E-007</v>
       </c>
+      <c r="E23" s="0"/>
+      <c r="F23" s="0"/>
+      <c r="G23" s="0"/>
+      <c r="H23" s="0"/>
+      <c r="I23" s="0"/>
+      <c r="J23" s="0"/>
+      <c r="K23" s="0"/>
+      <c r="L23" s="0"/>
+      <c r="M23" s="0"/>
+      <c r="N23" s="0"/>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="n">
@@ -3033,6 +3234,16 @@
         <f aca="false">ABS(F9-C24)</f>
         <v>9.99999999999997E-007</v>
       </c>
+      <c r="E24" s="0"/>
+      <c r="F24" s="0"/>
+      <c r="G24" s="0"/>
+      <c r="H24" s="0"/>
+      <c r="I24" s="0"/>
+      <c r="J24" s="0"/>
+      <c r="K24" s="0"/>
+      <c r="L24" s="0"/>
+      <c r="M24" s="0"/>
+      <c r="N24" s="0"/>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="n">
@@ -3048,6 +3259,16 @@
         <f aca="false">ABS(F5-C25)</f>
         <v>2.20000000000003E-006</v>
       </c>
+      <c r="E25" s="0"/>
+      <c r="F25" s="0"/>
+      <c r="G25" s="0"/>
+      <c r="H25" s="0"/>
+      <c r="I25" s="0"/>
+      <c r="J25" s="0"/>
+      <c r="K25" s="0"/>
+      <c r="L25" s="0"/>
+      <c r="M25" s="0"/>
+      <c r="N25" s="0"/>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="n">
@@ -3063,6 +3284,16 @@
         <f aca="false">ABS(F6-C26)</f>
         <v>1.2E-006</v>
       </c>
+      <c r="E26" s="0"/>
+      <c r="F26" s="0"/>
+      <c r="G26" s="0"/>
+      <c r="H26" s="0"/>
+      <c r="I26" s="0"/>
+      <c r="J26" s="0"/>
+      <c r="K26" s="0"/>
+      <c r="L26" s="0"/>
+      <c r="M26" s="0"/>
+      <c r="N26" s="0"/>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="n">
@@ -3078,6 +3309,16 @@
         <f aca="false">ABS(F7-C27)</f>
         <v>4.40000000000003E-006</v>
       </c>
+      <c r="E27" s="0"/>
+      <c r="F27" s="0"/>
+      <c r="G27" s="0"/>
+      <c r="H27" s="0"/>
+      <c r="I27" s="0"/>
+      <c r="J27" s="0"/>
+      <c r="K27" s="0"/>
+      <c r="L27" s="0"/>
+      <c r="M27" s="0"/>
+      <c r="N27" s="0"/>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="n">
@@ -3093,6 +3334,16 @@
         <f aca="false">ABS(F8-C28)</f>
         <v>3.4E-006</v>
       </c>
+      <c r="E28" s="0"/>
+      <c r="F28" s="0"/>
+      <c r="G28" s="0"/>
+      <c r="H28" s="0"/>
+      <c r="I28" s="0"/>
+      <c r="J28" s="0"/>
+      <c r="K28" s="0"/>
+      <c r="L28" s="0"/>
+      <c r="M28" s="0"/>
+      <c r="N28" s="0"/>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="n">
@@ -3108,12 +3359,51 @@
         <f aca="false">ABS(F9-C29)</f>
         <v>0</v>
       </c>
+      <c r="E29" s="0"/>
+      <c r="F29" s="0"/>
+      <c r="G29" s="0"/>
+      <c r="H29" s="0"/>
+      <c r="I29" s="0"/>
+      <c r="J29" s="0"/>
+      <c r="K29" s="0"/>
+      <c r="L29" s="0"/>
+      <c r="M29" s="0"/>
+      <c r="N29" s="0"/>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0"/>
+      <c r="B30" s="0"/>
       <c r="C30" s="1" t="n">
         <f aca="false">MIN(C5:C29)</f>
         <v>7.1E-005</v>
       </c>
+      <c r="D30" s="0"/>
+      <c r="E30" s="0"/>
+      <c r="F30" s="0"/>
+      <c r="G30" s="0"/>
+      <c r="H30" s="0"/>
+      <c r="I30" s="0"/>
+      <c r="J30" s="0"/>
+      <c r="K30" s="0"/>
+      <c r="L30" s="0"/>
+      <c r="M30" s="0"/>
+      <c r="N30" s="0"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0"/>
+      <c r="B31" s="0"/>
+      <c r="C31" s="0"/>
+      <c r="D31" s="0"/>
+      <c r="E31" s="0"/>
+      <c r="F31" s="0"/>
+      <c r="G31" s="0"/>
+      <c r="H31" s="0"/>
+      <c r="I31" s="0"/>
+      <c r="J31" s="0"/>
+      <c r="K31" s="0"/>
+      <c r="L31" s="0"/>
+      <c r="M31" s="0"/>
+      <c r="N31" s="0"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
@@ -3136,6 +3426,8 @@
         <v>39</v>
       </c>
       <c r="L32" s="8"/>
+      <c r="M32" s="0"/>
+      <c r="N32" s="0"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
@@ -3961,15 +4253,45 @@
         <v>0.000500000000006828</v>
       </c>
     </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0"/>
+      <c r="B49" s="0"/>
+      <c r="C49" s="0"/>
+      <c r="D49" s="0"/>
+      <c r="E49" s="0"/>
+      <c r="F49" s="0"/>
+      <c r="G49" s="0"/>
+      <c r="H49" s="0"/>
+      <c r="I49" s="0"/>
+      <c r="J49" s="0"/>
+      <c r="K49" s="0"/>
+      <c r="L49" s="0"/>
+      <c r="M49" s="0"/>
+      <c r="N49" s="0"/>
+    </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
         <v>19</v>
       </c>
+      <c r="B50" s="0"/>
+      <c r="C50" s="0"/>
+      <c r="D50" s="0"/>
+      <c r="E50" s="0"/>
+      <c r="F50" s="0"/>
+      <c r="G50" s="0"/>
+      <c r="H50" s="0"/>
+      <c r="I50" s="0"/>
+      <c r="J50" s="0"/>
+      <c r="K50" s="0"/>
+      <c r="L50" s="0"/>
+      <c r="M50" s="0"/>
+      <c r="N50" s="0"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="B51" s="0"/>
       <c r="C51" s="1" t="s">
         <v>15</v>
       </c>
@@ -4011,6 +4333,7 @@
       <c r="A52" s="1" t="n">
         <v>11</v>
       </c>
+      <c r="B52" s="0"/>
       <c r="C52" s="1" t="n">
         <f aca="false">AVERAGE(C34:C36)</f>
         <v>13.0768666666667</v>
@@ -4064,6 +4387,7 @@
       <c r="A53" s="1" t="n">
         <v>35</v>
       </c>
+      <c r="B53" s="0"/>
       <c r="C53" s="1" t="n">
         <f aca="false">AVERAGE(C37:C39)</f>
         <v>50.5148</v>
@@ -4117,6 +4441,7 @@
       <c r="A54" s="1" t="n">
         <v>55</v>
       </c>
+      <c r="B54" s="0"/>
       <c r="C54" s="1" t="n">
         <f aca="false">AVERAGE(C40:C42)</f>
         <v>88.9548666666667</v>
@@ -4170,6 +4495,7 @@
       <c r="A55" s="1" t="n">
         <v>85</v>
       </c>
+      <c r="B55" s="0"/>
       <c r="C55" s="1" t="n">
         <f aca="false">AVERAGE(C43:C45)</f>
         <v>185.339266666667</v>
@@ -4223,6 +4549,7 @@
       <c r="A56" s="1" t="n">
         <v>116</v>
       </c>
+      <c r="B56" s="0"/>
       <c r="C56" s="1" t="n">
         <f aca="false">AVERAGE(C46:C48)</f>
         <v>346.3414</v>
@@ -4273,6 +4600,10 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0"/>
+      <c r="B57" s="0"/>
+      <c r="C57" s="0"/>
+      <c r="D57" s="0"/>
       <c r="E57" s="1" t="n">
         <f aca="false">AVERAGE(E52:E56)</f>
         <v>1.52861619887262</v>
@@ -4281,6 +4612,8 @@
         <f aca="false">AVERAGE(F52:F56)</f>
         <v>0.0978747905390285</v>
       </c>
+      <c r="G57" s="0"/>
+      <c r="H57" s="0"/>
       <c r="I57" s="1" t="n">
         <f aca="false">AVERAGE(I52:I56)</f>
         <v>1.61710383532116</v>
@@ -4289,6 +4622,8 @@
         <f aca="false">AVERAGE(J52:J56)</f>
         <v>0.0688714678348874</v>
       </c>
+      <c r="K57" s="0"/>
+      <c r="L57" s="0"/>
       <c r="M57" s="1" t="n">
         <f aca="false">AVERAGE(M52:M56)</f>
         <v>1.11046510680917</v>
@@ -4298,16 +4633,31 @@
         <v>0.60234472545748</v>
       </c>
     </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0"/>
+      <c r="B58" s="0"/>
+      <c r="C58" s="0"/>
+      <c r="D58" s="0"/>
+      <c r="E58" s="0"/>
+      <c r="F58" s="0"/>
+      <c r="G58" s="0"/>
+      <c r="H58" s="0"/>
+      <c r="K58" s="0"/>
+      <c r="L58" s="0"/>
+    </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
         <v>43</v>
       </c>
+      <c r="B59" s="0"/>
       <c r="C59" s="1" t="s">
         <v>41</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>42</v>
       </c>
+      <c r="E59" s="0"/>
+      <c r="F59" s="0"/>
       <c r="G59" s="1" t="s">
         <v>41</v>
       </c>
@@ -4325,6 +4675,7 @@
       <c r="A60" s="1" t="n">
         <v>11</v>
       </c>
+      <c r="B60" s="0"/>
       <c r="C60" s="1" t="n">
         <f aca="false">AVERAGE(E34:E36)</f>
         <v>1.03677777777778</v>
@@ -4333,6 +4684,8 @@
         <f aca="false">AVERAGE(F34:F36)</f>
         <v>0.0759555555555552</v>
       </c>
+      <c r="E60" s="0"/>
+      <c r="F60" s="0"/>
       <c r="G60" s="1" t="n">
         <f aca="false">AVERAGE(I34:I36)</f>
         <v>0.940666666666667</v>
@@ -4354,6 +4707,7 @@
       <c r="A61" s="1" t="n">
         <v>35</v>
       </c>
+      <c r="B61" s="0"/>
       <c r="C61" s="1" t="n">
         <f aca="false">AVERAGE(E37:E39)</f>
         <v>1.73086666666667</v>
@@ -4362,6 +4716,8 @@
         <f aca="false">AVERAGE(F37:F39)</f>
         <v>0.256622222222224</v>
       </c>
+      <c r="E61" s="0"/>
+      <c r="F61" s="0"/>
       <c r="G61" s="1" t="n">
         <f aca="false">AVERAGE(I37:I39)</f>
         <v>1.68271111111111</v>
@@ -4383,6 +4739,7 @@
       <c r="A62" s="1" t="n">
         <v>55</v>
       </c>
+      <c r="B62" s="0"/>
       <c r="C62" s="1" t="n">
         <f aca="false">AVERAGE(E40:E42)</f>
         <v>0.348955555555558</v>
@@ -4391,6 +4748,8 @@
         <f aca="false">AVERAGE(F40:F42)</f>
         <v>0.189155555555556</v>
       </c>
+      <c r="E62" s="0"/>
+      <c r="F62" s="0"/>
       <c r="G62" s="1" t="n">
         <f aca="false">AVERAGE(I40:I42)</f>
         <v>0.357644444444446</v>
@@ -4412,6 +4771,7 @@
       <c r="A63" s="1" t="n">
         <v>85</v>
       </c>
+      <c r="B63" s="0"/>
       <c r="C63" s="1" t="n">
         <f aca="false">AVERAGE(E43:E45)</f>
         <v>0.951288888888882</v>
@@ -4420,6 +4780,8 @@
         <f aca="false">AVERAGE(F43:F45)</f>
         <v>0.349933333333335</v>
       </c>
+      <c r="E63" s="0"/>
+      <c r="F63" s="0"/>
       <c r="G63" s="1" t="n">
         <f aca="false">AVERAGE(I43:I45)</f>
         <v>0.970933333333325</v>
@@ -4441,6 +4803,7 @@
       <c r="A64" s="1" t="n">
         <v>116</v>
       </c>
+      <c r="B64" s="0"/>
       <c r="C64" s="1" t="n">
         <f aca="false">AVERAGE(E46:E48)</f>
         <v>1.67106666666668</v>
@@ -4449,6 +4812,8 @@
         <f aca="false">AVERAGE(F46:F48)</f>
         <v>4.01815555555555</v>
       </c>
+      <c r="E64" s="0"/>
+      <c r="F64" s="0"/>
       <c r="G64" s="1" t="n">
         <f aca="false">AVERAGE(I46:I48)</f>
         <v>1.45622222222223</v>
@@ -4467,14 +4832,22 @@
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0"/>
+      <c r="B65" s="0"/>
+      <c r="C65" s="0"/>
+      <c r="D65" s="0"/>
       <c r="E65" s="1" t="s">
         <v>44</v>
       </c>
+      <c r="F65" s="0"/>
+      <c r="G65" s="0"/>
+      <c r="H65" s="0"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
         <v>45</v>
       </c>
+      <c r="B66" s="0"/>
       <c r="C66" s="0" t="n">
         <f aca="false">G52/C52</f>
         <v>0.912366876876724</v>
@@ -4487,8 +4860,13 @@
         <f aca="false">ABS(D$71-D66)</f>
         <v>0.173710583171285</v>
       </c>
+      <c r="F66" s="0"/>
+      <c r="G66" s="0"/>
+      <c r="H66" s="0"/>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0"/>
+      <c r="B67" s="0"/>
       <c r="C67" s="0" t="n">
         <f aca="false">G53/C53</f>
         <v>0.965317755060563</v>
@@ -4501,8 +4879,13 @@
         <f aca="false">ABS(D$71-D67)</f>
         <v>0.00563635464201706</v>
       </c>
+      <c r="F67" s="0"/>
+      <c r="G67" s="0"/>
+      <c r="H67" s="0"/>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0"/>
+      <c r="B68" s="0"/>
       <c r="C68" s="0" t="n">
         <f aca="false">G54/C54</f>
         <v>0.972345151811068</v>
@@ -4515,8 +4898,13 @@
         <f aca="false">ABS(D$71-D68)</f>
         <v>0.037534775172141</v>
       </c>
+      <c r="F68" s="0"/>
+      <c r="G68" s="0"/>
+      <c r="H68" s="0"/>
     </row>
     <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0"/>
+      <c r="B69" s="0"/>
       <c r="C69" s="0" t="n">
         <f aca="false">G55/C55</f>
         <v>0.974434631409282</v>
@@ -4529,8 +4917,13 @@
         <f aca="false">ABS(D$71-D69)</f>
         <v>0.0602566326078107</v>
       </c>
+      <c r="F69" s="0"/>
+      <c r="G69" s="0"/>
+      <c r="H69" s="0"/>
     </row>
     <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0"/>
+      <c r="B70" s="0"/>
       <c r="C70" s="0" t="n">
         <f aca="false">G56/C56</f>
         <v>0.970811844420948</v>
@@ -4543,8 +4936,14 @@
         <f aca="false">ABS(D$71-D70)</f>
         <v>0.0702828207493168</v>
       </c>
+      <c r="F70" s="0"/>
+      <c r="G70" s="0"/>
+      <c r="H70" s="0"/>
     </row>
     <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0"/>
+      <c r="B71" s="0"/>
+      <c r="C71" s="0"/>
       <c r="D71" s="1" t="n">
         <f aca="false">AVERAGE(D66:D70)</f>
         <v>0.908813010415697</v>
@@ -4553,8 +4952,13 @@
         <f aca="false">AVERAGE(E66:E70)</f>
         <v>0.0694842332685142</v>
       </c>
+      <c r="F71" s="0"/>
+      <c r="G71" s="0"/>
+      <c r="H71" s="0"/>
     </row>
     <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0"/>
+      <c r="B72" s="0"/>
       <c r="C72" s="1" t="s">
         <v>24</v>
       </c>
@@ -4578,6 +4982,7 @@
       <c r="A73" s="1" t="s">
         <v>26</v>
       </c>
+      <c r="B73" s="0"/>
       <c r="C73" s="1" t="n">
         <f aca="false">SLOPE(C52:C56,$A$52:$A$56)</f>
         <v>3.14283802952001</v>
@@ -4671,15 +5076,15 @@
   </sheetPr>
   <dimension ref="B1:D37"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A16" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C38" activeCellId="0" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="9" width="27.5408163265306"/>
-    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="3" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="9" width="27.2704081632653"/>
+    <col collapsed="false" hidden="false" max="1025" min="5" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5090,4 +5495,2267 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H29"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.1020408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="6.98469387755102"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="13.2397959183673"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="9.90816326530612"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.62755102040816"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.37755102040816"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="10.0459183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="n">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>120.3339</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>12.5933</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <f aca="false">ABS(C$53-C3)</f>
+        <v>120.3339</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <f aca="false">ABS(D$53-D3)</f>
+        <v>12.5933</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>118.7848</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>12.5573</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <f aca="false">ABS(C$53-C4)</f>
+        <v>118.7848</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <f aca="false">ABS(D$53-D4)</f>
+        <v>12.5573</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>115.5851</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>12.532</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <f aca="false">ABS(C$53-C5)</f>
+        <v>115.5851</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <f aca="false">ABS(D$53-D5)</f>
+        <v>12.532</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="n">
+        <v>51</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>342.3194</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>35.7989</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <f aca="false">ABS(C$54-C6)</f>
+        <v>342.3194</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <f aca="false">ABS(D$54-D6)</f>
+        <v>35.7989</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>347.6656</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>35.5587</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <f aca="false">ABS(C$54-C7)</f>
+        <v>347.6656</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <f aca="false">ABS(D$54-D7)</f>
+        <v>35.5587</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>345.9944</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>36.2001</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <f aca="false">ABS(C$54-C8)</f>
+        <v>345.9944</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <f aca="false">ABS(D$54-D8)</f>
+        <v>36.2001</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="n">
+        <v>85</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>546.23</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>59.0627</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <f aca="false">ABS(C$55-C9)</f>
+        <v>546.23</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <f aca="false">ABS(D$55-D9)</f>
+        <v>59.0627</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>547.8033</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>59.3535</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <f aca="false">ABS(C$55-C10)</f>
+        <v>547.8033</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <f aca="false">ABS(D$55-D10)</f>
+        <v>59.3535</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>548.7295</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>58.9449</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <f aca="false">ABS(C$55-C11)</f>
+        <v>548.7295</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <f aca="false">ABS(D$55-D11)</f>
+        <v>58.9449</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="n">
+        <v>129</v>
+      </c>
+      <c r="B12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>868.9906</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>111.4689</v>
+      </c>
+      <c r="E12" s="1" t="n">
+        <f aca="false">ABS(C$56-C12)</f>
+        <v>868.9906</v>
+      </c>
+      <c r="F12" s="1" t="n">
+        <f aca="false">ABS(D$56-D12)</f>
+        <v>111.4689</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="n">
+        <v>129</v>
+      </c>
+      <c r="B13" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>868.381</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>123.6168</v>
+      </c>
+      <c r="E13" s="1" t="n">
+        <f aca="false">ABS(C$56-C13)</f>
+        <v>868.381</v>
+      </c>
+      <c r="F13" s="1" t="n">
+        <f aca="false">ABS(D$56-D13)</f>
+        <v>123.6168</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="n">
+        <v>129</v>
+      </c>
+      <c r="B14" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>875.6493</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>88.7706</v>
+      </c>
+      <c r="E14" s="1" t="n">
+        <f aca="false">ABS(C$56-C14)</f>
+        <v>875.6493</v>
+      </c>
+      <c r="F14" s="1" t="n">
+        <f aca="false">ABS(D$56-D14)</f>
+        <v>88.7706</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="n">
+        <v>173</v>
+      </c>
+      <c r="B15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>1068.876</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>119.2222</v>
+      </c>
+      <c r="E15" s="1" t="n">
+        <f aca="false">ABS(C$57-C15)</f>
+        <v>1068.876</v>
+      </c>
+      <c r="F15" s="1" t="n">
+        <f aca="false">ABS(D$57-D15)</f>
+        <v>119.2222</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="n">
+        <v>173</v>
+      </c>
+      <c r="B16" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>1152.8102</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>129.2446</v>
+      </c>
+      <c r="E16" s="1" t="n">
+        <f aca="false">ABS(C$57-C16)</f>
+        <v>1152.8102</v>
+      </c>
+      <c r="F16" s="1" t="n">
+        <f aca="false">ABS(D$57-D16)</f>
+        <v>129.2446</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="n">
+        <v>173</v>
+      </c>
+      <c r="B17" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>1064.039</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>119.6984</v>
+      </c>
+      <c r="E17" s="1" t="n">
+        <f aca="false">ABS(C$57-C17)</f>
+        <v>1064.039</v>
+      </c>
+      <c r="F17" s="1" t="n">
+        <f aca="false">ABS(D$57-D17)</f>
+        <v>119.6984</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="n">
+        <v>17</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <f aca="false">AVERAGE(C3:C5)</f>
+        <v>118.2346</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <f aca="false">AVERAGE(D3:D5)</f>
+        <v>12.5608666666667</v>
+      </c>
+      <c r="E21" s="1" t="n">
+        <f aca="false">AVERAGE(E3:E5)</f>
+        <v>118.2346</v>
+      </c>
+      <c r="F21" s="1" t="n">
+        <f aca="false">AVERAGE(F3:F5)</f>
+        <v>12.5608666666667</v>
+      </c>
+      <c r="G21" s="1" t="n">
+        <f aca="false">C21/D21</f>
+        <v>9.41293329016575</v>
+      </c>
+      <c r="H21" s="1" t="n">
+        <f aca="false">ABS($G$58-G21)</f>
+        <v>9.41293329016575</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="n">
+        <v>51</v>
+      </c>
+      <c r="C22" s="1" t="n">
+        <f aca="false">AVERAGE(C6:C8)</f>
+        <v>345.326466666667</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <f aca="false">AVERAGE(D6:D8)</f>
+        <v>35.8525666666667</v>
+      </c>
+      <c r="E22" s="1" t="n">
+        <f aca="false">AVERAGE(E6:E8)</f>
+        <v>345.326466666667</v>
+      </c>
+      <c r="F22" s="1" t="n">
+        <f aca="false">AVERAGE(F6:F8)</f>
+        <v>35.8525666666667</v>
+      </c>
+      <c r="G22" s="1" t="n">
+        <f aca="false">C22/D22</f>
+        <v>9.6318478360917</v>
+      </c>
+      <c r="H22" s="1" t="n">
+        <f aca="false">ABS($G$58-G22)</f>
+        <v>9.6318478360917</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="C23" s="1" t="n">
+        <f aca="false">AVERAGE(C9:C11)</f>
+        <v>547.5876</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <f aca="false">AVERAGE(D9:D11)</f>
+        <v>59.1203666666667</v>
+      </c>
+      <c r="E23" s="1" t="n">
+        <f aca="false">AVERAGE(E4:E9)</f>
+        <v>302.763216666667</v>
+      </c>
+      <c r="F23" s="1" t="n">
+        <f aca="false">AVERAGE(F4:F9)</f>
+        <v>31.9516166666667</v>
+      </c>
+      <c r="G23" s="1" t="n">
+        <f aca="false">C23/D23</f>
+        <v>9.26224972668753</v>
+      </c>
+      <c r="H23" s="1" t="n">
+        <f aca="false">ABS($G$58-G23)</f>
+        <v>9.26224972668753</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="n">
+        <v>129</v>
+      </c>
+      <c r="C24" s="1" t="n">
+        <f aca="false">AVERAGE(C12:C14)</f>
+        <v>871.006966666667</v>
+      </c>
+      <c r="D24" s="1" t="n">
+        <f aca="false">AVERAGE(D12:D14)</f>
+        <v>107.9521</v>
+      </c>
+      <c r="E24" s="1" t="n">
+        <f aca="false">AVERAGE(E12:E14)</f>
+        <v>871.006966666667</v>
+      </c>
+      <c r="F24" s="1" t="n">
+        <f aca="false">AVERAGE(F12:F14)</f>
+        <v>107.9521</v>
+      </c>
+      <c r="G24" s="1" t="n">
+        <f aca="false">C24/D24</f>
+        <v>8.06845783145179</v>
+      </c>
+      <c r="H24" s="1" t="n">
+        <f aca="false">ABS($G$58-G24)</f>
+        <v>8.06845783145179</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="n">
+        <v>173</v>
+      </c>
+      <c r="C25" s="1" t="n">
+        <f aca="false">AVERAGE(C15:C17)</f>
+        <v>1095.24173333333</v>
+      </c>
+      <c r="D25" s="1" t="n">
+        <f aca="false">AVERAGE(D15:D17)</f>
+        <v>122.721733333333</v>
+      </c>
+      <c r="E25" s="1" t="n">
+        <f aca="false">AVERAGE(E5:E10)</f>
+        <v>374.2663</v>
+      </c>
+      <c r="F25" s="1" t="n">
+        <f aca="false">AVERAGE(F5:F10)</f>
+        <v>39.7509833333333</v>
+      </c>
+      <c r="G25" s="1" t="n">
+        <f aca="false">C25/D25</f>
+        <v>8.92459471997897</v>
+      </c>
+      <c r="H25" s="1" t="n">
+        <f aca="false">ABS($G$58-G25)</f>
+        <v>8.92459471997897</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1" t="n">
+        <f aca="false">AVERAGE(G21:G25)</f>
+        <v>9.06001668087515</v>
+      </c>
+      <c r="H26" s="1" t="n">
+        <f aca="false">AVERAGE(H21:H25)</f>
+        <v>9.06001668087515</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="1" t="e">
+        <f aca="false">SLOPE(C21:C25,$A$53:$A$57)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D28" s="1" t="e">
+        <f aca="false">SLOPE(D21:D25,$A$53:$A$57)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="7"/>
+      <c r="B29" s="7"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="7" t="e">
+        <f aca="false">C28/D28</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:N43"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D9" activeCellId="0" sqref="D9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="13.4183673469388"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="7.36224489795918"/>
+    <col collapsed="false" hidden="false" max="4" min="3" style="0" width="13.9132653061224"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.8163265306122"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="13.9132653061224"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="13.8163265306122"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="13.9132653061224"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="0" width="9.54591836734694"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="0" width="10.6377551020408"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="0" width="9.25"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="0" width="9.35204081632653"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="0" width="8.95408163265306"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="0" width="10.6377551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="15" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="2"/>
+      <c r="C1" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="L1" s="8"/>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>11.5217</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>9.8314</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <f aca="false">ABS(C$52-C3)</f>
+        <v>11.5217</v>
+      </c>
+      <c r="F3" s="1" t="n">
+        <f aca="false">ABS(D$52-D3)</f>
+        <v>9.8314</v>
+      </c>
+      <c r="G3" s="1" t="n">
+        <v>10.5199</v>
+      </c>
+      <c r="H3" s="1" t="n">
+        <v>7.2581</v>
+      </c>
+      <c r="I3" s="1" t="n">
+        <f aca="false">ABS(G$52-G3)</f>
+        <v>10.5199</v>
+      </c>
+      <c r="J3" s="1" t="n">
+        <f aca="false">ABS(H$52-H3)</f>
+        <v>7.2581</v>
+      </c>
+      <c r="K3" s="1" t="n">
+        <f aca="false">C3-G3</f>
+        <v>1.0018</v>
+      </c>
+      <c r="L3" s="1" t="n">
+        <f aca="false">D3-H3</f>
+        <v>2.5733</v>
+      </c>
+      <c r="M3" s="1" t="n">
+        <f aca="false">ABS(K$52-K3)</f>
+        <v>1.0018</v>
+      </c>
+      <c r="N3" s="1" t="n">
+        <f aca="false">ABS(L$52-L3)</f>
+        <v>2.5733</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>14.4238</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>9.659</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <f aca="false">ABS(C$52-C4)</f>
+        <v>14.4238</v>
+      </c>
+      <c r="F4" s="1" t="n">
+        <f aca="false">ABS(D$52-D4)</f>
+        <v>9.659</v>
+      </c>
+      <c r="G4" s="1" t="n">
+        <v>13.1362</v>
+      </c>
+      <c r="H4" s="1" t="n">
+        <v>7.0731</v>
+      </c>
+      <c r="I4" s="1" t="n">
+        <f aca="false">ABS(G$52-G4)</f>
+        <v>13.1362</v>
+      </c>
+      <c r="J4" s="1" t="n">
+        <f aca="false">ABS(H$52-H4)</f>
+        <v>7.0731</v>
+      </c>
+      <c r="K4" s="1" t="n">
+        <f aca="false">C4-G4</f>
+        <v>1.2876</v>
+      </c>
+      <c r="L4" s="1" t="n">
+        <f aca="false">D4-H4</f>
+        <v>2.5859</v>
+      </c>
+      <c r="M4" s="1" t="n">
+        <f aca="false">ABS(K$52-K4)</f>
+        <v>1.2876</v>
+      </c>
+      <c r="N4" s="1" t="n">
+        <f aca="false">ABS(L$52-L4)</f>
+        <v>2.5859</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C5" s="1" t="n">
+        <v>13.2851</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>9.662</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <f aca="false">ABS(C$52-C5)</f>
+        <v>13.2851</v>
+      </c>
+      <c r="F5" s="1" t="n">
+        <f aca="false">ABS(D$52-D5)</f>
+        <v>9.662</v>
+      </c>
+      <c r="G5" s="1" t="n">
+        <v>12.1366</v>
+      </c>
+      <c r="H5" s="1" t="n">
+        <v>7.0988</v>
+      </c>
+      <c r="I5" s="1" t="n">
+        <f aca="false">ABS(G$52-G5)</f>
+        <v>12.1366</v>
+      </c>
+      <c r="J5" s="1" t="n">
+        <f aca="false">ABS(H$52-H5)</f>
+        <v>7.0988</v>
+      </c>
+      <c r="K5" s="1" t="n">
+        <f aca="false">C5-G5</f>
+        <v>1.1485</v>
+      </c>
+      <c r="L5" s="1" t="n">
+        <f aca="false">D5-H5</f>
+        <v>2.5632</v>
+      </c>
+      <c r="M5" s="1" t="n">
+        <f aca="false">ABS(K$52-K5)</f>
+        <v>1.1485</v>
+      </c>
+      <c r="N5" s="1" t="n">
+        <f aca="false">ABS(L$52-L5)</f>
+        <v>2.5632</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="n">
+        <v>35</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>53.1111</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>34.3539</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <f aca="false">ABS(C$53-C6)</f>
+        <v>53.1111</v>
+      </c>
+      <c r="F6" s="1" t="n">
+        <f aca="false">ABS(D$53-D6)</f>
+        <v>34.3539</v>
+      </c>
+      <c r="G6" s="1" t="n">
+        <v>51.2869</v>
+      </c>
+      <c r="H6" s="1" t="n">
+        <v>31.4538</v>
+      </c>
+      <c r="I6" s="1" t="n">
+        <f aca="false">ABS(G$53-G6)</f>
+        <v>51.2869</v>
+      </c>
+      <c r="J6" s="1" t="n">
+        <f aca="false">ABS(H$53-H6)</f>
+        <v>31.4538</v>
+      </c>
+      <c r="K6" s="1" t="n">
+        <f aca="false">C6-G6</f>
+        <v>1.8242</v>
+      </c>
+      <c r="L6" s="1" t="n">
+        <f aca="false">D6-H6</f>
+        <v>2.9001</v>
+      </c>
+      <c r="M6" s="1" t="n">
+        <f aca="false">ABS(K$53-K6)</f>
+        <v>1.8242</v>
+      </c>
+      <c r="N6" s="1" t="n">
+        <f aca="false">ABS(L$53-L6)</f>
+        <v>2.9001</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B7" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>49.4526</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>33.8754</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <f aca="false">ABS(C$53-C7)</f>
+        <v>49.4526</v>
+      </c>
+      <c r="F7" s="1" t="n">
+        <f aca="false">ABS(D$53-D7)</f>
+        <v>33.8754</v>
+      </c>
+      <c r="G7" s="1" t="n">
+        <v>47.7151</v>
+      </c>
+      <c r="H7" s="1" t="n">
+        <v>30.9728</v>
+      </c>
+      <c r="I7" s="1" t="n">
+        <f aca="false">ABS(G$53-G7)</f>
+        <v>47.7151</v>
+      </c>
+      <c r="J7" s="1" t="n">
+        <f aca="false">ABS(H$53-H7)</f>
+        <v>30.9728</v>
+      </c>
+      <c r="K7" s="1" t="n">
+        <f aca="false">C7-G7</f>
+        <v>1.7375</v>
+      </c>
+      <c r="L7" s="1" t="n">
+        <f aca="false">D7-H7</f>
+        <v>2.9026</v>
+      </c>
+      <c r="M7" s="1" t="n">
+        <f aca="false">ABS(K$53-K7)</f>
+        <v>1.7375</v>
+      </c>
+      <c r="N7" s="1" t="n">
+        <f aca="false">ABS(L$53-L7)</f>
+        <v>2.9026</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>48.9807</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>33.6776</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <f aca="false">ABS(C$53-C8)</f>
+        <v>48.9807</v>
+      </c>
+      <c r="F8" s="1" t="n">
+        <f aca="false">ABS(D$53-D8)</f>
+        <v>33.6776</v>
+      </c>
+      <c r="G8" s="1" t="n">
+        <v>47.2865</v>
+      </c>
+      <c r="H8" s="1" t="n">
+        <v>30.7621</v>
+      </c>
+      <c r="I8" s="1" t="n">
+        <f aca="false">ABS(G$53-G8)</f>
+        <v>47.2865</v>
+      </c>
+      <c r="J8" s="1" t="n">
+        <f aca="false">ABS(H$53-H8)</f>
+        <v>30.7621</v>
+      </c>
+      <c r="K8" s="1" t="n">
+        <f aca="false">C8-G8</f>
+        <v>1.6942</v>
+      </c>
+      <c r="L8" s="1" t="n">
+        <f aca="false">D8-H8</f>
+        <v>2.9155</v>
+      </c>
+      <c r="M8" s="1" t="n">
+        <f aca="false">ABS(K$53-K8)</f>
+        <v>1.6942</v>
+      </c>
+      <c r="N8" s="1" t="n">
+        <f aca="false">ABS(L$53-L8)</f>
+        <v>2.9155</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="2" t="n">
+        <v>55</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C9" s="1" t="n">
+        <v>88.6947</v>
+      </c>
+      <c r="D9" s="1" t="n">
+        <v>58.6917</v>
+      </c>
+      <c r="E9" s="1" t="n">
+        <f aca="false">ABS(C$54-C9)</f>
+        <v>88.6947</v>
+      </c>
+      <c r="F9" s="1" t="n">
+        <f aca="false">ABS(D$54-D9)</f>
+        <v>58.6917</v>
+      </c>
+      <c r="G9" s="1" t="n">
+        <v>86.2185</v>
+      </c>
+      <c r="H9" s="1" t="n">
+        <v>55.5258</v>
+      </c>
+      <c r="I9" s="1" t="n">
+        <f aca="false">ABS(G$54-G9)</f>
+        <v>86.2185</v>
+      </c>
+      <c r="J9" s="1" t="n">
+        <f aca="false">ABS(H$54-H9)</f>
+        <v>55.5258</v>
+      </c>
+      <c r="K9" s="1" t="n">
+        <f aca="false">C9-G9</f>
+        <v>2.47619999999999</v>
+      </c>
+      <c r="L9" s="1" t="n">
+        <f aca="false">D9-H9</f>
+        <v>3.1659</v>
+      </c>
+      <c r="M9" s="1" t="n">
+        <f aca="false">ABS(K$54-K9)</f>
+        <v>2.47619999999999</v>
+      </c>
+      <c r="N9" s="1" t="n">
+        <f aca="false">ABS(L$54-L9)</f>
+        <v>3.1659</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C10" s="1" t="n">
+        <v>89.4783</v>
+      </c>
+      <c r="D10" s="1" t="n">
+        <v>59.258</v>
+      </c>
+      <c r="E10" s="1" t="n">
+        <f aca="false">ABS(C$54-C10)</f>
+        <v>89.4783</v>
+      </c>
+      <c r="F10" s="1" t="n">
+        <f aca="false">ABS(D$54-D10)</f>
+        <v>59.258</v>
+      </c>
+      <c r="G10" s="1" t="n">
+        <v>87.0313</v>
+      </c>
+      <c r="H10" s="1" t="n">
+        <v>56.0749</v>
+      </c>
+      <c r="I10" s="1" t="n">
+        <f aca="false">ABS(G$54-G10)</f>
+        <v>87.0313</v>
+      </c>
+      <c r="J10" s="1" t="n">
+        <f aca="false">ABS(H$54-H10)</f>
+        <v>56.0749</v>
+      </c>
+      <c r="K10" s="1" t="n">
+        <f aca="false">C10-G10</f>
+        <v>2.447</v>
+      </c>
+      <c r="L10" s="1" t="n">
+        <f aca="false">D10-H10</f>
+        <v>3.1831</v>
+      </c>
+      <c r="M10" s="1" t="n">
+        <f aca="false">ABS(K$54-K10)</f>
+        <v>2.447</v>
+      </c>
+      <c r="N10" s="1" t="n">
+        <f aca="false">ABS(L$54-L10)</f>
+        <v>3.1831</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C11" s="1" t="n">
+        <v>88.6916</v>
+      </c>
+      <c r="D11" s="1" t="n">
+        <v>58.9731</v>
+      </c>
+      <c r="E11" s="1" t="n">
+        <f aca="false">ABS(C$54-C11)</f>
+        <v>88.6916</v>
+      </c>
+      <c r="F11" s="1" t="n">
+        <f aca="false">ABS(D$54-D11)</f>
+        <v>58.9731</v>
+      </c>
+      <c r="G11" s="1" t="n">
+        <v>86.2347</v>
+      </c>
+      <c r="H11" s="1" t="n">
+        <v>55.8298</v>
+      </c>
+      <c r="I11" s="1" t="n">
+        <f aca="false">ABS(G$54-G11)</f>
+        <v>86.2347</v>
+      </c>
+      <c r="J11" s="1" t="n">
+        <f aca="false">ABS(H$54-H11)</f>
+        <v>55.8298</v>
+      </c>
+      <c r="K11" s="1" t="n">
+        <f aca="false">C11-G11</f>
+        <v>2.45689999999999</v>
+      </c>
+      <c r="L11" s="1" t="n">
+        <f aca="false">D11-H11</f>
+        <v>3.1433</v>
+      </c>
+      <c r="M11" s="1" t="n">
+        <f aca="false">ABS(K$54-K11)</f>
+        <v>2.45689999999999</v>
+      </c>
+      <c r="N11" s="1" t="n">
+        <f aca="false">ABS(L$54-L11)</f>
+        <v>3.1433</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="2" t="n">
+        <v>85</v>
+      </c>
+      <c r="B12" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>184.4679</v>
+      </c>
+      <c r="D12" s="1" t="n">
+        <v>119.2639</v>
+      </c>
+      <c r="E12" s="1" t="n">
+        <f aca="false">ABS(C$55-C12)</f>
+        <v>184.4679</v>
+      </c>
+      <c r="F12" s="1" t="n">
+        <f aca="false">ABS(D$55-D12)</f>
+        <v>119.2639</v>
+      </c>
+      <c r="G12" s="1" t="n">
+        <v>179.7512</v>
+      </c>
+      <c r="H12" s="1" t="n">
+        <v>115.5621</v>
+      </c>
+      <c r="I12" s="1" t="n">
+        <f aca="false">ABS(G$55-G12)</f>
+        <v>179.7512</v>
+      </c>
+      <c r="J12" s="1" t="n">
+        <f aca="false">ABS(H$55-H12)</f>
+        <v>115.5621</v>
+      </c>
+      <c r="K12" s="1" t="n">
+        <f aca="false">C12-G12</f>
+        <v>4.71669999999997</v>
+      </c>
+      <c r="L12" s="1" t="n">
+        <f aca="false">D12-H12</f>
+        <v>3.70180000000001</v>
+      </c>
+      <c r="M12" s="1" t="n">
+        <f aca="false">ABS(K$55-K12)</f>
+        <v>4.71669999999997</v>
+      </c>
+      <c r="N12" s="1" t="n">
+        <f aca="false">ABS(L$55-L12)</f>
+        <v>3.70180000000001</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="B13" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C13" s="1" t="n">
+        <v>184.7837</v>
+      </c>
+      <c r="D13" s="1" t="n">
+        <v>120.0267</v>
+      </c>
+      <c r="E13" s="1" t="n">
+        <f aca="false">ABS(C$55-C13)</f>
+        <v>184.7837</v>
+      </c>
+      <c r="F13" s="1" t="n">
+        <f aca="false">ABS(D$55-D13)</f>
+        <v>120.0267</v>
+      </c>
+      <c r="G13" s="1" t="n">
+        <v>179.9944</v>
+      </c>
+      <c r="H13" s="1" t="n">
+        <v>116.3367</v>
+      </c>
+      <c r="I13" s="1" t="n">
+        <f aca="false">ABS(G$55-G13)</f>
+        <v>179.9944</v>
+      </c>
+      <c r="J13" s="1" t="n">
+        <f aca="false">ABS(H$55-H13)</f>
+        <v>116.3367</v>
+      </c>
+      <c r="K13" s="1" t="n">
+        <f aca="false">C13-G13</f>
+        <v>4.7893</v>
+      </c>
+      <c r="L13" s="1" t="n">
+        <f aca="false">D13-H13</f>
+        <v>3.69000000000001</v>
+      </c>
+      <c r="M13" s="1" t="n">
+        <f aca="false">ABS(K$55-K13)</f>
+        <v>4.7893</v>
+      </c>
+      <c r="N13" s="1" t="n">
+        <f aca="false">ABS(L$55-L13)</f>
+        <v>3.69000000000001</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="B14" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C14" s="1" t="n">
+        <v>186.7662</v>
+      </c>
+      <c r="D14" s="1" t="n">
+        <v>119.2148</v>
+      </c>
+      <c r="E14" s="1" t="n">
+        <f aca="false">ABS(C$55-C14)</f>
+        <v>186.7662</v>
+      </c>
+      <c r="F14" s="1" t="n">
+        <f aca="false">ABS(D$55-D14)</f>
+        <v>119.2148</v>
+      </c>
+      <c r="G14" s="1" t="n">
+        <v>182.0574</v>
+      </c>
+      <c r="H14" s="1" t="n">
+        <v>115.5179</v>
+      </c>
+      <c r="I14" s="1" t="n">
+        <f aca="false">ABS(G$55-G14)</f>
+        <v>182.0574</v>
+      </c>
+      <c r="J14" s="1" t="n">
+        <f aca="false">ABS(H$55-H14)</f>
+        <v>115.5179</v>
+      </c>
+      <c r="K14" s="1" t="n">
+        <f aca="false">C14-G14</f>
+        <v>4.7088</v>
+      </c>
+      <c r="L14" s="1" t="n">
+        <f aca="false">D14-H14</f>
+        <v>3.6969</v>
+      </c>
+      <c r="M14" s="1" t="n">
+        <f aca="false">ABS(K$55-K14)</f>
+        <v>4.7088</v>
+      </c>
+      <c r="N14" s="1" t="n">
+        <f aca="false">ABS(L$55-L14)</f>
+        <v>3.6969</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="n">
+        <v>116</v>
+      </c>
+      <c r="B15" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C15" s="1" t="n">
+        <v>348.4523</v>
+      </c>
+      <c r="D15" s="1" t="n">
+        <v>193.787</v>
+      </c>
+      <c r="E15" s="1" t="n">
+        <f aca="false">ABS(C$56-C15)</f>
+        <v>348.4523</v>
+      </c>
+      <c r="F15" s="1" t="n">
+        <f aca="false">ABS(D$56-D15)</f>
+        <v>193.787</v>
+      </c>
+      <c r="G15" s="1" t="n">
+        <v>337.951</v>
+      </c>
+      <c r="H15" s="1" t="n">
+        <v>189.6535</v>
+      </c>
+      <c r="I15" s="1" t="n">
+        <f aca="false">ABS(G$56-G15)</f>
+        <v>337.951</v>
+      </c>
+      <c r="J15" s="1" t="n">
+        <f aca="false">ABS(H$56-H15)</f>
+        <v>189.6535</v>
+      </c>
+      <c r="K15" s="1" t="n">
+        <f aca="false">C15-G15</f>
+        <v>10.5013</v>
+      </c>
+      <c r="L15" s="1" t="n">
+        <f aca="false">D15-H15</f>
+        <v>4.1335</v>
+      </c>
+      <c r="M15" s="1" t="n">
+        <f aca="false">ABS(K$56-K15)</f>
+        <v>10.5013</v>
+      </c>
+      <c r="N15" s="1" t="n">
+        <f aca="false">ABS(L$56-L15)</f>
+        <v>4.1335</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="n">
+        <v>116</v>
+      </c>
+      <c r="B16" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="C16" s="1" t="n">
+        <v>346.7371</v>
+      </c>
+      <c r="D16" s="1" t="n">
+        <v>203.8251</v>
+      </c>
+      <c r="E16" s="1" t="n">
+        <f aca="false">ABS(C$56-C16)</f>
+        <v>346.7371</v>
+      </c>
+      <c r="F16" s="1" t="n">
+        <f aca="false">ABS(D$56-D16)</f>
+        <v>203.8251</v>
+      </c>
+      <c r="G16" s="1" t="n">
+        <v>336.698</v>
+      </c>
+      <c r="H16" s="1" t="n">
+        <v>199.6895</v>
+      </c>
+      <c r="I16" s="1" t="n">
+        <f aca="false">ABS(G$56-G16)</f>
+        <v>336.698</v>
+      </c>
+      <c r="J16" s="1" t="n">
+        <f aca="false">ABS(H$56-H16)</f>
+        <v>199.6895</v>
+      </c>
+      <c r="K16" s="1" t="n">
+        <f aca="false">C16-G16</f>
+        <v>10.0391</v>
+      </c>
+      <c r="L16" s="1" t="n">
+        <f aca="false">D16-H16</f>
+        <v>4.13559999999998</v>
+      </c>
+      <c r="M16" s="1" t="n">
+        <f aca="false">ABS(K$56-K16)</f>
+        <v>10.0391</v>
+      </c>
+      <c r="N16" s="1" t="n">
+        <f aca="false">ABS(L$56-L16)</f>
+        <v>4.13559999999998</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="n">
+        <v>116</v>
+      </c>
+      <c r="B17" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>343.8348</v>
+      </c>
+      <c r="D17" s="1" t="n">
+        <v>195.7815</v>
+      </c>
+      <c r="E17" s="1" t="n">
+        <f aca="false">ABS(C$56-C17)</f>
+        <v>343.8348</v>
+      </c>
+      <c r="F17" s="1" t="n">
+        <f aca="false">ABS(D$56-D17)</f>
+        <v>195.7815</v>
+      </c>
+      <c r="G17" s="1" t="n">
+        <v>334.048</v>
+      </c>
+      <c r="H17" s="1" t="n">
+        <v>191.6462</v>
+      </c>
+      <c r="I17" s="1" t="n">
+        <f aca="false">ABS(G$56-G17)</f>
+        <v>334.048</v>
+      </c>
+      <c r="J17" s="1" t="n">
+        <f aca="false">ABS(H$56-H17)</f>
+        <v>191.6462</v>
+      </c>
+      <c r="K17" s="1" t="n">
+        <f aca="false">C17-G17</f>
+        <v>9.78679999999997</v>
+      </c>
+      <c r="L17" s="1" t="n">
+        <f aca="false">D17-H17</f>
+        <v>4.1353</v>
+      </c>
+      <c r="M17" s="1" t="n">
+        <f aca="false">ABS(K$56-K17)</f>
+        <v>9.78679999999997</v>
+      </c>
+      <c r="N17" s="1" t="n">
+        <f aca="false">ABS(L$56-L17)</f>
+        <v>4.1353</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="N20" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="C21" s="1" t="n">
+        <f aca="false">AVERAGE(C3:C5)</f>
+        <v>13.0768666666667</v>
+      </c>
+      <c r="D21" s="1" t="n">
+        <f aca="false">AVERAGE(D3:D5)</f>
+        <v>9.71746666666667</v>
+      </c>
+      <c r="E21" s="1" t="n">
+        <f aca="false">C21/D21</f>
+        <v>1.34570738601282</v>
+      </c>
+      <c r="F21" s="1" t="n">
+        <f aca="false">ABS(E$57-E21)</f>
+        <v>1.34570738601282</v>
+      </c>
+      <c r="G21" s="1" t="n">
+        <f aca="false">AVERAGE(G3:G5)</f>
+        <v>11.9309</v>
+      </c>
+      <c r="H21" s="1" t="n">
+        <f aca="false">AVERAGE(H3:H5)</f>
+        <v>7.14333333333333</v>
+      </c>
+      <c r="I21" s="1" t="n">
+        <f aca="false">G21/H21</f>
+        <v>1.67021465235651</v>
+      </c>
+      <c r="J21" s="1" t="n">
+        <f aca="false">ABS(I$57-I21)</f>
+        <v>1.67021465235651</v>
+      </c>
+      <c r="K21" s="1" t="n">
+        <f aca="false">AVERAGE(K3:K5)</f>
+        <v>1.14596666666667</v>
+      </c>
+      <c r="L21" s="1" t="n">
+        <f aca="false">AVERAGE(L3:L5)</f>
+        <v>2.57413333333333</v>
+      </c>
+      <c r="M21" s="1" t="n">
+        <f aca="false">K21/L21</f>
+        <v>0.445185434579923</v>
+      </c>
+      <c r="N21" s="1" t="n">
+        <f aca="false">ABS(M$57-M21)</f>
+        <v>0.445185434579923</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="C22" s="1" t="n">
+        <f aca="false">AVERAGE(C6:C8)</f>
+        <v>50.5148</v>
+      </c>
+      <c r="D22" s="1" t="n">
+        <f aca="false">AVERAGE(D6:D8)</f>
+        <v>33.9689666666667</v>
+      </c>
+      <c r="E22" s="1" t="n">
+        <f aca="false">C22/D22</f>
+        <v>1.48708674289965</v>
+      </c>
+      <c r="F22" s="1" t="n">
+        <f aca="false">ABS(E$57-E22)</f>
+        <v>1.48708674289965</v>
+      </c>
+      <c r="G22" s="1" t="n">
+        <f aca="false">AVERAGE(G6:G8)</f>
+        <v>48.7628333333333</v>
+      </c>
+      <c r="H22" s="1" t="n">
+        <f aca="false">AVERAGE(H6:H8)</f>
+        <v>31.0629</v>
+      </c>
+      <c r="I22" s="1" t="n">
+        <f aca="false">G22/H22</f>
+        <v>1.56980942968407</v>
+      </c>
+      <c r="J22" s="1" t="n">
+        <f aca="false">ABS(I$57-I22)</f>
+        <v>1.56980942968407</v>
+      </c>
+      <c r="K22" s="1" t="n">
+        <f aca="false">AVERAGE(K6:K8)</f>
+        <v>1.75196666666667</v>
+      </c>
+      <c r="L22" s="1" t="n">
+        <f aca="false">AVERAGE(L6:L8)</f>
+        <v>2.90606666666667</v>
+      </c>
+      <c r="M22" s="1" t="n">
+        <f aca="false">K22/L22</f>
+        <v>0.602865270353972</v>
+      </c>
+      <c r="N22" s="1" t="n">
+        <f aca="false">ABS(M$57-M22)</f>
+        <v>0.602865270353972</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="C23" s="1" t="n">
+        <f aca="false">AVERAGE(C9:C11)</f>
+        <v>88.9548666666667</v>
+      </c>
+      <c r="D23" s="1" t="n">
+        <f aca="false">AVERAGE(D9:D11)</f>
+        <v>58.9742666666667</v>
+      </c>
+      <c r="E23" s="1" t="n">
+        <f aca="false">C23/D23</f>
+        <v>1.50836749135781</v>
+      </c>
+      <c r="F23" s="1" t="n">
+        <f aca="false">ABS(E$57-E23)</f>
+        <v>1.50836749135781</v>
+      </c>
+      <c r="G23" s="1" t="n">
+        <f aca="false">AVERAGE(G9:G11)</f>
+        <v>86.4948333333333</v>
+      </c>
+      <c r="H23" s="1" t="n">
+        <f aca="false">AVERAGE(H9:H11)</f>
+        <v>55.8101666666667</v>
+      </c>
+      <c r="I23" s="1" t="n">
+        <f aca="false">G23/H23</f>
+        <v>1.54980424713538</v>
+      </c>
+      <c r="J23" s="1" t="n">
+        <f aca="false">ABS(I$57-I23)</f>
+        <v>1.54980424713538</v>
+      </c>
+      <c r="K23" s="1" t="n">
+        <f aca="false">AVERAGE(K9:K11)</f>
+        <v>2.46003333333333</v>
+      </c>
+      <c r="L23" s="1" t="n">
+        <f aca="false">AVERAGE(L9:L11)</f>
+        <v>3.1641</v>
+      </c>
+      <c r="M23" s="1" t="n">
+        <f aca="false">K23/L23</f>
+        <v>0.777482801849918</v>
+      </c>
+      <c r="N23" s="1" t="n">
+        <f aca="false">ABS(M$57-M23)</f>
+        <v>0.777482801849918</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="C24" s="1" t="n">
+        <f aca="false">AVERAGE(C12:C14)</f>
+        <v>185.339266666667</v>
+      </c>
+      <c r="D24" s="1" t="n">
+        <f aca="false">AVERAGE(D12:D14)</f>
+        <v>119.5018</v>
+      </c>
+      <c r="E24" s="1" t="n">
+        <f aca="false">C24/D24</f>
+        <v>1.55093284508406</v>
+      </c>
+      <c r="F24" s="1" t="n">
+        <f aca="false">ABS(E$57-E24)</f>
+        <v>1.55093284508406</v>
+      </c>
+      <c r="G24" s="1" t="n">
+        <f aca="false">AVERAGE(G12:G14)</f>
+        <v>180.601</v>
+      </c>
+      <c r="H24" s="1" t="n">
+        <f aca="false">AVERAGE(H12:H14)</f>
+        <v>115.805566666667</v>
+      </c>
+      <c r="I24" s="1" t="n">
+        <f aca="false">G24/H24</f>
+        <v>1.55951915955681</v>
+      </c>
+      <c r="J24" s="1" t="n">
+        <f aca="false">ABS(I$57-I24)</f>
+        <v>1.55951915955681</v>
+      </c>
+      <c r="K24" s="1" t="n">
+        <f aca="false">AVERAGE(K12:K14)</f>
+        <v>4.73826666666666</v>
+      </c>
+      <c r="L24" s="1" t="n">
+        <f aca="false">AVERAGE(L12:L14)</f>
+        <v>3.69623333333334</v>
+      </c>
+      <c r="M24" s="1" t="n">
+        <f aca="false">K24/L24</f>
+        <v>1.28191762785538</v>
+      </c>
+      <c r="N24" s="1" t="n">
+        <f aca="false">ABS(M$57-M24)</f>
+        <v>1.28191762785538</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1" t="n">
+        <v>116</v>
+      </c>
+      <c r="C25" s="1" t="n">
+        <f aca="false">AVERAGE(C15:C17)</f>
+        <v>346.3414</v>
+      </c>
+      <c r="D25" s="1" t="n">
+        <f aca="false">AVERAGE(D15:D17)</f>
+        <v>197.797866666667</v>
+      </c>
+      <c r="E25" s="1" t="n">
+        <f aca="false">C25/D25</f>
+        <v>1.75098652900874</v>
+      </c>
+      <c r="F25" s="1" t="n">
+        <f aca="false">ABS(E$57-E25)</f>
+        <v>1.75098652900874</v>
+      </c>
+      <c r="G25" s="1" t="n">
+        <f aca="false">AVERAGE(G15:G17)</f>
+        <v>336.232333333333</v>
+      </c>
+      <c r="H25" s="1" t="n">
+        <f aca="false">AVERAGE(H15:H17)</f>
+        <v>193.663066666667</v>
+      </c>
+      <c r="I25" s="1" t="n">
+        <f aca="false">G25/H25</f>
+        <v>1.73617168787303</v>
+      </c>
+      <c r="J25" s="1" t="n">
+        <f aca="false">ABS(I$57-I25)</f>
+        <v>1.73617168787303</v>
+      </c>
+      <c r="K25" s="1" t="n">
+        <f aca="false">AVERAGE(K15:K17)</f>
+        <v>10.1090666666666</v>
+      </c>
+      <c r="L25" s="1" t="n">
+        <f aca="false">AVERAGE(L15:L17)</f>
+        <v>4.13479999999999</v>
+      </c>
+      <c r="M25" s="1" t="n">
+        <f aca="false">K25/L25</f>
+        <v>2.44487439940666</v>
+      </c>
+      <c r="N25" s="1" t="n">
+        <f aca="false">ABS(M$57-M25)</f>
+        <v>2.44487439940666</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E26" s="1" t="n">
+        <f aca="false">AVERAGE(E21:E25)</f>
+        <v>1.52861619887262</v>
+      </c>
+      <c r="F26" s="1" t="n">
+        <f aca="false">AVERAGE(F21:F25)</f>
+        <v>1.52861619887262</v>
+      </c>
+      <c r="I26" s="1" t="n">
+        <f aca="false">AVERAGE(I21:I25)</f>
+        <v>1.61710383532116</v>
+      </c>
+      <c r="J26" s="1" t="n">
+        <f aca="false">AVERAGE(J21:J25)</f>
+        <v>1.61710383532116</v>
+      </c>
+      <c r="M26" s="1" t="n">
+        <f aca="false">AVERAGE(M21:M25)</f>
+        <v>1.11046510680917</v>
+      </c>
+      <c r="N26" s="1" t="n">
+        <f aca="false">AVERAGE(N21:N25)</f>
+        <v>1.11046510680917</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H28" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="L28" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="n">
+        <v>11</v>
+      </c>
+      <c r="C29" s="1" t="n">
+        <f aca="false">AVERAGE(E3:E5)</f>
+        <v>13.0768666666667</v>
+      </c>
+      <c r="D29" s="1" t="n">
+        <f aca="false">AVERAGE(F3:F5)</f>
+        <v>9.71746666666667</v>
+      </c>
+      <c r="G29" s="1" t="n">
+        <f aca="false">AVERAGE(I3:I5)</f>
+        <v>11.9309</v>
+      </c>
+      <c r="H29" s="1" t="n">
+        <f aca="false">AVERAGE(J3:J5)</f>
+        <v>7.14333333333333</v>
+      </c>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1" t="n">
+        <f aca="false">AVERAGE(M3:M5)</f>
+        <v>1.14596666666667</v>
+      </c>
+      <c r="L29" s="1" t="n">
+        <f aca="false">AVERAGE(N3:N5)</f>
+        <v>2.57413333333333</v>
+      </c>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1" t="n">
+        <v>35</v>
+      </c>
+      <c r="C30" s="1" t="n">
+        <f aca="false">AVERAGE(E6:E8)</f>
+        <v>50.5148</v>
+      </c>
+      <c r="D30" s="1" t="n">
+        <f aca="false">AVERAGE(F6:F8)</f>
+        <v>33.9689666666667</v>
+      </c>
+      <c r="G30" s="1" t="n">
+        <f aca="false">AVERAGE(I6:I8)</f>
+        <v>48.7628333333333</v>
+      </c>
+      <c r="H30" s="1" t="n">
+        <f aca="false">AVERAGE(J6:J8)</f>
+        <v>31.0629</v>
+      </c>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1" t="n">
+        <f aca="false">AVERAGE(M6:M8)</f>
+        <v>1.75196666666667</v>
+      </c>
+      <c r="L30" s="1" t="n">
+        <f aca="false">AVERAGE(N6:N8)</f>
+        <v>2.90606666666667</v>
+      </c>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="n">
+        <v>55</v>
+      </c>
+      <c r="C31" s="1" t="n">
+        <f aca="false">AVERAGE(E9:E11)</f>
+        <v>88.9548666666667</v>
+      </c>
+      <c r="D31" s="1" t="n">
+        <f aca="false">AVERAGE(F9:F11)</f>
+        <v>58.9742666666667</v>
+      </c>
+      <c r="G31" s="1" t="n">
+        <f aca="false">AVERAGE(I9:I11)</f>
+        <v>86.4948333333333</v>
+      </c>
+      <c r="H31" s="1" t="n">
+        <f aca="false">AVERAGE(J9:J11)</f>
+        <v>55.8101666666667</v>
+      </c>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1" t="n">
+        <f aca="false">AVERAGE(M9:M11)</f>
+        <v>2.46003333333333</v>
+      </c>
+      <c r="L31" s="1" t="n">
+        <f aca="false">AVERAGE(N9:N11)</f>
+        <v>3.1641</v>
+      </c>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="n">
+        <v>85</v>
+      </c>
+      <c r="C32" s="1" t="n">
+        <f aca="false">AVERAGE(E12:E14)</f>
+        <v>185.339266666667</v>
+      </c>
+      <c r="D32" s="1" t="n">
+        <f aca="false">AVERAGE(F12:F14)</f>
+        <v>119.5018</v>
+      </c>
+      <c r="G32" s="1" t="n">
+        <f aca="false">AVERAGE(I12:I14)</f>
+        <v>180.601</v>
+      </c>
+      <c r="H32" s="1" t="n">
+        <f aca="false">AVERAGE(J12:J14)</f>
+        <v>115.805566666667</v>
+      </c>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1" t="n">
+        <f aca="false">AVERAGE(M12:M14)</f>
+        <v>4.73826666666666</v>
+      </c>
+      <c r="L32" s="1" t="n">
+        <f aca="false">AVERAGE(N12:N14)</f>
+        <v>3.69623333333334</v>
+      </c>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="n">
+        <v>116</v>
+      </c>
+      <c r="C33" s="1" t="n">
+        <f aca="false">AVERAGE(E15:E17)</f>
+        <v>346.3414</v>
+      </c>
+      <c r="D33" s="1" t="n">
+        <f aca="false">AVERAGE(F15:F17)</f>
+        <v>197.797866666667</v>
+      </c>
+      <c r="G33" s="1" t="n">
+        <f aca="false">AVERAGE(I15:I17)</f>
+        <v>336.232333333333</v>
+      </c>
+      <c r="H33" s="1" t="n">
+        <f aca="false">AVERAGE(J15:J17)</f>
+        <v>193.663066666667</v>
+      </c>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1" t="n">
+        <f aca="false">AVERAGE(M15:M17)</f>
+        <v>10.1090666666666</v>
+      </c>
+      <c r="L33" s="1" t="n">
+        <f aca="false">AVERAGE(N15:N17)</f>
+        <v>4.13479999999999</v>
+      </c>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E34" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <f aca="false">G21/C21</f>
+        <v>0.912366876876724</v>
+      </c>
+      <c r="D35" s="1" t="n">
+        <f aca="false">H21/D21</f>
+        <v>0.735102427244412</v>
+      </c>
+      <c r="E35" s="1" t="n">
+        <f aca="false">ABS(D$71-D35)</f>
+        <v>0.735102427244412</v>
+      </c>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C36" s="0" t="n">
+        <f aca="false">G22/C22</f>
+        <v>0.965317755060563</v>
+      </c>
+      <c r="D36" s="1" t="n">
+        <f aca="false">H22/D22</f>
+        <v>0.914449365057715</v>
+      </c>
+      <c r="E36" s="1" t="n">
+        <f aca="false">ABS(D$71-D36)</f>
+        <v>0.914449365057715</v>
+      </c>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C37" s="0" t="n">
+        <f aca="false">G23/C23</f>
+        <v>0.972345151811068</v>
+      </c>
+      <c r="D37" s="1" t="n">
+        <f aca="false">H23/D23</f>
+        <v>0.946347785587838</v>
+      </c>
+      <c r="E37" s="1" t="n">
+        <f aca="false">ABS(D$71-D37)</f>
+        <v>0.946347785587838</v>
+      </c>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C38" s="0" t="n">
+        <f aca="false">G24/C24</f>
+        <v>0.974434631409282</v>
+      </c>
+      <c r="D38" s="1" t="n">
+        <f aca="false">H24/D24</f>
+        <v>0.969069643023508</v>
+      </c>
+      <c r="E38" s="1" t="n">
+        <f aca="false">ABS(D$71-D38)</f>
+        <v>0.969069643023508</v>
+      </c>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C39" s="0" t="n">
+        <f aca="false">G25/C25</f>
+        <v>0.970811844420948</v>
+      </c>
+      <c r="D39" s="1" t="n">
+        <f aca="false">H25/D25</f>
+        <v>0.979095831165014</v>
+      </c>
+      <c r="E39" s="1" t="n">
+        <f aca="false">ABS(D$71-D39)</f>
+        <v>0.979095831165014</v>
+      </c>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D40" s="1" t="n">
+        <f aca="false">AVERAGE(D35:D39)</f>
+        <v>0.908813010415697</v>
+      </c>
+      <c r="E40" s="1" t="n">
+        <f aca="false">AVERAGE(E35:E39)</f>
+        <v>0.908813010415697</v>
+      </c>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C41" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="F41" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="G41" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H41" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C42" s="1" t="e">
+        <f aca="false">SLOPE(C21:C25,$A$52:$A$56)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="D42" s="1" t="e">
+        <f aca="false">SLOPE(D21:D25,$A$52:$A$56)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E42" s="1" t="e">
+        <f aca="false">SLOPE(G21:G25,$A$52:$A$56)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F42" s="1" t="e">
+        <f aca="false">SLOPE(H21:H25,$A$52:$A$56)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G42" s="1" t="e">
+        <f aca="false">SLOPE(K21:K25,$A$52:$A$56)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="H42" s="1" t="e">
+        <f aca="false">SLOPE(L21:L25,$A$52:$A$56)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+      <c r="L42" s="1"/>
+      <c r="M42" s="1"/>
+      <c r="N42" s="1"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="7" t="e">
+        <f aca="false">C42/D42</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="E43" s="7"/>
+      <c r="F43" s="7" t="e">
+        <f aca="false">E42/F42</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="G43" s="7"/>
+      <c r="H43" s="7" t="e">
+        <f aca="false">G42/H42</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+      <c r="L43" s="1"/>
+      <c r="M43" s="1"/>
+      <c r="N43" s="1"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="K1:L1"/>
+  </mergeCells>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
updated the report with new rand weights results
</commit_message>
<xml_diff>
--- a/stats/stats_compilation.xlsx
+++ b/stats/stats_compilation.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="984" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="weights" sheetId="1" state="visible" r:id="rId2"/>
@@ -146,6 +146,9 @@
     <t xml:space="preserve">-----</t>
   </si>
   <si>
+    <t xml:space="preserve">batch_size (J)</t>
+  </si>
+  <si>
     <t xml:space="preserve">find_rewards</t>
   </si>
   <si>
@@ -192,9 +195,6 @@
   </si>
   <si>
     <t xml:space="preserve">gpu+-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">batch_size (J)</t>
   </si>
   <si>
     <t xml:space="preserve">congpu+-</t>
@@ -502,7 +502,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9924840" cy="9524520"/>
+          <a:ext cx="11337120" cy="9524520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -547,7 +547,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="0"/>
-          <a:ext cx="9924840" cy="9524520"/>
+          <a:ext cx="11337120" cy="9524520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -581,28 +581,29 @@
   </sheetPr>
   <dimension ref="A1:P65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C86" activeCellId="0" sqref="C86"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A78" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D94" activeCellId="0" sqref="D94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="1" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="12.1479591836735"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="7.96428571428571"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="6.88265306122449"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="6.0765306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="17" style="1" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="13.4285714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="7.26020408163265"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="13.6071428571429"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="13.6887755102041"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="13.780612244898"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.1683673469388"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="9.61224489795918"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="7.26020408163265"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.2602040816327"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="13.780612244898"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="13.1683673469388"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="9.61224489795918"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="8.39795918367347"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="7.26020408163265"/>
+    <col collapsed="false" hidden="false" max="1025" min="17" style="1" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2696,7 +2697,7 @@
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="1" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>4</v>
@@ -2727,7 +2728,7 @@
         <v>92.8932</v>
       </c>
       <c r="D65" s="1" t="n">
-        <v>12.5933</v>
+        <v>101.4049</v>
       </c>
       <c r="E65" s="1" t="n">
         <f aca="false">ABS(C$95-C65)</f>
@@ -2735,7 +2736,7 @@
       </c>
       <c r="F65" s="1" t="n">
         <f aca="false">ABS(D$95-D65)</f>
-        <v>0.0324333333333318</v>
+        <v>0.630933333333317</v>
       </c>
       <c r="G65" s="0"/>
       <c r="H65" s="0"/>
@@ -2751,7 +2752,7 @@
         <v>97.2039</v>
       </c>
       <c r="D66" s="1" t="n">
-        <v>12.5573</v>
+        <v>99.6621</v>
       </c>
       <c r="E66" s="1" t="n">
         <f aca="false">ABS(C$95-C66)</f>
@@ -2759,7 +2760,7 @@
       </c>
       <c r="F66" s="1" t="n">
         <f aca="false">ABS(D$95-D66)</f>
-        <v>0.00356666666666783</v>
+        <v>1.11186666666669</v>
       </c>
       <c r="G66" s="0"/>
       <c r="H66" s="0"/>
@@ -2775,7 +2776,7 @@
         <v>95.8503</v>
       </c>
       <c r="D67" s="1" t="n">
-        <v>12.532</v>
+        <v>101.2549</v>
       </c>
       <c r="E67" s="1" t="n">
         <f aca="false">ABS(C$95-C67)</f>
@@ -2783,7 +2784,7 @@
       </c>
       <c r="F67" s="1" t="n">
         <f aca="false">ABS(D$95-D67)</f>
-        <v>0.0288666666666675</v>
+        <v>0.480933333333326</v>
       </c>
       <c r="G67" s="0"/>
       <c r="H67" s="0"/>
@@ -2799,7 +2800,7 @@
         <v>206.2945</v>
       </c>
       <c r="D68" s="1" t="n">
-        <v>35.7989</v>
+        <v>101.0836</v>
       </c>
       <c r="E68" s="1" t="n">
         <f aca="false">ABS(C$96-C68)</f>
@@ -2807,7 +2808,7 @@
       </c>
       <c r="F68" s="1" t="n">
         <f aca="false">ABS(D$96-D68)</f>
-        <v>0.0536666666666648</v>
+        <v>0.00310000000000343</v>
       </c>
       <c r="G68" s="0"/>
       <c r="H68" s="0"/>
@@ -2823,7 +2824,7 @@
         <v>204.6409</v>
       </c>
       <c r="D69" s="1" t="n">
-        <v>35.5587</v>
+        <v>100.5115</v>
       </c>
       <c r="E69" s="1" t="n">
         <f aca="false">ABS(C$96-C69)</f>
@@ -2831,7 +2832,7 @@
       </c>
       <c r="F69" s="1" t="n">
         <f aca="false">ABS(D$96-D69)</f>
-        <v>0.293866666666666</v>
+        <v>0.57520000000001</v>
       </c>
       <c r="G69" s="0"/>
       <c r="H69" s="0"/>
@@ -2847,7 +2848,7 @@
         <v>195.377</v>
       </c>
       <c r="D70" s="1" t="n">
-        <v>36.2001</v>
+        <v>101.665</v>
       </c>
       <c r="E70" s="1" t="n">
         <f aca="false">ABS(C$96-C70)</f>
@@ -2855,7 +2856,7 @@
       </c>
       <c r="F70" s="1" t="n">
         <f aca="false">ABS(D$96-D70)</f>
-        <v>0.347533333333331</v>
+        <v>0.578299999999999</v>
       </c>
       <c r="G70" s="0"/>
       <c r="H70" s="0"/>
@@ -2871,7 +2872,7 @@
         <v>387.2138</v>
       </c>
       <c r="D71" s="1" t="n">
-        <v>59.0627</v>
+        <v>102.5469</v>
       </c>
       <c r="E71" s="1" t="n">
         <f aca="false">ABS(C$97-C71)</f>
@@ -2879,7 +2880,7 @@
       </c>
       <c r="F71" s="1" t="n">
         <f aca="false">ABS(D$97-D71)</f>
-        <v>0.0576666666666625</v>
+        <v>1.00020000000001</v>
       </c>
       <c r="G71" s="0"/>
       <c r="H71" s="0"/>
@@ -2895,7 +2896,7 @@
         <v>393.7993</v>
       </c>
       <c r="D72" s="1" t="n">
-        <v>59.3535</v>
+        <v>101.6901</v>
       </c>
       <c r="E72" s="1" t="n">
         <f aca="false">ABS(C$97-C72)</f>
@@ -2903,7 +2904,7 @@
       </c>
       <c r="F72" s="1" t="n">
         <f aca="false">ABS(D$97-D72)</f>
-        <v>0.233133333333335</v>
+        <v>0.143400000000014</v>
       </c>
       <c r="G72" s="0"/>
       <c r="H72" s="0"/>
@@ -2919,7 +2920,7 @@
         <v>393.3333</v>
       </c>
       <c r="D73" s="1" t="n">
-        <v>58.9449</v>
+        <v>100.4031</v>
       </c>
       <c r="E73" s="1" t="n">
         <f aca="false">ABS(C$97-C73)</f>
@@ -2927,7 +2928,7 @@
       </c>
       <c r="F73" s="1" t="n">
         <f aca="false">ABS(D$97-D73)</f>
-        <v>0.175466666666665</v>
+        <v>1.14359999999999</v>
       </c>
       <c r="G73" s="0"/>
       <c r="H73" s="0"/>
@@ -2943,7 +2944,7 @@
         <v>654.8508</v>
       </c>
       <c r="D74" s="1" t="n">
-        <v>111.4689</v>
+        <v>100.1242</v>
       </c>
       <c r="E74" s="1" t="n">
         <f aca="false">ABS(C$98-C74)</f>
@@ -2951,7 +2952,7 @@
       </c>
       <c r="F74" s="1" t="n">
         <f aca="false">ABS(D$98-D74)</f>
-        <v>3.51679999999999</v>
+        <v>0.500166666666672</v>
       </c>
       <c r="G74" s="0"/>
       <c r="H74" s="0"/>
@@ -2967,7 +2968,7 @@
         <v>653.6809</v>
       </c>
       <c r="D75" s="1" t="n">
-        <v>123.6168</v>
+        <v>100.7061</v>
       </c>
       <c r="E75" s="1" t="n">
         <f aca="false">ABS(C$98-C75)</f>
@@ -2975,7 +2976,7 @@
       </c>
       <c r="F75" s="1" t="n">
         <f aca="false">ABS(D$98-D75)</f>
-        <v>15.6647</v>
+        <v>0.0817333333333323</v>
       </c>
       <c r="G75" s="0"/>
       <c r="H75" s="0"/>
@@ -2991,7 +2992,7 @@
         <v>654.1779</v>
       </c>
       <c r="D76" s="1" t="n">
-        <v>88.7706</v>
+        <v>101.0428</v>
       </c>
       <c r="E76" s="1" t="n">
         <f aca="false">ABS(C$98-C76)</f>
@@ -2999,7 +3000,7 @@
       </c>
       <c r="F76" s="1" t="n">
         <f aca="false">ABS(D$98-D76)</f>
-        <v>19.1815</v>
+        <v>0.418433333333326</v>
       </c>
       <c r="G76" s="0"/>
       <c r="H76" s="0"/>
@@ -3015,7 +3016,7 @@
         <v>1002.5057</v>
       </c>
       <c r="D77" s="1" t="n">
-        <v>119.2222</v>
+        <v>109.6655</v>
       </c>
       <c r="E77" s="1" t="n">
         <f aca="false">ABS(C$99-C77)</f>
@@ -3023,7 +3024,7 @@
       </c>
       <c r="F77" s="1" t="n">
         <f aca="false">ABS(D$99-D77)</f>
-        <v>3.49953333333332</v>
+        <v>0.108033333333339</v>
       </c>
       <c r="G77" s="0"/>
       <c r="H77" s="0"/>
@@ -3039,7 +3040,7 @@
         <v>997.6372</v>
       </c>
       <c r="D78" s="1" t="n">
-        <v>129.2446</v>
+        <v>109.8494</v>
       </c>
       <c r="E78" s="1" t="n">
         <f aca="false">ABS(C$99-C78)</f>
@@ -3047,7 +3048,7 @@
       </c>
       <c r="F78" s="1" t="n">
         <f aca="false">ABS(D$99-D78)</f>
-        <v>6.52286666666667</v>
+        <v>0.0758666666666699</v>
       </c>
       <c r="G78" s="0"/>
       <c r="H78" s="0"/>
@@ -3063,7 +3064,7 @@
         <v>998.45</v>
       </c>
       <c r="D79" s="1" t="n">
-        <v>119.6984</v>
+        <v>109.8057</v>
       </c>
       <c r="E79" s="1" t="n">
         <f aca="false">ABS(C$99-C79)</f>
@@ -3071,7 +3072,7 @@
       </c>
       <c r="F79" s="1" t="n">
         <f aca="false">ABS(D$99-D79)</f>
-        <v>3.02333333333331</v>
+        <v>0.0321666666666687</v>
       </c>
       <c r="G79" s="0"/>
       <c r="H79" s="0"/>
@@ -3087,15 +3088,15 @@
         <v>1256.5199</v>
       </c>
       <c r="D80" s="1" t="n">
-        <v>119.2222</v>
+        <v>137.4039</v>
       </c>
       <c r="E80" s="1" t="n">
         <f aca="false">ABS(C$100-C80)</f>
-        <v>161.278166666667</v>
+        <v>8.2496666666666</v>
       </c>
       <c r="F80" s="1" t="n">
         <f aca="false">ABS(D$100-D80)</f>
-        <v>3.49953333333332</v>
+        <v>0.0539666666666676</v>
       </c>
       <c r="G80" s="0"/>
       <c r="H80" s="0"/>
@@ -3111,15 +3112,15 @@
         <v>1244.6403</v>
       </c>
       <c r="D81" s="1" t="n">
-        <v>129.2446</v>
+        <v>137.2518</v>
       </c>
       <c r="E81" s="1" t="n">
         <f aca="false">ABS(C$100-C81)</f>
-        <v>149.398566666667</v>
+        <v>3.62993333333338</v>
       </c>
       <c r="F81" s="1" t="n">
         <f aca="false">ABS(D$100-D81)</f>
-        <v>6.52286666666667</v>
+        <v>0.0981333333333225</v>
       </c>
       <c r="G81" s="0"/>
       <c r="H81" s="0"/>
@@ -3135,15 +3136,15 @@
         <v>1243.6505</v>
       </c>
       <c r="D82" s="1" t="n">
-        <v>119.6984</v>
+        <v>137.3941</v>
       </c>
       <c r="E82" s="1" t="n">
         <f aca="false">ABS(C$100-C82)</f>
-        <v>148.408766666667</v>
+        <v>4.61973333333344</v>
       </c>
       <c r="F82" s="1" t="n">
         <f aca="false">ABS(D$100-D82)</f>
-        <v>3.02333333333331</v>
+        <v>0.0441666666666833</v>
       </c>
       <c r="G82" s="0"/>
       <c r="H82" s="0"/>
@@ -3159,15 +3160,15 @@
         <v>1750.9063</v>
       </c>
       <c r="D83" s="1" t="n">
-        <v>119.2222</v>
+        <v>169.351</v>
       </c>
       <c r="E83" s="1" t="n">
         <f aca="false">ABS(C$101-C83)</f>
-        <v>230.3737</v>
+        <v>2.29900000000021</v>
       </c>
       <c r="F83" s="1" t="n">
         <f aca="false">ABS(D$101-D83)</f>
-        <v>3.49953333333332</v>
+        <v>0.18216666666666</v>
       </c>
       <c r="G83" s="0"/>
       <c r="H83" s="0"/>
@@ -3183,15 +3184,15 @@
         <v>1746.6525</v>
       </c>
       <c r="D84" s="1" t="n">
-        <v>129.2446</v>
+        <v>169.4748</v>
       </c>
       <c r="E84" s="1" t="n">
         <f aca="false">ABS(C$101-C84)</f>
-        <v>226.1199</v>
+        <v>1.95479999999998</v>
       </c>
       <c r="F84" s="1" t="n">
         <f aca="false">ABS(D$101-D84)</f>
-        <v>6.52286666666667</v>
+        <v>0.0583666666666716</v>
       </c>
       <c r="G84" s="0"/>
       <c r="H84" s="0"/>
@@ -3204,18 +3205,18 @@
         <v>3</v>
       </c>
       <c r="C85" s="1" t="n">
-        <v>1064.039</v>
+        <v>1748.2631</v>
       </c>
       <c r="D85" s="1" t="n">
-        <v>119.6984</v>
+        <v>169.7737</v>
       </c>
       <c r="E85" s="1" t="n">
         <f aca="false">ABS(C$101-C85)</f>
-        <v>456.4936</v>
+        <v>0.344200000000001</v>
       </c>
       <c r="F85" s="1" t="n">
         <f aca="false">ABS(D$101-D85)</f>
-        <v>3.02333333333331</v>
+        <v>0.240533333333332</v>
       </c>
       <c r="G85" s="0"/>
       <c r="H85" s="0"/>
@@ -3231,15 +3232,15 @@
         <v>2278.1319</v>
       </c>
       <c r="D86" s="1" t="n">
-        <v>119.2222</v>
+        <v>224.2459</v>
       </c>
       <c r="E86" s="1" t="n">
         <f aca="false">ABS(C$102-C86)</f>
-        <v>403.546266666667</v>
+        <v>1.76516666666657</v>
       </c>
       <c r="F86" s="1" t="n">
         <f aca="false">ABS(D$102-D86)</f>
-        <v>3.49953333333332</v>
+        <v>0.107600000000019</v>
       </c>
       <c r="G86" s="0"/>
       <c r="H86" s="0"/>
@@ -3255,15 +3256,15 @@
         <v>2281.586</v>
       </c>
       <c r="D87" s="1" t="n">
-        <v>129.2446</v>
+        <v>224.2434</v>
       </c>
       <c r="E87" s="1" t="n">
         <f aca="false">ABS(C$102-C87)</f>
-        <v>407.000366666666</v>
+        <v>1.68893333333335</v>
       </c>
       <c r="F87" s="1" t="n">
         <f aca="false">ABS(D$102-D87)</f>
-        <v>6.52286666666667</v>
+        <v>0.105100000000022</v>
       </c>
       <c r="G87" s="0"/>
       <c r="H87" s="0"/>
@@ -3276,18 +3277,18 @@
         <v>3</v>
       </c>
       <c r="C88" s="1" t="n">
-        <v>1064.039</v>
+        <v>2279.9733</v>
       </c>
       <c r="D88" s="1" t="n">
-        <v>119.6984</v>
+        <v>223.9256</v>
       </c>
       <c r="E88" s="1" t="n">
         <f aca="false">ABS(C$102-C88)</f>
-        <v>810.546633333333</v>
+        <v>0.0762333333336755</v>
       </c>
       <c r="F88" s="1" t="n">
         <f aca="false">ABS(D$102-D88)</f>
-        <v>3.02333333333331</v>
+        <v>0.212699999999984</v>
       </c>
       <c r="G88" s="0"/>
       <c r="H88" s="0"/>
@@ -3303,15 +3304,15 @@
         <v>2832.4094</v>
       </c>
       <c r="D89" s="1" t="n">
-        <v>119.2222</v>
+        <v>269.0916</v>
       </c>
       <c r="E89" s="1" t="n">
         <f aca="false">ABS(C$103-C89)</f>
-        <v>617.2739</v>
+        <v>55.2567333333332</v>
       </c>
       <c r="F89" s="1" t="n">
         <f aca="false">ABS(D$103-D89)</f>
-        <v>3.49953333333332</v>
+        <v>0.110066666666626</v>
       </c>
       <c r="G89" s="0"/>
       <c r="H89" s="0"/>
@@ -3327,15 +3328,15 @@
         <v>2748.9581</v>
       </c>
       <c r="D90" s="1" t="n">
-        <v>129.2446</v>
+        <v>269.1411</v>
       </c>
       <c r="E90" s="1" t="n">
         <f aca="false">ABS(C$103-C90)</f>
-        <v>533.8226</v>
+        <v>28.194566666667</v>
       </c>
       <c r="F90" s="1" t="n">
         <f aca="false">ABS(D$103-D90)</f>
-        <v>6.52286666666667</v>
+        <v>0.0605666666666593</v>
       </c>
       <c r="G90" s="0"/>
       <c r="H90" s="0"/>
@@ -3348,18 +3349,18 @@
         <v>3</v>
       </c>
       <c r="C91" s="1" t="n">
-        <v>1064.039</v>
+        <v>2750.0905</v>
       </c>
       <c r="D91" s="1" t="n">
-        <v>119.6984</v>
+        <v>269.3723</v>
       </c>
       <c r="E91" s="1" t="n">
         <f aca="false">ABS(C$103-C91)</f>
-        <v>1151.0965</v>
+        <v>27.0621666666671</v>
       </c>
       <c r="F91" s="1" t="n">
         <f aca="false">ABS(D$103-D91)</f>
-        <v>3.02333333333331</v>
+        <v>0.170633333333342</v>
       </c>
       <c r="G91" s="0"/>
       <c r="H91" s="0"/>
@@ -3388,7 +3389,7 @@
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="B94" s="0"/>
       <c r="C94" s="1" t="s">
@@ -3421,7 +3422,7 @@
       </c>
       <c r="D95" s="1" t="n">
         <f aca="false">AVERAGE(D65:D67)</f>
-        <v>12.5608666666667</v>
+        <v>100.773966666667</v>
       </c>
       <c r="E95" s="1" t="n">
         <f aca="false">AVERAGE(E65:E67)</f>
@@ -3429,15 +3430,15 @@
       </c>
       <c r="F95" s="1" t="n">
         <f aca="false">AVERAGE(F65:F67)</f>
-        <v>0.0216222222222224</v>
+        <v>0.741244444444443</v>
       </c>
       <c r="G95" s="1" t="n">
         <f aca="false">C95/D95</f>
-        <v>7.58831396984285</v>
+        <v>0.945837532775495</v>
       </c>
       <c r="H95" s="1" t="n">
         <f aca="false">ABS($G$58-G95)</f>
-        <v>1.4717027110323</v>
+        <v>8.11417914809965</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3451,7 +3452,7 @@
       </c>
       <c r="D96" s="1" t="n">
         <f aca="false">AVERAGE(D68:D70)</f>
-        <v>35.8525666666667</v>
+        <v>101.0867</v>
       </c>
       <c r="E96" s="1" t="n">
         <f aca="false">AVERAGE(E68:E70)</f>
@@ -3459,15 +3460,15 @@
       </c>
       <c r="F96" s="1" t="n">
         <f aca="false">AVERAGE(F68:F70)</f>
-        <v>0.231688888888887</v>
+        <v>0.385533333333337</v>
       </c>
       <c r="G96" s="1" t="n">
         <f aca="false">C96/D96</f>
-        <v>5.63708967372861</v>
+        <v>1.99931477962317</v>
       </c>
       <c r="H96" s="1" t="n">
         <f aca="false">ABS($G$58-G96)</f>
-        <v>3.42292700714653</v>
+        <v>7.06070190125198</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3481,7 +3482,7 @@
       </c>
       <c r="D97" s="1" t="n">
         <f aca="false">AVERAGE(D71:D73)</f>
-        <v>59.1203666666667</v>
+        <v>101.5467</v>
       </c>
       <c r="E97" s="1" t="n">
         <f aca="false">AVERAGE(E71:E73)</f>
@@ -3489,15 +3490,15 @@
       </c>
       <c r="F97" s="1" t="n">
         <f aca="false">AVERAGE(F71:F73)</f>
-        <v>0.155422222222221</v>
+        <v>0.762400000000004</v>
       </c>
       <c r="G97" s="1" t="n">
         <f aca="false">C97/D97</f>
-        <v>6.6212173920888</v>
+        <v>3.8548648060449</v>
       </c>
       <c r="H97" s="1" t="n">
         <f aca="false">ABS($G$58-G97)</f>
-        <v>2.43879928878635</v>
+        <v>5.20515187483024</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3511,7 +3512,7 @@
       </c>
       <c r="D98" s="1" t="n">
         <f aca="false">AVERAGE(D74:D76)</f>
-        <v>107.9521</v>
+        <v>100.624366666667</v>
       </c>
       <c r="E98" s="1" t="n">
         <f aca="false">AVERAGE(E74:E76)</f>
@@ -3519,15 +3520,15 @@
       </c>
       <c r="F98" s="1" t="n">
         <f aca="false">AVERAGE(F74:F76)</f>
-        <v>12.7876666666667</v>
+        <v>0.333444444444443</v>
       </c>
       <c r="G98" s="1" t="n">
         <f aca="false">C98/D98</f>
-        <v>6.06043359354133</v>
+        <v>6.50177044592579</v>
       </c>
       <c r="H98" s="1" t="n">
         <f aca="false">ABS($G$58-G98)</f>
-        <v>2.99958308733381</v>
+        <v>2.55824623494936</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3541,7 +3542,7 @@
       </c>
       <c r="D99" s="1" t="n">
         <f aca="false">AVERAGE(D77:D79)</f>
-        <v>122.721733333333</v>
+        <v>109.773533333333</v>
       </c>
       <c r="E99" s="1" t="n">
         <f aca="false">AVERAGE(E77:E79)</f>
@@ -3549,15 +3550,15 @@
       </c>
       <c r="F99" s="1" t="n">
         <f aca="false">AVERAGE(F77:F79)</f>
-        <v>4.34857777777777</v>
+        <v>0.0720222222222257</v>
       </c>
       <c r="G99" s="1" t="n">
         <f aca="false">C99/D99</f>
-        <v>8.14469401236184</v>
+        <v>9.10539122059173</v>
       </c>
       <c r="H99" s="1" t="n">
         <f aca="false">ABS($G$58-G99)</f>
-        <v>0.915322668513305</v>
+        <v>0.0453745397165797</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3567,27 +3568,27 @@
       <c r="B100" s="0"/>
       <c r="C100" s="1" t="n">
         <f aca="false">AVERAGE(C80:C82)</f>
-        <v>1095.24173333333</v>
+        <v>1248.27023333333</v>
       </c>
       <c r="D100" s="1" t="n">
         <f aca="false">AVERAGE(D80:D82)</f>
-        <v>122.721733333333</v>
+        <v>137.349933333333</v>
       </c>
       <c r="E100" s="1" t="n">
         <f aca="false">AVERAGE(E80:E82)</f>
-        <v>153.0285</v>
+        <v>5.49977777777781</v>
       </c>
       <c r="F100" s="1" t="n">
         <f aca="false">AVERAGE(F80:F82)</f>
-        <v>4.34857777777777</v>
+        <v>0.0654222222222245</v>
       </c>
       <c r="G100" s="1" t="n">
         <f aca="false">C100/D100</f>
-        <v>8.92459471997897</v>
+        <v>9.08824782829648</v>
       </c>
       <c r="H100" s="1" t="n">
         <f aca="false">ABS($G$58-G100)</f>
-        <v>0.135421960896181</v>
+        <v>0.0282311474213355</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3597,27 +3598,27 @@
       <c r="B101" s="0"/>
       <c r="C101" s="1" t="n">
         <f aca="false">AVERAGE(C83:C85)</f>
-        <v>1520.5326</v>
+        <v>1748.6073</v>
       </c>
       <c r="D101" s="1" t="n">
         <f aca="false">AVERAGE(D83:D85)</f>
-        <v>122.721733333333</v>
+        <v>169.533166666667</v>
       </c>
       <c r="E101" s="1" t="n">
         <f aca="false">AVERAGE(E83:E85)</f>
-        <v>304.329066666667</v>
+        <v>1.53266666666673</v>
       </c>
       <c r="F101" s="1" t="n">
         <f aca="false">AVERAGE(F83:F85)</f>
-        <v>4.34857777777777</v>
+        <v>0.160355555555554</v>
       </c>
       <c r="G101" s="1" t="n">
         <f aca="false">C101/D101</f>
-        <v>12.3900841252785</v>
+        <v>10.3142490309173</v>
       </c>
       <c r="H101" s="1" t="n">
         <f aca="false">ABS($G$58-G101)</f>
-        <v>3.3300674444034</v>
+        <v>1.25423235004211</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3627,27 +3628,27 @@
       <c r="B102" s="0"/>
       <c r="C102" s="1" t="n">
         <f aca="false">AVERAGE(C86:C88)</f>
-        <v>1874.58563333333</v>
+        <v>2279.89706666667</v>
       </c>
       <c r="D102" s="1" t="n">
         <f aca="false">AVERAGE(D86:D88)</f>
-        <v>122.721733333333</v>
+        <v>224.1383</v>
       </c>
       <c r="E102" s="1" t="n">
         <f aca="false">AVERAGE(E86:E88)</f>
-        <v>540.364422222222</v>
+        <v>1.17677777777787</v>
       </c>
       <c r="F102" s="1" t="n">
         <f aca="false">AVERAGE(F86:F88)</f>
-        <v>4.34857777777777</v>
+        <v>0.141800000000008</v>
       </c>
       <c r="G102" s="1" t="n">
         <f aca="false">C102/D102</f>
-        <v>15.2750909102762</v>
+        <v>10.1718317068822</v>
       </c>
       <c r="H102" s="1" t="n">
         <f aca="false">ABS($G$58-G102)</f>
-        <v>6.215074229401</v>
+        <v>1.11181502600702</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3657,27 +3658,27 @@
       <c r="B103" s="0"/>
       <c r="C103" s="1" t="n">
         <f aca="false">AVERAGE(C89:C91)</f>
-        <v>2215.1355</v>
+        <v>2777.15266666667</v>
       </c>
       <c r="D103" s="1" t="n">
         <f aca="false">AVERAGE(D89:D91)</f>
-        <v>122.721733333333</v>
+        <v>269.201666666667</v>
       </c>
       <c r="E103" s="1" t="n">
         <f aca="false">AVERAGE(E89:E91)</f>
-        <v>767.397666666667</v>
+        <v>36.8378222222224</v>
       </c>
       <c r="F103" s="1" t="n">
         <f aca="false">AVERAGE(F89:F91)</f>
-        <v>4.34857777777777</v>
+        <v>0.113755555555542</v>
       </c>
       <c r="G103" s="1" t="n">
         <f aca="false">C103/D103</f>
-        <v>18.0500669264776</v>
+        <v>10.3162536140811</v>
       </c>
       <c r="H103" s="1" t="n">
         <f aca="false">ABS($G$58-G103)</f>
-        <v>8.99005024560243</v>
+        <v>1.256236933206</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3687,11 +3688,11 @@
       <c r="D104" s="0"/>
       <c r="G104" s="1" t="n">
         <f aca="false">AVERAGE(G95:G99)</f>
-        <v>6.81034972831269</v>
+        <v>4.48143575699222</v>
       </c>
       <c r="H104" s="1" t="n">
         <f aca="false">AVERAGE(H95:H99)</f>
-        <v>2.24966695256246</v>
+        <v>4.59673073976956</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3715,7 +3716,7 @@
       </c>
       <c r="D106" s="1" t="n">
         <f aca="false">SLOPE(D95:D99,$A$95:$A$99)</f>
-        <v>1.11292773280133</v>
+        <v>0.0666212619749801</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3724,7 +3725,7 @@
       <c r="C107" s="7"/>
       <c r="D107" s="7" t="n">
         <f aca="false">C106/D106</f>
-        <v>7.72781084979304</v>
+        <v>129.095348145876</v>
       </c>
     </row>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -3791,7 +3792,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B2" s="0"/>
       <c r="C2" s="0"/>
@@ -3812,7 +3813,7 @@
         <v>3</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="C3" s="0"/>
       <c r="D3" s="0"/>
@@ -3821,10 +3822,10 @@
       <c r="G3" s="0"/>
       <c r="H3" s="0"/>
       <c r="I3" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="K3" s="0"/>
       <c r="L3" s="0"/>
@@ -3833,25 +3834,25 @@
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D4" s="0"/>
       <c r="E4" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G4" s="0"/>
       <c r="H4" s="0"/>
       <c r="I4" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="J4" s="1" t="n">
         <v>0.000234784733038</v>
@@ -3888,7 +3889,7 @@
       </c>
       <c r="H5" s="0"/>
       <c r="I5" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="J5" s="1" t="n">
         <v>0.000400919205276</v>
@@ -4081,10 +4082,10 @@
         <v>1.12E-005</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="G11" s="0"/>
       <c r="H11" s="0"/>
@@ -4611,19 +4612,19 @@
       </c>
       <c r="B32" s="2"/>
       <c r="C32" s="8" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D32" s="8"/>
       <c r="E32" s="9"/>
       <c r="F32" s="9"/>
       <c r="G32" s="10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H32" s="10"/>
       <c r="I32" s="9"/>
       <c r="J32" s="9"/>
       <c r="K32" s="11" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L32" s="11"/>
       <c r="M32" s="0"/>
@@ -4631,7 +4632,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>4</v>
@@ -4643,10 +4644,10 @@
         <v>16</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F33" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G33" s="13" t="s">
         <v>15</v>
@@ -4655,10 +4656,10 @@
         <v>16</v>
       </c>
       <c r="I33" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J33" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K33" s="14" t="s">
         <v>15</v>
@@ -4667,10 +4668,10 @@
         <v>16</v>
       </c>
       <c r="M33" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="N33" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6113,7 +6114,7 @@
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="1" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="B63" s="0"/>
       <c r="C63" s="12" t="s">
@@ -6687,28 +6688,28 @@
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="B75" s="0"/>
       <c r="C75" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="D75" s="12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="E75" s="0"/>
       <c r="F75" s="0"/>
       <c r="G75" s="13" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H75" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="K75" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="K75" s="14" t="s">
-        <v>42</v>
-      </c>
       <c r="L75" s="14" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7342,7 +7343,7 @@
         <v>5</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8396,25 +8397,25 @@
       </c>
       <c r="B1" s="2"/>
       <c r="C1" s="11" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D1" s="11"/>
       <c r="E1" s="9"/>
       <c r="F1" s="9"/>
       <c r="G1" s="10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="H1" s="10"/>
       <c r="I1" s="9"/>
       <c r="J1" s="9"/>
       <c r="K1" s="8" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="L1" s="8"/>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>4</v>
@@ -8426,10 +8427,10 @@
         <v>16</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="G2" s="13" t="s">
         <v>15</v>
@@ -8438,10 +8439,10 @@
         <v>16</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="K2" s="12" t="s">
         <v>15</v>
@@ -8450,10 +8451,10 @@
         <v>16</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9881,7 +9882,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>44</v>
+        <v>28</v>
       </c>
       <c r="C32" s="14" t="s">
         <v>15</v>
@@ -10443,27 +10444,27 @@
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="D44" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C44" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="D44" s="14" t="s">
+      <c r="G44" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G44" s="13" t="s">
-        <v>42</v>
-      </c>
       <c r="H44" s="13" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I44" s="1"/>
       <c r="J44" s="1"/>
       <c r="K44" s="12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="L44" s="12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="M44" s="1"/>
       <c r="N44" s="1"/>

</xml_diff>